<commit_message>
Updated data for 8Jun22 to include Salt River and Buck Island sites. Create updated KML
</commit_message>
<xml_diff>
--- a/Data/Genotype_Samples_2022.xlsx
+++ b/Data/Genotype_Samples_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4935" uniqueCount="1464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5374" uniqueCount="1597">
   <si>
     <t>Date</t>
   </si>
@@ -4301,6 +4301,405 @@
   </si>
   <si>
     <t>G1678</t>
+  </si>
+  <si>
+    <t>SRA_046</t>
+  </si>
+  <si>
+    <t>G1606</t>
+  </si>
+  <si>
+    <t>SRA_047</t>
+  </si>
+  <si>
+    <t>SRA_048</t>
+  </si>
+  <si>
+    <t>G1607</t>
+  </si>
+  <si>
+    <t>SRA_049</t>
+  </si>
+  <si>
+    <t>G1608</t>
+  </si>
+  <si>
+    <t>SRA_050</t>
+  </si>
+  <si>
+    <t>G1616</t>
+  </si>
+  <si>
+    <t>SRA_051</t>
+  </si>
+  <si>
+    <t>G1609</t>
+  </si>
+  <si>
+    <t>Disease; sampled from non diseased side</t>
+  </si>
+  <si>
+    <t>SRA_052</t>
+  </si>
+  <si>
+    <t>G1610</t>
+  </si>
+  <si>
+    <t>SRA_053</t>
+  </si>
+  <si>
+    <t>G1617</t>
+  </si>
+  <si>
+    <t>SRA_054</t>
+  </si>
+  <si>
+    <t>G1626</t>
+  </si>
+  <si>
+    <t>SRA_055</t>
+  </si>
+  <si>
+    <t>SRA_056</t>
+  </si>
+  <si>
+    <t>G1618</t>
+  </si>
+  <si>
+    <t>SRA_057</t>
+  </si>
+  <si>
+    <t>G1636</t>
+  </si>
+  <si>
+    <t>SRA_058</t>
+  </si>
+  <si>
+    <t>SRA_059</t>
+  </si>
+  <si>
+    <t>G1619</t>
+  </si>
+  <si>
+    <t>SRA_060</t>
+  </si>
+  <si>
+    <t>G1620</t>
+  </si>
+  <si>
+    <t>SRA_061</t>
+  </si>
+  <si>
+    <t>G1627</t>
+  </si>
+  <si>
+    <t>SRA_062</t>
+  </si>
+  <si>
+    <t>SRA_063</t>
+  </si>
+  <si>
+    <t>G1628</t>
+  </si>
+  <si>
+    <t>SRA_064</t>
+  </si>
+  <si>
+    <t>SRA_065</t>
+  </si>
+  <si>
+    <t>G1637</t>
+  </si>
+  <si>
+    <t>SRA_066</t>
+  </si>
+  <si>
+    <t>SRA_067</t>
+  </si>
+  <si>
+    <t>G1022</t>
+  </si>
+  <si>
+    <t>SRA_068</t>
+  </si>
+  <si>
+    <t>SRA_069</t>
+  </si>
+  <si>
+    <t>G1023</t>
+  </si>
+  <si>
+    <t>SRA_070</t>
+  </si>
+  <si>
+    <t>SRA_071</t>
+  </si>
+  <si>
+    <t>G1208</t>
+  </si>
+  <si>
+    <t>SRA_072</t>
+  </si>
+  <si>
+    <t>G1209</t>
+  </si>
+  <si>
+    <t>SRA_073</t>
+  </si>
+  <si>
+    <t>G1216</t>
+  </si>
+  <si>
+    <t>SRA_074</t>
+  </si>
+  <si>
+    <t>G1210</t>
+  </si>
+  <si>
+    <t>SRA_075</t>
+  </si>
+  <si>
+    <t>G1217</t>
+  </si>
+  <si>
+    <t>SRA_076</t>
+  </si>
+  <si>
+    <t>G1218</t>
+  </si>
+  <si>
+    <t>SRA_077</t>
+  </si>
+  <si>
+    <t>G1226</t>
+  </si>
+  <si>
+    <t>SRA_078</t>
+  </si>
+  <si>
+    <t>SRA_079</t>
+  </si>
+  <si>
+    <t>G1219</t>
+  </si>
+  <si>
+    <t>SRA_080</t>
+  </si>
+  <si>
+    <t>G1220</t>
+  </si>
+  <si>
+    <t>SRA_081</t>
+  </si>
+  <si>
+    <t>G1227</t>
+  </si>
+  <si>
+    <t>SRA_082</t>
+  </si>
+  <si>
+    <t>G1228</t>
+  </si>
+  <si>
+    <t>SRA_083</t>
+  </si>
+  <si>
+    <t>G1236</t>
+  </si>
+  <si>
+    <t>SRA_084</t>
+  </si>
+  <si>
+    <t>G1229</t>
+  </si>
+  <si>
+    <t>SRA_085</t>
+  </si>
+  <si>
+    <t>G1230</t>
+  </si>
+  <si>
+    <t>SRA_086</t>
+  </si>
+  <si>
+    <t>G1237</t>
+  </si>
+  <si>
+    <t>SRA_087</t>
+  </si>
+  <si>
+    <t>G1238</t>
+  </si>
+  <si>
+    <t>SRA_088</t>
+  </si>
+  <si>
+    <t>G1239</t>
+  </si>
+  <si>
+    <t>SRA_089</t>
+  </si>
+  <si>
+    <t>G1240</t>
+  </si>
+  <si>
+    <t>SRA_090</t>
+  </si>
+  <si>
+    <t>G1246</t>
+  </si>
+  <si>
+    <t>SRA_091</t>
+  </si>
+  <si>
+    <t>G1247</t>
+  </si>
+  <si>
+    <t>BIA_001</t>
+  </si>
+  <si>
+    <t>G1856</t>
+  </si>
+  <si>
+    <t>BIA_002</t>
+  </si>
+  <si>
+    <t>G1857</t>
+  </si>
+  <si>
+    <t>BIA_003</t>
+  </si>
+  <si>
+    <t>BIA_004</t>
+  </si>
+  <si>
+    <t>G1866</t>
+  </si>
+  <si>
+    <t>BIA_005</t>
+  </si>
+  <si>
+    <t>BIA_006</t>
+  </si>
+  <si>
+    <t>G1858</t>
+  </si>
+  <si>
+    <t>BIA_007</t>
+  </si>
+  <si>
+    <t>BIA_008</t>
+  </si>
+  <si>
+    <t>G1859</t>
+  </si>
+  <si>
+    <t>BIA_009</t>
+  </si>
+  <si>
+    <t>BIA_010</t>
+  </si>
+  <si>
+    <t>G1867</t>
+  </si>
+  <si>
+    <t>BIA_011</t>
+  </si>
+  <si>
+    <t>G1868</t>
+  </si>
+  <si>
+    <t>BIA_012</t>
+  </si>
+  <si>
+    <t>BIA_013</t>
+  </si>
+  <si>
+    <t>G1860</t>
+  </si>
+  <si>
+    <t>BIA_014</t>
+  </si>
+  <si>
+    <t>BIA_015</t>
+  </si>
+  <si>
+    <t>G1851</t>
+  </si>
+  <si>
+    <t>BIA_016</t>
+  </si>
+  <si>
+    <t>BIA_017</t>
+  </si>
+  <si>
+    <t>G1852</t>
+  </si>
+  <si>
+    <t>BIA_018</t>
+  </si>
+  <si>
+    <t>BIA_019</t>
+  </si>
+  <si>
+    <t>G1853</t>
+  </si>
+  <si>
+    <t>BIA_020</t>
+  </si>
+  <si>
+    <t>BIA_021</t>
+  </si>
+  <si>
+    <t>G1854</t>
+  </si>
+  <si>
+    <t>BIA_022</t>
+  </si>
+  <si>
+    <t>BIA_023</t>
+  </si>
+  <si>
+    <t>G1855</t>
+  </si>
+  <si>
+    <t>BIA_024</t>
+  </si>
+  <si>
+    <t>BIA_025</t>
+  </si>
+  <si>
+    <t>G1863</t>
+  </si>
+  <si>
+    <t>BIA_026</t>
+  </si>
+  <si>
+    <t>BIA_027</t>
+  </si>
+  <si>
+    <t>G1864</t>
+  </si>
+  <si>
+    <t>BIA_028</t>
+  </si>
+  <si>
+    <t>BIA_029</t>
+  </si>
+  <si>
+    <t>G1865</t>
+  </si>
+  <si>
+    <t>BIA_030</t>
+  </si>
+  <si>
+    <t>BIA_031</t>
+  </si>
+  <si>
+    <t>G1861</t>
+  </si>
+  <si>
+    <t>BIA_032</t>
   </si>
   <si>
     <t>Site_ID</t>
@@ -4819,9 +5218,8 @@
     <col customWidth="1" min="6" max="6" width="10.38"/>
     <col customWidth="1" min="7" max="7" width="7.88"/>
     <col customWidth="1" min="8" max="8" width="17.0"/>
-    <col customWidth="1" min="9" max="9" width="22.25"/>
-    <col customWidth="1" min="10" max="10" width="19.63"/>
-    <col customWidth="1" min="11" max="11" width="19.13"/>
+    <col customWidth="1" min="9" max="9" width="12.88"/>
+    <col customWidth="1" min="10" max="11" width="12.38"/>
     <col customWidth="1" min="12" max="12" width="12.0"/>
     <col customWidth="1" min="13" max="13" width="29.88"/>
     <col customWidth="1" min="14" max="14" width="19.25"/>
@@ -33971,238 +34369,2647 @@
       </c>
     </row>
     <row r="895">
-      <c r="A895" s="24"/>
+      <c r="A895" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B895" s="7" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C895" s="7" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D895" s="7">
+        <v>77.0</v>
+      </c>
+      <c r="E895" s="8">
+        <v>0.3506944444444444</v>
+      </c>
+      <c r="F895" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G895" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H895" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J895" s="11">
+        <v>17.7819174807519</v>
+      </c>
+      <c r="K895" s="11">
+        <v>-64.7565879207104</v>
+      </c>
+      <c r="M895" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="896">
-      <c r="A896" s="24"/>
+      <c r="A896" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B896" s="7" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C896" s="7" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D896" s="7">
+        <v>71.0</v>
+      </c>
+      <c r="E896" s="8">
+        <v>0.3506944444444444</v>
+      </c>
+      <c r="F896" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G896" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H896" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J896" s="11">
+        <v>17.7819174807519</v>
+      </c>
+      <c r="K896" s="11">
+        <v>-64.7565879207104</v>
+      </c>
+      <c r="M896" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="897">
-      <c r="A897" s="24"/>
+      <c r="A897" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B897" s="7" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C897" s="7" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D897" s="7">
+        <v>72.0</v>
+      </c>
+      <c r="E897" s="8">
+        <v>0.35555555555555557</v>
+      </c>
+      <c r="F897" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G897" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H897" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J897" s="11">
+        <v>17.7817620802671</v>
+      </c>
+      <c r="K897" s="11">
+        <v>-64.7563694883138</v>
+      </c>
     </row>
     <row r="898">
-      <c r="A898" s="24"/>
+      <c r="A898" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B898" s="7" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C898" s="7" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D898" s="7">
+        <v>74.0</v>
+      </c>
+      <c r="E898" s="8">
+        <v>0.3590277777777778</v>
+      </c>
+      <c r="F898" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G898" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H898" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J898" s="11">
+        <v>17.7817265409976</v>
+      </c>
+      <c r="K898" s="11">
+        <v>-64.7562093939632</v>
+      </c>
     </row>
     <row r="899">
-      <c r="A899" s="24"/>
+      <c r="A899" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B899" s="7" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C899" s="7" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D899" s="7">
+        <v>76.0</v>
+      </c>
+      <c r="E899" s="8">
+        <v>0.36319444444444443</v>
+      </c>
+      <c r="F899" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G899" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H899" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J899" s="11">
+        <v>17.7817099448293</v>
+      </c>
+      <c r="K899" s="11">
+        <v>-64.7562126629055</v>
+      </c>
     </row>
     <row r="900">
-      <c r="A900" s="24"/>
+      <c r="A900" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B900" s="7" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C900" s="7" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D900" s="7">
+        <v>82.0</v>
+      </c>
+      <c r="E900" s="8">
+        <v>0.36736111111111114</v>
+      </c>
+      <c r="F900" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G900" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H900" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J900" s="11">
+        <v>17.7816565521061</v>
+      </c>
+      <c r="K900" s="11">
+        <v>-64.7561439312994</v>
+      </c>
+      <c r="M900" s="7" t="s">
+        <v>1440</v>
+      </c>
     </row>
     <row r="901">
-      <c r="A901" s="24"/>
+      <c r="A901" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B901" s="7" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C901" s="7" t="s">
+        <v>1442</v>
+      </c>
+      <c r="D901" s="7">
+        <v>73.0</v>
+      </c>
+      <c r="E901" s="8">
+        <v>0.37083333333333335</v>
+      </c>
+      <c r="F901" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G901" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H901" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J901" s="11">
+        <v>17.7815993037075</v>
+      </c>
+      <c r="K901" s="11">
+        <v>-64.7560552507639</v>
+      </c>
     </row>
     <row r="902">
-      <c r="A902" s="24"/>
+      <c r="A902" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B902" s="7" t="s">
+        <v>1443</v>
+      </c>
+      <c r="C902" s="7" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D902" s="7">
+        <v>89.0</v>
+      </c>
+      <c r="E902" s="8">
+        <v>0.37430555555555556</v>
+      </c>
+      <c r="F902" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G902" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H902" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J902" s="11">
+        <v>17.7815461624414</v>
+      </c>
+      <c r="K902" s="11">
+        <v>-64.7560591902584</v>
+      </c>
     </row>
     <row r="903">
-      <c r="A903" s="24"/>
+      <c r="A903" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B903" s="7" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C903" s="7" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D903" s="7">
+        <v>88.0</v>
+      </c>
+      <c r="E903" s="8">
+        <v>0.3763888888888889</v>
+      </c>
+      <c r="F903" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G903" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H903" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J903" s="11">
+        <v>17.7814851421863</v>
+      </c>
+      <c r="K903" s="11">
+        <v>-64.7560161910951</v>
+      </c>
     </row>
     <row r="904">
-      <c r="A904" s="24"/>
+      <c r="A904" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B904" s="7" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C904" s="7" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D904" s="7">
+        <v>78.0</v>
+      </c>
+      <c r="E904" s="8">
+        <v>0.3763888888888889</v>
+      </c>
+      <c r="F904" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G904" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H904" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J904" s="11">
+        <v>17.7814851421863</v>
+      </c>
+      <c r="K904" s="11">
+        <v>-64.7560161910951</v>
+      </c>
+      <c r="M904" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="905">
-      <c r="A905" s="24"/>
+      <c r="A905" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B905" s="7" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C905" s="7" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D905" s="7">
+        <v>83.0</v>
+      </c>
+      <c r="E905" s="8">
+        <v>0.38125</v>
+      </c>
+      <c r="F905" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G905" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H905" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J905" s="11">
+        <v>17.7814946975559</v>
+      </c>
+      <c r="K905" s="11">
+        <v>-64.756076624617</v>
+      </c>
+      <c r="M905" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="906">
-      <c r="A906" s="24"/>
+      <c r="A906" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B906" s="7" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C906" s="7" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D906" s="7">
+        <v>81.0</v>
+      </c>
+      <c r="E906" s="8">
+        <v>0.3840277777777778</v>
+      </c>
+      <c r="F906" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G906" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H906" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J906" s="11">
+        <v>17.7814807835966</v>
+      </c>
+      <c r="K906" s="11">
+        <v>-64.7561170253903</v>
+      </c>
+      <c r="M906" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="907">
-      <c r="A907" s="24"/>
+      <c r="A907" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B907" s="7" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C907" s="7" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D907" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="E907" s="8">
+        <v>0.3840277777777778</v>
+      </c>
+      <c r="F907" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G907" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H907" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J907" s="11">
+        <v>17.7814807835966</v>
+      </c>
+      <c r="K907" s="11">
+        <v>-64.7561170253903</v>
+      </c>
+      <c r="M907" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="908">
-      <c r="A908" s="24"/>
+      <c r="A908" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B908" s="7" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C908" s="7" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D908" s="7">
+        <v>79.0</v>
+      </c>
+      <c r="E908" s="8">
+        <v>0.3875</v>
+      </c>
+      <c r="F908" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G908" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H908" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J908" s="11">
+        <v>17.7815262973309</v>
+      </c>
+      <c r="K908" s="11">
+        <v>-64.7561557497829</v>
+      </c>
     </row>
     <row r="909">
-      <c r="A909" s="24"/>
+      <c r="A909" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B909" s="7" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C909" s="7" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D909" s="7">
+        <v>87.0</v>
+      </c>
+      <c r="E909" s="8">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="F909" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G909" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H909" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J909" s="11">
+        <v>17.7815222740173</v>
+      </c>
+      <c r="K909" s="11">
+        <v>-64.7562963981181</v>
+      </c>
     </row>
     <row r="910">
-      <c r="A910" s="24"/>
+      <c r="A910" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B910" s="7" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C910" s="7" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D910" s="7">
+        <v>75.0</v>
+      </c>
+      <c r="E910" s="8">
+        <v>0.3951388888888889</v>
+      </c>
+      <c r="F910" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G910" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H910" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J910" s="11">
+        <v>17.7815523650497</v>
+      </c>
+      <c r="K910" s="11">
+        <v>-64.7562997508794</v>
+      </c>
+      <c r="M910" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="911">
-      <c r="A911" s="24"/>
+      <c r="A911" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B911" s="7" t="s">
+        <v>1459</v>
+      </c>
+      <c r="C911" s="7" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D911" s="7">
+        <v>84.0</v>
+      </c>
+      <c r="E911" s="8">
+        <v>0.3951388888888889</v>
+      </c>
+      <c r="F911" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G911" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H911" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J911" s="11">
+        <v>17.7815523650497</v>
+      </c>
+      <c r="K911" s="11">
+        <v>-64.7562997508794</v>
+      </c>
+      <c r="M911" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="912">
-      <c r="A912" s="24"/>
+      <c r="A912" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B912" s="7" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C912" s="7" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D912" s="7">
+        <v>85.0</v>
+      </c>
+      <c r="E912" s="8">
+        <v>0.3993055555555556</v>
+      </c>
+      <c r="F912" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G912" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H912" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J912" s="11">
+        <v>17.7816207613796</v>
+      </c>
+      <c r="K912" s="11">
+        <v>-64.756335625425</v>
+      </c>
+      <c r="M912" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="913">
-      <c r="A913" s="24"/>
+      <c r="A913" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B913" s="7" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C913" s="7" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D913" s="7">
+        <v>90.0</v>
+      </c>
+      <c r="E913" s="8">
+        <v>0.3993055555555556</v>
+      </c>
+      <c r="F913" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G913" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H913" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J913" s="11">
+        <v>17.7816207613796</v>
+      </c>
+      <c r="K913" s="11">
+        <v>-64.756335625425</v>
+      </c>
+      <c r="M913" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="914">
-      <c r="A914" s="24"/>
+      <c r="A914" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B914" s="7" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C914" s="7" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D914" s="7">
+        <v>86.0</v>
+      </c>
+      <c r="E914" s="8">
+        <v>0.40555555555555556</v>
+      </c>
+      <c r="F914" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G914" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H914" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J914" s="11">
+        <v>17.7816595695913</v>
+      </c>
+      <c r="K914" s="11">
+        <v>-64.7564747650176</v>
+      </c>
+      <c r="M914" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="915">
-      <c r="A915" s="24"/>
+      <c r="A915" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B915" s="7" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C915" s="7" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D915" s="7">
+        <v>51.0</v>
+      </c>
+      <c r="E915" s="8">
+        <v>0.40555555555555556</v>
+      </c>
+      <c r="F915" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G915" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H915" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J915" s="11">
+        <v>17.7816595695913</v>
+      </c>
+      <c r="K915" s="11">
+        <v>-64.7564747650176</v>
+      </c>
+      <c r="M915" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="916">
-      <c r="A916" s="24"/>
+      <c r="A916" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B916" s="7" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C916" s="7" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D916" s="7">
+        <v>25.0</v>
+      </c>
+      <c r="E916" s="8">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="F916" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G916" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H916" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J916" s="11">
+        <v>17.7817656006664</v>
+      </c>
+      <c r="K916" s="11">
+        <v>-64.7563759423792</v>
+      </c>
+      <c r="M916" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="917">
-      <c r="A917" s="24"/>
+      <c r="A917" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B917" s="7" t="s">
+        <v>1468</v>
+      </c>
+      <c r="C917" s="7" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D917" s="7">
+        <v>24.0</v>
+      </c>
+      <c r="E917" s="8">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="F917" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G917" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H917" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J917" s="11">
+        <v>17.7817656006664</v>
+      </c>
+      <c r="K917" s="11">
+        <v>-64.7563759423792</v>
+      </c>
+      <c r="M917" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="918">
-      <c r="A918" s="24"/>
+      <c r="A918" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B918" s="7" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C918" s="7" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D918" s="7">
+        <v>15.0</v>
+      </c>
+      <c r="E918" s="8">
+        <v>0.35625</v>
+      </c>
+      <c r="F918" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G918" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H918" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J918" s="11">
+        <v>17.7817426342517</v>
+      </c>
+      <c r="K918" s="11">
+        <v>-64.7563581727445</v>
+      </c>
+      <c r="M918" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="919">
-      <c r="A919" s="24"/>
+      <c r="A919" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B919" s="7" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C919" s="7" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D919" s="7">
+        <v>23.0</v>
+      </c>
+      <c r="E919" s="8">
+        <v>0.35625</v>
+      </c>
+      <c r="F919" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G919" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H919" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J919" s="11">
+        <v>17.7817426342517</v>
+      </c>
+      <c r="K919" s="11">
+        <v>-64.7563581727445</v>
+      </c>
+      <c r="M919" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="920">
-      <c r="A920" s="24"/>
+      <c r="A920" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B920" s="7" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C920" s="7" t="s">
+        <v>1473</v>
+      </c>
+      <c r="D920" s="7">
+        <v>22.0</v>
+      </c>
+      <c r="E920" s="8">
+        <v>0.36319444444444443</v>
+      </c>
+      <c r="F920" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G920" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H920" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J920" s="11">
+        <v>17.7817099448293</v>
+      </c>
+      <c r="K920" s="11">
+        <v>-64.7562126629055</v>
+      </c>
     </row>
     <row r="921">
-      <c r="A921" s="24"/>
+      <c r="A921" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B921" s="7" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C921" s="7" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D921" s="7">
+        <v>32.0</v>
+      </c>
+      <c r="E921" s="8">
+        <v>0.36736111111111114</v>
+      </c>
+      <c r="F921" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G921" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H921" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J921" s="11">
+        <v>17.7816565521061</v>
+      </c>
+      <c r="K921" s="11">
+        <v>-64.7561439312994</v>
+      </c>
     </row>
     <row r="922">
-      <c r="A922" s="24"/>
+      <c r="A922" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B922" s="7" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C922" s="7" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D922" s="7">
+        <v>21.0</v>
+      </c>
+      <c r="E922" s="8">
+        <v>0.3701388888888889</v>
+      </c>
+      <c r="F922" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G922" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H922" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J922" s="11">
+        <v>17.7816057577729</v>
+      </c>
+      <c r="K922" s="11">
+        <v>-64.7560409177095</v>
+      </c>
     </row>
     <row r="923">
-      <c r="A923" s="24"/>
+      <c r="A923" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B923" s="7" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C923" s="7" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D923" s="7">
+        <v>20.0</v>
+      </c>
+      <c r="E923" s="8">
+        <v>0.3729166666666667</v>
+      </c>
+      <c r="F923" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G923" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H923" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J923" s="11">
+        <v>17.7815495990217</v>
+      </c>
+      <c r="K923" s="11">
+        <v>-64.7560643032193</v>
+      </c>
     </row>
     <row r="924">
-      <c r="A924" s="24"/>
+      <c r="A924" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B924" s="7" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C924" s="7" t="s">
+        <v>1481</v>
+      </c>
+      <c r="D924" s="7">
+        <v>19.0</v>
+      </c>
+      <c r="E924" s="8">
+        <v>0.37430555555555556</v>
+      </c>
+      <c r="F924" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G924" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H924" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J924" s="11">
+        <v>17.7815461624414</v>
+      </c>
+      <c r="K924" s="11">
+        <v>-64.7560591902584</v>
+      </c>
     </row>
     <row r="925">
-      <c r="A925" s="24"/>
+      <c r="A925" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B925" s="7" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C925" s="7" t="s">
+        <v>1483</v>
+      </c>
+      <c r="D925" s="7">
+        <v>18.0</v>
+      </c>
+      <c r="E925" s="8">
+        <v>0.37569444444444444</v>
+      </c>
+      <c r="F925" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G925" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H925" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J925" s="11">
+        <v>17.7815184183419</v>
+      </c>
+      <c r="K925" s="11">
+        <v>-64.7560270037502</v>
+      </c>
     </row>
     <row r="926">
-      <c r="A926" s="24"/>
+      <c r="A926" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B926" s="7" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C926" s="7" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D926" s="7">
+        <v>16.0</v>
+      </c>
+      <c r="E926" s="8">
+        <v>0.3784722222222222</v>
+      </c>
+      <c r="F926" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G926" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H926" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J926" s="11">
+        <v>17.7814824599773</v>
+      </c>
+      <c r="K926" s="11">
+        <v>-64.7560669854283</v>
+      </c>
+      <c r="M926" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="927">
-      <c r="A927" s="24"/>
+      <c r="A927" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B927" s="7" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C927" s="7" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D927" s="7">
+        <v>17.0</v>
+      </c>
+      <c r="E927" s="8">
+        <v>0.3784722222222222</v>
+      </c>
+      <c r="F927" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G927" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H927" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J927" s="11">
+        <v>17.7814824599773</v>
+      </c>
+      <c r="K927" s="11">
+        <v>-64.7560669854283</v>
+      </c>
+      <c r="M927" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="928">
-      <c r="A928" s="24"/>
+      <c r="A928" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B928" s="7" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C928" s="7" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D928" s="7">
+        <v>14.0</v>
+      </c>
+      <c r="E928" s="8">
+        <v>0.38125</v>
+      </c>
+      <c r="F928" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G928" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H928" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J928" s="11">
+        <v>17.7814946975559</v>
+      </c>
+      <c r="K928" s="11">
+        <v>-64.756076624617</v>
+      </c>
     </row>
     <row r="929">
-      <c r="A929" s="24"/>
+      <c r="A929" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B929" s="7" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C929" s="7" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D929" s="7">
+        <v>13.0</v>
+      </c>
+      <c r="E929" s="8">
+        <v>0.38333333333333336</v>
+      </c>
+      <c r="F929" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G929" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H929" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J929" s="11">
+        <v>17.7814743295312</v>
+      </c>
+      <c r="K929" s="11">
+        <v>-64.7561107389629</v>
+      </c>
     </row>
     <row r="930">
-      <c r="A930" s="24"/>
+      <c r="A930" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B930" s="7" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C930" s="7" t="s">
+        <v>1492</v>
+      </c>
+      <c r="D930" s="7">
+        <v>12.0</v>
+      </c>
+      <c r="E930" s="8">
+        <v>0.3840277777777778</v>
+      </c>
+      <c r="F930" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G930" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H930" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J930" s="11">
+        <v>17.7814807835966</v>
+      </c>
+      <c r="K930" s="11">
+        <v>-64.7561170253903</v>
+      </c>
     </row>
     <row r="931">
-      <c r="A931" s="24"/>
+      <c r="A931" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B931" s="7" t="s">
+        <v>1493</v>
+      </c>
+      <c r="C931" s="7" t="s">
+        <v>1494</v>
+      </c>
+      <c r="D931" s="7">
+        <v>11.0</v>
+      </c>
+      <c r="E931" s="8">
+        <v>0.3875</v>
+      </c>
+      <c r="F931" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G931" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H931" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J931" s="11">
+        <v>17.7815262973309</v>
+      </c>
+      <c r="K931" s="11">
+        <v>-64.7561557497829</v>
+      </c>
     </row>
     <row r="932">
-      <c r="A932" s="24"/>
+      <c r="A932" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B932" s="7" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C932" s="7" t="s">
+        <v>1496</v>
+      </c>
+      <c r="D932" s="7">
+        <v>10.0</v>
+      </c>
+      <c r="E932" s="8">
+        <v>0.38958333333333334</v>
+      </c>
+      <c r="F932" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G932" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H932" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J932" s="11">
+        <v>17.7815435640514</v>
+      </c>
+      <c r="K932" s="11">
+        <v>-64.7561756987125</v>
+      </c>
     </row>
     <row r="933">
-      <c r="A933" s="24"/>
+      <c r="A933" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B933" s="7" t="s">
+        <v>1497</v>
+      </c>
+      <c r="C933" s="7" t="s">
+        <v>1498</v>
+      </c>
+      <c r="D933" s="7">
+        <v>9.0</v>
+      </c>
+      <c r="E933" s="8">
+        <v>0.3909722222222222</v>
+      </c>
+      <c r="F933" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G933" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H933" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J933" s="11">
+        <v>17.7814968768507</v>
+      </c>
+      <c r="K933" s="11">
+        <v>-64.7562160156667</v>
+      </c>
     </row>
     <row r="934">
-      <c r="A934" s="24"/>
+      <c r="A934" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B934" s="7" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C934" s="7" t="s">
+        <v>1500</v>
+      </c>
+      <c r="D934" s="7">
+        <v>8.0</v>
+      </c>
+      <c r="E934" s="8">
+        <v>0.39375</v>
+      </c>
+      <c r="F934" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G934" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H934" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J934" s="11">
+        <v>17.781553119421</v>
+      </c>
+      <c r="K934" s="11">
+        <v>-64.7563174366951</v>
+      </c>
     </row>
     <row r="935">
-      <c r="A935" s="24"/>
+      <c r="A935" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B935" s="7" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C935" s="7" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D935" s="7">
+        <v>7.0</v>
+      </c>
+      <c r="E935" s="8">
+        <v>0.3951388888888889</v>
+      </c>
+      <c r="F935" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G935" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H935" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J935" s="11">
+        <v>17.7815523650497</v>
+      </c>
+      <c r="K935" s="11">
+        <v>-64.7562997508794</v>
+      </c>
     </row>
     <row r="936">
-      <c r="A936" s="24"/>
+      <c r="A936" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B936" s="7" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C936" s="7" t="s">
+        <v>1504</v>
+      </c>
+      <c r="D936" s="7">
+        <v>43.0</v>
+      </c>
+      <c r="E936" s="8">
+        <v>0.39791666666666664</v>
+      </c>
+      <c r="F936" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G936" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H936" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J936" s="11">
+        <v>17.7816149778664</v>
+      </c>
+      <c r="K936" s="11">
+        <v>-64.7563520539552</v>
+      </c>
     </row>
     <row r="937">
-      <c r="A937" s="24"/>
+      <c r="A937" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B937" s="7" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C937" s="7" t="s">
+        <v>1506</v>
+      </c>
+      <c r="D937" s="7">
+        <v>6.0</v>
+      </c>
+      <c r="E937" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="F937" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G937" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H937" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J937" s="11">
+        <v>17.7816146425903</v>
+      </c>
+      <c r="K937" s="11">
+        <v>-64.7563414089382</v>
+      </c>
     </row>
     <row r="938">
-      <c r="A938" s="24"/>
+      <c r="A938" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B938" s="7" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C938" s="7" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D938" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="E938" s="8">
+        <v>0.4027777777777778</v>
+      </c>
+      <c r="F938" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G938" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H938" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J938" s="11">
+        <v>17.7816606592387</v>
+      </c>
+      <c r="K938" s="11">
+        <v>-64.7564590070397</v>
+      </c>
     </row>
     <row r="939">
-      <c r="A939" s="24"/>
+      <c r="A939" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B939" s="7" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C939" s="7" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D939" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="E939" s="8">
+        <v>0.40625</v>
+      </c>
+      <c r="F939" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G939" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H939" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J939" s="11">
+        <v>17.7816710527986</v>
+      </c>
+      <c r="K939" s="11">
+        <v>-64.7565150819719</v>
+      </c>
     </row>
     <row r="940">
-      <c r="A940" s="24"/>
+      <c r="A940" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B940" s="7" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C940" s="7" t="s">
+        <v>1512</v>
+      </c>
+      <c r="D940" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="E940" s="8">
+        <v>0.4083333333333333</v>
+      </c>
+      <c r="F940" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G940" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H940" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J940" s="11">
+        <v>17.7817664388567</v>
+      </c>
+      <c r="K940" s="11">
+        <v>-64.7566398046911</v>
+      </c>
     </row>
     <row r="941">
-      <c r="A941" s="24"/>
+      <c r="A941" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B941" s="7" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C941" s="7" t="s">
+        <v>1514</v>
+      </c>
+      <c r="D941" s="7">
+        <v>73.0</v>
+      </c>
+      <c r="E941" s="8">
+        <v>0.63125</v>
+      </c>
+      <c r="F941" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G941" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H941" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J941" s="11">
+        <v>17.7872969862074</v>
+      </c>
+      <c r="K941" s="11">
+        <v>-64.6095775533468</v>
+      </c>
     </row>
     <row r="942">
-      <c r="A942" s="24"/>
+      <c r="A942" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B942" s="7" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C942" s="7" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D942" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="E942" s="8">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="F942" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G942" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H942" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J942" s="11">
+        <v>17.7872059587389</v>
+      </c>
+      <c r="K942" s="11">
+        <v>-64.6095987595618</v>
+      </c>
+      <c r="M942" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="943">
-      <c r="A943" s="24"/>
+      <c r="A943" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B943" s="7" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C943" s="7" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D943" s="7">
+        <v>85.0</v>
+      </c>
+      <c r="E943" s="8">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="F943" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G943" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H943" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J943" s="11">
+        <v>17.7872059587389</v>
+      </c>
+      <c r="K943" s="11">
+        <v>-64.6095987595618</v>
+      </c>
+      <c r="M943" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="944">
-      <c r="A944" s="24"/>
+      <c r="A944" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B944" s="7" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C944" s="7" t="s">
+        <v>1519</v>
+      </c>
+      <c r="D944" s="7">
+        <v>90.0</v>
+      </c>
+      <c r="E944" s="8">
+        <v>0.6375</v>
+      </c>
+      <c r="F944" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G944" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H944" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J944" s="11">
+        <v>17.7871865127236</v>
+      </c>
+      <c r="K944" s="11">
+        <v>-64.6095527429134</v>
+      </c>
+      <c r="M944" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="945">
-      <c r="A945" s="24"/>
+      <c r="A945" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B945" s="7" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C945" s="7" t="s">
+        <v>1519</v>
+      </c>
+      <c r="D945" s="7">
+        <v>88.0</v>
+      </c>
+      <c r="E945" s="8">
+        <v>0.6375</v>
+      </c>
+      <c r="F945" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G945" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H945" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J945" s="11">
+        <v>17.7871865127236</v>
+      </c>
+      <c r="K945" s="11">
+        <v>-64.6095527429134</v>
+      </c>
+      <c r="M945" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="946">
-      <c r="A946" s="24"/>
+      <c r="A946" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B946" s="7" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C946" s="7" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D946" s="7">
+        <v>72.0</v>
+      </c>
+      <c r="E946" s="8">
+        <v>0.6423611111111112</v>
+      </c>
+      <c r="F946" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G946" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H946" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J946" s="11">
+        <v>17.7870855946094</v>
+      </c>
+      <c r="K946" s="11">
+        <v>-64.6095788944513</v>
+      </c>
+      <c r="M946" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="947">
-      <c r="A947" s="24"/>
+      <c r="A947" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B947" s="7" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C947" s="7" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D947" s="7">
+        <v>77.0</v>
+      </c>
+      <c r="E947" s="8">
+        <v>0.6423611111111112</v>
+      </c>
+      <c r="F947" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G947" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H947" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J947" s="11">
+        <v>17.7870855946094</v>
+      </c>
+      <c r="K947" s="11">
+        <v>-64.6095788944513</v>
+      </c>
+      <c r="M947" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="948">
-      <c r="A948" s="24"/>
+      <c r="A948" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B948" s="7" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C948" s="7" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D948" s="7">
+        <v>81.0</v>
+      </c>
+      <c r="E948" s="8">
+        <v>0.6465277777777778</v>
+      </c>
+      <c r="F948" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G948" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H948" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J948" s="11">
+        <v>17.7869964111596</v>
+      </c>
+      <c r="K948" s="11">
+        <v>-64.6094797365367</v>
+      </c>
+      <c r="M948" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="949">
-      <c r="A949" s="24"/>
+      <c r="A949" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B949" s="7" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C949" s="7" t="s">
+        <v>1525</v>
+      </c>
+      <c r="D949" s="7">
+        <v>84.0</v>
+      </c>
+      <c r="E949" s="8">
+        <v>0.6465277777777778</v>
+      </c>
+      <c r="F949" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G949" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H949" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J949" s="11">
+        <v>17.7869964111596</v>
+      </c>
+      <c r="K949" s="11">
+        <v>-64.6094797365367</v>
+      </c>
+      <c r="M949" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="950">
-      <c r="A950" s="24"/>
+      <c r="A950" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B950" s="7" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C950" s="7" t="s">
+        <v>1528</v>
+      </c>
+      <c r="D950" s="7">
+        <v>79.0</v>
+      </c>
+      <c r="E950" s="8">
+        <v>0.6513888888888889</v>
+      </c>
+      <c r="F950" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G950" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H950" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J950" s="11">
+        <v>17.7869213093072</v>
+      </c>
+      <c r="K950" s="11">
+        <v>-64.6095244958997</v>
+      </c>
     </row>
     <row r="951">
-      <c r="A951" s="24"/>
+      <c r="A951" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B951" s="7" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C951" s="7" t="s">
+        <v>1530</v>
+      </c>
+      <c r="D951" s="7">
+        <v>71.0</v>
+      </c>
+      <c r="E951" s="8">
+        <v>0.6548611111111111</v>
+      </c>
+      <c r="F951" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G951" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H951" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J951" s="11">
+        <v>17.7868501469493</v>
+      </c>
+      <c r="K951" s="11">
+        <v>-64.6096182055771</v>
+      </c>
+      <c r="M951" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="952">
-      <c r="A952" s="24"/>
+      <c r="A952" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B952" s="7" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C952" s="7" t="s">
+        <v>1530</v>
+      </c>
+      <c r="D952" s="7">
+        <v>75.0</v>
+      </c>
+      <c r="E952" s="8">
+        <v>0.6548611111111111</v>
+      </c>
+      <c r="F952" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G952" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H952" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J952" s="11">
+        <v>17.7868501469493</v>
+      </c>
+      <c r="K952" s="11">
+        <v>-64.6096182055771</v>
+      </c>
+      <c r="M952" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="953">
-      <c r="A953" s="24"/>
+      <c r="A953" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B953" s="7" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C953" s="7" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D953" s="7">
+        <v>76.0</v>
+      </c>
+      <c r="E953" s="8">
+        <v>0.6604166666666667</v>
+      </c>
+      <c r="F953" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G953" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H953" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J953" s="11">
+        <v>17.7867736201733</v>
+      </c>
+      <c r="K953" s="11">
+        <v>-64.6096846740693</v>
+      </c>
+      <c r="M953" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="954">
-      <c r="A954" s="24"/>
+      <c r="A954" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B954" s="7" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C954" s="7" t="s">
+        <v>1533</v>
+      </c>
+      <c r="D954" s="7">
+        <v>86.0</v>
+      </c>
+      <c r="E954" s="8">
+        <v>0.6604166666666667</v>
+      </c>
+      <c r="F954" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G954" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H954" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J954" s="11">
+        <v>17.7867736201733</v>
+      </c>
+      <c r="K954" s="11">
+        <v>-64.6096846740693</v>
+      </c>
+      <c r="M954" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="955">
-      <c r="A955" s="24"/>
+      <c r="A955" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B955" s="7" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C955" s="7" t="s">
+        <v>1536</v>
+      </c>
+      <c r="D955" s="7">
+        <v>36.0</v>
+      </c>
+      <c r="E955" s="8">
+        <v>0.6340277777777777</v>
+      </c>
+      <c r="F955" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G955" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H955" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J955" s="11">
+        <v>17.787216771394</v>
+      </c>
+      <c r="K955" s="11">
+        <v>-64.609633795917</v>
+      </c>
+      <c r="M955" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="956">
-      <c r="A956" s="24"/>
+      <c r="A956" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B956" s="7" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C956" s="7" t="s">
+        <v>1536</v>
+      </c>
+      <c r="D956" s="7">
+        <v>47.0</v>
+      </c>
+      <c r="E956" s="8">
+        <v>0.6340277777777777</v>
+      </c>
+      <c r="F956" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G956" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H956" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J956" s="11">
+        <v>17.787216771394</v>
+      </c>
+      <c r="K956" s="11">
+        <v>-64.609633795917</v>
+      </c>
+      <c r="M956" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="957">
-      <c r="A957" s="24"/>
+      <c r="A957" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B957" s="7" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C957" s="7" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D957" s="7">
+        <v>49.0</v>
+      </c>
+      <c r="E957" s="8">
+        <v>0.6368055555555555</v>
+      </c>
+      <c r="F957" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G957" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H957" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J957" s="11">
+        <v>17.7871963195503</v>
+      </c>
+      <c r="K957" s="11">
+        <v>-64.6096187923104</v>
+      </c>
+      <c r="M957" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="958">
-      <c r="A958" s="24"/>
+      <c r="A958" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B958" s="7" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C958" s="7" t="s">
+        <v>1539</v>
+      </c>
+      <c r="D958" s="7">
+        <v>35.0</v>
+      </c>
+      <c r="E958" s="8">
+        <v>0.6368055555555555</v>
+      </c>
+      <c r="F958" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G958" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H958" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J958" s="11">
+        <v>17.7871963195503</v>
+      </c>
+      <c r="K958" s="11">
+        <v>-64.6096187923104</v>
+      </c>
+      <c r="M958" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="959">
-      <c r="A959" s="24"/>
+      <c r="A959" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B959" s="7" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C959" s="7" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D959" s="7">
+        <v>41.0</v>
+      </c>
+      <c r="E959" s="8">
+        <v>0.6416666666666667</v>
+      </c>
+      <c r="F959" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G959" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H959" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J959" s="11">
+        <v>17.7870947308838</v>
+      </c>
+      <c r="K959" s="11">
+        <v>-64.6096144337207</v>
+      </c>
+      <c r="M959" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="960">
-      <c r="A960" s="24"/>
+      <c r="A960" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B960" s="7" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C960" s="7" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D960" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="E960" s="8">
+        <v>0.6416666666666667</v>
+      </c>
+      <c r="F960" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G960" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H960" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J960" s="11">
+        <v>17.7870947308838</v>
+      </c>
+      <c r="K960" s="11">
+        <v>-64.6096144337207</v>
+      </c>
+      <c r="M960" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="961">
-      <c r="A961" s="24"/>
+      <c r="A961" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B961" s="7" t="s">
+        <v>1544</v>
+      </c>
+      <c r="C961" s="7" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D961" s="7">
+        <v>44.0</v>
+      </c>
+      <c r="E961" s="8">
+        <v>0.6465277777777778</v>
+      </c>
+      <c r="F961" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G961" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H961" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J961" s="11">
+        <v>17.7869964111596</v>
+      </c>
+      <c r="K961" s="11">
+        <v>-64.6094797365367</v>
+      </c>
+      <c r="M961" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="962">
-      <c r="A962" s="24"/>
+      <c r="A962" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B962" s="7" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C962" s="7" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D962" s="7">
+        <v>29.0</v>
+      </c>
+      <c r="E962" s="8">
+        <v>0.6465277777777778</v>
+      </c>
+      <c r="F962" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G962" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H962" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J962" s="11">
+        <v>17.7869964111596</v>
+      </c>
+      <c r="K962" s="11">
+        <v>-64.6094797365367</v>
+      </c>
+      <c r="M962" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="963">
-      <c r="A963" s="24"/>
+      <c r="A963" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B963" s="7" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C963" s="7" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D963" s="7">
+        <v>39.0</v>
+      </c>
+      <c r="E963" s="8">
+        <v>0.6493055555555556</v>
+      </c>
+      <c r="F963" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G963" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H963" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J963" s="11">
+        <v>17.786920806393</v>
+      </c>
+      <c r="K963" s="11">
+        <v>-64.6095093246549</v>
+      </c>
+      <c r="M963" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="964">
-      <c r="A964" s="24"/>
+      <c r="A964" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B964" s="7" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C964" s="7" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D964" s="7">
+        <v>34.0</v>
+      </c>
+      <c r="E964" s="8">
+        <v>0.6493055555555556</v>
+      </c>
+      <c r="F964" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G964" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H964" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J964" s="11">
+        <v>17.786920806393</v>
+      </c>
+      <c r="K964" s="11">
+        <v>-64.6095093246549</v>
+      </c>
+      <c r="M964" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="965">
-      <c r="A965" s="24"/>
+      <c r="A965" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B965" s="7" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C965" s="7" t="s">
+        <v>1551</v>
+      </c>
+      <c r="D965" s="7">
+        <v>42.0</v>
+      </c>
+      <c r="E965" s="8">
+        <v>0.6520833333333333</v>
+      </c>
+      <c r="F965" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G965" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H965" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J965" s="11">
+        <v>17.7869192138314</v>
+      </c>
+      <c r="K965" s="11">
+        <v>-64.609570261091</v>
+      </c>
+      <c r="M965" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="966">
-      <c r="A966" s="24"/>
+      <c r="A966" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B966" s="7" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C966" s="7" t="s">
+        <v>1551</v>
+      </c>
+      <c r="D966" s="7">
+        <v>28.0</v>
+      </c>
+      <c r="E966" s="8">
+        <v>0.6520833333333333</v>
+      </c>
+      <c r="F966" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G966" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H966" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J966" s="11">
+        <v>17.7869192138314</v>
+      </c>
+      <c r="K966" s="11">
+        <v>-64.609570261091</v>
+      </c>
+      <c r="M966" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="967">
-      <c r="A967" s="24"/>
+      <c r="A967" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B967" s="7" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C967" s="7" t="s">
+        <v>1554</v>
+      </c>
+      <c r="D967" s="7">
+        <v>48.0</v>
+      </c>
+      <c r="E967" s="8">
+        <v>0.6541666666666667</v>
+      </c>
+      <c r="F967" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G967" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H967" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J967" s="11">
+        <v>17.786907395348</v>
+      </c>
+      <c r="K967" s="11">
+        <v>-64.6095876954496</v>
+      </c>
+      <c r="M967" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="968">
-      <c r="A968" s="24"/>
+      <c r="A968" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B968" s="7" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C968" s="7" t="s">
+        <v>1554</v>
+      </c>
+      <c r="D968" s="7">
+        <v>46.0</v>
+      </c>
+      <c r="E968" s="8">
+        <v>0.6541666666666667</v>
+      </c>
+      <c r="F968" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G968" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H968" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J968" s="11">
+        <v>17.786907395348</v>
+      </c>
+      <c r="K968" s="11">
+        <v>-64.6095876954496</v>
+      </c>
+      <c r="M968" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="969">
-      <c r="A969" s="24"/>
+      <c r="A969" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B969" s="7" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C969" s="7" t="s">
+        <v>1557</v>
+      </c>
+      <c r="D969" s="7">
+        <v>37.0</v>
+      </c>
+      <c r="E969" s="8">
+        <v>0.6583333333333333</v>
+      </c>
+      <c r="F969" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G969" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H969" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J969" s="11">
+        <v>17.7867669984698</v>
+      </c>
+      <c r="K969" s="11">
+        <v>-64.6096779685467</v>
+      </c>
+      <c r="M969" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="970">
-      <c r="A970" s="24"/>
+      <c r="A970" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B970" s="7" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C970" s="7" t="s">
+        <v>1557</v>
+      </c>
+      <c r="D970" s="7">
+        <v>45.0</v>
+      </c>
+      <c r="E970" s="8">
+        <v>0.6583333333333333</v>
+      </c>
+      <c r="F970" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G970" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H970" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J970" s="11">
+        <v>17.7867669984698</v>
+      </c>
+      <c r="K970" s="11">
+        <v>-64.6096779685467</v>
+      </c>
+      <c r="M970" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="971">
-      <c r="A971" s="24"/>
+      <c r="A971" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B971" s="7" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C971" s="7" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D971" s="7">
+        <v>27.0</v>
+      </c>
+      <c r="E971" s="8">
+        <v>0.6611111111111111</v>
+      </c>
+      <c r="F971" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G971" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H971" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J971" s="11">
+        <v>17.7867658250034</v>
+      </c>
+      <c r="K971" s="11">
+        <v>-64.6096836682409</v>
+      </c>
+      <c r="M971" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="972">
-      <c r="A972" s="24"/>
+      <c r="A972" s="6">
+        <v>44719.0</v>
+      </c>
+      <c r="B972" s="7" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C972" s="7" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D972" s="7">
+        <v>30.0</v>
+      </c>
+      <c r="E972" s="8">
+        <v>0.6611111111111111</v>
+      </c>
+      <c r="F972" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G972" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H972" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J972" s="11">
+        <v>17.7867658250034</v>
+      </c>
+      <c r="K972" s="11">
+        <v>-64.6096836682409</v>
+      </c>
+      <c r="M972" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="973">
       <c r="A973" s="24"/>
@@ -34305,19 +37112,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>1429</v>
+        <v>1562</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>1430</v>
+        <v>1563</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>1431</v>
+        <v>1564</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>1432</v>
+        <v>1565</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>1433</v>
+        <v>1566</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>7</v>
@@ -34341,21 +37148,21 @@
         <v>51</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>1434</v>
+        <v>1567</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>145</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>1435</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>1436</v>
+        <v>1569</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1437</v>
+        <v>1570</v>
       </c>
       <c r="C2" s="7">
         <v>7.0</v>
@@ -34367,33 +37174,33 @@
         <v>44688.0</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>1438</v>
+        <v>1571</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>1438</v>
+        <v>1571</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>1438</v>
+        <v>1571</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>1438</v>
+        <v>1571</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>1438</v>
+        <v>1571</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>1439</v>
+        <v>1572</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>1440</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>1441</v>
+        <v>1574</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>1442</v>
+        <v>1575</v>
       </c>
       <c r="C3" s="7">
         <v>25.0</v>
@@ -34404,10 +37211,10 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>1443</v>
+        <v>1576</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="C4" s="7">
         <v>15.0</v>
@@ -34419,18 +37226,18 @@
         <v>44690.0</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>1445</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>1446</v>
+        <v>1579</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>1447</v>
+        <v>1580</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>1448</v>
+        <v>1581</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>20</v>
@@ -34438,10 +37245,10 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>1449</v>
+        <v>1582</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>1450</v>
+        <v>1583</v>
       </c>
       <c r="C6" s="7">
         <v>20.0</v>
@@ -34473,10 +37280,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>1451</v>
+        <v>1584</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>1452</v>
+        <v>1585</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>78</v>
@@ -34508,7 +37315,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1436</v>
+        <v>1569</v>
       </c>
       <c r="C2" s="7">
         <v>2.0</v>
@@ -34537,7 +37344,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>1443</v>
+        <v>1576</v>
       </c>
       <c r="C3" s="7">
         <v>5.0</v>
@@ -34566,7 +37373,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>1441</v>
+        <v>1574</v>
       </c>
       <c r="F4" s="7">
         <v>17.0</v>
@@ -34589,7 +37396,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>1449</v>
+        <v>1582</v>
       </c>
       <c r="F5" s="7">
         <v>6.0</v>
@@ -34612,7 +37419,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>1453</v>
+        <v>1586</v>
       </c>
       <c r="F6" s="7">
         <v>11.0</v>
@@ -34655,16 +37462,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="26" t="s">
-        <v>1454</v>
+        <v>1587</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>1455</v>
+        <v>1588</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>1456</v>
+        <v>1589</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>12</v>
@@ -34694,7 +37501,7 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B2" s="6">
         <v>44690.0</v>
@@ -34709,7 +37516,7 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B3" s="6">
         <v>44690.0</v>
@@ -34724,7 +37531,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B4" s="6">
         <v>44690.0</v>
@@ -34739,7 +37546,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B5" s="6">
         <v>44690.0</v>
@@ -34754,7 +37561,7 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B6" s="6">
         <v>44690.0</v>
@@ -34769,7 +37576,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B7" s="6">
         <v>44690.0</v>
@@ -34784,7 +37591,7 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B8" s="6">
         <v>44690.0</v>
@@ -34799,7 +37606,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B9" s="6">
         <v>44690.0</v>
@@ -34814,7 +37621,7 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B10" s="6">
         <v>44690.0</v>
@@ -34829,7 +37636,7 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B11" s="6">
         <v>44690.0</v>
@@ -34844,7 +37651,7 @@
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B12" s="6">
         <v>44690.0</v>
@@ -34859,7 +37666,7 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B13" s="6">
         <v>44690.0</v>
@@ -34874,7 +37681,7 @@
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B14" s="6">
         <v>44690.0</v>
@@ -34889,7 +37696,7 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B15" s="6">
         <v>44690.0</v>
@@ -34904,7 +37711,7 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B16" s="6">
         <v>44690.0</v>
@@ -34919,7 +37726,7 @@
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B17" s="6">
         <v>44690.0</v>
@@ -34935,7 +37742,7 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B18" s="6">
         <v>44690.0</v>
@@ -34951,7 +37758,7 @@
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B19" s="6">
         <v>44690.0</v>
@@ -34966,7 +37773,7 @@
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B20" s="6">
         <v>44690.0</v>
@@ -34981,7 +37788,7 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B21" s="6">
         <v>44690.0</v>
@@ -34996,7 +37803,7 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B22" s="6">
         <v>44690.0</v>
@@ -35011,7 +37818,7 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B23" s="6">
         <v>44690.0</v>
@@ -35026,7 +37833,7 @@
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B24" s="6">
         <v>44690.0</v>
@@ -35041,7 +37848,7 @@
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B25" s="6">
         <v>44690.0</v>
@@ -35056,7 +37863,7 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B26" s="6">
         <v>44690.0</v>
@@ -35071,7 +37878,7 @@
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B27" s="6">
         <v>44690.0</v>
@@ -35086,7 +37893,7 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B28" s="6">
         <v>44690.0</v>
@@ -35101,7 +37908,7 @@
     </row>
     <row r="29">
       <c r="A29" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B29" s="6">
         <v>44690.0</v>
@@ -35116,7 +37923,7 @@
     </row>
     <row r="30">
       <c r="A30" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B30" s="6">
         <v>44690.0</v>
@@ -35131,7 +37938,7 @@
     </row>
     <row r="31">
       <c r="A31" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B31" s="6">
         <v>44690.0</v>
@@ -35146,7 +37953,7 @@
     </row>
     <row r="32">
       <c r="A32" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B32" s="6">
         <v>44690.0</v>
@@ -35161,7 +37968,7 @@
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B33" s="6">
         <v>44690.0</v>
@@ -35176,7 +37983,7 @@
     </row>
     <row r="34">
       <c r="A34" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B34" s="6">
         <v>44690.0</v>
@@ -35191,7 +37998,7 @@
     </row>
     <row r="35">
       <c r="A35" s="7" t="s">
-        <v>1444</v>
+        <v>1577</v>
       </c>
       <c r="B35" s="6">
         <v>44690.0</v>
@@ -35206,7 +38013,7 @@
     </row>
     <row r="36">
       <c r="A36" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B36" s="6">
         <v>44704.0</v>
@@ -35221,7 +38028,7 @@
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B37" s="6">
         <v>44704.0</v>
@@ -35236,7 +38043,7 @@
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B38" s="6">
         <v>44704.0</v>
@@ -35248,12 +38055,12 @@
         <v>22.0</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>1458</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B39" s="6">
         <v>44704.0</v>
@@ -35268,7 +38075,7 @@
     </row>
     <row r="40">
       <c r="A40" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B40" s="6">
         <v>44704.0</v>
@@ -35280,12 +38087,12 @@
         <v>34.0</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>1458</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B41" s="6">
         <v>44704.0</v>
@@ -35300,7 +38107,7 @@
     </row>
     <row r="42">
       <c r="A42" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B42" s="6">
         <v>44704.0</v>
@@ -35315,7 +38122,7 @@
     </row>
     <row r="43">
       <c r="A43" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B43" s="6">
         <v>44704.0</v>
@@ -35330,7 +38137,7 @@
     </row>
     <row r="44">
       <c r="A44" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B44" s="6">
         <v>44704.0</v>
@@ -35342,12 +38149,12 @@
         <v>6.0</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>1458</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B45" s="6">
         <v>44704.0</v>
@@ -35362,7 +38169,7 @@
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B46" s="6">
         <v>44704.0</v>
@@ -35377,7 +38184,7 @@
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B47" s="6">
         <v>44704.0</v>
@@ -35392,7 +38199,7 @@
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B48" s="6">
         <v>44704.0</v>
@@ -35407,7 +38214,7 @@
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B49" s="6">
         <v>44704.0</v>
@@ -35422,7 +38229,7 @@
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B50" s="6">
         <v>44704.0</v>
@@ -35437,7 +38244,7 @@
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B51" s="6">
         <v>44704.0</v>
@@ -35452,7 +38259,7 @@
     </row>
     <row r="52">
       <c r="A52" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B52" s="6">
         <v>44704.0</v>
@@ -35467,7 +38274,7 @@
     </row>
     <row r="53">
       <c r="A53" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B53" s="6">
         <v>44704.0</v>
@@ -35482,7 +38289,7 @@
     </row>
     <row r="54">
       <c r="A54" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B54" s="6">
         <v>44704.0</v>
@@ -35497,7 +38304,7 @@
     </row>
     <row r="55">
       <c r="A55" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B55" s="6">
         <v>44704.0</v>
@@ -35512,7 +38319,7 @@
     </row>
     <row r="56">
       <c r="A56" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B56" s="6">
         <v>44704.0</v>
@@ -35527,7 +38334,7 @@
     </row>
     <row r="57">
       <c r="A57" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B57" s="6">
         <v>44704.0</v>
@@ -35542,7 +38349,7 @@
     </row>
     <row r="58">
       <c r="A58" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B58" s="6">
         <v>44704.0</v>
@@ -35557,7 +38364,7 @@
     </row>
     <row r="59">
       <c r="A59" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B59" s="6">
         <v>44704.0</v>
@@ -35572,7 +38379,7 @@
     </row>
     <row r="60">
       <c r="A60" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B60" s="6">
         <v>44704.0</v>
@@ -35587,7 +38394,7 @@
     </row>
     <row r="61">
       <c r="A61" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B61" s="6">
         <v>44704.0</v>
@@ -35602,7 +38409,7 @@
     </row>
     <row r="62">
       <c r="A62" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B62" s="6">
         <v>44704.0</v>
@@ -35617,7 +38424,7 @@
     </row>
     <row r="63">
       <c r="A63" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B63" s="6">
         <v>44704.0</v>
@@ -35632,7 +38439,7 @@
     </row>
     <row r="64">
       <c r="A64" s="7" t="s">
-        <v>1457</v>
+        <v>1590</v>
       </c>
       <c r="B64" s="6">
         <v>44704.0</v>
@@ -35647,7 +38454,7 @@
     </row>
     <row r="65">
       <c r="A65" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B65" s="6">
         <v>44704.0</v>
@@ -35662,7 +38469,7 @@
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B66" s="6">
         <v>44704.0</v>
@@ -35677,7 +38484,7 @@
     </row>
     <row r="67">
       <c r="A67" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B67" s="6">
         <v>44704.0</v>
@@ -35692,7 +38499,7 @@
     </row>
     <row r="68">
       <c r="A68" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B68" s="6">
         <v>44704.0</v>
@@ -35707,7 +38514,7 @@
     </row>
     <row r="69">
       <c r="A69" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B69" s="6">
         <v>44704.0</v>
@@ -35722,7 +38529,7 @@
     </row>
     <row r="70">
       <c r="A70" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B70" s="6">
         <v>44704.0</v>
@@ -35737,7 +38544,7 @@
     </row>
     <row r="71">
       <c r="A71" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B71" s="6">
         <v>44704.0</v>
@@ -35752,7 +38559,7 @@
     </row>
     <row r="72">
       <c r="A72" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B72" s="6">
         <v>44704.0</v>
@@ -35767,7 +38574,7 @@
     </row>
     <row r="73">
       <c r="A73" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B73" s="6">
         <v>44704.0</v>
@@ -35782,7 +38589,7 @@
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B74" s="6">
         <v>44704.0</v>
@@ -35797,7 +38604,7 @@
     </row>
     <row r="75">
       <c r="A75" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B75" s="6">
         <v>44704.0</v>
@@ -35812,7 +38619,7 @@
     </row>
     <row r="76">
       <c r="A76" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B76" s="6">
         <v>44704.0</v>
@@ -35827,7 +38634,7 @@
     </row>
     <row r="77">
       <c r="A77" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B77" s="6">
         <v>44704.0</v>
@@ -35842,7 +38649,7 @@
     </row>
     <row r="78">
       <c r="A78" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B78" s="6">
         <v>44704.0</v>
@@ -35857,7 +38664,7 @@
     </row>
     <row r="79">
       <c r="A79" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B79" s="6">
         <v>44704.0</v>
@@ -35872,7 +38679,7 @@
     </row>
     <row r="80">
       <c r="A80" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B80" s="6">
         <v>44704.0</v>
@@ -35887,7 +38694,7 @@
     </row>
     <row r="81">
       <c r="A81" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B81" s="6">
         <v>44704.0</v>
@@ -35902,7 +38709,7 @@
     </row>
     <row r="82">
       <c r="A82" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B82" s="6">
         <v>44704.0</v>
@@ -35917,7 +38724,7 @@
     </row>
     <row r="83">
       <c r="A83" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B83" s="6">
         <v>44704.0</v>
@@ -35932,7 +38739,7 @@
     </row>
     <row r="84">
       <c r="A84" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B84" s="6">
         <v>44704.0</v>
@@ -35947,7 +38754,7 @@
     </row>
     <row r="85">
       <c r="A85" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B85" s="6">
         <v>44704.0</v>
@@ -35962,7 +38769,7 @@
     </row>
     <row r="86">
       <c r="A86" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B86" s="6">
         <v>44704.0</v>
@@ -35977,7 +38784,7 @@
     </row>
     <row r="87">
       <c r="A87" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B87" s="6">
         <v>44704.0</v>
@@ -35992,7 +38799,7 @@
     </row>
     <row r="88">
       <c r="A88" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B88" s="6">
         <v>44704.0</v>
@@ -36007,7 +38814,7 @@
     </row>
     <row r="89">
       <c r="A89" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B89" s="6">
         <v>44704.0</v>
@@ -36022,7 +38829,7 @@
     </row>
     <row r="90">
       <c r="A90" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B90" s="6">
         <v>44704.0</v>
@@ -36037,7 +38844,7 @@
     </row>
     <row r="91">
       <c r="A91" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B91" s="6">
         <v>44704.0</v>
@@ -36052,7 +38859,7 @@
     </row>
     <row r="92">
       <c r="A92" s="7" t="s">
-        <v>1459</v>
+        <v>1592</v>
       </c>
       <c r="B92" s="6">
         <v>44704.0</v>
@@ -36067,7 +38874,7 @@
     </row>
     <row r="93">
       <c r="A93" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B93" s="6">
         <v>44705.0</v>
@@ -36082,7 +38889,7 @@
     </row>
     <row r="94">
       <c r="A94" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B94" s="6">
         <v>44705.0</v>
@@ -36097,7 +38904,7 @@
     </row>
     <row r="95">
       <c r="A95" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B95" s="6">
         <v>44705.0</v>
@@ -36112,7 +38919,7 @@
     </row>
     <row r="96">
       <c r="A96" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B96" s="6">
         <v>44705.0</v>
@@ -36127,7 +38934,7 @@
     </row>
     <row r="97">
       <c r="A97" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B97" s="6">
         <v>44705.0</v>
@@ -36142,7 +38949,7 @@
     </row>
     <row r="98">
       <c r="A98" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B98" s="6">
         <v>44705.0</v>
@@ -36157,7 +38964,7 @@
     </row>
     <row r="99">
       <c r="A99" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B99" s="6">
         <v>44705.0</v>
@@ -36172,7 +38979,7 @@
     </row>
     <row r="100">
       <c r="A100" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B100" s="6">
         <v>44705.0</v>
@@ -36187,7 +38994,7 @@
     </row>
     <row r="101">
       <c r="A101" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B101" s="6">
         <v>44705.0</v>
@@ -36202,7 +39009,7 @@
     </row>
     <row r="102">
       <c r="A102" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B102" s="6">
         <v>44705.0</v>
@@ -36217,7 +39024,7 @@
     </row>
     <row r="103">
       <c r="A103" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B103" s="6">
         <v>44705.0</v>
@@ -36232,7 +39039,7 @@
     </row>
     <row r="104">
       <c r="A104" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B104" s="6">
         <v>44705.0</v>
@@ -36247,7 +39054,7 @@
     </row>
     <row r="105">
       <c r="A105" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B105" s="6">
         <v>44705.0</v>
@@ -36262,7 +39069,7 @@
     </row>
     <row r="106">
       <c r="A106" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B106" s="6">
         <v>44705.0</v>
@@ -36277,7 +39084,7 @@
     </row>
     <row r="107">
       <c r="A107" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B107" s="6">
         <v>44705.0</v>
@@ -36292,7 +39099,7 @@
     </row>
     <row r="108">
       <c r="A108" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B108" s="6">
         <v>44705.0</v>
@@ -36307,7 +39114,7 @@
     </row>
     <row r="109">
       <c r="A109" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B109" s="6">
         <v>44705.0</v>
@@ -36322,7 +39129,7 @@
     </row>
     <row r="110">
       <c r="A110" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B110" s="6">
         <v>44705.0</v>
@@ -36337,7 +39144,7 @@
     </row>
     <row r="111">
       <c r="A111" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B111" s="6">
         <v>44705.0</v>
@@ -36352,7 +39159,7 @@
     </row>
     <row r="112">
       <c r="A112" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B112" s="6">
         <v>44705.0</v>
@@ -36367,7 +39174,7 @@
     </row>
     <row r="113">
       <c r="A113" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B113" s="6">
         <v>44705.0</v>
@@ -36382,7 +39189,7 @@
     </row>
     <row r="114">
       <c r="A114" s="7" t="s">
-        <v>1460</v>
+        <v>1593</v>
       </c>
       <c r="B114" s="6">
         <v>44705.0</v>
@@ -36397,7 +39204,7 @@
     </row>
     <row r="115">
       <c r="A115" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B115" s="6">
         <v>44708.0</v>
@@ -36412,7 +39219,7 @@
     </row>
     <row r="116">
       <c r="A116" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B116" s="6">
         <v>44708.0</v>
@@ -36427,7 +39234,7 @@
     </row>
     <row r="117">
       <c r="A117" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B117" s="6">
         <v>44708.0</v>
@@ -36442,7 +39249,7 @@
     </row>
     <row r="118">
       <c r="A118" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B118" s="6">
         <v>44708.0</v>
@@ -36454,12 +39261,12 @@
         <v>39.0</v>
       </c>
       <c r="E118" s="29" t="s">
-        <v>1458</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B119" s="6">
         <v>44708.0</v>
@@ -36474,7 +39281,7 @@
     </row>
     <row r="120">
       <c r="A120" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B120" s="6">
         <v>44708.0</v>
@@ -36489,7 +39296,7 @@
     </row>
     <row r="121">
       <c r="A121" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B121" s="6">
         <v>44708.0</v>
@@ -36504,7 +39311,7 @@
     </row>
     <row r="122">
       <c r="A122" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B122" s="6">
         <v>44708.0</v>
@@ -36519,7 +39326,7 @@
     </row>
     <row r="123">
       <c r="A123" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B123" s="6">
         <v>44708.0</v>
@@ -36534,7 +39341,7 @@
     </row>
     <row r="124">
       <c r="A124" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B124" s="6">
         <v>44708.0</v>
@@ -36549,7 +39356,7 @@
     </row>
     <row r="125">
       <c r="A125" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B125" s="6">
         <v>44708.0</v>
@@ -36564,7 +39371,7 @@
     </row>
     <row r="126">
       <c r="A126" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B126" s="6">
         <v>44708.0</v>
@@ -36579,7 +39386,7 @@
     </row>
     <row r="127">
       <c r="A127" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B127" s="6">
         <v>44708.0</v>
@@ -36591,12 +39398,12 @@
         <v>11.0</v>
       </c>
       <c r="E127" s="29" t="s">
-        <v>1458</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B128" s="6">
         <v>44708.0</v>
@@ -36611,7 +39418,7 @@
     </row>
     <row r="129">
       <c r="A129" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B129" s="6">
         <v>44708.0</v>
@@ -36623,12 +39430,12 @@
         <v>40.0</v>
       </c>
       <c r="E129" s="29" t="s">
-        <v>1458</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B130" s="6">
         <v>44708.0</v>
@@ -36643,7 +39450,7 @@
     </row>
     <row r="131">
       <c r="A131" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B131" s="6">
         <v>44708.0</v>
@@ -36658,7 +39465,7 @@
     </row>
     <row r="132">
       <c r="A132" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B132" s="6">
         <v>44708.0</v>
@@ -36673,7 +39480,7 @@
     </row>
     <row r="133">
       <c r="A133" s="7" t="s">
-        <v>1461</v>
+        <v>1594</v>
       </c>
       <c r="B133" s="6">
         <v>44708.0</v>
@@ -36688,7 +39495,7 @@
     </row>
     <row r="134">
       <c r="A134" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B134" s="6">
         <v>44713.0</v>
@@ -36700,12 +39507,12 @@
         <v>1298</v>
       </c>
       <c r="E134" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B135" s="6">
         <v>44713.0</v>
@@ -36717,12 +39524,12 @@
         <v>1300</v>
       </c>
       <c r="E135" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B136" s="6">
         <v>44713.0</v>
@@ -36734,12 +39541,12 @@
         <v>1302</v>
       </c>
       <c r="E136" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B137" s="6">
         <v>44713.0</v>
@@ -36751,12 +39558,12 @@
         <v>1304</v>
       </c>
       <c r="E137" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B138" s="6">
         <v>44713.0</v>
@@ -36768,12 +39575,12 @@
         <v>1306</v>
       </c>
       <c r="E138" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B139" s="6">
         <v>44713.0</v>
@@ -36785,12 +39592,12 @@
         <v>1309</v>
       </c>
       <c r="E139" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B140" s="6">
         <v>44713.0</v>
@@ -36802,12 +39609,12 @@
         <v>1312</v>
       </c>
       <c r="E140" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B141" s="6">
         <v>44713.0</v>
@@ -36819,12 +39626,12 @@
         <v>1315</v>
       </c>
       <c r="E141" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B142" s="6">
         <v>44713.0</v>
@@ -36836,12 +39643,12 @@
         <v>1318</v>
       </c>
       <c r="E142" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B143" s="6">
         <v>44713.0</v>
@@ -36853,12 +39660,12 @@
         <v>1321</v>
       </c>
       <c r="E143" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B144" s="6">
         <v>44713.0</v>
@@ -36870,12 +39677,12 @@
         <v>1323</v>
       </c>
       <c r="E144" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B145" s="6">
         <v>44713.0</v>
@@ -36887,12 +39694,12 @@
         <v>1325</v>
       </c>
       <c r="E145" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B146" s="6">
         <v>44713.0</v>
@@ -36904,12 +39711,12 @@
         <v>1327</v>
       </c>
       <c r="E146" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B147" s="6">
         <v>44713.0</v>
@@ -36921,12 +39728,12 @@
         <v>1329</v>
       </c>
       <c r="E147" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B148" s="6">
         <v>44713.0</v>
@@ -36938,12 +39745,12 @@
         <v>1331</v>
       </c>
       <c r="E148" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B149" s="6">
         <v>44713.0</v>
@@ -36955,12 +39762,12 @@
         <v>1333</v>
       </c>
       <c r="E149" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B150" s="6">
         <v>44713.0</v>
@@ -36972,12 +39779,12 @@
         <v>1335</v>
       </c>
       <c r="E150" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B151" s="6">
         <v>44713.0</v>
@@ -36989,12 +39796,12 @@
         <v>1337</v>
       </c>
       <c r="E151" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B152" s="6">
         <v>44713.0</v>
@@ -37006,12 +39813,12 @@
         <v>1340</v>
       </c>
       <c r="E152" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B153" s="6">
         <v>44713.0</v>
@@ -37023,12 +39830,12 @@
         <v>1342</v>
       </c>
       <c r="E153" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B154" s="6">
         <v>44713.0</v>
@@ -37040,12 +39847,12 @@
         <v>1344</v>
       </c>
       <c r="E154" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B155" s="6">
         <v>44713.0</v>
@@ -37057,12 +39864,12 @@
         <v>1346</v>
       </c>
       <c r="E155" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B156" s="6">
         <v>44713.0</v>
@@ -37074,12 +39881,12 @@
         <v>1348</v>
       </c>
       <c r="E156" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="7" t="s">
-        <v>1462</v>
+        <v>1595</v>
       </c>
       <c r="B157" s="6">
         <v>44713.0</v>
@@ -37091,7 +39898,7 @@
         <v>1350</v>
       </c>
       <c r="E157" s="29" t="s">
-        <v>1463</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="158">

</xml_diff>

<commit_message>
Updated data and gps for 18June2022
</commit_message>
<xml_diff>
--- a/Data/Genotype_Samples_2022.xlsx
+++ b/Data/Genotype_Samples_2022.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7033" uniqueCount="2103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7181" uniqueCount="2139">
   <si>
     <t>Date</t>
   </si>
@@ -6168,6 +6168,114 @@
   </si>
   <si>
     <t>G1532</t>
+  </si>
+  <si>
+    <t>BUT_026</t>
+  </si>
+  <si>
+    <t>G1890</t>
+  </si>
+  <si>
+    <t>BUT_027</t>
+  </si>
+  <si>
+    <t>BUT_028</t>
+  </si>
+  <si>
+    <t>G1897</t>
+  </si>
+  <si>
+    <t>BUT_029</t>
+  </si>
+  <si>
+    <t>BUT_030</t>
+  </si>
+  <si>
+    <t>G1896</t>
+  </si>
+  <si>
+    <t>BUT_031</t>
+  </si>
+  <si>
+    <t>BUT_032</t>
+  </si>
+  <si>
+    <t>G1898</t>
+  </si>
+  <si>
+    <t>BUT_033</t>
+  </si>
+  <si>
+    <t>BUT_034</t>
+  </si>
+  <si>
+    <t>G1899</t>
+  </si>
+  <si>
+    <t>BUT_035</t>
+  </si>
+  <si>
+    <t>BUT_036</t>
+  </si>
+  <si>
+    <t>BUT_037</t>
+  </si>
+  <si>
+    <t>BUT_038</t>
+  </si>
+  <si>
+    <t>G1889</t>
+  </si>
+  <si>
+    <t>BUT_039</t>
+  </si>
+  <si>
+    <t>BUT_040</t>
+  </si>
+  <si>
+    <t>BUT_041</t>
+  </si>
+  <si>
+    <t>G1888</t>
+  </si>
+  <si>
+    <t>BUT_042</t>
+  </si>
+  <si>
+    <t>BUT_043</t>
+  </si>
+  <si>
+    <t>G1880</t>
+  </si>
+  <si>
+    <t>BUT_044</t>
+  </si>
+  <si>
+    <t>BUT_045</t>
+  </si>
+  <si>
+    <t>BUT_046</t>
+  </si>
+  <si>
+    <t>G1592</t>
+  </si>
+  <si>
+    <t>BUT_047</t>
+  </si>
+  <si>
+    <t>BUT_048</t>
+  </si>
+  <si>
+    <t>BUT_049</t>
+  </si>
+  <si>
+    <t>G1879</t>
+  </si>
+  <si>
+    <t>BUT_050</t>
+  </si>
+  <si>
+    <t>G1370</t>
   </si>
   <si>
     <t>Site_ID</t>
@@ -48203,94 +48311,870 @@
       </c>
     </row>
     <row r="1262">
-      <c r="A1262" s="24"/>
+      <c r="A1262" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1262" s="7" t="s">
+        <v>2051</v>
+      </c>
+      <c r="C1262" s="7" t="s">
+        <v>2052</v>
+      </c>
+      <c r="D1262" s="7">
+        <v>76.0</v>
+      </c>
+      <c r="E1262" s="8">
+        <v>0.4465277777777778</v>
+      </c>
+      <c r="F1262" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1262" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1262" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1262" s="11">
+        <v>17.7481494750828</v>
+      </c>
+      <c r="K1262" s="11">
+        <v>-64.8955184686929</v>
+      </c>
+      <c r="M1262" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1263">
-      <c r="A1263" s="24"/>
+      <c r="A1263" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1263" s="7" t="s">
+        <v>2053</v>
+      </c>
+      <c r="C1263" s="7" t="s">
+        <v>2052</v>
+      </c>
+      <c r="D1263" s="7">
+        <v>45.0</v>
+      </c>
+      <c r="E1263" s="8">
+        <v>0.4465277777777778</v>
+      </c>
+      <c r="F1263" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1263" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1263" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1263" s="11">
+        <v>17.7481494750828</v>
+      </c>
+      <c r="K1263" s="11">
+        <v>-64.8955184686929</v>
+      </c>
+      <c r="M1263" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1264">
-      <c r="A1264" s="24"/>
+      <c r="A1264" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1264" s="7" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C1264" s="7" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D1264" s="7">
+        <v>12.0</v>
+      </c>
+      <c r="E1264" s="8">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="F1264" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1264" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1264" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1264" s="11">
+        <v>17.7480897121131</v>
+      </c>
+      <c r="K1264" s="11">
+        <v>-64.8955574445426</v>
+      </c>
+      <c r="M1264" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1265">
-      <c r="A1265" s="24"/>
+      <c r="A1265" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1265" s="7" t="s">
+        <v>2056</v>
+      </c>
+      <c r="C1265" s="7" t="s">
+        <v>2055</v>
+      </c>
+      <c r="D1265" s="7">
+        <v>81.0</v>
+      </c>
+      <c r="E1265" s="8">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="F1265" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1265" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1265" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1265" s="11">
+        <v>17.7480897121131</v>
+      </c>
+      <c r="K1265" s="11">
+        <v>-64.8955574445426</v>
+      </c>
+      <c r="M1265" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1266">
-      <c r="A1266" s="24"/>
+      <c r="A1266" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1266" s="7" t="s">
+        <v>2057</v>
+      </c>
+      <c r="C1266" s="7" t="s">
+        <v>2058</v>
+      </c>
+      <c r="D1266" s="7">
+        <v>21.0</v>
+      </c>
+      <c r="E1266" s="8">
+        <v>0.4527777777777778</v>
+      </c>
+      <c r="F1266" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1266" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1266" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1266" s="11">
+        <v>17.7480458747596</v>
+      </c>
+      <c r="K1266" s="11">
+        <v>-64.8954984359443</v>
+      </c>
+      <c r="M1266" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1267">
-      <c r="A1267" s="24"/>
+      <c r="A1267" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1267" s="7" t="s">
+        <v>2059</v>
+      </c>
+      <c r="C1267" s="7" t="s">
+        <v>2058</v>
+      </c>
+      <c r="D1267" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="E1267" s="8">
+        <v>0.4527777777777778</v>
+      </c>
+      <c r="F1267" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1267" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1267" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1267" s="11">
+        <v>17.7480458747596</v>
+      </c>
+      <c r="K1267" s="11">
+        <v>-64.8954984359443</v>
+      </c>
+      <c r="M1267" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1268">
-      <c r="A1268" s="24"/>
+      <c r="A1268" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1268" s="7" t="s">
+        <v>2060</v>
+      </c>
+      <c r="C1268" s="7" t="s">
+        <v>2061</v>
+      </c>
+      <c r="D1268" s="7">
+        <v>35.0</v>
+      </c>
+      <c r="E1268" s="8">
+        <v>0.45555555555555555</v>
+      </c>
+      <c r="F1268" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1268" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1268" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1268" s="11">
+        <v>17.7481688372791</v>
+      </c>
+      <c r="K1268" s="11">
+        <v>-64.8954471386969</v>
+      </c>
+      <c r="M1268" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1269">
-      <c r="A1269" s="24"/>
+      <c r="A1269" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1269" s="7" t="s">
+        <v>2062</v>
+      </c>
+      <c r="C1269" s="7" t="s">
+        <v>2061</v>
+      </c>
+      <c r="D1269" s="7">
+        <v>84.0</v>
+      </c>
+      <c r="E1269" s="8">
+        <v>0.45555555555555555</v>
+      </c>
+      <c r="F1269" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1269" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1269" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1269" s="11">
+        <v>17.7481688372791</v>
+      </c>
+      <c r="K1269" s="11">
+        <v>-64.8954471386969</v>
+      </c>
+      <c r="M1269" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1270">
-      <c r="A1270" s="24"/>
+      <c r="A1270" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1270" s="7" t="s">
+        <v>2063</v>
+      </c>
+      <c r="C1270" s="7" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D1270" s="7">
+        <v>8.0</v>
+      </c>
+      <c r="E1270" s="8">
+        <v>0.4583333333333333</v>
+      </c>
+      <c r="F1270" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1270" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1270" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1270" s="11">
+        <v>17.7481514029205</v>
+      </c>
+      <c r="K1270" s="11">
+        <v>-64.895434230566</v>
+      </c>
+      <c r="M1270" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1271">
-      <c r="A1271" s="24"/>
+      <c r="A1271" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1271" s="7" t="s">
+        <v>2065</v>
+      </c>
+      <c r="C1271" s="7" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D1271" s="7">
+        <v>44.0</v>
+      </c>
+      <c r="E1271" s="8">
+        <v>0.4583333333333333</v>
+      </c>
+      <c r="F1271" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1271" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1271" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1271" s="11">
+        <v>17.7481514029205</v>
+      </c>
+      <c r="K1271" s="11">
+        <v>-64.895434230566</v>
+      </c>
+      <c r="M1271" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1272">
-      <c r="A1272" s="24"/>
-      <c r="B1272" s="7"/>
+      <c r="A1272" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1272" s="7" t="s">
+        <v>2066</v>
+      </c>
+      <c r="C1272" s="7" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D1272" s="7">
+        <v>90.0</v>
+      </c>
+      <c r="E1272" s="8">
+        <v>0.4583333333333333</v>
+      </c>
+      <c r="F1272" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1272" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1272" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1272" s="11">
+        <v>17.7481514029205</v>
+      </c>
+      <c r="K1272" s="11">
+        <v>-64.895434230566</v>
+      </c>
+      <c r="M1272" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1273">
-      <c r="A1273" s="24"/>
-      <c r="B1273" s="7"/>
+      <c r="A1273" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1273" s="7" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C1273" s="7" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D1273" s="7">
+        <v>72.0</v>
+      </c>
+      <c r="E1273" s="8">
+        <v>0.4583333333333333</v>
+      </c>
+      <c r="F1273" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1273" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1273" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1273" s="11">
+        <v>17.7481514029205</v>
+      </c>
+      <c r="K1273" s="11">
+        <v>-64.895434230566</v>
+      </c>
+      <c r="M1273" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1274">
-      <c r="A1274" s="24"/>
-      <c r="B1274" s="7"/>
+      <c r="A1274" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1274" s="7" t="s">
+        <v>2068</v>
+      </c>
+      <c r="C1274" s="7" t="s">
+        <v>2069</v>
+      </c>
+      <c r="D1274" s="7">
+        <v>101.0</v>
+      </c>
+      <c r="E1274" s="8">
+        <v>0.46319444444444446</v>
+      </c>
+      <c r="F1274" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1274" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1274" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1274" s="11">
+        <v>17.7483710087836</v>
+      </c>
+      <c r="K1274" s="11">
+        <v>-64.8953836038709</v>
+      </c>
+      <c r="M1274" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1275">
-      <c r="A1275" s="24"/>
-      <c r="B1275" s="7"/>
+      <c r="A1275" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1275" s="7" t="s">
+        <v>2070</v>
+      </c>
+      <c r="C1275" s="7" t="s">
+        <v>2069</v>
+      </c>
+      <c r="D1275" s="7">
+        <v>73.0</v>
+      </c>
+      <c r="E1275" s="8">
+        <v>0.46319444444444446</v>
+      </c>
+      <c r="F1275" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1275" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1275" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1275" s="11">
+        <v>17.7483710087836</v>
+      </c>
+      <c r="K1275" s="11">
+        <v>-64.8953836038709</v>
+      </c>
+      <c r="M1275" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1276">
-      <c r="A1276" s="24"/>
-      <c r="B1276" s="7"/>
+      <c r="A1276" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1276" s="7" t="s">
+        <v>2071</v>
+      </c>
+      <c r="C1276" s="7" t="s">
+        <v>2069</v>
+      </c>
+      <c r="D1276" s="7">
+        <v>79.0</v>
+      </c>
+      <c r="E1276" s="8">
+        <v>0.46319444444444446</v>
+      </c>
+      <c r="F1276" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1276" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1276" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1276" s="11">
+        <v>17.7483710087836</v>
+      </c>
+      <c r="K1276" s="11">
+        <v>-64.8953836038709</v>
+      </c>
+      <c r="M1276" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1277">
-      <c r="A1277" s="24"/>
-      <c r="B1277" s="7"/>
+      <c r="A1277" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1277" s="7" t="s">
+        <v>2072</v>
+      </c>
+      <c r="C1277" s="7" t="s">
+        <v>2073</v>
+      </c>
+      <c r="D1277" s="7">
+        <v>77.0</v>
+      </c>
+      <c r="E1277" s="8">
+        <v>0.46805555555555556</v>
+      </c>
+      <c r="F1277" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1277" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1277" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1277" s="11">
+        <v>17.7483722660691</v>
+      </c>
+      <c r="K1277" s="11">
+        <v>-64.895315207541</v>
+      </c>
+      <c r="M1277" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1278">
-      <c r="A1278" s="24"/>
-      <c r="B1278" s="7"/>
+      <c r="A1278" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1278" s="7" t="s">
+        <v>2074</v>
+      </c>
+      <c r="C1278" s="7" t="s">
+        <v>2073</v>
+      </c>
+      <c r="D1278" s="7">
+        <v>9.0</v>
+      </c>
+      <c r="E1278" s="8">
+        <v>0.46805555555555556</v>
+      </c>
+      <c r="F1278" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1278" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1278" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1278" s="11">
+        <v>17.7483722660691</v>
+      </c>
+      <c r="K1278" s="11">
+        <v>-64.895315207541</v>
+      </c>
+      <c r="M1278" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1279">
-      <c r="A1279" s="24"/>
-      <c r="B1279" s="7"/>
+      <c r="A1279" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1279" s="7" t="s">
+        <v>2075</v>
+      </c>
+      <c r="C1279" s="7" t="s">
+        <v>2076</v>
+      </c>
+      <c r="D1279" s="7">
+        <v>27.0</v>
+      </c>
+      <c r="E1279" s="8">
+        <v>0.4701388888888889</v>
+      </c>
+      <c r="F1279" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1279" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1279" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1279" s="11">
+        <v>17.7483629621565</v>
+      </c>
+      <c r="K1279" s="11">
+        <v>-64.8953643254936</v>
+      </c>
+      <c r="M1279" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1280">
-      <c r="A1280" s="24"/>
-      <c r="B1280" s="7"/>
+      <c r="A1280" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1280" s="7" t="s">
+        <v>2077</v>
+      </c>
+      <c r="C1280" s="7" t="s">
+        <v>2076</v>
+      </c>
+      <c r="D1280" s="7">
+        <v>28.0</v>
+      </c>
+      <c r="E1280" s="8">
+        <v>0.4701388888888889</v>
+      </c>
+      <c r="F1280" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1280" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1280" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1280" s="11">
+        <v>17.7483629621565</v>
+      </c>
+      <c r="K1280" s="11">
+        <v>-64.8953643254936</v>
+      </c>
+      <c r="M1280" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1281">
-      <c r="A1281" s="24"/>
-      <c r="B1281" s="7"/>
+      <c r="A1281" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1281" s="7" t="s">
+        <v>2078</v>
+      </c>
+      <c r="C1281" s="7" t="s">
+        <v>2076</v>
+      </c>
+      <c r="D1281" s="7">
+        <v>47.0</v>
+      </c>
+      <c r="E1281" s="8">
+        <v>0.4701388888888889</v>
+      </c>
+      <c r="F1281" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1281" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1281" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1281" s="11">
+        <v>17.7483629621565</v>
+      </c>
+      <c r="K1281" s="11">
+        <v>-64.8953643254936</v>
+      </c>
+      <c r="M1281" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1282">
-      <c r="A1282" s="24"/>
-      <c r="B1282" s="7"/>
+      <c r="A1282" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1282" s="7" t="s">
+        <v>2079</v>
+      </c>
+      <c r="C1282" s="7" t="s">
+        <v>2080</v>
+      </c>
+      <c r="D1282" s="7">
+        <v>29.0</v>
+      </c>
+      <c r="E1282" s="8">
+        <v>0.4736111111111111</v>
+      </c>
+      <c r="F1282" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1282" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1282" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1282" s="11">
+        <v>17.7483405824751</v>
+      </c>
+      <c r="K1282" s="11">
+        <v>-64.8953629843891</v>
+      </c>
+      <c r="M1282" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1283">
-      <c r="A1283" s="24"/>
-      <c r="B1283" s="7"/>
+      <c r="A1283" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1283" s="7" t="s">
+        <v>2081</v>
+      </c>
+      <c r="C1283" s="7" t="s">
+        <v>2080</v>
+      </c>
+      <c r="D1283" s="7">
+        <v>49.0</v>
+      </c>
+      <c r="E1283" s="8">
+        <v>0.4736111111111111</v>
+      </c>
+      <c r="F1283" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1283" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1283" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1283" s="11">
+        <v>17.7483405824751</v>
+      </c>
+      <c r="K1283" s="11">
+        <v>-64.8953629843891</v>
+      </c>
+      <c r="M1283" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1284">
-      <c r="A1284" s="24"/>
-      <c r="B1284" s="7"/>
+      <c r="A1284" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1284" s="7" t="s">
+        <v>2082</v>
+      </c>
+      <c r="C1284" s="7" t="s">
+        <v>2080</v>
+      </c>
+      <c r="E1284" s="8">
+        <v>0.4736111111111111</v>
+      </c>
+      <c r="F1284" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1284" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1284" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1284" s="11">
+        <v>17.7483405824751</v>
+      </c>
+      <c r="K1284" s="11">
+        <v>-64.8953629843891</v>
+      </c>
+      <c r="M1284" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1285">
-      <c r="A1285" s="24"/>
-      <c r="B1285" s="7"/>
+      <c r="A1285" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1285" s="7" t="s">
+        <v>2083</v>
+      </c>
+      <c r="C1285" s="7" t="s">
+        <v>2084</v>
+      </c>
+      <c r="D1285" s="7">
+        <v>75.0</v>
+      </c>
+      <c r="E1285" s="8">
+        <v>0.47638888888888886</v>
+      </c>
+      <c r="F1285" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1285" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1285" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1285" s="11">
+        <v>17.7483918797225</v>
+      </c>
+      <c r="K1285" s="11">
+        <v>-64.8954082466662</v>
+      </c>
     </row>
     <row r="1286">
-      <c r="A1286" s="24"/>
-      <c r="B1286" s="7"/>
+      <c r="A1286" s="6">
+        <v>44730.0</v>
+      </c>
+      <c r="B1286" s="7" t="s">
+        <v>2085</v>
+      </c>
+      <c r="C1286" s="7" t="s">
+        <v>2086</v>
+      </c>
+      <c r="D1286" s="7">
+        <v>104.0</v>
+      </c>
+      <c r="E1286" s="8">
+        <v>0.47708333333333336</v>
+      </c>
+      <c r="F1286" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1286" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1286" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1286" s="11">
+        <v>17.748340498656</v>
+      </c>
+      <c r="K1286" s="11">
+        <v>-64.8953986912966</v>
+      </c>
     </row>
     <row r="1287">
       <c r="A1287" s="24"/>
@@ -51139,10 +52023,6 @@
     <row r="1998">
       <c r="A1998" s="24"/>
       <c r="B1998" s="7"/>
-    </row>
-    <row r="1999">
-      <c r="A1999" s="24"/>
-      <c r="B1999" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -51161,19 +52041,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>2051</v>
+        <v>2087</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2052</v>
+        <v>2088</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2053</v>
+        <v>2089</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2054</v>
+        <v>2090</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2055</v>
+        <v>2091</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>7</v>
@@ -51197,21 +52077,21 @@
         <v>51</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>2056</v>
+        <v>2092</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>145</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>2057</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>2058</v>
+        <v>2094</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2059</v>
+        <v>2095</v>
       </c>
       <c r="C2" s="7">
         <v>7.0</v>
@@ -51223,33 +52103,33 @@
         <v>44688.0</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>2060</v>
+        <v>2096</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>2060</v>
+        <v>2096</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>2060</v>
+        <v>2096</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>2060</v>
+        <v>2096</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>2060</v>
+        <v>2096</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>2061</v>
+        <v>2097</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>2062</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>2063</v>
+        <v>2099</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2064</v>
+        <v>2100</v>
       </c>
       <c r="C3" s="7">
         <v>25.0</v>
@@ -51260,10 +52140,10 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>2065</v>
+        <v>2101</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="C4" s="7">
         <v>15.0</v>
@@ -51275,18 +52155,18 @@
         <v>44690.0</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>2067</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>2068</v>
+        <v>2104</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2069</v>
+        <v>2105</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2070</v>
+        <v>2106</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>20</v>
@@ -51294,10 +52174,10 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>2071</v>
+        <v>2107</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2072</v>
+        <v>2108</v>
       </c>
       <c r="C6" s="7">
         <v>20.0</v>
@@ -51329,10 +52209,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>2073</v>
+        <v>2109</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2074</v>
+        <v>2110</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>78</v>
@@ -51364,7 +52244,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2058</v>
+        <v>2094</v>
       </c>
       <c r="C2" s="7">
         <v>2.0</v>
@@ -51393,7 +52273,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2065</v>
+        <v>2101</v>
       </c>
       <c r="C3" s="7">
         <v>5.0</v>
@@ -51422,7 +52302,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2063</v>
+        <v>2099</v>
       </c>
       <c r="F4" s="7">
         <v>17.0</v>
@@ -51445,7 +52325,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2071</v>
+        <v>2107</v>
       </c>
       <c r="F5" s="7">
         <v>6.0</v>
@@ -51468,7 +52348,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2075</v>
+        <v>2111</v>
       </c>
       <c r="F6" s="7">
         <v>11.0</v>
@@ -51511,16 +52391,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="26" t="s">
-        <v>2076</v>
+        <v>2112</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>2077</v>
+        <v>2113</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>2078</v>
+        <v>2114</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>12</v>
@@ -51550,7 +52430,7 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B2" s="6">
         <v>44690.0</v>
@@ -51565,7 +52445,7 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B3" s="6">
         <v>44690.0</v>
@@ -51580,7 +52460,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B4" s="6">
         <v>44690.0</v>
@@ -51595,7 +52475,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B5" s="6">
         <v>44690.0</v>
@@ -51610,7 +52490,7 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B6" s="6">
         <v>44690.0</v>
@@ -51625,7 +52505,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B7" s="6">
         <v>44690.0</v>
@@ -51640,7 +52520,7 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B8" s="6">
         <v>44690.0</v>
@@ -51655,7 +52535,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B9" s="6">
         <v>44690.0</v>
@@ -51670,7 +52550,7 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B10" s="6">
         <v>44690.0</v>
@@ -51685,7 +52565,7 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B11" s="6">
         <v>44690.0</v>
@@ -51700,7 +52580,7 @@
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B12" s="6">
         <v>44690.0</v>
@@ -51715,7 +52595,7 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B13" s="6">
         <v>44690.0</v>
@@ -51730,7 +52610,7 @@
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B14" s="6">
         <v>44690.0</v>
@@ -51745,7 +52625,7 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B15" s="6">
         <v>44690.0</v>
@@ -51760,7 +52640,7 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B16" s="6">
         <v>44690.0</v>
@@ -51775,7 +52655,7 @@
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B17" s="6">
         <v>44690.0</v>
@@ -51791,7 +52671,7 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B18" s="6">
         <v>44690.0</v>
@@ -51807,7 +52687,7 @@
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B19" s="6">
         <v>44690.0</v>
@@ -51822,7 +52702,7 @@
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B20" s="6">
         <v>44690.0</v>
@@ -51837,7 +52717,7 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B21" s="6">
         <v>44690.0</v>
@@ -51852,7 +52732,7 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B22" s="6">
         <v>44690.0</v>
@@ -51867,7 +52747,7 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B23" s="6">
         <v>44690.0</v>
@@ -51882,7 +52762,7 @@
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B24" s="6">
         <v>44690.0</v>
@@ -51897,7 +52777,7 @@
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B25" s="6">
         <v>44690.0</v>
@@ -51912,7 +52792,7 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B26" s="6">
         <v>44690.0</v>
@@ -51927,7 +52807,7 @@
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B27" s="6">
         <v>44690.0</v>
@@ -51942,7 +52822,7 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B28" s="6">
         <v>44690.0</v>
@@ -51957,7 +52837,7 @@
     </row>
     <row r="29">
       <c r="A29" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B29" s="6">
         <v>44690.0</v>
@@ -51972,7 +52852,7 @@
     </row>
     <row r="30">
       <c r="A30" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B30" s="6">
         <v>44690.0</v>
@@ -51987,7 +52867,7 @@
     </row>
     <row r="31">
       <c r="A31" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B31" s="6">
         <v>44690.0</v>
@@ -52002,7 +52882,7 @@
     </row>
     <row r="32">
       <c r="A32" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B32" s="6">
         <v>44690.0</v>
@@ -52017,7 +52897,7 @@
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B33" s="6">
         <v>44690.0</v>
@@ -52032,7 +52912,7 @@
     </row>
     <row r="34">
       <c r="A34" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B34" s="6">
         <v>44690.0</v>
@@ -52047,7 +52927,7 @@
     </row>
     <row r="35">
       <c r="A35" s="7" t="s">
-        <v>2066</v>
+        <v>2102</v>
       </c>
       <c r="B35" s="6">
         <v>44690.0</v>
@@ -52062,7 +52942,7 @@
     </row>
     <row r="36">
       <c r="A36" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B36" s="6">
         <v>44704.0</v>
@@ -52077,7 +52957,7 @@
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B37" s="6">
         <v>44704.0</v>
@@ -52092,7 +52972,7 @@
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B38" s="6">
         <v>44704.0</v>
@@ -52104,12 +52984,12 @@
         <v>22.0</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>2080</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B39" s="6">
         <v>44704.0</v>
@@ -52124,7 +53004,7 @@
     </row>
     <row r="40">
       <c r="A40" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B40" s="6">
         <v>44704.0</v>
@@ -52136,12 +53016,12 @@
         <v>34.0</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>2080</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B41" s="6">
         <v>44704.0</v>
@@ -52156,7 +53036,7 @@
     </row>
     <row r="42">
       <c r="A42" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B42" s="6">
         <v>44704.0</v>
@@ -52171,7 +53051,7 @@
     </row>
     <row r="43">
       <c r="A43" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B43" s="6">
         <v>44704.0</v>
@@ -52186,7 +53066,7 @@
     </row>
     <row r="44">
       <c r="A44" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B44" s="6">
         <v>44704.0</v>
@@ -52198,12 +53078,12 @@
         <v>6.0</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>2080</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B45" s="6">
         <v>44704.0</v>
@@ -52218,7 +53098,7 @@
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B46" s="6">
         <v>44704.0</v>
@@ -52233,7 +53113,7 @@
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B47" s="6">
         <v>44704.0</v>
@@ -52248,7 +53128,7 @@
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B48" s="6">
         <v>44704.0</v>
@@ -52263,7 +53143,7 @@
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B49" s="6">
         <v>44704.0</v>
@@ -52278,7 +53158,7 @@
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B50" s="6">
         <v>44704.0</v>
@@ -52293,7 +53173,7 @@
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B51" s="6">
         <v>44704.0</v>
@@ -52308,7 +53188,7 @@
     </row>
     <row r="52">
       <c r="A52" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B52" s="6">
         <v>44704.0</v>
@@ -52323,7 +53203,7 @@
     </row>
     <row r="53">
       <c r="A53" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B53" s="6">
         <v>44704.0</v>
@@ -52338,7 +53218,7 @@
     </row>
     <row r="54">
       <c r="A54" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B54" s="6">
         <v>44704.0</v>
@@ -52353,7 +53233,7 @@
     </row>
     <row r="55">
       <c r="A55" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B55" s="6">
         <v>44704.0</v>
@@ -52368,7 +53248,7 @@
     </row>
     <row r="56">
       <c r="A56" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B56" s="6">
         <v>44704.0</v>
@@ -52383,7 +53263,7 @@
     </row>
     <row r="57">
       <c r="A57" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B57" s="6">
         <v>44704.0</v>
@@ -52398,7 +53278,7 @@
     </row>
     <row r="58">
       <c r="A58" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B58" s="6">
         <v>44704.0</v>
@@ -52413,7 +53293,7 @@
     </row>
     <row r="59">
       <c r="A59" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B59" s="6">
         <v>44704.0</v>
@@ -52428,7 +53308,7 @@
     </row>
     <row r="60">
       <c r="A60" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B60" s="6">
         <v>44704.0</v>
@@ -52443,7 +53323,7 @@
     </row>
     <row r="61">
       <c r="A61" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B61" s="6">
         <v>44704.0</v>
@@ -52458,7 +53338,7 @@
     </row>
     <row r="62">
       <c r="A62" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B62" s="6">
         <v>44704.0</v>
@@ -52473,7 +53353,7 @@
     </row>
     <row r="63">
       <c r="A63" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B63" s="6">
         <v>44704.0</v>
@@ -52488,7 +53368,7 @@
     </row>
     <row r="64">
       <c r="A64" s="7" t="s">
-        <v>2079</v>
+        <v>2115</v>
       </c>
       <c r="B64" s="6">
         <v>44704.0</v>
@@ -52503,7 +53383,7 @@
     </row>
     <row r="65">
       <c r="A65" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B65" s="6">
         <v>44704.0</v>
@@ -52518,7 +53398,7 @@
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B66" s="6">
         <v>44704.0</v>
@@ -52533,7 +53413,7 @@
     </row>
     <row r="67">
       <c r="A67" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B67" s="6">
         <v>44704.0</v>
@@ -52548,7 +53428,7 @@
     </row>
     <row r="68">
       <c r="A68" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B68" s="6">
         <v>44704.0</v>
@@ -52563,7 +53443,7 @@
     </row>
     <row r="69">
       <c r="A69" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B69" s="6">
         <v>44704.0</v>
@@ -52578,7 +53458,7 @@
     </row>
     <row r="70">
       <c r="A70" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B70" s="6">
         <v>44704.0</v>
@@ -52593,7 +53473,7 @@
     </row>
     <row r="71">
       <c r="A71" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B71" s="6">
         <v>44704.0</v>
@@ -52608,7 +53488,7 @@
     </row>
     <row r="72">
       <c r="A72" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B72" s="6">
         <v>44704.0</v>
@@ -52623,7 +53503,7 @@
     </row>
     <row r="73">
       <c r="A73" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B73" s="6">
         <v>44704.0</v>
@@ -52638,7 +53518,7 @@
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B74" s="6">
         <v>44704.0</v>
@@ -52653,7 +53533,7 @@
     </row>
     <row r="75">
       <c r="A75" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B75" s="6">
         <v>44704.0</v>
@@ -52668,7 +53548,7 @@
     </row>
     <row r="76">
       <c r="A76" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B76" s="6">
         <v>44704.0</v>
@@ -52683,7 +53563,7 @@
     </row>
     <row r="77">
       <c r="A77" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B77" s="6">
         <v>44704.0</v>
@@ -52698,7 +53578,7 @@
     </row>
     <row r="78">
       <c r="A78" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B78" s="6">
         <v>44704.0</v>
@@ -52713,7 +53593,7 @@
     </row>
     <row r="79">
       <c r="A79" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B79" s="6">
         <v>44704.0</v>
@@ -52728,7 +53608,7 @@
     </row>
     <row r="80">
       <c r="A80" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B80" s="6">
         <v>44704.0</v>
@@ -52743,7 +53623,7 @@
     </row>
     <row r="81">
       <c r="A81" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B81" s="6">
         <v>44704.0</v>
@@ -52758,7 +53638,7 @@
     </row>
     <row r="82">
       <c r="A82" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B82" s="6">
         <v>44704.0</v>
@@ -52773,7 +53653,7 @@
     </row>
     <row r="83">
       <c r="A83" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B83" s="6">
         <v>44704.0</v>
@@ -52788,7 +53668,7 @@
     </row>
     <row r="84">
       <c r="A84" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B84" s="6">
         <v>44704.0</v>
@@ -52803,7 +53683,7 @@
     </row>
     <row r="85">
       <c r="A85" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B85" s="6">
         <v>44704.0</v>
@@ -52818,7 +53698,7 @@
     </row>
     <row r="86">
       <c r="A86" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B86" s="6">
         <v>44704.0</v>
@@ -52833,7 +53713,7 @@
     </row>
     <row r="87">
       <c r="A87" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B87" s="6">
         <v>44704.0</v>
@@ -52848,7 +53728,7 @@
     </row>
     <row r="88">
       <c r="A88" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B88" s="6">
         <v>44704.0</v>
@@ -52863,7 +53743,7 @@
     </row>
     <row r="89">
       <c r="A89" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B89" s="6">
         <v>44704.0</v>
@@ -52878,7 +53758,7 @@
     </row>
     <row r="90">
       <c r="A90" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B90" s="6">
         <v>44704.0</v>
@@ -52893,7 +53773,7 @@
     </row>
     <row r="91">
       <c r="A91" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B91" s="6">
         <v>44704.0</v>
@@ -52908,7 +53788,7 @@
     </row>
     <row r="92">
       <c r="A92" s="7" t="s">
-        <v>2081</v>
+        <v>2117</v>
       </c>
       <c r="B92" s="6">
         <v>44704.0</v>
@@ -52923,7 +53803,7 @@
     </row>
     <row r="93">
       <c r="A93" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B93" s="6">
         <v>44705.0</v>
@@ -52938,7 +53818,7 @@
     </row>
     <row r="94">
       <c r="A94" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B94" s="6">
         <v>44705.0</v>
@@ -52953,7 +53833,7 @@
     </row>
     <row r="95">
       <c r="A95" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B95" s="6">
         <v>44705.0</v>
@@ -52968,7 +53848,7 @@
     </row>
     <row r="96">
       <c r="A96" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B96" s="6">
         <v>44705.0</v>
@@ -52983,7 +53863,7 @@
     </row>
     <row r="97">
       <c r="A97" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B97" s="6">
         <v>44705.0</v>
@@ -52998,7 +53878,7 @@
     </row>
     <row r="98">
       <c r="A98" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B98" s="6">
         <v>44705.0</v>
@@ -53013,7 +53893,7 @@
     </row>
     <row r="99">
       <c r="A99" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B99" s="6">
         <v>44705.0</v>
@@ -53028,7 +53908,7 @@
     </row>
     <row r="100">
       <c r="A100" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B100" s="6">
         <v>44705.0</v>
@@ -53043,7 +53923,7 @@
     </row>
     <row r="101">
       <c r="A101" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B101" s="6">
         <v>44705.0</v>
@@ -53058,7 +53938,7 @@
     </row>
     <row r="102">
       <c r="A102" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B102" s="6">
         <v>44705.0</v>
@@ -53073,7 +53953,7 @@
     </row>
     <row r="103">
       <c r="A103" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B103" s="6">
         <v>44705.0</v>
@@ -53088,7 +53968,7 @@
     </row>
     <row r="104">
       <c r="A104" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B104" s="6">
         <v>44705.0</v>
@@ -53103,7 +53983,7 @@
     </row>
     <row r="105">
       <c r="A105" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B105" s="6">
         <v>44705.0</v>
@@ -53118,7 +53998,7 @@
     </row>
     <row r="106">
       <c r="A106" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B106" s="6">
         <v>44705.0</v>
@@ -53133,7 +54013,7 @@
     </row>
     <row r="107">
       <c r="A107" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B107" s="6">
         <v>44705.0</v>
@@ -53148,7 +54028,7 @@
     </row>
     <row r="108">
       <c r="A108" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B108" s="6">
         <v>44705.0</v>
@@ -53163,7 +54043,7 @@
     </row>
     <row r="109">
       <c r="A109" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B109" s="6">
         <v>44705.0</v>
@@ -53178,7 +54058,7 @@
     </row>
     <row r="110">
       <c r="A110" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B110" s="6">
         <v>44705.0</v>
@@ -53193,7 +54073,7 @@
     </row>
     <row r="111">
       <c r="A111" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B111" s="6">
         <v>44705.0</v>
@@ -53208,7 +54088,7 @@
     </row>
     <row r="112">
       <c r="A112" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B112" s="6">
         <v>44705.0</v>
@@ -53223,7 +54103,7 @@
     </row>
     <row r="113">
       <c r="A113" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B113" s="6">
         <v>44705.0</v>
@@ -53238,7 +54118,7 @@
     </row>
     <row r="114">
       <c r="A114" s="7" t="s">
-        <v>2082</v>
+        <v>2118</v>
       </c>
       <c r="B114" s="6">
         <v>44705.0</v>
@@ -53253,7 +54133,7 @@
     </row>
     <row r="115">
       <c r="A115" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B115" s="6">
         <v>44708.0</v>
@@ -53268,7 +54148,7 @@
     </row>
     <row r="116">
       <c r="A116" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B116" s="6">
         <v>44708.0</v>
@@ -53283,7 +54163,7 @@
     </row>
     <row r="117">
       <c r="A117" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B117" s="6">
         <v>44708.0</v>
@@ -53298,7 +54178,7 @@
     </row>
     <row r="118">
       <c r="A118" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B118" s="6">
         <v>44708.0</v>
@@ -53310,12 +54190,12 @@
         <v>39.0</v>
       </c>
       <c r="E118" s="29" t="s">
-        <v>2080</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B119" s="6">
         <v>44708.0</v>
@@ -53330,7 +54210,7 @@
     </row>
     <row r="120">
       <c r="A120" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B120" s="6">
         <v>44708.0</v>
@@ -53345,7 +54225,7 @@
     </row>
     <row r="121">
       <c r="A121" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B121" s="6">
         <v>44708.0</v>
@@ -53360,7 +54240,7 @@
     </row>
     <row r="122">
       <c r="A122" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B122" s="6">
         <v>44708.0</v>
@@ -53375,7 +54255,7 @@
     </row>
     <row r="123">
       <c r="A123" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B123" s="6">
         <v>44708.0</v>
@@ -53390,7 +54270,7 @@
     </row>
     <row r="124">
       <c r="A124" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B124" s="6">
         <v>44708.0</v>
@@ -53405,7 +54285,7 @@
     </row>
     <row r="125">
       <c r="A125" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B125" s="6">
         <v>44708.0</v>
@@ -53420,7 +54300,7 @@
     </row>
     <row r="126">
       <c r="A126" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B126" s="6">
         <v>44708.0</v>
@@ -53435,7 +54315,7 @@
     </row>
     <row r="127">
       <c r="A127" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B127" s="6">
         <v>44708.0</v>
@@ -53447,12 +54327,12 @@
         <v>11.0</v>
       </c>
       <c r="E127" s="29" t="s">
-        <v>2080</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B128" s="6">
         <v>44708.0</v>
@@ -53467,7 +54347,7 @@
     </row>
     <row r="129">
       <c r="A129" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B129" s="6">
         <v>44708.0</v>
@@ -53479,12 +54359,12 @@
         <v>40.0</v>
       </c>
       <c r="E129" s="29" t="s">
-        <v>2080</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B130" s="6">
         <v>44708.0</v>
@@ -53499,7 +54379,7 @@
     </row>
     <row r="131">
       <c r="A131" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B131" s="6">
         <v>44708.0</v>
@@ -53514,7 +54394,7 @@
     </row>
     <row r="132">
       <c r="A132" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B132" s="6">
         <v>44708.0</v>
@@ -53529,7 +54409,7 @@
     </row>
     <row r="133">
       <c r="A133" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="B133" s="6">
         <v>44708.0</v>
@@ -53544,7 +54424,7 @@
     </row>
     <row r="134">
       <c r="A134" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B134" s="6">
         <v>44713.0</v>
@@ -53556,12 +54436,12 @@
         <v>1298</v>
       </c>
       <c r="E134" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B135" s="6">
         <v>44713.0</v>
@@ -53573,12 +54453,12 @@
         <v>1300</v>
       </c>
       <c r="E135" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B136" s="6">
         <v>44713.0</v>
@@ -53590,12 +54470,12 @@
         <v>1302</v>
       </c>
       <c r="E136" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B137" s="6">
         <v>44713.0</v>
@@ -53607,12 +54487,12 @@
         <v>1304</v>
       </c>
       <c r="E137" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B138" s="6">
         <v>44713.0</v>
@@ -53624,12 +54504,12 @@
         <v>1306</v>
       </c>
       <c r="E138" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B139" s="6">
         <v>44713.0</v>
@@ -53641,12 +54521,12 @@
         <v>1309</v>
       </c>
       <c r="E139" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B140" s="6">
         <v>44713.0</v>
@@ -53658,12 +54538,12 @@
         <v>1312</v>
       </c>
       <c r="E140" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B141" s="6">
         <v>44713.0</v>
@@ -53675,12 +54555,12 @@
         <v>1315</v>
       </c>
       <c r="E141" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B142" s="6">
         <v>44713.0</v>
@@ -53692,12 +54572,12 @@
         <v>1318</v>
       </c>
       <c r="E142" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B143" s="6">
         <v>44713.0</v>
@@ -53709,12 +54589,12 @@
         <v>1321</v>
       </c>
       <c r="E143" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B144" s="6">
         <v>44713.0</v>
@@ -53726,12 +54606,12 @@
         <v>1323</v>
       </c>
       <c r="E144" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B145" s="6">
         <v>44713.0</v>
@@ -53743,12 +54623,12 @@
         <v>1325</v>
       </c>
       <c r="E145" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B146" s="6">
         <v>44713.0</v>
@@ -53760,12 +54640,12 @@
         <v>1327</v>
       </c>
       <c r="E146" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B147" s="6">
         <v>44713.0</v>
@@ -53777,12 +54657,12 @@
         <v>1329</v>
       </c>
       <c r="E147" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B148" s="6">
         <v>44713.0</v>
@@ -53794,12 +54674,12 @@
         <v>1331</v>
       </c>
       <c r="E148" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B149" s="6">
         <v>44713.0</v>
@@ -53811,12 +54691,12 @@
         <v>1333</v>
       </c>
       <c r="E149" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B150" s="6">
         <v>44713.0</v>
@@ -53828,12 +54708,12 @@
         <v>1335</v>
       </c>
       <c r="E150" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B151" s="6">
         <v>44713.0</v>
@@ -53845,12 +54725,12 @@
         <v>1337</v>
       </c>
       <c r="E151" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B152" s="6">
         <v>44713.0</v>
@@ -53862,12 +54742,12 @@
         <v>1340</v>
       </c>
       <c r="E152" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B153" s="6">
         <v>44713.0</v>
@@ -53879,12 +54759,12 @@
         <v>1342</v>
       </c>
       <c r="E153" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B154" s="6">
         <v>44713.0</v>
@@ -53896,12 +54776,12 @@
         <v>1344</v>
       </c>
       <c r="E154" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B155" s="6">
         <v>44713.0</v>
@@ -53913,12 +54793,12 @@
         <v>1346</v>
       </c>
       <c r="E155" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B156" s="6">
         <v>44713.0</v>
@@ -53930,12 +54810,12 @@
         <v>1348</v>
       </c>
       <c r="E156" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="7" t="s">
-        <v>2084</v>
+        <v>2120</v>
       </c>
       <c r="B157" s="6">
         <v>44713.0</v>
@@ -53947,7 +54827,7 @@
         <v>1350</v>
       </c>
       <c r="E157" s="29" t="s">
-        <v>2085</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="158">
@@ -56499,22 +57379,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2086</v>
+        <v>2122</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2087</v>
+        <v>2123</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2088</v>
+        <v>2124</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2089</v>
+        <v>2125</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>2090</v>
+        <v>2126</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>2091</v>
+        <v>2127</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>12</v>
@@ -56525,17 +57405,17 @@
         <v>44690.0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2092</v>
+        <v>2128</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>2065</v>
+        <v>2101</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7" t="s">
-        <v>2093</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="3">
@@ -56543,7 +57423,7 @@
         <v>44692.0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2094</v>
+        <v>2130</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="7" t="s">
@@ -56564,10 +57444,10 @@
         <v>44694.0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2095</v>
+        <v>2131</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>2071</v>
+        <v>2107</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
@@ -56582,7 +57462,7 @@
         <v>2.5</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>2096</v>
+        <v>2132</v>
       </c>
     </row>
     <row r="5">
@@ -56590,10 +57470,10 @@
         <v>44695.0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2097</v>
+        <v>2133</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2075</v>
+        <v>2111</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -56613,10 +57493,10 @@
         <v>44697.0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2098</v>
+        <v>2134</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>2099</v>
+        <v>2135</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -56636,10 +57516,10 @@
         <v>44698.0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>2083</v>
+        <v>2119</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>2100</v>
+        <v>2136</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -56659,10 +57539,10 @@
         <v>44726.0</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>2101</v>
+        <v>2137</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>2102</v>
+        <v>2138</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>1353</v>

</xml_diff>

<commit_message>
Updated everything for 19Jun2022 (CBE)
</commit_message>
<xml_diff>
--- a/Data/Genotype_Samples_2022.xlsx
+++ b/Data/Genotype_Samples_2022.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7181" uniqueCount="2139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7535" uniqueCount="2224">
   <si>
     <t>Date</t>
   </si>
@@ -6276,6 +6276,261 @@
   </si>
   <si>
     <t>G1370</t>
+  </si>
+  <si>
+    <t>CBE_001</t>
+  </si>
+  <si>
+    <t>G1392</t>
+  </si>
+  <si>
+    <t>CBE_002</t>
+  </si>
+  <si>
+    <t>CBE_003</t>
+  </si>
+  <si>
+    <t>G2343</t>
+  </si>
+  <si>
+    <t>CBE_004</t>
+  </si>
+  <si>
+    <t>CBE_005</t>
+  </si>
+  <si>
+    <t>CBE_006</t>
+  </si>
+  <si>
+    <t>*Tag used for multiple corals; maybe ofra?</t>
+  </si>
+  <si>
+    <t>CBE_007</t>
+  </si>
+  <si>
+    <t>G2344</t>
+  </si>
+  <si>
+    <t>CBE_008</t>
+  </si>
+  <si>
+    <t>CBE_009</t>
+  </si>
+  <si>
+    <t>G2345</t>
+  </si>
+  <si>
+    <t>CBE_010</t>
+  </si>
+  <si>
+    <t>CBE_011</t>
+  </si>
+  <si>
+    <t>CBE_012</t>
+  </si>
+  <si>
+    <t>*Tag used for multiple corals; 4-5ft from tag</t>
+  </si>
+  <si>
+    <t>CBE_013</t>
+  </si>
+  <si>
+    <t>G1092</t>
+  </si>
+  <si>
+    <t>CBE_014</t>
+  </si>
+  <si>
+    <t>CBE_015</t>
+  </si>
+  <si>
+    <t>*Tag used for multiple corals; maybe ofav?</t>
+  </si>
+  <si>
+    <t>CBE_016</t>
+  </si>
+  <si>
+    <t>G1094</t>
+  </si>
+  <si>
+    <t>CBE_017</t>
+  </si>
+  <si>
+    <t>CBE_018</t>
+  </si>
+  <si>
+    <t>*Tag used for multiple corals; disease</t>
+  </si>
+  <si>
+    <t>CBE_019</t>
+  </si>
+  <si>
+    <t>G2342</t>
+  </si>
+  <si>
+    <t>CBE_020</t>
+  </si>
+  <si>
+    <t>CBE_021</t>
+  </si>
+  <si>
+    <t>CBE_022</t>
+  </si>
+  <si>
+    <t>CBE_023</t>
+  </si>
+  <si>
+    <t>CBE_024</t>
+  </si>
+  <si>
+    <t>G2400</t>
+  </si>
+  <si>
+    <t>CBE_025</t>
+  </si>
+  <si>
+    <t>CBE_026</t>
+  </si>
+  <si>
+    <t>CBE_027</t>
+  </si>
+  <si>
+    <t>G1095</t>
+  </si>
+  <si>
+    <t>CBE_028</t>
+  </si>
+  <si>
+    <t>CBE_029</t>
+  </si>
+  <si>
+    <t>CBE_030</t>
+  </si>
+  <si>
+    <t>G2334</t>
+  </si>
+  <si>
+    <t>CBE_031</t>
+  </si>
+  <si>
+    <t>CBE_032</t>
+  </si>
+  <si>
+    <t>G1248</t>
+  </si>
+  <si>
+    <t>CBE_033</t>
+  </si>
+  <si>
+    <t>CBE_034</t>
+  </si>
+  <si>
+    <t>G1249</t>
+  </si>
+  <si>
+    <t>CBE_035</t>
+  </si>
+  <si>
+    <t>CBE_036</t>
+  </si>
+  <si>
+    <t>CBE_037</t>
+  </si>
+  <si>
+    <t>G1250</t>
+  </si>
+  <si>
+    <t>CBE_038</t>
+  </si>
+  <si>
+    <t>CBE_039</t>
+  </si>
+  <si>
+    <t>G1687</t>
+  </si>
+  <si>
+    <t>CBE_040</t>
+  </si>
+  <si>
+    <t>CBE_041</t>
+  </si>
+  <si>
+    <t>G1688</t>
+  </si>
+  <si>
+    <t>CBE_042</t>
+  </si>
+  <si>
+    <t>CBE_043</t>
+  </si>
+  <si>
+    <t>G1680</t>
+  </si>
+  <si>
+    <t>*Tag used for multiple corals; MAYBE OFRA?</t>
+  </si>
+  <si>
+    <t>CBE_044</t>
+  </si>
+  <si>
+    <t>CBE_045</t>
+  </si>
+  <si>
+    <t>CBE_046</t>
+  </si>
+  <si>
+    <t>G1673</t>
+  </si>
+  <si>
+    <t>CBE_047</t>
+  </si>
+  <si>
+    <t>CBE_048</t>
+  </si>
+  <si>
+    <t>CBE_049</t>
+  </si>
+  <si>
+    <t>G1813</t>
+  </si>
+  <si>
+    <t>CBE_050</t>
+  </si>
+  <si>
+    <t>CBE_051</t>
+  </si>
+  <si>
+    <t>G1814</t>
+  </si>
+  <si>
+    <t>CBE_052</t>
+  </si>
+  <si>
+    <t>CBE_053</t>
+  </si>
+  <si>
+    <t>G1815</t>
+  </si>
+  <si>
+    <t>CBE_054</t>
+  </si>
+  <si>
+    <t>CBE_055</t>
+  </si>
+  <si>
+    <t>CBE_056</t>
+  </si>
+  <si>
+    <t>G1821</t>
+  </si>
+  <si>
+    <t>CBE_057</t>
+  </si>
+  <si>
+    <t>CBE_058</t>
+  </si>
+  <si>
+    <t>CBE_059</t>
   </si>
   <si>
     <t>Site_ID</t>
@@ -49090,6 +49345,9 @@
       <c r="C1284" s="7" t="s">
         <v>2080</v>
       </c>
+      <c r="D1284" s="7">
+        <v>113.0</v>
+      </c>
       <c r="E1284" s="8">
         <v>0.4736111111111111</v>
       </c>
@@ -49177,240 +49435,2069 @@
       </c>
     </row>
     <row r="1287">
-      <c r="A1287" s="24"/>
-      <c r="B1287" s="7"/>
+      <c r="A1287" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1287" s="7" t="s">
+        <v>2087</v>
+      </c>
+      <c r="C1287" s="7" t="s">
+        <v>2088</v>
+      </c>
+      <c r="D1287" s="7">
+        <v>113.0</v>
+      </c>
+      <c r="E1287" s="8">
+        <v>0.5013888888888889</v>
+      </c>
+      <c r="F1287" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1287" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1287" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1287" s="11">
+        <v>17.7741564251482</v>
+      </c>
+      <c r="K1287" s="11">
+        <v>-64.8125196900219</v>
+      </c>
+      <c r="M1287" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1288">
-      <c r="A1288" s="24"/>
-      <c r="B1288" s="7"/>
+      <c r="A1288" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1288" s="7" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C1288" s="7" t="s">
+        <v>2088</v>
+      </c>
+      <c r="D1288" s="7">
+        <v>72.0</v>
+      </c>
+      <c r="E1288" s="8">
+        <v>0.5013888888888889</v>
+      </c>
+      <c r="F1288" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1288" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1288" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1288" s="11">
+        <v>17.7741564251482</v>
+      </c>
+      <c r="K1288" s="11">
+        <v>-64.8125196900219</v>
+      </c>
+      <c r="M1288" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1289">
-      <c r="A1289" s="24"/>
-      <c r="B1289" s="7"/>
+      <c r="A1289" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1289" s="7" t="s">
+        <v>2090</v>
+      </c>
+      <c r="C1289" s="7" t="s">
+        <v>2091</v>
+      </c>
+      <c r="D1289" s="7">
+        <v>21.0</v>
+      </c>
+      <c r="E1289" s="8">
+        <v>0.5048611111111111</v>
+      </c>
+      <c r="F1289" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1289" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1289" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1289" s="11">
+        <v>17.7740425989032</v>
+      </c>
+      <c r="K1289" s="11">
+        <v>-64.8125653713942</v>
+      </c>
+      <c r="M1289" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1290">
-      <c r="A1290" s="24"/>
-      <c r="B1290" s="7"/>
+      <c r="A1290" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1290" s="7" t="s">
+        <v>2092</v>
+      </c>
+      <c r="C1290" s="7" t="s">
+        <v>2091</v>
+      </c>
+      <c r="D1290" s="7">
+        <v>47.0</v>
+      </c>
+      <c r="E1290" s="8">
+        <v>0.5048611111111111</v>
+      </c>
+      <c r="F1290" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1290" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1290" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1290" s="11">
+        <v>17.7740425989032</v>
+      </c>
+      <c r="K1290" s="11">
+        <v>-64.8125653713942</v>
+      </c>
+      <c r="M1290" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1291">
-      <c r="A1291" s="24"/>
-      <c r="B1291" s="7"/>
+      <c r="A1291" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1291" s="7" t="s">
+        <v>2093</v>
+      </c>
+      <c r="C1291" s="7" t="s">
+        <v>2091</v>
+      </c>
+      <c r="D1291" s="7">
+        <v>84.0</v>
+      </c>
+      <c r="E1291" s="8">
+        <v>0.5048611111111111</v>
+      </c>
+      <c r="F1291" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1291" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1291" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1291" s="11">
+        <v>17.7740425989032</v>
+      </c>
+      <c r="K1291" s="11">
+        <v>-64.8125653713942</v>
+      </c>
+      <c r="M1291" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1292">
-      <c r="A1292" s="24"/>
-      <c r="B1292" s="7"/>
+      <c r="A1292" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1292" s="7" t="s">
+        <v>2094</v>
+      </c>
+      <c r="C1292" s="7" t="s">
+        <v>2091</v>
+      </c>
+      <c r="D1292" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="E1292" s="8">
+        <v>0.5111111111111111</v>
+      </c>
+      <c r="F1292" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1292" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1292" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1292" s="11">
+        <v>17.7740533277392</v>
+      </c>
+      <c r="K1292" s="11">
+        <v>-64.8126666247845</v>
+      </c>
+      <c r="M1292" s="7" t="s">
+        <v>2095</v>
+      </c>
     </row>
     <row r="1293">
-      <c r="A1293" s="24"/>
-      <c r="B1293" s="7"/>
+      <c r="A1293" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1293" s="7" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C1293" s="7" t="s">
+        <v>2097</v>
+      </c>
+      <c r="D1293" s="7">
+        <v>76.0</v>
+      </c>
+      <c r="E1293" s="8">
+        <v>0.5111111111111111</v>
+      </c>
+      <c r="F1293" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1293" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1293" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1293" s="11">
+        <v>17.7740533277392</v>
+      </c>
+      <c r="K1293" s="11">
+        <v>-64.8126666247845</v>
+      </c>
+      <c r="M1293" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1294">
-      <c r="A1294" s="24"/>
-      <c r="B1294" s="7"/>
+      <c r="A1294" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1294" s="7" t="s">
+        <v>2098</v>
+      </c>
+      <c r="C1294" s="7" t="s">
+        <v>2097</v>
+      </c>
+      <c r="D1294" s="7">
+        <v>79.0</v>
+      </c>
+      <c r="E1294" s="8">
+        <v>0.5111111111111111</v>
+      </c>
+      <c r="F1294" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1294" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1294" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1294" s="11">
+        <v>17.7740533277392</v>
+      </c>
+      <c r="K1294" s="11">
+        <v>-64.8126666247845</v>
+      </c>
+      <c r="M1294" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1295">
-      <c r="A1295" s="24"/>
-      <c r="B1295" s="7"/>
+      <c r="A1295" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1295" s="7" t="s">
+        <v>2099</v>
+      </c>
+      <c r="C1295" s="7" t="s">
+        <v>2100</v>
+      </c>
+      <c r="D1295" s="7">
+        <v>44.0</v>
+      </c>
+      <c r="E1295" s="8">
+        <v>0.5166666666666667</v>
+      </c>
+      <c r="F1295" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1295" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1295" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1295" s="11">
+        <v>17.7740880288184</v>
+      </c>
+      <c r="K1295" s="11">
+        <v>-64.8127294052392</v>
+      </c>
+      <c r="M1295" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1296">
-      <c r="A1296" s="24"/>
-      <c r="B1296" s="7"/>
+      <c r="A1296" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1296" s="7" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C1296" s="7" t="s">
+        <v>2100</v>
+      </c>
+      <c r="D1296" s="7">
+        <v>45.0</v>
+      </c>
+      <c r="E1296" s="8">
+        <v>0.5166666666666667</v>
+      </c>
+      <c r="F1296" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1296" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1296" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1296" s="11">
+        <v>17.7740880288184</v>
+      </c>
+      <c r="K1296" s="11">
+        <v>-64.8127294052392</v>
+      </c>
+      <c r="M1296" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1297">
-      <c r="A1297" s="24"/>
-      <c r="B1297" s="7"/>
+      <c r="A1297" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1297" s="7" t="s">
+        <v>2102</v>
+      </c>
+      <c r="C1297" s="7" t="s">
+        <v>2100</v>
+      </c>
+      <c r="D1297" s="7">
+        <v>28.0</v>
+      </c>
+      <c r="E1297" s="8">
+        <v>0.5166666666666667</v>
+      </c>
+      <c r="F1297" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1297" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1297" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1297" s="11">
+        <v>17.7740880288184</v>
+      </c>
+      <c r="K1297" s="11">
+        <v>-64.8127294052392</v>
+      </c>
+      <c r="M1297" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1298">
-      <c r="A1298" s="24"/>
-      <c r="B1298" s="7"/>
+      <c r="A1298" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1298" s="7" t="s">
+        <v>2103</v>
+      </c>
+      <c r="C1298" s="7" t="s">
+        <v>2100</v>
+      </c>
+      <c r="D1298" s="7">
+        <v>12.0</v>
+      </c>
+      <c r="E1298" s="8">
+        <v>0.5166666666666667</v>
+      </c>
+      <c r="F1298" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1298" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1298" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1298" s="11">
+        <v>17.7740880288184</v>
+      </c>
+      <c r="K1298" s="11">
+        <v>-64.8127294052392</v>
+      </c>
+      <c r="M1298" s="7" t="s">
+        <v>2104</v>
+      </c>
     </row>
     <row r="1299">
-      <c r="A1299" s="24"/>
-      <c r="B1299" s="7"/>
+      <c r="A1299" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1299" s="7" t="s">
+        <v>2105</v>
+      </c>
+      <c r="C1299" s="7" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D1299" s="7">
+        <v>8.0</v>
+      </c>
+      <c r="E1299" s="8">
+        <v>0.525</v>
+      </c>
+      <c r="F1299" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1299" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1299" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1299" s="11">
+        <v>17.773931119591</v>
+      </c>
+      <c r="K1299" s="11">
+        <v>-64.8127095401287</v>
+      </c>
+      <c r="M1299" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1300">
-      <c r="A1300" s="24"/>
-      <c r="B1300" s="7"/>
+      <c r="A1300" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1300" s="7" t="s">
+        <v>2107</v>
+      </c>
+      <c r="C1300" s="7" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D1300" s="7">
+        <v>90.0</v>
+      </c>
+      <c r="E1300" s="8">
+        <v>0.525</v>
+      </c>
+      <c r="F1300" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1300" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1300" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1300" s="11">
+        <v>17.773931119591</v>
+      </c>
+      <c r="K1300" s="11">
+        <v>-64.8127095401287</v>
+      </c>
+      <c r="M1300" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1301">
-      <c r="A1301" s="24"/>
-      <c r="B1301" s="7"/>
+      <c r="A1301" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1301" s="7" t="s">
+        <v>2108</v>
+      </c>
+      <c r="C1301" s="7" t="s">
+        <v>2106</v>
+      </c>
+      <c r="D1301" s="7">
+        <v>49.0</v>
+      </c>
+      <c r="E1301" s="8">
+        <v>0.525</v>
+      </c>
+      <c r="F1301" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1301" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1301" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1301" s="11">
+        <v>17.773931119591</v>
+      </c>
+      <c r="K1301" s="11">
+        <v>-64.8127095401287</v>
+      </c>
+      <c r="M1301" s="7" t="s">
+        <v>2109</v>
+      </c>
     </row>
     <row r="1302">
-      <c r="A1302" s="24"/>
-      <c r="B1302" s="7"/>
+      <c r="A1302" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1302" s="7" t="s">
+        <v>2110</v>
+      </c>
+      <c r="C1302" s="7" t="s">
+        <v>2111</v>
+      </c>
+      <c r="D1302" s="7">
+        <v>81.0</v>
+      </c>
+      <c r="E1302" s="8">
+        <v>0.5305555555555556</v>
+      </c>
+      <c r="F1302" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1302" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1302" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1302" s="11">
+        <v>17.7739307004958</v>
+      </c>
+      <c r="K1302" s="11">
+        <v>-64.8127145692706</v>
+      </c>
+      <c r="M1302" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1303">
-      <c r="A1303" s="24"/>
-      <c r="B1303" s="7"/>
+      <c r="A1303" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1303" s="7" t="s">
+        <v>2112</v>
+      </c>
+      <c r="C1303" s="7" t="s">
+        <v>2111</v>
+      </c>
+      <c r="D1303" s="7">
+        <v>9.0</v>
+      </c>
+      <c r="E1303" s="8">
+        <v>0.5305555555555556</v>
+      </c>
+      <c r="F1303" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1303" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1303" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1303" s="11">
+        <v>17.7739307004958</v>
+      </c>
+      <c r="K1303" s="11">
+        <v>-64.8127145692706</v>
+      </c>
+      <c r="M1303" s="7" t="s">
+        <v>2095</v>
+      </c>
     </row>
     <row r="1304">
-      <c r="A1304" s="24"/>
-      <c r="B1304" s="7"/>
+      <c r="A1304" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1304" s="7" t="s">
+        <v>2113</v>
+      </c>
+      <c r="C1304" s="7" t="s">
+        <v>2111</v>
+      </c>
+      <c r="D1304" s="7">
+        <v>29.0</v>
+      </c>
+      <c r="E1304" s="8">
+        <v>0.5305555555555556</v>
+      </c>
+      <c r="F1304" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1304" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1304" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1304" s="11">
+        <v>17.7739307004958</v>
+      </c>
+      <c r="K1304" s="11">
+        <v>-64.8127145692706</v>
+      </c>
+      <c r="M1304" s="7" t="s">
+        <v>2114</v>
+      </c>
     </row>
     <row r="1305">
-      <c r="A1305" s="24"/>
-      <c r="B1305" s="7"/>
+      <c r="A1305" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1305" s="7" t="s">
+        <v>2115</v>
+      </c>
+      <c r="C1305" s="7" t="s">
+        <v>2116</v>
+      </c>
+      <c r="D1305" s="7">
+        <v>35.0</v>
+      </c>
+      <c r="E1305" s="8">
+        <v>0.5361111111111111</v>
+      </c>
+      <c r="F1305" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1305" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1305" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1305" s="11">
+        <v>17.7738813310862</v>
+      </c>
+      <c r="K1305" s="11">
+        <v>-64.812773829326</v>
+      </c>
+      <c r="M1305" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1306">
-      <c r="A1306" s="24"/>
-      <c r="B1306" s="7"/>
+      <c r="A1306" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1306" s="7" t="s">
+        <v>2117</v>
+      </c>
+      <c r="C1306" s="7" t="s">
+        <v>2116</v>
+      </c>
+      <c r="D1306" s="7">
+        <v>75.0</v>
+      </c>
+      <c r="E1306" s="8">
+        <v>0.5361111111111111</v>
+      </c>
+      <c r="F1306" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1306" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1306" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1306" s="11">
+        <v>17.7738813310862</v>
+      </c>
+      <c r="K1306" s="11">
+        <v>-64.812773829326</v>
+      </c>
+      <c r="M1306" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1307">
-      <c r="A1307" s="24"/>
-      <c r="B1307" s="7"/>
+      <c r="A1307" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1307" s="7" t="s">
+        <v>2118</v>
+      </c>
+      <c r="C1307" s="7" t="s">
+        <v>2116</v>
+      </c>
+      <c r="D1307" s="7">
+        <v>27.0</v>
+      </c>
+      <c r="E1307" s="8">
+        <v>0.5361111111111111</v>
+      </c>
+      <c r="F1307" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1307" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1307" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1307" s="11">
+        <v>17.7738813310862</v>
+      </c>
+      <c r="K1307" s="11">
+        <v>-64.812773829326</v>
+      </c>
+      <c r="M1307" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1308">
-      <c r="A1308" s="24"/>
-      <c r="B1308" s="7"/>
+      <c r="A1308" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1308" s="7" t="s">
+        <v>2119</v>
+      </c>
+      <c r="C1308" s="7" t="s">
+        <v>2116</v>
+      </c>
+      <c r="D1308" s="7">
+        <v>101.0</v>
+      </c>
+      <c r="E1308" s="8">
+        <v>0.5361111111111111</v>
+      </c>
+      <c r="F1308" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1308" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1308" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1308" s="11">
+        <v>17.7738813310862</v>
+      </c>
+      <c r="K1308" s="11">
+        <v>-64.812773829326</v>
+      </c>
+      <c r="M1308" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1309">
-      <c r="A1309" s="24"/>
-      <c r="B1309" s="7"/>
+      <c r="A1309" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1309" s="7" t="s">
+        <v>2120</v>
+      </c>
+      <c r="C1309" s="7" t="s">
+        <v>2116</v>
+      </c>
+      <c r="D1309" s="7">
+        <v>104.0</v>
+      </c>
+      <c r="E1309" s="8">
+        <v>0.5361111111111111</v>
+      </c>
+      <c r="F1309" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1309" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1309" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1309" s="11">
+        <v>17.7738813310862</v>
+      </c>
+      <c r="K1309" s="11">
+        <v>-64.812773829326</v>
+      </c>
+      <c r="M1309" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1310">
-      <c r="A1310" s="24"/>
-      <c r="B1310" s="7"/>
+      <c r="A1310" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1310" s="7" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C1310" s="7" t="s">
+        <v>2122</v>
+      </c>
+      <c r="D1310" s="7">
+        <v>77.0</v>
+      </c>
+      <c r="E1310" s="8">
+        <v>0.5465277777777777</v>
+      </c>
+      <c r="F1310" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1310" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1310" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1310" s="11">
+        <v>17.7738169580698</v>
+      </c>
+      <c r="K1310" s="11">
+        <v>-64.8127914313227</v>
+      </c>
+      <c r="M1310" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1311">
-      <c r="A1311" s="24"/>
-      <c r="B1311" s="7"/>
+      <c r="A1311" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1311" s="7" t="s">
+        <v>2123</v>
+      </c>
+      <c r="C1311" s="7" t="s">
+        <v>2122</v>
+      </c>
+      <c r="D1311" s="7">
+        <v>73.0</v>
+      </c>
+      <c r="E1311" s="8">
+        <v>0.5465277777777777</v>
+      </c>
+      <c r="F1311" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1311" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1311" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1311" s="11">
+        <v>17.7738169580698</v>
+      </c>
+      <c r="K1311" s="11">
+        <v>-64.8127914313227</v>
+      </c>
+      <c r="M1311" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1312">
-      <c r="A1312" s="24"/>
-      <c r="B1312" s="7"/>
+      <c r="A1312" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1312" s="7" t="s">
+        <v>2124</v>
+      </c>
+      <c r="C1312" s="7" t="s">
+        <v>2122</v>
+      </c>
+      <c r="D1312" s="7">
+        <v>71.0</v>
+      </c>
+      <c r="E1312" s="8">
+        <v>0.5465277777777777</v>
+      </c>
+      <c r="F1312" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1312" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1312" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1312" s="11">
+        <v>17.7738169580698</v>
+      </c>
+      <c r="K1312" s="11">
+        <v>-64.8127914313227</v>
+      </c>
+      <c r="M1312" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1313">
-      <c r="A1313" s="24"/>
-      <c r="B1313" s="7"/>
+      <c r="A1313" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1313" s="7" t="s">
+        <v>2125</v>
+      </c>
+      <c r="C1313" s="7" t="s">
+        <v>2126</v>
+      </c>
+      <c r="D1313" s="7">
+        <v>218.0</v>
+      </c>
+      <c r="E1313" s="8">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="F1313" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1313" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1313" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1313" s="11">
+        <v>17.7737949974835</v>
+      </c>
+      <c r="K1313" s="11">
+        <v>-64.8128112126142</v>
+      </c>
+      <c r="M1313" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1314">
-      <c r="A1314" s="24"/>
-      <c r="B1314" s="7"/>
+      <c r="A1314" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1314" s="7" t="s">
+        <v>2127</v>
+      </c>
+      <c r="C1314" s="7" t="s">
+        <v>2126</v>
+      </c>
+      <c r="D1314" s="7">
+        <v>102.0</v>
+      </c>
+      <c r="E1314" s="8">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="F1314" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1314" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1314" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1314" s="11">
+        <v>17.7737949974835</v>
+      </c>
+      <c r="K1314" s="11">
+        <v>-64.8128112126142</v>
+      </c>
+      <c r="M1314" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1315">
-      <c r="A1315" s="24"/>
-      <c r="B1315" s="7"/>
+      <c r="A1315" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1315" s="7" t="s">
+        <v>2128</v>
+      </c>
+      <c r="C1315" s="7" t="s">
+        <v>2126</v>
+      </c>
+      <c r="D1315" s="7">
+        <v>108.0</v>
+      </c>
+      <c r="E1315" s="8">
+        <v>0.5534722222222223</v>
+      </c>
+      <c r="F1315" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1315" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1315" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1315" s="11">
+        <v>17.7737949974835</v>
+      </c>
+      <c r="K1315" s="11">
+        <v>-64.8128112126142</v>
+      </c>
+      <c r="M1315" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1316">
-      <c r="A1316" s="24"/>
-      <c r="B1316" s="7"/>
+      <c r="A1316" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1316" s="7" t="s">
+        <v>2129</v>
+      </c>
+      <c r="C1316" s="7" t="s">
+        <v>2130</v>
+      </c>
+      <c r="D1316" s="7">
+        <v>115.0</v>
+      </c>
+      <c r="E1316" s="8">
+        <v>0.5569444444444445</v>
+      </c>
+      <c r="F1316" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1316" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1316" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1316" s="11">
+        <v>17.7738100849092</v>
+      </c>
+      <c r="K1316" s="11">
+        <v>-64.8128307424486</v>
+      </c>
+      <c r="M1316" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1317">
-      <c r="A1317" s="24"/>
-      <c r="B1317" s="7"/>
+      <c r="A1317" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1317" s="7" t="s">
+        <v>2131</v>
+      </c>
+      <c r="C1317" s="7" t="s">
+        <v>2130</v>
+      </c>
+      <c r="D1317" s="7">
+        <v>120.0</v>
+      </c>
+      <c r="E1317" s="8">
+        <v>0.5569444444444445</v>
+      </c>
+      <c r="F1317" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1317" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1317" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1317" s="11">
+        <v>17.7738100849092</v>
+      </c>
+      <c r="K1317" s="11">
+        <v>-64.8128307424486</v>
+      </c>
+      <c r="M1317" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1318">
-      <c r="A1318" s="24"/>
-      <c r="B1318" s="7"/>
+      <c r="A1318" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1318" s="7" t="s">
+        <v>2132</v>
+      </c>
+      <c r="C1318" s="7" t="s">
+        <v>2133</v>
+      </c>
+      <c r="D1318" s="7">
+        <v>52.0</v>
+      </c>
+      <c r="E1318" s="8">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="F1318" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1318" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1318" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1318" s="11">
+        <v>17.7740512322634</v>
+      </c>
+      <c r="K1318" s="11">
+        <v>-64.8126670438796</v>
+      </c>
+      <c r="M1318" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1319">
-      <c r="A1319" s="24"/>
-      <c r="B1319" s="7"/>
+      <c r="A1319" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1319" s="7" t="s">
+        <v>2134</v>
+      </c>
+      <c r="C1319" s="7" t="s">
+        <v>2133</v>
+      </c>
+      <c r="D1319" s="7">
+        <v>53.0</v>
+      </c>
+      <c r="E1319" s="8">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="F1319" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1319" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1319" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1319" s="11">
+        <v>17.7740512322634</v>
+      </c>
+      <c r="K1319" s="11">
+        <v>-64.8126670438796</v>
+      </c>
+      <c r="M1319" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1320">
-      <c r="A1320" s="24"/>
-      <c r="B1320" s="7"/>
+      <c r="A1320" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1320" s="7" t="s">
+        <v>2135</v>
+      </c>
+      <c r="C1320" s="7" t="s">
+        <v>2136</v>
+      </c>
+      <c r="D1320" s="7">
+        <v>59.0</v>
+      </c>
+      <c r="E1320" s="8">
+        <v>0.5145833333333333</v>
+      </c>
+      <c r="F1320" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1320" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1320" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1320" s="11">
+        <v>17.7740921359509</v>
+      </c>
+      <c r="K1320" s="11">
+        <v>-64.8127265553921</v>
+      </c>
+      <c r="M1320" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1321">
-      <c r="A1321" s="24"/>
-      <c r="B1321" s="7"/>
+      <c r="A1321" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1321" s="7" t="s">
+        <v>2137</v>
+      </c>
+      <c r="C1321" s="7" t="s">
+        <v>2136</v>
+      </c>
+      <c r="D1321" s="7">
+        <v>58.0</v>
+      </c>
+      <c r="E1321" s="8">
+        <v>0.5145833333333333</v>
+      </c>
+      <c r="F1321" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1321" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1321" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1321" s="11">
+        <v>17.7740921359509</v>
+      </c>
+      <c r="K1321" s="11">
+        <v>-64.8127265553921</v>
+      </c>
+      <c r="M1321" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1322">
-      <c r="A1322" s="24"/>
-      <c r="B1322" s="7"/>
+      <c r="A1322" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1322" s="7" t="s">
+        <v>2138</v>
+      </c>
+      <c r="C1322" s="7" t="s">
+        <v>2136</v>
+      </c>
+      <c r="D1322" s="7">
+        <v>60.0</v>
+      </c>
+      <c r="E1322" s="8">
+        <v>0.5145833333333333</v>
+      </c>
+      <c r="F1322" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1322" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1322" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1322" s="11">
+        <v>17.7740921359509</v>
+      </c>
+      <c r="K1322" s="11">
+        <v>-64.8127265553921</v>
+      </c>
+      <c r="M1322" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1323">
-      <c r="A1323" s="24"/>
-      <c r="B1323" s="7"/>
+      <c r="A1323" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1323" s="7" t="s">
+        <v>2139</v>
+      </c>
+      <c r="C1323" s="7" t="s">
+        <v>2140</v>
+      </c>
+      <c r="D1323" s="7">
+        <v>57.0</v>
+      </c>
+      <c r="E1323" s="8">
+        <v>0.5215277777777778</v>
+      </c>
+      <c r="F1323" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1323" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1323" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1323" s="11">
+        <v>17.7739343885332</v>
+      </c>
+      <c r="K1323" s="11">
+        <v>-64.8127095401287</v>
+      </c>
+      <c r="M1323" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1324">
-      <c r="A1324" s="24"/>
-      <c r="B1324" s="7"/>
+      <c r="A1324" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1324" s="7" t="s">
+        <v>2141</v>
+      </c>
+      <c r="C1324" s="7" t="s">
+        <v>2140</v>
+      </c>
+      <c r="D1324" s="7">
+        <v>56.0</v>
+      </c>
+      <c r="E1324" s="8">
+        <v>0.5215277777777778</v>
+      </c>
+      <c r="F1324" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1324" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1324" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1324" s="11">
+        <v>17.7739343885332</v>
+      </c>
+      <c r="K1324" s="11">
+        <v>-64.8127095401287</v>
+      </c>
+      <c r="M1324" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1325">
-      <c r="A1325" s="24"/>
-      <c r="B1325" s="7"/>
+      <c r="A1325" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1325" s="7" t="s">
+        <v>2142</v>
+      </c>
+      <c r="C1325" s="7" t="s">
+        <v>2143</v>
+      </c>
+      <c r="D1325" s="7">
+        <v>54.0</v>
+      </c>
+      <c r="E1325" s="8">
+        <v>0.5263888888888889</v>
+      </c>
+      <c r="F1325" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1325" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1325" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1325" s="11">
+        <v>17.7739305328578</v>
+      </c>
+      <c r="K1325" s="11">
+        <v>-64.8127094563097</v>
+      </c>
+      <c r="M1325" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1326">
-      <c r="A1326" s="24"/>
-      <c r="B1326" s="7"/>
+      <c r="A1326" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1326" s="7" t="s">
+        <v>2144</v>
+      </c>
+      <c r="C1326" s="7" t="s">
+        <v>2143</v>
+      </c>
+      <c r="D1326" s="7">
+        <v>55.0</v>
+      </c>
+      <c r="E1326" s="8">
+        <v>0.5263888888888889</v>
+      </c>
+      <c r="F1326" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1326" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1326" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1326" s="11">
+        <v>17.7739305328578</v>
+      </c>
+      <c r="K1326" s="11">
+        <v>-64.8127094563097</v>
+      </c>
+      <c r="M1326" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1327">
-      <c r="A1327" s="24"/>
-      <c r="B1327" s="7"/>
+      <c r="A1327" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1327" s="7" t="s">
+        <v>2145</v>
+      </c>
+      <c r="C1327" s="7" t="s">
+        <v>2146</v>
+      </c>
+      <c r="D1327" s="7">
+        <v>61.0</v>
+      </c>
+      <c r="E1327" s="8">
+        <v>0.5319444444444444</v>
+      </c>
+      <c r="F1327" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1327" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1327" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1327" s="11">
+        <v>17.7738779783249</v>
+      </c>
+      <c r="K1327" s="11">
+        <v>-64.81276310049</v>
+      </c>
+      <c r="M1327" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1328">
-      <c r="A1328" s="24"/>
-      <c r="B1328" s="7"/>
+      <c r="A1328" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1328" s="7" t="s">
+        <v>2147</v>
+      </c>
+      <c r="C1328" s="7" t="s">
+        <v>2146</v>
+      </c>
+      <c r="D1328" s="7">
+        <v>62.0</v>
+      </c>
+      <c r="E1328" s="8">
+        <v>0.5319444444444444</v>
+      </c>
+      <c r="F1328" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1328" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1328" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1328" s="11">
+        <v>17.7738779783249</v>
+      </c>
+      <c r="K1328" s="11">
+        <v>-64.81276310049</v>
+      </c>
+      <c r="M1328" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1329">
-      <c r="A1329" s="24"/>
-      <c r="B1329" s="7"/>
+      <c r="A1329" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1329" s="7" t="s">
+        <v>2148</v>
+      </c>
+      <c r="C1329" s="7" t="s">
+        <v>2149</v>
+      </c>
+      <c r="D1329" s="7">
+        <v>63.0</v>
+      </c>
+      <c r="E1329" s="8">
+        <v>0.5361111111111111</v>
+      </c>
+      <c r="F1329" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1329" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1329" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1329" s="11">
+        <v>17.7738813310862</v>
+      </c>
+      <c r="K1329" s="11">
+        <v>-64.812773829326</v>
+      </c>
+      <c r="M1329" s="7" t="s">
+        <v>2150</v>
+      </c>
     </row>
     <row r="1330">
-      <c r="A1330" s="24"/>
-      <c r="B1330" s="7"/>
+      <c r="A1330" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1330" s="7" t="s">
+        <v>2151</v>
+      </c>
+      <c r="C1330" s="7" t="s">
+        <v>2149</v>
+      </c>
+      <c r="D1330" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="E1330" s="8">
+        <v>0.5361111111111111</v>
+      </c>
+      <c r="F1330" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1330" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1330" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1330" s="11">
+        <v>17.7738813310862</v>
+      </c>
+      <c r="K1330" s="11">
+        <v>-64.812773829326</v>
+      </c>
+      <c r="M1330" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1331">
-      <c r="A1331" s="24"/>
-      <c r="B1331" s="7"/>
+      <c r="A1331" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1331" s="7" t="s">
+        <v>2152</v>
+      </c>
+      <c r="C1331" s="7" t="s">
+        <v>2149</v>
+      </c>
+      <c r="D1331" s="7">
+        <v>46.0</v>
+      </c>
+      <c r="E1331" s="8">
+        <v>0.5361111111111111</v>
+      </c>
+      <c r="F1331" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1331" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1331" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1331" s="11">
+        <v>17.7738813310862</v>
+      </c>
+      <c r="K1331" s="11">
+        <v>-64.812773829326</v>
+      </c>
+      <c r="M1331" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1332">
-      <c r="A1332" s="24"/>
-      <c r="B1332" s="7"/>
+      <c r="A1332" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1332" s="7" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C1332" s="7" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D1332" s="7">
+        <v>64.0</v>
+      </c>
+      <c r="E1332" s="8">
+        <v>0.5409722222222222</v>
+      </c>
+      <c r="F1332" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1332" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1332" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1332" s="11">
+        <v>17.7738768886775</v>
+      </c>
+      <c r="K1332" s="11">
+        <v>-64.8127766791731</v>
+      </c>
+      <c r="M1332" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1333">
-      <c r="A1333" s="24"/>
-      <c r="B1333" s="7"/>
+      <c r="A1333" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1333" s="7" t="s">
+        <v>2155</v>
+      </c>
+      <c r="C1333" s="7" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D1333" s="7">
+        <v>65.0</v>
+      </c>
+      <c r="E1333" s="8">
+        <v>0.5409722222222222</v>
+      </c>
+      <c r="F1333" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1333" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1333" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1333" s="11">
+        <v>17.7738768886775</v>
+      </c>
+      <c r="K1333" s="11">
+        <v>-64.8127766791731</v>
+      </c>
+      <c r="M1333" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1334">
-      <c r="A1334" s="24"/>
-      <c r="B1334" s="7"/>
+      <c r="A1334" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1334" s="7" t="s">
+        <v>2156</v>
+      </c>
+      <c r="C1334" s="7" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D1334" s="7">
+        <v>69.0</v>
+      </c>
+      <c r="E1334" s="8">
+        <v>0.5409722222222222</v>
+      </c>
+      <c r="F1334" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1334" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1334" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1334" s="11">
+        <v>17.7738768886775</v>
+      </c>
+      <c r="K1334" s="11">
+        <v>-64.8127766791731</v>
+      </c>
+      <c r="M1334" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1335">
-      <c r="A1335" s="24"/>
-      <c r="B1335" s="7"/>
+      <c r="A1335" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1335" s="7" t="s">
+        <v>2157</v>
+      </c>
+      <c r="C1335" s="7" t="s">
+        <v>2158</v>
+      </c>
+      <c r="D1335" s="7">
+        <v>66.0</v>
+      </c>
+      <c r="E1335" s="8">
+        <v>0.5472222222222223</v>
+      </c>
+      <c r="F1335" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1335" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1335" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1335" s="11">
+        <v>17.7738104201853</v>
+      </c>
+      <c r="K1335" s="11">
+        <v>-64.8127903416753</v>
+      </c>
+      <c r="M1335" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1336">
-      <c r="A1336" s="24"/>
-      <c r="B1336" s="7"/>
+      <c r="A1336" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1336" s="7" t="s">
+        <v>2159</v>
+      </c>
+      <c r="C1336" s="7" t="s">
+        <v>2158</v>
+      </c>
+      <c r="D1336" s="7">
+        <v>83.0</v>
+      </c>
+      <c r="E1336" s="8">
+        <v>0.5472222222222223</v>
+      </c>
+      <c r="F1336" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1336" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1336" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1336" s="11">
+        <v>17.7738104201853</v>
+      </c>
+      <c r="K1336" s="11">
+        <v>-64.8127903416753</v>
+      </c>
+      <c r="M1336" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1337">
-      <c r="A1337" s="24"/>
-      <c r="B1337" s="7"/>
+      <c r="A1337" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1337" s="7" t="s">
+        <v>2160</v>
+      </c>
+      <c r="C1337" s="7" t="s">
+        <v>2161</v>
+      </c>
+      <c r="D1337" s="7">
+        <v>67.0</v>
+      </c>
+      <c r="E1337" s="8">
+        <v>0.5513888888888889</v>
+      </c>
+      <c r="F1337" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1337" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1337" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1337" s="11">
+        <v>17.7738205622882</v>
+      </c>
+      <c r="K1337" s="11">
+        <v>-64.8127822112292</v>
+      </c>
+      <c r="M1337" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1338">
-      <c r="A1338" s="24"/>
-      <c r="B1338" s="7"/>
+      <c r="A1338" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1338" s="7" t="s">
+        <v>2162</v>
+      </c>
+      <c r="C1338" s="7" t="s">
+        <v>2161</v>
+      </c>
+      <c r="D1338" s="7">
+        <v>68.0</v>
+      </c>
+      <c r="E1338" s="8">
+        <v>0.5513888888888889</v>
+      </c>
+      <c r="F1338" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1338" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1338" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1338" s="11">
+        <v>17.7738205622882</v>
+      </c>
+      <c r="K1338" s="11">
+        <v>-64.8127822112292</v>
+      </c>
+      <c r="M1338" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1339">
-      <c r="A1339" s="24"/>
-      <c r="B1339" s="7"/>
+      <c r="A1339" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1339" s="7" t="s">
+        <v>2163</v>
+      </c>
+      <c r="C1339" s="7" t="s">
+        <v>2164</v>
+      </c>
+      <c r="D1339" s="7">
+        <v>70.0</v>
+      </c>
+      <c r="E1339" s="8">
+        <v>0.5576388888888889</v>
+      </c>
+      <c r="F1339" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1339" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1339" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1339" s="11">
+        <v>17.7738102525473</v>
+      </c>
+      <c r="K1339" s="11">
+        <v>-64.812824036926</v>
+      </c>
+      <c r="M1339" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1340">
-      <c r="A1340" s="24"/>
-      <c r="B1340" s="7"/>
+      <c r="A1340" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1340" s="7" t="s">
+        <v>2165</v>
+      </c>
+      <c r="C1340" s="7" t="s">
+        <v>2164</v>
+      </c>
+      <c r="D1340" s="7">
+        <v>82.0</v>
+      </c>
+      <c r="E1340" s="8">
+        <v>0.5576388888888889</v>
+      </c>
+      <c r="F1340" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1340" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1340" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1340" s="11">
+        <v>17.7738102525473</v>
+      </c>
+      <c r="K1340" s="11">
+        <v>-64.812824036926</v>
+      </c>
+      <c r="M1340" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1341">
-      <c r="A1341" s="24"/>
-      <c r="B1341" s="7"/>
+      <c r="A1341" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1341" s="7" t="s">
+        <v>2166</v>
+      </c>
+      <c r="C1341" s="7" t="s">
+        <v>2164</v>
+      </c>
+      <c r="D1341" s="7">
+        <v>78.0</v>
+      </c>
+      <c r="E1341" s="8">
+        <v>0.5576388888888889</v>
+      </c>
+      <c r="F1341" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1341" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1341" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1341" s="11">
+        <v>17.7738102525473</v>
+      </c>
+      <c r="K1341" s="11">
+        <v>-64.812824036926</v>
+      </c>
+      <c r="M1341" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1342">
-      <c r="A1342" s="24"/>
-      <c r="B1342" s="7"/>
+      <c r="A1342" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1342" s="7" t="s">
+        <v>2167</v>
+      </c>
+      <c r="C1342" s="7" t="s">
+        <v>2168</v>
+      </c>
+      <c r="D1342" s="7">
+        <v>87.0</v>
+      </c>
+      <c r="E1342" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="F1342" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1342" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1342" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1342" s="11">
+        <v>17.7737263496965</v>
+      </c>
+      <c r="K1342" s="11">
+        <v>-64.8128720652312</v>
+      </c>
+      <c r="M1342" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1343">
-      <c r="A1343" s="24"/>
-      <c r="B1343" s="7"/>
+      <c r="A1343" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1343" s="7" t="s">
+        <v>2169</v>
+      </c>
+      <c r="C1343" s="7" t="s">
+        <v>2168</v>
+      </c>
+      <c r="D1343" s="7">
+        <v>89.0</v>
+      </c>
+      <c r="E1343" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="F1343" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1343" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1343" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1343" s="11">
+        <v>17.7737263496965</v>
+      </c>
+      <c r="K1343" s="11">
+        <v>-64.8128720652312</v>
+      </c>
+      <c r="M1343" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1344">
-      <c r="A1344" s="24"/>
-      <c r="B1344" s="7"/>
+      <c r="A1344" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1344" s="7" t="s">
+        <v>2170</v>
+      </c>
+      <c r="C1344" s="7" t="s">
+        <v>2168</v>
+      </c>
+      <c r="D1344" s="7">
+        <v>51.0</v>
+      </c>
+      <c r="E1344" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="F1344" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1344" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1344" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1344" s="11">
+        <v>17.7737263496965</v>
+      </c>
+      <c r="K1344" s="11">
+        <v>-64.8128720652312</v>
+      </c>
+      <c r="M1344" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1345">
-      <c r="A1345" s="24"/>
-      <c r="B1345" s="7"/>
+      <c r="A1345" s="6">
+        <v>44731.0</v>
+      </c>
+      <c r="B1345" s="7" t="s">
+        <v>2171</v>
+      </c>
+      <c r="C1345" s="7" t="s">
+        <v>2168</v>
+      </c>
+      <c r="D1345" s="7">
+        <v>74.0</v>
+      </c>
+      <c r="E1345" s="8">
+        <v>0.5625</v>
+      </c>
+      <c r="F1345" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1345" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1345" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1345" s="11">
+        <v>17.7737263496965</v>
+      </c>
+      <c r="K1345" s="11">
+        <v>-64.8128720652312</v>
+      </c>
+      <c r="M1345" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1346">
       <c r="A1346" s="24"/>
@@ -52041,19 +54128,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>2087</v>
+        <v>2172</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2088</v>
+        <v>2173</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2089</v>
+        <v>2174</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2090</v>
+        <v>2175</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2091</v>
+        <v>2176</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>7</v>
@@ -52077,21 +54164,21 @@
         <v>51</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>2092</v>
+        <v>2177</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>145</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>2093</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>2094</v>
+        <v>2179</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2095</v>
+        <v>2180</v>
       </c>
       <c r="C2" s="7">
         <v>7.0</v>
@@ -52103,33 +54190,33 @@
         <v>44688.0</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>2096</v>
+        <v>2181</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>2096</v>
+        <v>2181</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>2096</v>
+        <v>2181</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>2096</v>
+        <v>2181</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>2096</v>
+        <v>2181</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>2097</v>
+        <v>2182</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>2098</v>
+        <v>2183</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>2099</v>
+        <v>2184</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2100</v>
+        <v>2185</v>
       </c>
       <c r="C3" s="7">
         <v>25.0</v>
@@ -52140,10 +54227,10 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>2101</v>
+        <v>2186</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="C4" s="7">
         <v>15.0</v>
@@ -52155,18 +54242,18 @@
         <v>44690.0</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>2103</v>
+        <v>2188</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>2104</v>
+        <v>2189</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2105</v>
+        <v>2190</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2106</v>
+        <v>2191</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>20</v>
@@ -52174,10 +54261,10 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>2107</v>
+        <v>2192</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2108</v>
+        <v>2193</v>
       </c>
       <c r="C6" s="7">
         <v>20.0</v>
@@ -52209,10 +54296,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>2109</v>
+        <v>2194</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2110</v>
+        <v>2195</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>78</v>
@@ -52244,7 +54331,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2094</v>
+        <v>2179</v>
       </c>
       <c r="C2" s="7">
         <v>2.0</v>
@@ -52273,7 +54360,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2101</v>
+        <v>2186</v>
       </c>
       <c r="C3" s="7">
         <v>5.0</v>
@@ -52302,7 +54389,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2099</v>
+        <v>2184</v>
       </c>
       <c r="F4" s="7">
         <v>17.0</v>
@@ -52325,7 +54412,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2107</v>
+        <v>2192</v>
       </c>
       <c r="F5" s="7">
         <v>6.0</v>
@@ -52348,7 +54435,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2111</v>
+        <v>2196</v>
       </c>
       <c r="F6" s="7">
         <v>11.0</v>
@@ -52391,16 +54478,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="26" t="s">
-        <v>2112</v>
+        <v>2197</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>2113</v>
+        <v>2198</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>2114</v>
+        <v>2199</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>12</v>
@@ -52430,7 +54517,7 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B2" s="6">
         <v>44690.0</v>
@@ -52445,7 +54532,7 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B3" s="6">
         <v>44690.0</v>
@@ -52460,7 +54547,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B4" s="6">
         <v>44690.0</v>
@@ -52475,7 +54562,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B5" s="6">
         <v>44690.0</v>
@@ -52490,7 +54577,7 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B6" s="6">
         <v>44690.0</v>
@@ -52505,7 +54592,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B7" s="6">
         <v>44690.0</v>
@@ -52520,7 +54607,7 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B8" s="6">
         <v>44690.0</v>
@@ -52535,7 +54622,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B9" s="6">
         <v>44690.0</v>
@@ -52550,7 +54637,7 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B10" s="6">
         <v>44690.0</v>
@@ -52565,7 +54652,7 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B11" s="6">
         <v>44690.0</v>
@@ -52580,7 +54667,7 @@
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B12" s="6">
         <v>44690.0</v>
@@ -52595,7 +54682,7 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B13" s="6">
         <v>44690.0</v>
@@ -52610,7 +54697,7 @@
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B14" s="6">
         <v>44690.0</v>
@@ -52625,7 +54712,7 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B15" s="6">
         <v>44690.0</v>
@@ -52640,7 +54727,7 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B16" s="6">
         <v>44690.0</v>
@@ -52655,7 +54742,7 @@
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B17" s="6">
         <v>44690.0</v>
@@ -52671,7 +54758,7 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B18" s="6">
         <v>44690.0</v>
@@ -52687,7 +54774,7 @@
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B19" s="6">
         <v>44690.0</v>
@@ -52702,7 +54789,7 @@
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B20" s="6">
         <v>44690.0</v>
@@ -52717,7 +54804,7 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B21" s="6">
         <v>44690.0</v>
@@ -52732,7 +54819,7 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B22" s="6">
         <v>44690.0</v>
@@ -52747,7 +54834,7 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B23" s="6">
         <v>44690.0</v>
@@ -52762,7 +54849,7 @@
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B24" s="6">
         <v>44690.0</v>
@@ -52777,7 +54864,7 @@
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B25" s="6">
         <v>44690.0</v>
@@ -52792,7 +54879,7 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B26" s="6">
         <v>44690.0</v>
@@ -52807,7 +54894,7 @@
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B27" s="6">
         <v>44690.0</v>
@@ -52822,7 +54909,7 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B28" s="6">
         <v>44690.0</v>
@@ -52837,7 +54924,7 @@
     </row>
     <row r="29">
       <c r="A29" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B29" s="6">
         <v>44690.0</v>
@@ -52852,7 +54939,7 @@
     </row>
     <row r="30">
       <c r="A30" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B30" s="6">
         <v>44690.0</v>
@@ -52867,7 +54954,7 @@
     </row>
     <row r="31">
       <c r="A31" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B31" s="6">
         <v>44690.0</v>
@@ -52882,7 +54969,7 @@
     </row>
     <row r="32">
       <c r="A32" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B32" s="6">
         <v>44690.0</v>
@@ -52897,7 +54984,7 @@
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B33" s="6">
         <v>44690.0</v>
@@ -52912,7 +54999,7 @@
     </row>
     <row r="34">
       <c r="A34" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B34" s="6">
         <v>44690.0</v>
@@ -52927,7 +55014,7 @@
     </row>
     <row r="35">
       <c r="A35" s="7" t="s">
-        <v>2102</v>
+        <v>2187</v>
       </c>
       <c r="B35" s="6">
         <v>44690.0</v>
@@ -52942,7 +55029,7 @@
     </row>
     <row r="36">
       <c r="A36" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B36" s="6">
         <v>44704.0</v>
@@ -52957,7 +55044,7 @@
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B37" s="6">
         <v>44704.0</v>
@@ -52972,7 +55059,7 @@
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B38" s="6">
         <v>44704.0</v>
@@ -52984,12 +55071,12 @@
         <v>22.0</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>2116</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B39" s="6">
         <v>44704.0</v>
@@ -53004,7 +55091,7 @@
     </row>
     <row r="40">
       <c r="A40" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B40" s="6">
         <v>44704.0</v>
@@ -53016,12 +55103,12 @@
         <v>34.0</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>2116</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B41" s="6">
         <v>44704.0</v>
@@ -53036,7 +55123,7 @@
     </row>
     <row r="42">
       <c r="A42" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B42" s="6">
         <v>44704.0</v>
@@ -53051,7 +55138,7 @@
     </row>
     <row r="43">
       <c r="A43" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B43" s="6">
         <v>44704.0</v>
@@ -53066,7 +55153,7 @@
     </row>
     <row r="44">
       <c r="A44" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B44" s="6">
         <v>44704.0</v>
@@ -53078,12 +55165,12 @@
         <v>6.0</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>2116</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B45" s="6">
         <v>44704.0</v>
@@ -53098,7 +55185,7 @@
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B46" s="6">
         <v>44704.0</v>
@@ -53113,7 +55200,7 @@
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B47" s="6">
         <v>44704.0</v>
@@ -53128,7 +55215,7 @@
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B48" s="6">
         <v>44704.0</v>
@@ -53143,7 +55230,7 @@
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B49" s="6">
         <v>44704.0</v>
@@ -53158,7 +55245,7 @@
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B50" s="6">
         <v>44704.0</v>
@@ -53173,7 +55260,7 @@
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B51" s="6">
         <v>44704.0</v>
@@ -53188,7 +55275,7 @@
     </row>
     <row r="52">
       <c r="A52" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B52" s="6">
         <v>44704.0</v>
@@ -53203,7 +55290,7 @@
     </row>
     <row r="53">
       <c r="A53" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B53" s="6">
         <v>44704.0</v>
@@ -53218,7 +55305,7 @@
     </row>
     <row r="54">
       <c r="A54" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B54" s="6">
         <v>44704.0</v>
@@ -53233,7 +55320,7 @@
     </row>
     <row r="55">
       <c r="A55" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B55" s="6">
         <v>44704.0</v>
@@ -53248,7 +55335,7 @@
     </row>
     <row r="56">
       <c r="A56" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B56" s="6">
         <v>44704.0</v>
@@ -53263,7 +55350,7 @@
     </row>
     <row r="57">
       <c r="A57" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B57" s="6">
         <v>44704.0</v>
@@ -53278,7 +55365,7 @@
     </row>
     <row r="58">
       <c r="A58" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B58" s="6">
         <v>44704.0</v>
@@ -53293,7 +55380,7 @@
     </row>
     <row r="59">
       <c r="A59" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B59" s="6">
         <v>44704.0</v>
@@ -53308,7 +55395,7 @@
     </row>
     <row r="60">
       <c r="A60" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B60" s="6">
         <v>44704.0</v>
@@ -53323,7 +55410,7 @@
     </row>
     <row r="61">
       <c r="A61" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B61" s="6">
         <v>44704.0</v>
@@ -53338,7 +55425,7 @@
     </row>
     <row r="62">
       <c r="A62" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B62" s="6">
         <v>44704.0</v>
@@ -53353,7 +55440,7 @@
     </row>
     <row r="63">
       <c r="A63" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B63" s="6">
         <v>44704.0</v>
@@ -53368,7 +55455,7 @@
     </row>
     <row r="64">
       <c r="A64" s="7" t="s">
-        <v>2115</v>
+        <v>2200</v>
       </c>
       <c r="B64" s="6">
         <v>44704.0</v>
@@ -53383,7 +55470,7 @@
     </row>
     <row r="65">
       <c r="A65" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B65" s="6">
         <v>44704.0</v>
@@ -53398,7 +55485,7 @@
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B66" s="6">
         <v>44704.0</v>
@@ -53413,7 +55500,7 @@
     </row>
     <row r="67">
       <c r="A67" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B67" s="6">
         <v>44704.0</v>
@@ -53428,7 +55515,7 @@
     </row>
     <row r="68">
       <c r="A68" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B68" s="6">
         <v>44704.0</v>
@@ -53443,7 +55530,7 @@
     </row>
     <row r="69">
       <c r="A69" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B69" s="6">
         <v>44704.0</v>
@@ -53458,7 +55545,7 @@
     </row>
     <row r="70">
       <c r="A70" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B70" s="6">
         <v>44704.0</v>
@@ -53473,7 +55560,7 @@
     </row>
     <row r="71">
       <c r="A71" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B71" s="6">
         <v>44704.0</v>
@@ -53488,7 +55575,7 @@
     </row>
     <row r="72">
       <c r="A72" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B72" s="6">
         <v>44704.0</v>
@@ -53503,7 +55590,7 @@
     </row>
     <row r="73">
       <c r="A73" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B73" s="6">
         <v>44704.0</v>
@@ -53518,7 +55605,7 @@
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B74" s="6">
         <v>44704.0</v>
@@ -53533,7 +55620,7 @@
     </row>
     <row r="75">
       <c r="A75" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B75" s="6">
         <v>44704.0</v>
@@ -53548,7 +55635,7 @@
     </row>
     <row r="76">
       <c r="A76" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B76" s="6">
         <v>44704.0</v>
@@ -53563,7 +55650,7 @@
     </row>
     <row r="77">
       <c r="A77" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B77" s="6">
         <v>44704.0</v>
@@ -53578,7 +55665,7 @@
     </row>
     <row r="78">
       <c r="A78" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B78" s="6">
         <v>44704.0</v>
@@ -53593,7 +55680,7 @@
     </row>
     <row r="79">
       <c r="A79" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B79" s="6">
         <v>44704.0</v>
@@ -53608,7 +55695,7 @@
     </row>
     <row r="80">
       <c r="A80" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B80" s="6">
         <v>44704.0</v>
@@ -53623,7 +55710,7 @@
     </row>
     <row r="81">
       <c r="A81" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B81" s="6">
         <v>44704.0</v>
@@ -53638,7 +55725,7 @@
     </row>
     <row r="82">
       <c r="A82" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B82" s="6">
         <v>44704.0</v>
@@ -53653,7 +55740,7 @@
     </row>
     <row r="83">
       <c r="A83" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B83" s="6">
         <v>44704.0</v>
@@ -53668,7 +55755,7 @@
     </row>
     <row r="84">
       <c r="A84" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B84" s="6">
         <v>44704.0</v>
@@ -53683,7 +55770,7 @@
     </row>
     <row r="85">
       <c r="A85" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B85" s="6">
         <v>44704.0</v>
@@ -53698,7 +55785,7 @@
     </row>
     <row r="86">
       <c r="A86" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B86" s="6">
         <v>44704.0</v>
@@ -53713,7 +55800,7 @@
     </row>
     <row r="87">
       <c r="A87" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B87" s="6">
         <v>44704.0</v>
@@ -53728,7 +55815,7 @@
     </row>
     <row r="88">
       <c r="A88" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B88" s="6">
         <v>44704.0</v>
@@ -53743,7 +55830,7 @@
     </row>
     <row r="89">
       <c r="A89" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B89" s="6">
         <v>44704.0</v>
@@ -53758,7 +55845,7 @@
     </row>
     <row r="90">
       <c r="A90" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B90" s="6">
         <v>44704.0</v>
@@ -53773,7 +55860,7 @@
     </row>
     <row r="91">
       <c r="A91" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B91" s="6">
         <v>44704.0</v>
@@ -53788,7 +55875,7 @@
     </row>
     <row r="92">
       <c r="A92" s="7" t="s">
-        <v>2117</v>
+        <v>2202</v>
       </c>
       <c r="B92" s="6">
         <v>44704.0</v>
@@ -53803,7 +55890,7 @@
     </row>
     <row r="93">
       <c r="A93" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B93" s="6">
         <v>44705.0</v>
@@ -53818,7 +55905,7 @@
     </row>
     <row r="94">
       <c r="A94" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B94" s="6">
         <v>44705.0</v>
@@ -53833,7 +55920,7 @@
     </row>
     <row r="95">
       <c r="A95" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B95" s="6">
         <v>44705.0</v>
@@ -53848,7 +55935,7 @@
     </row>
     <row r="96">
       <c r="A96" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B96" s="6">
         <v>44705.0</v>
@@ -53863,7 +55950,7 @@
     </row>
     <row r="97">
       <c r="A97" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B97" s="6">
         <v>44705.0</v>
@@ -53878,7 +55965,7 @@
     </row>
     <row r="98">
       <c r="A98" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B98" s="6">
         <v>44705.0</v>
@@ -53893,7 +55980,7 @@
     </row>
     <row r="99">
       <c r="A99" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B99" s="6">
         <v>44705.0</v>
@@ -53908,7 +55995,7 @@
     </row>
     <row r="100">
       <c r="A100" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B100" s="6">
         <v>44705.0</v>
@@ -53923,7 +56010,7 @@
     </row>
     <row r="101">
       <c r="A101" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B101" s="6">
         <v>44705.0</v>
@@ -53938,7 +56025,7 @@
     </row>
     <row r="102">
       <c r="A102" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B102" s="6">
         <v>44705.0</v>
@@ -53953,7 +56040,7 @@
     </row>
     <row r="103">
       <c r="A103" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B103" s="6">
         <v>44705.0</v>
@@ -53968,7 +56055,7 @@
     </row>
     <row r="104">
       <c r="A104" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B104" s="6">
         <v>44705.0</v>
@@ -53983,7 +56070,7 @@
     </row>
     <row r="105">
       <c r="A105" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B105" s="6">
         <v>44705.0</v>
@@ -53998,7 +56085,7 @@
     </row>
     <row r="106">
       <c r="A106" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B106" s="6">
         <v>44705.0</v>
@@ -54013,7 +56100,7 @@
     </row>
     <row r="107">
       <c r="A107" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B107" s="6">
         <v>44705.0</v>
@@ -54028,7 +56115,7 @@
     </row>
     <row r="108">
       <c r="A108" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B108" s="6">
         <v>44705.0</v>
@@ -54043,7 +56130,7 @@
     </row>
     <row r="109">
       <c r="A109" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B109" s="6">
         <v>44705.0</v>
@@ -54058,7 +56145,7 @@
     </row>
     <row r="110">
       <c r="A110" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B110" s="6">
         <v>44705.0</v>
@@ -54073,7 +56160,7 @@
     </row>
     <row r="111">
       <c r="A111" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B111" s="6">
         <v>44705.0</v>
@@ -54088,7 +56175,7 @@
     </row>
     <row r="112">
       <c r="A112" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B112" s="6">
         <v>44705.0</v>
@@ -54103,7 +56190,7 @@
     </row>
     <row r="113">
       <c r="A113" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B113" s="6">
         <v>44705.0</v>
@@ -54118,7 +56205,7 @@
     </row>
     <row r="114">
       <c r="A114" s="7" t="s">
-        <v>2118</v>
+        <v>2203</v>
       </c>
       <c r="B114" s="6">
         <v>44705.0</v>
@@ -54133,7 +56220,7 @@
     </row>
     <row r="115">
       <c r="A115" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B115" s="6">
         <v>44708.0</v>
@@ -54148,7 +56235,7 @@
     </row>
     <row r="116">
       <c r="A116" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B116" s="6">
         <v>44708.0</v>
@@ -54163,7 +56250,7 @@
     </row>
     <row r="117">
       <c r="A117" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B117" s="6">
         <v>44708.0</v>
@@ -54178,7 +56265,7 @@
     </row>
     <row r="118">
       <c r="A118" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B118" s="6">
         <v>44708.0</v>
@@ -54190,12 +56277,12 @@
         <v>39.0</v>
       </c>
       <c r="E118" s="29" t="s">
-        <v>2116</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B119" s="6">
         <v>44708.0</v>
@@ -54210,7 +56297,7 @@
     </row>
     <row r="120">
       <c r="A120" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B120" s="6">
         <v>44708.0</v>
@@ -54225,7 +56312,7 @@
     </row>
     <row r="121">
       <c r="A121" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B121" s="6">
         <v>44708.0</v>
@@ -54240,7 +56327,7 @@
     </row>
     <row r="122">
       <c r="A122" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B122" s="6">
         <v>44708.0</v>
@@ -54255,7 +56342,7 @@
     </row>
     <row r="123">
       <c r="A123" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B123" s="6">
         <v>44708.0</v>
@@ -54270,7 +56357,7 @@
     </row>
     <row r="124">
       <c r="A124" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B124" s="6">
         <v>44708.0</v>
@@ -54285,7 +56372,7 @@
     </row>
     <row r="125">
       <c r="A125" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B125" s="6">
         <v>44708.0</v>
@@ -54300,7 +56387,7 @@
     </row>
     <row r="126">
       <c r="A126" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B126" s="6">
         <v>44708.0</v>
@@ -54315,7 +56402,7 @@
     </row>
     <row r="127">
       <c r="A127" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B127" s="6">
         <v>44708.0</v>
@@ -54327,12 +56414,12 @@
         <v>11.0</v>
       </c>
       <c r="E127" s="29" t="s">
-        <v>2116</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B128" s="6">
         <v>44708.0</v>
@@ -54347,7 +56434,7 @@
     </row>
     <row r="129">
       <c r="A129" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B129" s="6">
         <v>44708.0</v>
@@ -54359,12 +56446,12 @@
         <v>40.0</v>
       </c>
       <c r="E129" s="29" t="s">
-        <v>2116</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B130" s="6">
         <v>44708.0</v>
@@ -54379,7 +56466,7 @@
     </row>
     <row r="131">
       <c r="A131" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B131" s="6">
         <v>44708.0</v>
@@ -54394,7 +56481,7 @@
     </row>
     <row r="132">
       <c r="A132" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B132" s="6">
         <v>44708.0</v>
@@ -54409,7 +56496,7 @@
     </row>
     <row r="133">
       <c r="A133" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="B133" s="6">
         <v>44708.0</v>
@@ -54424,7 +56511,7 @@
     </row>
     <row r="134">
       <c r="A134" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B134" s="6">
         <v>44713.0</v>
@@ -54436,12 +56523,12 @@
         <v>1298</v>
       </c>
       <c r="E134" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B135" s="6">
         <v>44713.0</v>
@@ -54453,12 +56540,12 @@
         <v>1300</v>
       </c>
       <c r="E135" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B136" s="6">
         <v>44713.0</v>
@@ -54470,12 +56557,12 @@
         <v>1302</v>
       </c>
       <c r="E136" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B137" s="6">
         <v>44713.0</v>
@@ -54487,12 +56574,12 @@
         <v>1304</v>
       </c>
       <c r="E137" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B138" s="6">
         <v>44713.0</v>
@@ -54504,12 +56591,12 @@
         <v>1306</v>
       </c>
       <c r="E138" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B139" s="6">
         <v>44713.0</v>
@@ -54521,12 +56608,12 @@
         <v>1309</v>
       </c>
       <c r="E139" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B140" s="6">
         <v>44713.0</v>
@@ -54538,12 +56625,12 @@
         <v>1312</v>
       </c>
       <c r="E140" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B141" s="6">
         <v>44713.0</v>
@@ -54555,12 +56642,12 @@
         <v>1315</v>
       </c>
       <c r="E141" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B142" s="6">
         <v>44713.0</v>
@@ -54572,12 +56659,12 @@
         <v>1318</v>
       </c>
       <c r="E142" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B143" s="6">
         <v>44713.0</v>
@@ -54589,12 +56676,12 @@
         <v>1321</v>
       </c>
       <c r="E143" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B144" s="6">
         <v>44713.0</v>
@@ -54606,12 +56693,12 @@
         <v>1323</v>
       </c>
       <c r="E144" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B145" s="6">
         <v>44713.0</v>
@@ -54623,12 +56710,12 @@
         <v>1325</v>
       </c>
       <c r="E145" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B146" s="6">
         <v>44713.0</v>
@@ -54640,12 +56727,12 @@
         <v>1327</v>
       </c>
       <c r="E146" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B147" s="6">
         <v>44713.0</v>
@@ -54657,12 +56744,12 @@
         <v>1329</v>
       </c>
       <c r="E147" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B148" s="6">
         <v>44713.0</v>
@@ -54674,12 +56761,12 @@
         <v>1331</v>
       </c>
       <c r="E148" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B149" s="6">
         <v>44713.0</v>
@@ -54691,12 +56778,12 @@
         <v>1333</v>
       </c>
       <c r="E149" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B150" s="6">
         <v>44713.0</v>
@@ -54708,12 +56795,12 @@
         <v>1335</v>
       </c>
       <c r="E150" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B151" s="6">
         <v>44713.0</v>
@@ -54725,12 +56812,12 @@
         <v>1337</v>
       </c>
       <c r="E151" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B152" s="6">
         <v>44713.0</v>
@@ -54742,12 +56829,12 @@
         <v>1340</v>
       </c>
       <c r="E152" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B153" s="6">
         <v>44713.0</v>
@@ -54759,12 +56846,12 @@
         <v>1342</v>
       </c>
       <c r="E153" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B154" s="6">
         <v>44713.0</v>
@@ -54776,12 +56863,12 @@
         <v>1344</v>
       </c>
       <c r="E154" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B155" s="6">
         <v>44713.0</v>
@@ -54793,12 +56880,12 @@
         <v>1346</v>
       </c>
       <c r="E155" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B156" s="6">
         <v>44713.0</v>
@@ -54810,12 +56897,12 @@
         <v>1348</v>
       </c>
       <c r="E156" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="7" t="s">
-        <v>2120</v>
+        <v>2205</v>
       </c>
       <c r="B157" s="6">
         <v>44713.0</v>
@@ -54827,7 +56914,7 @@
         <v>1350</v>
       </c>
       <c r="E157" s="29" t="s">
-        <v>2121</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="158">
@@ -57379,22 +59466,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2122</v>
+        <v>2207</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2123</v>
+        <v>2208</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2124</v>
+        <v>2209</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2125</v>
+        <v>2210</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>2126</v>
+        <v>2211</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>2127</v>
+        <v>2212</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>12</v>
@@ -57405,17 +59492,17 @@
         <v>44690.0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2128</v>
+        <v>2213</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>2101</v>
+        <v>2186</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7" t="s">
-        <v>2129</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="3">
@@ -57423,7 +59510,7 @@
         <v>44692.0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2130</v>
+        <v>2215</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="7" t="s">
@@ -57444,10 +59531,10 @@
         <v>44694.0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2131</v>
+        <v>2216</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>2107</v>
+        <v>2192</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
@@ -57462,7 +59549,7 @@
         <v>2.5</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>2132</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="5">
@@ -57470,10 +59557,10 @@
         <v>44695.0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2133</v>
+        <v>2218</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2111</v>
+        <v>2196</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -57493,10 +59580,10 @@
         <v>44697.0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2134</v>
+        <v>2219</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>2135</v>
+        <v>2220</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -57516,10 +59603,10 @@
         <v>44698.0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>2119</v>
+        <v>2204</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>2136</v>
+        <v>2221</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -57539,10 +59626,10 @@
         <v>44726.0</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>2137</v>
+        <v>2222</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>2138</v>
+        <v>2223</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>1353</v>

</xml_diff>

<commit_message>
Updated species counts and KML file for THO on 25Jun2022
</commit_message>
<xml_diff>
--- a/Data/Genotype_Samples_2022.xlsx
+++ b/Data/Genotype_Samples_2022.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8089" uniqueCount="2412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8349" uniqueCount="2484">
   <si>
     <t>Date</t>
   </si>
@@ -7095,6 +7095,222 @@
   </si>
   <si>
     <t>G1413</t>
+  </si>
+  <si>
+    <t>THO_001</t>
+  </si>
+  <si>
+    <t>G1651</t>
+  </si>
+  <si>
+    <t>THO_002</t>
+  </si>
+  <si>
+    <t>THO_003</t>
+  </si>
+  <si>
+    <t>G1654</t>
+  </si>
+  <si>
+    <t>THO_004</t>
+  </si>
+  <si>
+    <t>THO_005</t>
+  </si>
+  <si>
+    <t>THO_006</t>
+  </si>
+  <si>
+    <t>G1652</t>
+  </si>
+  <si>
+    <t>THO_007</t>
+  </si>
+  <si>
+    <t>THO_008</t>
+  </si>
+  <si>
+    <t>THO_009</t>
+  </si>
+  <si>
+    <t>G1653</t>
+  </si>
+  <si>
+    <t>THO_010</t>
+  </si>
+  <si>
+    <t>THO_011</t>
+  </si>
+  <si>
+    <t>THO_012</t>
+  </si>
+  <si>
+    <t>G1655</t>
+  </si>
+  <si>
+    <t>THO_013</t>
+  </si>
+  <si>
+    <t>THO_014</t>
+  </si>
+  <si>
+    <t>THO_015</t>
+  </si>
+  <si>
+    <t>G1661</t>
+  </si>
+  <si>
+    <t>THO_016</t>
+  </si>
+  <si>
+    <t>THO_017</t>
+  </si>
+  <si>
+    <t>THO_018</t>
+  </si>
+  <si>
+    <t>G1662</t>
+  </si>
+  <si>
+    <t>THO_019</t>
+  </si>
+  <si>
+    <t>THO_020</t>
+  </si>
+  <si>
+    <t>THO_021</t>
+  </si>
+  <si>
+    <t>G1663</t>
+  </si>
+  <si>
+    <t>THO_022</t>
+  </si>
+  <si>
+    <t>THO_023</t>
+  </si>
+  <si>
+    <t>THO_024</t>
+  </si>
+  <si>
+    <t>G1945</t>
+  </si>
+  <si>
+    <t>THO_025</t>
+  </si>
+  <si>
+    <t>THO_026</t>
+  </si>
+  <si>
+    <t>THO_027</t>
+  </si>
+  <si>
+    <t>G1944</t>
+  </si>
+  <si>
+    <t>THO_028</t>
+  </si>
+  <si>
+    <t>THO_029</t>
+  </si>
+  <si>
+    <t>THO_030</t>
+  </si>
+  <si>
+    <t>G1942</t>
+  </si>
+  <si>
+    <t>THO_031</t>
+  </si>
+  <si>
+    <t>THO_032</t>
+  </si>
+  <si>
+    <t>THO_033</t>
+  </si>
+  <si>
+    <t>G1941</t>
+  </si>
+  <si>
+    <t>THO_034</t>
+  </si>
+  <si>
+    <t>THO_035</t>
+  </si>
+  <si>
+    <t>THO_036</t>
+  </si>
+  <si>
+    <t>G1664</t>
+  </si>
+  <si>
+    <t>THO_037</t>
+  </si>
+  <si>
+    <t>THO_038</t>
+  </si>
+  <si>
+    <t>THO_039</t>
+  </si>
+  <si>
+    <t>G1665</t>
+  </si>
+  <si>
+    <t>THO_040</t>
+  </si>
+  <si>
+    <t>THO_041</t>
+  </si>
+  <si>
+    <t>THO_042</t>
+  </si>
+  <si>
+    <t>G1943</t>
+  </si>
+  <si>
+    <t>THO_043</t>
+  </si>
+  <si>
+    <t>THO_044</t>
+  </si>
+  <si>
+    <t>THO_045</t>
+  </si>
+  <si>
+    <t>G1671</t>
+  </si>
+  <si>
+    <t>THO_046</t>
+  </si>
+  <si>
+    <t>G1672</t>
+  </si>
+  <si>
+    <t>THO_047</t>
+  </si>
+  <si>
+    <t>G1935</t>
+  </si>
+  <si>
+    <t>THO_048</t>
+  </si>
+  <si>
+    <t>THO_049</t>
+  </si>
+  <si>
+    <t>G1934</t>
+  </si>
+  <si>
+    <t>THO_050</t>
+  </si>
+  <si>
+    <t>THO_051</t>
+  </si>
+  <si>
+    <t>THO_052</t>
+  </si>
+  <si>
+    <t>G1674</t>
   </si>
   <si>
     <t>Site_ID</t>
@@ -55486,206 +55702,1668 @@
       </c>
     </row>
     <row r="1452">
-      <c r="A1452" s="24"/>
+      <c r="A1452" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1452" s="7" t="s">
+        <v>2360</v>
+      </c>
+      <c r="C1452" s="7" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D1452" s="7">
+        <v>16.0</v>
+      </c>
+      <c r="E1452" s="8">
+        <v>0.46805555555555556</v>
+      </c>
+      <c r="F1452" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1452" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1452" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1452" s="11">
+        <v>17.737940736115</v>
+      </c>
+      <c r="K1452" s="11">
+        <v>-64.6041779313236</v>
+      </c>
     </row>
     <row r="1453">
-      <c r="A1453" s="24"/>
+      <c r="A1453" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1453" s="7" t="s">
+        <v>2362</v>
+      </c>
+      <c r="C1453" s="7" t="s">
+        <v>2361</v>
+      </c>
+      <c r="D1453" s="7">
+        <v>207.0</v>
+      </c>
+      <c r="E1453" s="8">
+        <v>0.46805555555555556</v>
+      </c>
+      <c r="F1453" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1453" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1453" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1453" s="11">
+        <v>17.737940736115</v>
+      </c>
+      <c r="K1453" s="11">
+        <v>-64.6041779313236</v>
+      </c>
     </row>
     <row r="1454">
-      <c r="A1454" s="24"/>
+      <c r="A1454" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1454" s="7" t="s">
+        <v>2363</v>
+      </c>
+      <c r="C1454" s="7" t="s">
+        <v>2364</v>
+      </c>
+      <c r="D1454" s="7">
+        <v>204.0</v>
+      </c>
+      <c r="E1454" s="8">
+        <v>0.47152777777777777</v>
+      </c>
+      <c r="F1454" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1454" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1454" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1454" s="11">
+        <v>17.7378968987614</v>
+      </c>
+      <c r="K1454" s="11">
+        <v>-64.6040979679674</v>
+      </c>
     </row>
     <row r="1455">
-      <c r="A1455" s="24"/>
+      <c r="A1455" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1455" s="7" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C1455" s="7" t="s">
+        <v>2364</v>
+      </c>
+      <c r="D1455" s="7">
+        <v>109.0</v>
+      </c>
+      <c r="E1455" s="8">
+        <v>0.47152777777777777</v>
+      </c>
+      <c r="F1455" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1455" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1455" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1455" s="11">
+        <v>17.7378968987614</v>
+      </c>
+      <c r="K1455" s="11">
+        <v>-64.6040979679674</v>
+      </c>
     </row>
     <row r="1456">
-      <c r="A1456" s="24"/>
+      <c r="A1456" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1456" s="7" t="s">
+        <v>2366</v>
+      </c>
+      <c r="C1456" s="7" t="s">
+        <v>2364</v>
+      </c>
+      <c r="D1456" s="7">
+        <v>219.0</v>
+      </c>
+      <c r="E1456" s="8">
+        <v>0.47152777777777777</v>
+      </c>
+      <c r="F1456" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1456" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1456" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1456" s="11">
+        <v>17.7378968987614</v>
+      </c>
+      <c r="K1456" s="11">
+        <v>-64.6040979679674</v>
+      </c>
     </row>
     <row r="1457">
-      <c r="A1457" s="24"/>
+      <c r="A1457" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1457" s="7" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C1457" s="7" t="s">
+        <v>2368</v>
+      </c>
+      <c r="D1457" s="7">
+        <v>85.0</v>
+      </c>
+      <c r="E1457" s="8">
+        <v>0.47638888888888886</v>
+      </c>
+      <c r="F1457" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1457" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1457" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1457" s="11">
+        <v>17.7378632873297</v>
+      </c>
+      <c r="K1457" s="11">
+        <v>-64.6040884964168</v>
+      </c>
     </row>
     <row r="1458">
-      <c r="A1458" s="24"/>
-      <c r="B1458" s="7"/>
+      <c r="A1458" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1458" s="7" t="s">
+        <v>2369</v>
+      </c>
+      <c r="C1458" s="7" t="s">
+        <v>2368</v>
+      </c>
+      <c r="D1458" s="7">
+        <v>34.0</v>
+      </c>
+      <c r="E1458" s="8">
+        <v>0.47638888888888886</v>
+      </c>
+      <c r="F1458" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1458" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1458" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1458" s="11">
+        <v>17.7378632873297</v>
+      </c>
+      <c r="K1458" s="11">
+        <v>-64.6040884964168</v>
+      </c>
     </row>
     <row r="1459">
-      <c r="A1459" s="24"/>
-      <c r="B1459" s="7"/>
+      <c r="A1459" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1459" s="7" t="s">
+        <v>2370</v>
+      </c>
+      <c r="C1459" s="7" t="s">
+        <v>2368</v>
+      </c>
+      <c r="D1459" s="7">
+        <v>106.0</v>
+      </c>
+      <c r="E1459" s="8">
+        <v>0.47638888888888886</v>
+      </c>
+      <c r="F1459" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1459" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1459" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1459" s="11">
+        <v>17.7378632873297</v>
+      </c>
+      <c r="K1459" s="11">
+        <v>-64.6040884964168</v>
+      </c>
     </row>
     <row r="1460">
-      <c r="A1460" s="24"/>
-      <c r="B1460" s="7"/>
+      <c r="A1460" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1460" s="7" t="s">
+        <v>2371</v>
+      </c>
+      <c r="C1460" s="7" t="s">
+        <v>2372</v>
+      </c>
+      <c r="D1460" s="7">
+        <v>201.0</v>
+      </c>
+      <c r="E1460" s="8">
+        <v>0.48125</v>
+      </c>
+      <c r="F1460" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1460" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1460" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1460" s="11">
+        <v>17.7378211263567</v>
+      </c>
+      <c r="K1460" s="11">
+        <v>-64.6040576510131</v>
+      </c>
     </row>
     <row r="1461">
-      <c r="A1461" s="24"/>
-      <c r="B1461" s="7"/>
+      <c r="A1461" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1461" s="7" t="s">
+        <v>2373</v>
+      </c>
+      <c r="C1461" s="7" t="s">
+        <v>2372</v>
+      </c>
+      <c r="D1461" s="7">
+        <v>25.0</v>
+      </c>
+      <c r="E1461" s="8">
+        <v>0.48125</v>
+      </c>
+      <c r="F1461" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1461" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1461" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1461" s="11">
+        <v>17.7378211263567</v>
+      </c>
+      <c r="K1461" s="11">
+        <v>-64.6040576510131</v>
+      </c>
     </row>
     <row r="1462">
-      <c r="A1462" s="24"/>
-      <c r="B1462" s="7"/>
+      <c r="A1462" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1462" s="7" t="s">
+        <v>2374</v>
+      </c>
+      <c r="C1462" s="7" t="s">
+        <v>2372</v>
+      </c>
+      <c r="D1462" s="7">
+        <v>73.0</v>
+      </c>
+      <c r="E1462" s="8">
+        <v>0.48125</v>
+      </c>
+      <c r="F1462" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1462" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1462" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1462" s="11">
+        <v>17.7378211263567</v>
+      </c>
+      <c r="K1462" s="11">
+        <v>-64.6040576510131</v>
+      </c>
     </row>
     <row r="1463">
-      <c r="A1463" s="24"/>
-      <c r="B1463" s="7"/>
+      <c r="A1463" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1463" s="7" t="s">
+        <v>2375</v>
+      </c>
+      <c r="C1463" s="7" t="s">
+        <v>2376</v>
+      </c>
+      <c r="D1463" s="7">
+        <v>20.0</v>
+      </c>
+      <c r="E1463" s="8">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="F1463" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1463" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1463" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1463" s="11">
+        <v>17.7377644646913</v>
+      </c>
+      <c r="K1463" s="11">
+        <v>-64.6040355227888</v>
+      </c>
     </row>
     <row r="1464">
-      <c r="A1464" s="24"/>
-      <c r="B1464" s="7"/>
+      <c r="A1464" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1464" s="7" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C1464" s="7" t="s">
+        <v>2376</v>
+      </c>
+      <c r="D1464" s="7">
+        <v>209.0</v>
+      </c>
+      <c r="E1464" s="8">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="F1464" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1464" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1464" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1464" s="11">
+        <v>17.7377644646913</v>
+      </c>
+      <c r="K1464" s="11">
+        <v>-64.6040355227888</v>
+      </c>
     </row>
     <row r="1465">
-      <c r="A1465" s="24"/>
-      <c r="B1465" s="7"/>
+      <c r="A1465" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1465" s="7" t="s">
+        <v>2378</v>
+      </c>
+      <c r="C1465" s="7" t="s">
+        <v>2376</v>
+      </c>
+      <c r="D1465" s="7">
+        <v>31.0</v>
+      </c>
+      <c r="E1465" s="8">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="F1465" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1465" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1465" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1465" s="11">
+        <v>17.7377644646913</v>
+      </c>
+      <c r="K1465" s="11">
+        <v>-64.6040355227888</v>
+      </c>
     </row>
     <row r="1466">
-      <c r="A1466" s="24"/>
-      <c r="B1466" s="7"/>
+      <c r="A1466" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1466" s="7" t="s">
+        <v>2379</v>
+      </c>
+      <c r="C1466" s="7" t="s">
+        <v>2380</v>
+      </c>
+      <c r="D1466" s="7">
+        <v>19.0</v>
+      </c>
+      <c r="E1466" s="8">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="F1466" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1466" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1466" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1466" s="11">
+        <v>17.7377297636122</v>
+      </c>
+      <c r="K1466" s="11">
+        <v>-64.6040692180395</v>
+      </c>
     </row>
     <row r="1467">
-      <c r="A1467" s="24"/>
-      <c r="B1467" s="7"/>
+      <c r="A1467" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1467" s="7" t="s">
+        <v>2381</v>
+      </c>
+      <c r="C1467" s="7" t="s">
+        <v>2380</v>
+      </c>
+      <c r="D1467" s="7">
+        <v>215.0</v>
+      </c>
+      <c r="E1467" s="8">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="F1467" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1467" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1467" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1467" s="11">
+        <v>17.7377297636122</v>
+      </c>
+      <c r="K1467" s="11">
+        <v>-64.6040692180395</v>
+      </c>
     </row>
     <row r="1468">
-      <c r="A1468" s="24"/>
-      <c r="B1468" s="7"/>
+      <c r="A1468" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1468" s="7" t="s">
+        <v>2382</v>
+      </c>
+      <c r="C1468" s="7" t="s">
+        <v>2380</v>
+      </c>
+      <c r="D1468" s="7">
+        <v>38.0</v>
+      </c>
+      <c r="E1468" s="8">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="F1468" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1468" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1468" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1468" s="11">
+        <v>17.7377297636122</v>
+      </c>
+      <c r="K1468" s="11">
+        <v>-64.6040692180395</v>
+      </c>
     </row>
     <row r="1469">
-      <c r="A1469" s="24"/>
-      <c r="B1469" s="7"/>
+      <c r="A1469" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1469" s="7" t="s">
+        <v>2383</v>
+      </c>
+      <c r="C1469" s="7" t="s">
+        <v>2384</v>
+      </c>
+      <c r="D1469" s="7">
+        <v>86.0</v>
+      </c>
+      <c r="E1469" s="8">
+        <v>0.49027777777777776</v>
+      </c>
+      <c r="F1469" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1469" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1469" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1469" s="11">
+        <v>17.7377620339394</v>
+      </c>
+      <c r="K1469" s="11">
+        <v>-64.6040841378272</v>
+      </c>
     </row>
     <row r="1470">
-      <c r="A1470" s="24"/>
-      <c r="B1470" s="7"/>
+      <c r="A1470" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1470" s="7" t="s">
+        <v>2385</v>
+      </c>
+      <c r="C1470" s="7" t="s">
+        <v>2384</v>
+      </c>
+      <c r="D1470" s="7">
+        <v>15.0</v>
+      </c>
+      <c r="E1470" s="8">
+        <v>0.49027777777777776</v>
+      </c>
+      <c r="F1470" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1470" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1470" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1470" s="11">
+        <v>17.7377620339394</v>
+      </c>
+      <c r="K1470" s="11">
+        <v>-64.6040841378272</v>
+      </c>
     </row>
     <row r="1471">
-      <c r="A1471" s="24"/>
-      <c r="B1471" s="7"/>
+      <c r="A1471" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1471" s="7" t="s">
+        <v>2386</v>
+      </c>
+      <c r="C1471" s="7" t="s">
+        <v>2384</v>
+      </c>
+      <c r="D1471" s="7">
+        <v>75.0</v>
+      </c>
+      <c r="E1471" s="8">
+        <v>0.49027777777777776</v>
+      </c>
+      <c r="F1471" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1471" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1471" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1471" s="11">
+        <v>17.7377620339394</v>
+      </c>
+      <c r="K1471" s="11">
+        <v>-64.6040841378272</v>
+      </c>
     </row>
     <row r="1472">
-      <c r="A1472" s="24"/>
-      <c r="B1472" s="7"/>
+      <c r="A1472" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1472" s="7" t="s">
+        <v>2387</v>
+      </c>
+      <c r="C1472" s="7" t="s">
+        <v>2388</v>
+      </c>
+      <c r="D1472" s="7">
+        <v>208.0</v>
+      </c>
+      <c r="E1472" s="8">
+        <v>0.49375</v>
+      </c>
+      <c r="F1472" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1472" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1472" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1472" s="11">
+        <v>17.7377782110125</v>
+      </c>
+      <c r="K1472" s="11">
+        <v>-64.6041248738766</v>
+      </c>
     </row>
     <row r="1473">
-      <c r="A1473" s="24"/>
-      <c r="B1473" s="7"/>
+      <c r="A1473" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1473" s="7" t="s">
+        <v>2389</v>
+      </c>
+      <c r="C1473" s="7" t="s">
+        <v>2388</v>
+      </c>
+      <c r="D1473" s="7">
+        <v>52.0</v>
+      </c>
+      <c r="E1473" s="8">
+        <v>0.49375</v>
+      </c>
+      <c r="F1473" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1473" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1473" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1473" s="11">
+        <v>17.7377782110125</v>
+      </c>
+      <c r="K1473" s="11">
+        <v>-64.6041248738766</v>
+      </c>
     </row>
     <row r="1474">
-      <c r="A1474" s="24"/>
-      <c r="B1474" s="7"/>
+      <c r="A1474" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1474" s="7" t="s">
+        <v>2390</v>
+      </c>
+      <c r="C1474" s="7" t="s">
+        <v>2388</v>
+      </c>
+      <c r="D1474" s="7">
+        <v>58.0</v>
+      </c>
+      <c r="E1474" s="8">
+        <v>0.49375</v>
+      </c>
+      <c r="F1474" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1474" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1474" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1474" s="11">
+        <v>17.7377782110125</v>
+      </c>
+      <c r="K1474" s="11">
+        <v>-64.6041248738766</v>
+      </c>
     </row>
     <row r="1475">
-      <c r="A1475" s="24"/>
-      <c r="B1475" s="7"/>
+      <c r="A1475" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1475" s="7" t="s">
+        <v>2391</v>
+      </c>
+      <c r="C1475" s="7" t="s">
+        <v>2392</v>
+      </c>
+      <c r="D1475" s="7">
+        <v>33.0</v>
+      </c>
+      <c r="E1475" s="8">
+        <v>0.49722222222222223</v>
+      </c>
+      <c r="F1475" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1475" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1475" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1475" s="11">
+        <v>17.7377729304135</v>
+      </c>
+      <c r="K1475" s="11">
+        <v>-64.6041493490338</v>
+      </c>
     </row>
     <row r="1476">
-      <c r="A1476" s="24"/>
-      <c r="B1476" s="7"/>
+      <c r="A1476" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1476" s="7" t="s">
+        <v>2393</v>
+      </c>
+      <c r="C1476" s="7" t="s">
+        <v>2392</v>
+      </c>
+      <c r="D1476" s="7">
+        <v>200.0</v>
+      </c>
+      <c r="E1476" s="8">
+        <v>0.49722222222222223</v>
+      </c>
+      <c r="F1476" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1476" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1476" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1476" s="11">
+        <v>17.7377729304135</v>
+      </c>
+      <c r="K1476" s="11">
+        <v>-64.6041493490338</v>
+      </c>
     </row>
     <row r="1477">
-      <c r="A1477" s="24"/>
-      <c r="B1477" s="7"/>
+      <c r="A1477" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1477" s="7" t="s">
+        <v>2394</v>
+      </c>
+      <c r="C1477" s="7" t="s">
+        <v>2392</v>
+      </c>
+      <c r="D1477" s="7">
+        <v>205.0</v>
+      </c>
+      <c r="E1477" s="8">
+        <v>0.49722222222222223</v>
+      </c>
+      <c r="F1477" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1477" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1477" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1477" s="11">
+        <v>17.7377729304135</v>
+      </c>
+      <c r="K1477" s="11">
+        <v>-64.6041493490338</v>
+      </c>
     </row>
     <row r="1478">
-      <c r="A1478" s="24"/>
-      <c r="B1478" s="7"/>
+      <c r="A1478" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1478" s="7" t="s">
+        <v>2395</v>
+      </c>
+      <c r="C1478" s="7" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D1478" s="7">
+        <v>210.0</v>
+      </c>
+      <c r="E1478" s="8">
+        <v>0.5013888888888889</v>
+      </c>
+      <c r="F1478" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1478" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1478" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1478" s="11">
+        <v>17.7378396503627</v>
+      </c>
+      <c r="K1478" s="11">
+        <v>-64.6041179168969</v>
+      </c>
     </row>
     <row r="1479">
-      <c r="A1479" s="24"/>
-      <c r="B1479" s="7"/>
+      <c r="A1479" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1479" s="7" t="s">
+        <v>2397</v>
+      </c>
+      <c r="C1479" s="7" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D1479" s="7">
+        <v>37.0</v>
+      </c>
+      <c r="E1479" s="8">
+        <v>0.5013888888888889</v>
+      </c>
+      <c r="F1479" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1479" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1479" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1479" s="11">
+        <v>17.7378396503627</v>
+      </c>
+      <c r="K1479" s="11">
+        <v>-64.6041179168969</v>
+      </c>
     </row>
     <row r="1480">
-      <c r="A1480" s="24"/>
-      <c r="B1480" s="7"/>
+      <c r="A1480" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1480" s="7" t="s">
+        <v>2398</v>
+      </c>
+      <c r="C1480" s="7" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D1480" s="7">
+        <v>23.0</v>
+      </c>
+      <c r="E1480" s="8">
+        <v>0.5013888888888889</v>
+      </c>
+      <c r="F1480" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1480" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1480" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1480" s="11">
+        <v>17.7378396503627</v>
+      </c>
+      <c r="K1480" s="11">
+        <v>-64.6041179168969</v>
+      </c>
     </row>
     <row r="1481">
-      <c r="A1481" s="24"/>
-      <c r="B1481" s="7"/>
+      <c r="A1481" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1481" s="7" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C1481" s="7" t="s">
+        <v>2400</v>
+      </c>
+      <c r="D1481" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="E1481" s="8">
+        <v>0.5076388888888889</v>
+      </c>
+      <c r="F1481" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1481" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1481" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1481" s="11">
+        <v>17.7377805579454</v>
+      </c>
+      <c r="K1481" s="11">
+        <v>-64.6042035799474</v>
+      </c>
     </row>
     <row r="1482">
-      <c r="A1482" s="24"/>
-      <c r="B1482" s="7"/>
+      <c r="A1482" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1482" s="7" t="s">
+        <v>2401</v>
+      </c>
+      <c r="C1482" s="7" t="s">
+        <v>2400</v>
+      </c>
+      <c r="D1482" s="7">
+        <v>29.0</v>
+      </c>
+      <c r="E1482" s="8">
+        <v>0.5076388888888889</v>
+      </c>
+      <c r="F1482" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1482" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1482" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1482" s="11">
+        <v>17.7377805579454</v>
+      </c>
+      <c r="K1482" s="11">
+        <v>-64.6042035799474</v>
+      </c>
     </row>
     <row r="1483">
-      <c r="A1483" s="24"/>
-      <c r="B1483" s="7"/>
+      <c r="A1483" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1483" s="7" t="s">
+        <v>2402</v>
+      </c>
+      <c r="C1483" s="7" t="s">
+        <v>2400</v>
+      </c>
+      <c r="D1483" s="7">
+        <v>28.0</v>
+      </c>
+      <c r="E1483" s="8">
+        <v>0.5076388888888889</v>
+      </c>
+      <c r="F1483" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1483" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1483" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1483" s="11">
+        <v>17.7377805579454</v>
+      </c>
+      <c r="K1483" s="11">
+        <v>-64.6042035799474</v>
+      </c>
     </row>
     <row r="1484">
-      <c r="A1484" s="24"/>
-      <c r="B1484" s="7"/>
+      <c r="A1484" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1484" s="7" t="s">
+        <v>2403</v>
+      </c>
+      <c r="C1484" s="7" t="s">
+        <v>2404</v>
+      </c>
+      <c r="D1484" s="7">
+        <v>102.0</v>
+      </c>
+      <c r="E1484" s="8">
+        <v>0.5111111111111111</v>
+      </c>
+      <c r="F1484" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1484" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1484" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1484" s="11">
+        <v>17.7377038635314</v>
+      </c>
+      <c r="K1484" s="11">
+        <v>-64.6043516043574</v>
+      </c>
     </row>
     <row r="1485">
-      <c r="A1485" s="24"/>
-      <c r="B1485" s="7"/>
+      <c r="A1485" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1485" s="7" t="s">
+        <v>2405</v>
+      </c>
+      <c r="C1485" s="7" t="s">
+        <v>2404</v>
+      </c>
+      <c r="D1485" s="7">
+        <v>35.0</v>
+      </c>
+      <c r="E1485" s="8">
+        <v>0.5111111111111111</v>
+      </c>
+      <c r="F1485" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1485" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1485" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1485" s="11">
+        <v>17.7377038635314</v>
+      </c>
+      <c r="K1485" s="11">
+        <v>-64.6043516043574</v>
+      </c>
     </row>
     <row r="1486">
-      <c r="A1486" s="24"/>
-      <c r="B1486" s="7"/>
+      <c r="A1486" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1486" s="7" t="s">
+        <v>2406</v>
+      </c>
+      <c r="C1486" s="7" t="s">
+        <v>2404</v>
+      </c>
+      <c r="D1486" s="7">
+        <v>8.0</v>
+      </c>
+      <c r="E1486" s="8">
+        <v>0.5111111111111111</v>
+      </c>
+      <c r="F1486" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1486" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1486" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1486" s="11">
+        <v>17.7377038635314</v>
+      </c>
+      <c r="K1486" s="11">
+        <v>-64.6043516043574</v>
+      </c>
     </row>
     <row r="1487">
-      <c r="A1487" s="24"/>
-      <c r="B1487" s="7"/>
+      <c r="A1487" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1487" s="7" t="s">
+        <v>2407</v>
+      </c>
+      <c r="C1487" s="7" t="s">
+        <v>2408</v>
+      </c>
+      <c r="D1487" s="7">
+        <v>69.0</v>
+      </c>
+      <c r="E1487" s="8">
+        <v>0.5152777777777777</v>
+      </c>
+      <c r="F1487" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1487" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1487" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1487" s="11">
+        <v>17.7376589365304</v>
+      </c>
+      <c r="K1487" s="11">
+        <v>-64.6043306495994</v>
+      </c>
     </row>
     <row r="1488">
-      <c r="A1488" s="24"/>
-      <c r="B1488" s="7"/>
+      <c r="A1488" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1488" s="7" t="s">
+        <v>2409</v>
+      </c>
+      <c r="C1488" s="7" t="s">
+        <v>2408</v>
+      </c>
+      <c r="D1488" s="7">
+        <v>218.0</v>
+      </c>
+      <c r="E1488" s="8">
+        <v>0.5152777777777777</v>
+      </c>
+      <c r="F1488" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1488" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1488" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1488" s="11">
+        <v>17.7376589365304</v>
+      </c>
+      <c r="K1488" s="11">
+        <v>-64.6043306495994</v>
+      </c>
     </row>
     <row r="1489">
-      <c r="A1489" s="24"/>
-      <c r="B1489" s="7"/>
+      <c r="A1489" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1489" s="7" t="s">
+        <v>2410</v>
+      </c>
+      <c r="C1489" s="7" t="s">
+        <v>2408</v>
+      </c>
+      <c r="D1489" s="7">
+        <v>9.0</v>
+      </c>
+      <c r="E1489" s="8">
+        <v>0.5152777777777777</v>
+      </c>
+      <c r="F1489" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1489" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1489" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1489" s="11">
+        <v>17.7376589365304</v>
+      </c>
+      <c r="K1489" s="11">
+        <v>-64.6043306495994</v>
+      </c>
     </row>
     <row r="1490">
-      <c r="A1490" s="24"/>
-      <c r="B1490" s="7"/>
+      <c r="A1490" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1490" s="7" t="s">
+        <v>2411</v>
+      </c>
+      <c r="C1490" s="7" t="s">
+        <v>2412</v>
+      </c>
+      <c r="D1490" s="7">
+        <v>113.0</v>
+      </c>
+      <c r="E1490" s="8">
+        <v>0.5222222222222223</v>
+      </c>
+      <c r="F1490" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1490" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1490" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1490" s="11">
+        <v>17.7376535721123</v>
+      </c>
+      <c r="K1490" s="11">
+        <v>-64.6044316515327</v>
+      </c>
     </row>
     <row r="1491">
-      <c r="A1491" s="24"/>
-      <c r="B1491" s="7"/>
+      <c r="A1491" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1491" s="7" t="s">
+        <v>2413</v>
+      </c>
+      <c r="C1491" s="7" t="s">
+        <v>2412</v>
+      </c>
+      <c r="D1491" s="7">
+        <v>44.0</v>
+      </c>
+      <c r="E1491" s="8">
+        <v>0.5222222222222223</v>
+      </c>
+      <c r="F1491" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1491" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1491" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1491" s="11">
+        <v>17.7376535721123</v>
+      </c>
+      <c r="K1491" s="11">
+        <v>-64.6044316515327</v>
+      </c>
     </row>
     <row r="1492">
-      <c r="A1492" s="24"/>
-      <c r="B1492" s="7"/>
+      <c r="A1492" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1492" s="7" t="s">
+        <v>2414</v>
+      </c>
+      <c r="C1492" s="7" t="s">
+        <v>2412</v>
+      </c>
+      <c r="D1492" s="7">
+        <v>104.0</v>
+      </c>
+      <c r="E1492" s="8">
+        <v>0.5222222222222223</v>
+      </c>
+      <c r="F1492" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1492" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1492" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1492" s="11">
+        <v>17.7376535721123</v>
+      </c>
+      <c r="K1492" s="11">
+        <v>-64.6044316515327</v>
+      </c>
     </row>
     <row r="1493">
-      <c r="A1493" s="24"/>
-      <c r="B1493" s="7"/>
+      <c r="A1493" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1493" s="7" t="s">
+        <v>2415</v>
+      </c>
+      <c r="C1493" s="7" t="s">
+        <v>2416</v>
+      </c>
+      <c r="D1493" s="7">
+        <v>12.0</v>
+      </c>
+      <c r="E1493" s="8">
+        <v>0.5263888888888889</v>
+      </c>
+      <c r="F1493" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1493" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1493" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1493" s="11">
+        <v>17.7376163564622</v>
+      </c>
+      <c r="K1493" s="11">
+        <v>-64.6044947672635</v>
+      </c>
     </row>
     <row r="1494">
-      <c r="A1494" s="24"/>
-      <c r="B1494" s="7"/>
+      <c r="A1494" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1494" s="7" t="s">
+        <v>2417</v>
+      </c>
+      <c r="C1494" s="7" t="s">
+        <v>2416</v>
+      </c>
+      <c r="D1494" s="7">
+        <v>108.0</v>
+      </c>
+      <c r="E1494" s="8">
+        <v>0.5263888888888889</v>
+      </c>
+      <c r="F1494" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1494" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1494" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1494" s="11">
+        <v>17.7376163564622</v>
+      </c>
+      <c r="K1494" s="11">
+        <v>-64.6044947672635</v>
+      </c>
     </row>
     <row r="1495">
-      <c r="A1495" s="24"/>
-      <c r="B1495" s="7"/>
+      <c r="A1495" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1495" s="7" t="s">
+        <v>2418</v>
+      </c>
+      <c r="C1495" s="7" t="s">
+        <v>2416</v>
+      </c>
+      <c r="D1495" s="7">
+        <v>57.0</v>
+      </c>
+      <c r="E1495" s="8">
+        <v>0.5263888888888889</v>
+      </c>
+      <c r="F1495" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1495" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1495" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1495" s="11">
+        <v>17.7376163564622</v>
+      </c>
+      <c r="K1495" s="11">
+        <v>-64.6044947672635</v>
+      </c>
     </row>
     <row r="1496">
-      <c r="A1496" s="24"/>
-      <c r="B1496" s="7"/>
+      <c r="A1496" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1496" s="7" t="s">
+        <v>2419</v>
+      </c>
+      <c r="C1496" s="7" t="s">
+        <v>2420</v>
+      </c>
+      <c r="D1496" s="7">
+        <v>47.0</v>
+      </c>
+      <c r="E1496" s="8">
+        <v>0.5291666666666667</v>
+      </c>
+      <c r="F1496" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1496" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1496" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1496" s="11">
+        <v>17.7376375626773</v>
+      </c>
+      <c r="K1496" s="11">
+        <v>-64.6045222599059</v>
+      </c>
     </row>
     <row r="1497">
-      <c r="A1497" s="24"/>
-      <c r="B1497" s="7"/>
+      <c r="A1497" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1497" s="7" t="s">
+        <v>2421</v>
+      </c>
+      <c r="C1497" s="7" t="s">
+        <v>2422</v>
+      </c>
+      <c r="D1497" s="7">
+        <v>27.0</v>
+      </c>
+      <c r="E1497" s="8">
+        <v>0.5298611111111111</v>
+      </c>
+      <c r="F1497" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1497" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1497" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1497" s="11">
+        <v>17.7375903725624</v>
+      </c>
+      <c r="K1497" s="11">
+        <v>-64.6045558713377</v>
+      </c>
     </row>
     <row r="1498">
-      <c r="A1498" s="24"/>
-      <c r="B1498" s="7"/>
+      <c r="A1498" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1498" s="7" t="s">
+        <v>2423</v>
+      </c>
+      <c r="C1498" s="7" t="s">
+        <v>2424</v>
+      </c>
+      <c r="D1498" s="7">
+        <v>77.0</v>
+      </c>
+      <c r="E1498" s="8">
+        <v>0.5326388888888889</v>
+      </c>
+      <c r="F1498" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1498" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1498" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1498" s="11">
+        <v>17.7375637181103</v>
+      </c>
+      <c r="K1498" s="11">
+        <v>-64.604570120573</v>
+      </c>
     </row>
     <row r="1499">
-      <c r="A1499" s="24"/>
-      <c r="B1499" s="7"/>
+      <c r="A1499" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1499" s="7" t="s">
+        <v>2425</v>
+      </c>
+      <c r="C1499" s="7" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D1499" s="7">
+        <v>115.0</v>
+      </c>
+      <c r="E1499" s="8">
+        <v>0.5340277777777778</v>
+      </c>
+      <c r="F1499" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1499" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1499" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1499" s="11">
+        <v>17.7375161089003</v>
+      </c>
+      <c r="K1499" s="11">
+        <v>-64.6045708749443</v>
+      </c>
     </row>
     <row r="1500">
-      <c r="A1500" s="24"/>
-      <c r="B1500" s="7"/>
+      <c r="A1500" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1500" s="7" t="s">
+        <v>2426</v>
+      </c>
+      <c r="C1500" s="7" t="s">
+        <v>2427</v>
+      </c>
+      <c r="D1500" s="7">
+        <v>84.0</v>
+      </c>
+      <c r="E1500" s="8">
+        <v>0.5354166666666667</v>
+      </c>
+      <c r="F1500" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1500" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1500" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1500" s="11">
+        <v>17.7375410869718</v>
+      </c>
+      <c r="K1500" s="11">
+        <v>-64.6046808455139</v>
+      </c>
     </row>
     <row r="1501">
-      <c r="A1501" s="24"/>
-      <c r="B1501" s="7"/>
+      <c r="A1501" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1501" s="7" t="s">
+        <v>2428</v>
+      </c>
+      <c r="C1501" s="7" t="s">
+        <v>2427</v>
+      </c>
+      <c r="D1501" s="7">
+        <v>46.0</v>
+      </c>
+      <c r="E1501" s="8">
+        <v>0.5354166666666667</v>
+      </c>
+      <c r="F1501" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1501" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1501" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1501" s="11">
+        <v>17.7375410869718</v>
+      </c>
+      <c r="K1501" s="11">
+        <v>-64.6046808455139</v>
+      </c>
     </row>
     <row r="1502">
-      <c r="A1502" s="24"/>
-      <c r="B1502" s="7"/>
+      <c r="A1502" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1502" s="7" t="s">
+        <v>2429</v>
+      </c>
+      <c r="C1502" s="7" t="s">
+        <v>2427</v>
+      </c>
+      <c r="D1502" s="7">
+        <v>71.0</v>
+      </c>
+      <c r="E1502" s="8">
+        <v>0.5354166666666667</v>
+      </c>
+      <c r="F1502" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1502" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1502" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1502" s="11">
+        <v>17.7375410869718</v>
+      </c>
+      <c r="K1502" s="11">
+        <v>-64.6046808455139</v>
+      </c>
     </row>
     <row r="1503">
-      <c r="A1503" s="24"/>
-      <c r="B1503" s="7"/>
+      <c r="A1503" s="6">
+        <v>44737.0</v>
+      </c>
+      <c r="B1503" s="7" t="s">
+        <v>2430</v>
+      </c>
+      <c r="C1503" s="7" t="s">
+        <v>2431</v>
+      </c>
+      <c r="D1503" s="7">
+        <v>120.0</v>
+      </c>
+      <c r="E1503" s="8">
+        <v>0.5402777777777777</v>
+      </c>
+      <c r="F1503" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1503" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1503" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1503" s="11">
+        <v>17.7375373989344</v>
+      </c>
+      <c r="K1503" s="11">
+        <v>-64.6047618146986</v>
+      </c>
     </row>
     <row r="1504">
       <c r="A1504" s="24"/>
@@ -57684,19 +59362,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>2360</v>
+        <v>2432</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2361</v>
+        <v>2433</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2362</v>
+        <v>2434</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2363</v>
+        <v>2435</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2364</v>
+        <v>2436</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>7</v>
@@ -57720,21 +59398,21 @@
         <v>51</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>2365</v>
+        <v>2437</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>145</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>2366</v>
+        <v>2438</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>2367</v>
+        <v>2439</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2368</v>
+        <v>2440</v>
       </c>
       <c r="C2" s="7">
         <v>7.0</v>
@@ -57746,33 +59424,33 @@
         <v>44688.0</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>2369</v>
+        <v>2441</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>2369</v>
+        <v>2441</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>2369</v>
+        <v>2441</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>2369</v>
+        <v>2441</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>2369</v>
+        <v>2441</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>2370</v>
+        <v>2442</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>2371</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>2372</v>
+        <v>2444</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2373</v>
+        <v>2445</v>
       </c>
       <c r="C3" s="7">
         <v>25.0</v>
@@ -57783,10 +59461,10 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>2374</v>
+        <v>2446</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="C4" s="7">
         <v>15.0</v>
@@ -57798,18 +59476,18 @@
         <v>44690.0</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>2376</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>2377</v>
+        <v>2449</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2378</v>
+        <v>2450</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2379</v>
+        <v>2451</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>20</v>
@@ -57817,10 +59495,10 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>2380</v>
+        <v>2452</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2381</v>
+        <v>2453</v>
       </c>
       <c r="C6" s="7">
         <v>20.0</v>
@@ -57852,10 +59530,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>2382</v>
+        <v>2454</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2383</v>
+        <v>2455</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>78</v>
@@ -57887,7 +59565,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2367</v>
+        <v>2439</v>
       </c>
       <c r="C2" s="7">
         <v>2.0</v>
@@ -57916,7 +59594,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2374</v>
+        <v>2446</v>
       </c>
       <c r="C3" s="7">
         <v>5.0</v>
@@ -57945,7 +59623,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2372</v>
+        <v>2444</v>
       </c>
       <c r="F4" s="7">
         <v>17.0</v>
@@ -57968,7 +59646,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2380</v>
+        <v>2452</v>
       </c>
       <c r="F5" s="7">
         <v>6.0</v>
@@ -57991,7 +59669,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2384</v>
+        <v>2456</v>
       </c>
       <c r="F6" s="7">
         <v>11.0</v>
@@ -58034,16 +59712,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="26" t="s">
-        <v>2385</v>
+        <v>2457</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>2386</v>
+        <v>2458</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>2387</v>
+        <v>2459</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>12</v>
@@ -58073,7 +59751,7 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B2" s="6">
         <v>44690.0</v>
@@ -58088,7 +59766,7 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B3" s="6">
         <v>44690.0</v>
@@ -58103,7 +59781,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B4" s="6">
         <v>44690.0</v>
@@ -58118,7 +59796,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B5" s="6">
         <v>44690.0</v>
@@ -58133,7 +59811,7 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B6" s="6">
         <v>44690.0</v>
@@ -58148,7 +59826,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B7" s="6">
         <v>44690.0</v>
@@ -58163,7 +59841,7 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B8" s="6">
         <v>44690.0</v>
@@ -58178,7 +59856,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B9" s="6">
         <v>44690.0</v>
@@ -58193,7 +59871,7 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B10" s="6">
         <v>44690.0</v>
@@ -58208,7 +59886,7 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B11" s="6">
         <v>44690.0</v>
@@ -58223,7 +59901,7 @@
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B12" s="6">
         <v>44690.0</v>
@@ -58238,7 +59916,7 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B13" s="6">
         <v>44690.0</v>
@@ -58253,7 +59931,7 @@
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B14" s="6">
         <v>44690.0</v>
@@ -58268,7 +59946,7 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B15" s="6">
         <v>44690.0</v>
@@ -58283,7 +59961,7 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B16" s="6">
         <v>44690.0</v>
@@ -58298,7 +59976,7 @@
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B17" s="6">
         <v>44690.0</v>
@@ -58314,7 +59992,7 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B18" s="6">
         <v>44690.0</v>
@@ -58330,7 +60008,7 @@
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B19" s="6">
         <v>44690.0</v>
@@ -58345,7 +60023,7 @@
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B20" s="6">
         <v>44690.0</v>
@@ -58360,7 +60038,7 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B21" s="6">
         <v>44690.0</v>
@@ -58375,7 +60053,7 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B22" s="6">
         <v>44690.0</v>
@@ -58390,7 +60068,7 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B23" s="6">
         <v>44690.0</v>
@@ -58405,7 +60083,7 @@
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B24" s="6">
         <v>44690.0</v>
@@ -58420,7 +60098,7 @@
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B25" s="6">
         <v>44690.0</v>
@@ -58435,7 +60113,7 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B26" s="6">
         <v>44690.0</v>
@@ -58450,7 +60128,7 @@
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B27" s="6">
         <v>44690.0</v>
@@ -58465,7 +60143,7 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B28" s="6">
         <v>44690.0</v>
@@ -58480,7 +60158,7 @@
     </row>
     <row r="29">
       <c r="A29" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B29" s="6">
         <v>44690.0</v>
@@ -58495,7 +60173,7 @@
     </row>
     <row r="30">
       <c r="A30" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B30" s="6">
         <v>44690.0</v>
@@ -58510,7 +60188,7 @@
     </row>
     <row r="31">
       <c r="A31" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B31" s="6">
         <v>44690.0</v>
@@ -58525,7 +60203,7 @@
     </row>
     <row r="32">
       <c r="A32" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B32" s="6">
         <v>44690.0</v>
@@ -58540,7 +60218,7 @@
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B33" s="6">
         <v>44690.0</v>
@@ -58555,7 +60233,7 @@
     </row>
     <row r="34">
       <c r="A34" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B34" s="6">
         <v>44690.0</v>
@@ -58570,7 +60248,7 @@
     </row>
     <row r="35">
       <c r="A35" s="7" t="s">
-        <v>2375</v>
+        <v>2447</v>
       </c>
       <c r="B35" s="6">
         <v>44690.0</v>
@@ -58585,7 +60263,7 @@
     </row>
     <row r="36">
       <c r="A36" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B36" s="6">
         <v>44704.0</v>
@@ -58600,7 +60278,7 @@
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B37" s="6">
         <v>44704.0</v>
@@ -58615,7 +60293,7 @@
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B38" s="6">
         <v>44704.0</v>
@@ -58627,12 +60305,12 @@
         <v>22.0</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>2389</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B39" s="6">
         <v>44704.0</v>
@@ -58647,7 +60325,7 @@
     </row>
     <row r="40">
       <c r="A40" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B40" s="6">
         <v>44704.0</v>
@@ -58659,12 +60337,12 @@
         <v>34.0</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>2389</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B41" s="6">
         <v>44704.0</v>
@@ -58679,7 +60357,7 @@
     </row>
     <row r="42">
       <c r="A42" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B42" s="6">
         <v>44704.0</v>
@@ -58694,7 +60372,7 @@
     </row>
     <row r="43">
       <c r="A43" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B43" s="6">
         <v>44704.0</v>
@@ -58709,7 +60387,7 @@
     </row>
     <row r="44">
       <c r="A44" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B44" s="6">
         <v>44704.0</v>
@@ -58721,12 +60399,12 @@
         <v>6.0</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>2389</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B45" s="6">
         <v>44704.0</v>
@@ -58741,7 +60419,7 @@
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B46" s="6">
         <v>44704.0</v>
@@ -58756,7 +60434,7 @@
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B47" s="6">
         <v>44704.0</v>
@@ -58771,7 +60449,7 @@
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B48" s="6">
         <v>44704.0</v>
@@ -58786,7 +60464,7 @@
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B49" s="6">
         <v>44704.0</v>
@@ -58801,7 +60479,7 @@
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B50" s="6">
         <v>44704.0</v>
@@ -58816,7 +60494,7 @@
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B51" s="6">
         <v>44704.0</v>
@@ -58831,7 +60509,7 @@
     </row>
     <row r="52">
       <c r="A52" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B52" s="6">
         <v>44704.0</v>
@@ -58846,7 +60524,7 @@
     </row>
     <row r="53">
       <c r="A53" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B53" s="6">
         <v>44704.0</v>
@@ -58861,7 +60539,7 @@
     </row>
     <row r="54">
       <c r="A54" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B54" s="6">
         <v>44704.0</v>
@@ -58876,7 +60554,7 @@
     </row>
     <row r="55">
       <c r="A55" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B55" s="6">
         <v>44704.0</v>
@@ -58891,7 +60569,7 @@
     </row>
     <row r="56">
       <c r="A56" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B56" s="6">
         <v>44704.0</v>
@@ -58906,7 +60584,7 @@
     </row>
     <row r="57">
       <c r="A57" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B57" s="6">
         <v>44704.0</v>
@@ -58921,7 +60599,7 @@
     </row>
     <row r="58">
       <c r="A58" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B58" s="6">
         <v>44704.0</v>
@@ -58936,7 +60614,7 @@
     </row>
     <row r="59">
       <c r="A59" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B59" s="6">
         <v>44704.0</v>
@@ -58951,7 +60629,7 @@
     </row>
     <row r="60">
       <c r="A60" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B60" s="6">
         <v>44704.0</v>
@@ -58966,7 +60644,7 @@
     </row>
     <row r="61">
       <c r="A61" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B61" s="6">
         <v>44704.0</v>
@@ -58981,7 +60659,7 @@
     </row>
     <row r="62">
       <c r="A62" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B62" s="6">
         <v>44704.0</v>
@@ -58996,7 +60674,7 @@
     </row>
     <row r="63">
       <c r="A63" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B63" s="6">
         <v>44704.0</v>
@@ -59011,7 +60689,7 @@
     </row>
     <row r="64">
       <c r="A64" s="7" t="s">
-        <v>2388</v>
+        <v>2460</v>
       </c>
       <c r="B64" s="6">
         <v>44704.0</v>
@@ -59026,7 +60704,7 @@
     </row>
     <row r="65">
       <c r="A65" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B65" s="6">
         <v>44704.0</v>
@@ -59041,7 +60719,7 @@
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B66" s="6">
         <v>44704.0</v>
@@ -59056,7 +60734,7 @@
     </row>
     <row r="67">
       <c r="A67" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B67" s="6">
         <v>44704.0</v>
@@ -59071,7 +60749,7 @@
     </row>
     <row r="68">
       <c r="A68" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B68" s="6">
         <v>44704.0</v>
@@ -59086,7 +60764,7 @@
     </row>
     <row r="69">
       <c r="A69" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B69" s="6">
         <v>44704.0</v>
@@ -59101,7 +60779,7 @@
     </row>
     <row r="70">
       <c r="A70" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B70" s="6">
         <v>44704.0</v>
@@ -59116,7 +60794,7 @@
     </row>
     <row r="71">
       <c r="A71" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B71" s="6">
         <v>44704.0</v>
@@ -59131,7 +60809,7 @@
     </row>
     <row r="72">
       <c r="A72" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B72" s="6">
         <v>44704.0</v>
@@ -59146,7 +60824,7 @@
     </row>
     <row r="73">
       <c r="A73" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B73" s="6">
         <v>44704.0</v>
@@ -59161,7 +60839,7 @@
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B74" s="6">
         <v>44704.0</v>
@@ -59176,7 +60854,7 @@
     </row>
     <row r="75">
       <c r="A75" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B75" s="6">
         <v>44704.0</v>
@@ -59191,7 +60869,7 @@
     </row>
     <row r="76">
       <c r="A76" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B76" s="6">
         <v>44704.0</v>
@@ -59206,7 +60884,7 @@
     </row>
     <row r="77">
       <c r="A77" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B77" s="6">
         <v>44704.0</v>
@@ -59221,7 +60899,7 @@
     </row>
     <row r="78">
       <c r="A78" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B78" s="6">
         <v>44704.0</v>
@@ -59236,7 +60914,7 @@
     </row>
     <row r="79">
       <c r="A79" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B79" s="6">
         <v>44704.0</v>
@@ -59251,7 +60929,7 @@
     </row>
     <row r="80">
       <c r="A80" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B80" s="6">
         <v>44704.0</v>
@@ -59266,7 +60944,7 @@
     </row>
     <row r="81">
       <c r="A81" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B81" s="6">
         <v>44704.0</v>
@@ -59281,7 +60959,7 @@
     </row>
     <row r="82">
       <c r="A82" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B82" s="6">
         <v>44704.0</v>
@@ -59296,7 +60974,7 @@
     </row>
     <row r="83">
       <c r="A83" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B83" s="6">
         <v>44704.0</v>
@@ -59311,7 +60989,7 @@
     </row>
     <row r="84">
       <c r="A84" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B84" s="6">
         <v>44704.0</v>
@@ -59326,7 +61004,7 @@
     </row>
     <row r="85">
       <c r="A85" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B85" s="6">
         <v>44704.0</v>
@@ -59341,7 +61019,7 @@
     </row>
     <row r="86">
       <c r="A86" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B86" s="6">
         <v>44704.0</v>
@@ -59356,7 +61034,7 @@
     </row>
     <row r="87">
       <c r="A87" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B87" s="6">
         <v>44704.0</v>
@@ -59371,7 +61049,7 @@
     </row>
     <row r="88">
       <c r="A88" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B88" s="6">
         <v>44704.0</v>
@@ -59386,7 +61064,7 @@
     </row>
     <row r="89">
       <c r="A89" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B89" s="6">
         <v>44704.0</v>
@@ -59401,7 +61079,7 @@
     </row>
     <row r="90">
       <c r="A90" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B90" s="6">
         <v>44704.0</v>
@@ -59416,7 +61094,7 @@
     </row>
     <row r="91">
       <c r="A91" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B91" s="6">
         <v>44704.0</v>
@@ -59431,7 +61109,7 @@
     </row>
     <row r="92">
       <c r="A92" s="7" t="s">
-        <v>2390</v>
+        <v>2462</v>
       </c>
       <c r="B92" s="6">
         <v>44704.0</v>
@@ -59446,7 +61124,7 @@
     </row>
     <row r="93">
       <c r="A93" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B93" s="6">
         <v>44705.0</v>
@@ -59461,7 +61139,7 @@
     </row>
     <row r="94">
       <c r="A94" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B94" s="6">
         <v>44705.0</v>
@@ -59476,7 +61154,7 @@
     </row>
     <row r="95">
       <c r="A95" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B95" s="6">
         <v>44705.0</v>
@@ -59491,7 +61169,7 @@
     </row>
     <row r="96">
       <c r="A96" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B96" s="6">
         <v>44705.0</v>
@@ -59506,7 +61184,7 @@
     </row>
     <row r="97">
       <c r="A97" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B97" s="6">
         <v>44705.0</v>
@@ -59521,7 +61199,7 @@
     </row>
     <row r="98">
       <c r="A98" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B98" s="6">
         <v>44705.0</v>
@@ -59536,7 +61214,7 @@
     </row>
     <row r="99">
       <c r="A99" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B99" s="6">
         <v>44705.0</v>
@@ -59551,7 +61229,7 @@
     </row>
     <row r="100">
       <c r="A100" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B100" s="6">
         <v>44705.0</v>
@@ -59566,7 +61244,7 @@
     </row>
     <row r="101">
       <c r="A101" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B101" s="6">
         <v>44705.0</v>
@@ -59581,7 +61259,7 @@
     </row>
     <row r="102">
       <c r="A102" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B102" s="6">
         <v>44705.0</v>
@@ -59596,7 +61274,7 @@
     </row>
     <row r="103">
       <c r="A103" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B103" s="6">
         <v>44705.0</v>
@@ -59611,7 +61289,7 @@
     </row>
     <row r="104">
       <c r="A104" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B104" s="6">
         <v>44705.0</v>
@@ -59626,7 +61304,7 @@
     </row>
     <row r="105">
       <c r="A105" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B105" s="6">
         <v>44705.0</v>
@@ -59641,7 +61319,7 @@
     </row>
     <row r="106">
       <c r="A106" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B106" s="6">
         <v>44705.0</v>
@@ -59656,7 +61334,7 @@
     </row>
     <row r="107">
       <c r="A107" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B107" s="6">
         <v>44705.0</v>
@@ -59671,7 +61349,7 @@
     </row>
     <row r="108">
       <c r="A108" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B108" s="6">
         <v>44705.0</v>
@@ -59686,7 +61364,7 @@
     </row>
     <row r="109">
       <c r="A109" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B109" s="6">
         <v>44705.0</v>
@@ -59701,7 +61379,7 @@
     </row>
     <row r="110">
       <c r="A110" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B110" s="6">
         <v>44705.0</v>
@@ -59716,7 +61394,7 @@
     </row>
     <row r="111">
       <c r="A111" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B111" s="6">
         <v>44705.0</v>
@@ -59731,7 +61409,7 @@
     </row>
     <row r="112">
       <c r="A112" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B112" s="6">
         <v>44705.0</v>
@@ -59746,7 +61424,7 @@
     </row>
     <row r="113">
       <c r="A113" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B113" s="6">
         <v>44705.0</v>
@@ -59761,7 +61439,7 @@
     </row>
     <row r="114">
       <c r="A114" s="7" t="s">
-        <v>2391</v>
+        <v>2463</v>
       </c>
       <c r="B114" s="6">
         <v>44705.0</v>
@@ -59776,7 +61454,7 @@
     </row>
     <row r="115">
       <c r="A115" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B115" s="6">
         <v>44708.0</v>
@@ -59791,7 +61469,7 @@
     </row>
     <row r="116">
       <c r="A116" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B116" s="6">
         <v>44708.0</v>
@@ -59806,7 +61484,7 @@
     </row>
     <row r="117">
       <c r="A117" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B117" s="6">
         <v>44708.0</v>
@@ -59821,7 +61499,7 @@
     </row>
     <row r="118">
       <c r="A118" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B118" s="6">
         <v>44708.0</v>
@@ -59833,12 +61511,12 @@
         <v>39.0</v>
       </c>
       <c r="E118" s="29" t="s">
-        <v>2389</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B119" s="6">
         <v>44708.0</v>
@@ -59853,7 +61531,7 @@
     </row>
     <row r="120">
       <c r="A120" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B120" s="6">
         <v>44708.0</v>
@@ -59868,7 +61546,7 @@
     </row>
     <row r="121">
       <c r="A121" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B121" s="6">
         <v>44708.0</v>
@@ -59883,7 +61561,7 @@
     </row>
     <row r="122">
       <c r="A122" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B122" s="6">
         <v>44708.0</v>
@@ -59898,7 +61576,7 @@
     </row>
     <row r="123">
       <c r="A123" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B123" s="6">
         <v>44708.0</v>
@@ -59913,7 +61591,7 @@
     </row>
     <row r="124">
       <c r="A124" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B124" s="6">
         <v>44708.0</v>
@@ -59928,7 +61606,7 @@
     </row>
     <row r="125">
       <c r="A125" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B125" s="6">
         <v>44708.0</v>
@@ -59943,7 +61621,7 @@
     </row>
     <row r="126">
       <c r="A126" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B126" s="6">
         <v>44708.0</v>
@@ -59958,7 +61636,7 @@
     </row>
     <row r="127">
       <c r="A127" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B127" s="6">
         <v>44708.0</v>
@@ -59970,12 +61648,12 @@
         <v>11.0</v>
       </c>
       <c r="E127" s="29" t="s">
-        <v>2389</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B128" s="6">
         <v>44708.0</v>
@@ -59990,7 +61668,7 @@
     </row>
     <row r="129">
       <c r="A129" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B129" s="6">
         <v>44708.0</v>
@@ -60002,12 +61680,12 @@
         <v>40.0</v>
       </c>
       <c r="E129" s="29" t="s">
-        <v>2389</v>
+        <v>2461</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B130" s="6">
         <v>44708.0</v>
@@ -60022,7 +61700,7 @@
     </row>
     <row r="131">
       <c r="A131" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B131" s="6">
         <v>44708.0</v>
@@ -60037,7 +61715,7 @@
     </row>
     <row r="132">
       <c r="A132" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B132" s="6">
         <v>44708.0</v>
@@ -60052,7 +61730,7 @@
     </row>
     <row r="133">
       <c r="A133" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="B133" s="6">
         <v>44708.0</v>
@@ -60067,7 +61745,7 @@
     </row>
     <row r="134">
       <c r="A134" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B134" s="6">
         <v>44713.0</v>
@@ -60079,12 +61757,12 @@
         <v>1298</v>
       </c>
       <c r="E134" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B135" s="6">
         <v>44713.0</v>
@@ -60096,12 +61774,12 @@
         <v>1300</v>
       </c>
       <c r="E135" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B136" s="6">
         <v>44713.0</v>
@@ -60113,12 +61791,12 @@
         <v>1302</v>
       </c>
       <c r="E136" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B137" s="6">
         <v>44713.0</v>
@@ -60130,12 +61808,12 @@
         <v>1304</v>
       </c>
       <c r="E137" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B138" s="6">
         <v>44713.0</v>
@@ -60147,12 +61825,12 @@
         <v>1306</v>
       </c>
       <c r="E138" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B139" s="6">
         <v>44713.0</v>
@@ -60164,12 +61842,12 @@
         <v>1309</v>
       </c>
       <c r="E139" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B140" s="6">
         <v>44713.0</v>
@@ -60181,12 +61859,12 @@
         <v>1312</v>
       </c>
       <c r="E140" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B141" s="6">
         <v>44713.0</v>
@@ -60198,12 +61876,12 @@
         <v>1315</v>
       </c>
       <c r="E141" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B142" s="6">
         <v>44713.0</v>
@@ -60215,12 +61893,12 @@
         <v>1318</v>
       </c>
       <c r="E142" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B143" s="6">
         <v>44713.0</v>
@@ -60232,12 +61910,12 @@
         <v>1321</v>
       </c>
       <c r="E143" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B144" s="6">
         <v>44713.0</v>
@@ -60249,12 +61927,12 @@
         <v>1323</v>
       </c>
       <c r="E144" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B145" s="6">
         <v>44713.0</v>
@@ -60266,12 +61944,12 @@
         <v>1325</v>
       </c>
       <c r="E145" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B146" s="6">
         <v>44713.0</v>
@@ -60283,12 +61961,12 @@
         <v>1327</v>
       </c>
       <c r="E146" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B147" s="6">
         <v>44713.0</v>
@@ -60300,12 +61978,12 @@
         <v>1329</v>
       </c>
       <c r="E147" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B148" s="6">
         <v>44713.0</v>
@@ -60317,12 +61995,12 @@
         <v>1331</v>
       </c>
       <c r="E148" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B149" s="6">
         <v>44713.0</v>
@@ -60334,12 +62012,12 @@
         <v>1333</v>
       </c>
       <c r="E149" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B150" s="6">
         <v>44713.0</v>
@@ -60351,12 +62029,12 @@
         <v>1335</v>
       </c>
       <c r="E150" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B151" s="6">
         <v>44713.0</v>
@@ -60368,12 +62046,12 @@
         <v>1337</v>
       </c>
       <c r="E151" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B152" s="6">
         <v>44713.0</v>
@@ -60385,12 +62063,12 @@
         <v>1340</v>
       </c>
       <c r="E152" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B153" s="6">
         <v>44713.0</v>
@@ -60402,12 +62080,12 @@
         <v>1342</v>
       </c>
       <c r="E153" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B154" s="6">
         <v>44713.0</v>
@@ -60419,12 +62097,12 @@
         <v>1344</v>
       </c>
       <c r="E154" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B155" s="6">
         <v>44713.0</v>
@@ -60436,12 +62114,12 @@
         <v>1346</v>
       </c>
       <c r="E155" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B156" s="6">
         <v>44713.0</v>
@@ -60453,12 +62131,12 @@
         <v>1348</v>
       </c>
       <c r="E156" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="7" t="s">
-        <v>2393</v>
+        <v>2465</v>
       </c>
       <c r="B157" s="6">
         <v>44713.0</v>
@@ -60470,7 +62148,7 @@
         <v>1350</v>
       </c>
       <c r="E157" s="29" t="s">
-        <v>2394</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="158">
@@ -63022,22 +64700,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2395</v>
+        <v>2467</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2396</v>
+        <v>2468</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2397</v>
+        <v>2469</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2398</v>
+        <v>2470</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>2399</v>
+        <v>2471</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>2400</v>
+        <v>2472</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>12</v>
@@ -63048,17 +64726,17 @@
         <v>44690.0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2401</v>
+        <v>2473</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>2374</v>
+        <v>2446</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7" t="s">
-        <v>2402</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="3">
@@ -63066,7 +64744,7 @@
         <v>44692.0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2403</v>
+        <v>2475</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="7" t="s">
@@ -63087,10 +64765,10 @@
         <v>44694.0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2404</v>
+        <v>2476</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>2380</v>
+        <v>2452</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
@@ -63105,7 +64783,7 @@
         <v>2.5</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>2405</v>
+        <v>2477</v>
       </c>
     </row>
     <row r="5">
@@ -63113,10 +64791,10 @@
         <v>44695.0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2406</v>
+        <v>2478</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2384</v>
+        <v>2456</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -63136,10 +64814,10 @@
         <v>44697.0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2407</v>
+        <v>2479</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>2408</v>
+        <v>2480</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -63159,10 +64837,10 @@
         <v>44698.0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>2392</v>
+        <v>2464</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>2409</v>
+        <v>2481</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -63182,10 +64860,10 @@
         <v>44726.0</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>2410</v>
+        <v>2482</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>2411</v>
+        <v>2483</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>1353</v>

</xml_diff>

<commit_message>
Updated to include second day of sampling at CBE on 26Jun2022
</commit_message>
<xml_diff>
--- a/Data/Genotype_Samples_2022.xlsx
+++ b/Data/Genotype_Samples_2022.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8349" uniqueCount="2484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8606" uniqueCount="2584">
   <si>
     <t>Date</t>
   </si>
@@ -7311,6 +7311,306 @@
   </si>
   <si>
     <t>G1674</t>
+  </si>
+  <si>
+    <t>CBE_060</t>
+  </si>
+  <si>
+    <t>G1506</t>
+  </si>
+  <si>
+    <t>Erin/Sesno</t>
+  </si>
+  <si>
+    <t>CBE_061</t>
+  </si>
+  <si>
+    <t>G1507</t>
+  </si>
+  <si>
+    <t>CBE_062</t>
+  </si>
+  <si>
+    <t>G1508</t>
+  </si>
+  <si>
+    <t>CBE_063</t>
+  </si>
+  <si>
+    <t>G1516</t>
+  </si>
+  <si>
+    <t>CBE_064</t>
+  </si>
+  <si>
+    <t>G1509</t>
+  </si>
+  <si>
+    <t>CBE_065</t>
+  </si>
+  <si>
+    <t>G1510</t>
+  </si>
+  <si>
+    <t>Lone lobe (large)</t>
+  </si>
+  <si>
+    <t>CBE_066</t>
+  </si>
+  <si>
+    <t>G1517</t>
+  </si>
+  <si>
+    <t>CBE_067</t>
+  </si>
+  <si>
+    <t>G1519</t>
+  </si>
+  <si>
+    <t>CBE_068</t>
+  </si>
+  <si>
+    <t>G1518</t>
+  </si>
+  <si>
+    <t>CBE_069</t>
+  </si>
+  <si>
+    <t>G1526</t>
+  </si>
+  <si>
+    <t>CBE_070</t>
+  </si>
+  <si>
+    <t>CBE_071</t>
+  </si>
+  <si>
+    <t>G1520</t>
+  </si>
+  <si>
+    <t>CBE_072</t>
+  </si>
+  <si>
+    <t>G1527</t>
+  </si>
+  <si>
+    <t>CBE_073</t>
+  </si>
+  <si>
+    <t>G1528</t>
+  </si>
+  <si>
+    <t>CBE_074</t>
+  </si>
+  <si>
+    <t>G1536</t>
+  </si>
+  <si>
+    <t>CBE_075</t>
+  </si>
+  <si>
+    <t>G1529</t>
+  </si>
+  <si>
+    <t>CBE_076</t>
+  </si>
+  <si>
+    <t>G1537</t>
+  </si>
+  <si>
+    <t>CBE_077</t>
+  </si>
+  <si>
+    <t>G1530</t>
+  </si>
+  <si>
+    <t>CBE_078</t>
+  </si>
+  <si>
+    <t>G1546</t>
+  </si>
+  <si>
+    <t>CBE_079</t>
+  </si>
+  <si>
+    <t>G1538</t>
+  </si>
+  <si>
+    <t>CBE_080</t>
+  </si>
+  <si>
+    <t>G1539</t>
+  </si>
+  <si>
+    <t>CBE_081</t>
+  </si>
+  <si>
+    <t>G1547</t>
+  </si>
+  <si>
+    <t>CBE_082</t>
+  </si>
+  <si>
+    <t>G1540</t>
+  </si>
+  <si>
+    <t>CBE_083</t>
+  </si>
+  <si>
+    <t>G1548</t>
+  </si>
+  <si>
+    <t>CBE_084</t>
+  </si>
+  <si>
+    <t>G1445</t>
+  </si>
+  <si>
+    <t>CBE_085</t>
+  </si>
+  <si>
+    <t>G1444</t>
+  </si>
+  <si>
+    <t>CBE_086</t>
+  </si>
+  <si>
+    <t>G1443</t>
+  </si>
+  <si>
+    <t>Disease</t>
+  </si>
+  <si>
+    <t>CBE_087</t>
+  </si>
+  <si>
+    <t>G1442</t>
+  </si>
+  <si>
+    <t>CBE_088</t>
+  </si>
+  <si>
+    <t>G1431</t>
+  </si>
+  <si>
+    <t>CBE_089</t>
+  </si>
+  <si>
+    <t>G1441</t>
+  </si>
+  <si>
+    <t>CBE_090</t>
+  </si>
+  <si>
+    <t>G1422</t>
+  </si>
+  <si>
+    <t>CBE_091</t>
+  </si>
+  <si>
+    <t>G1435</t>
+  </si>
+  <si>
+    <t>CBE_092</t>
+  </si>
+  <si>
+    <t>G1434</t>
+  </si>
+  <si>
+    <t>CBE_093</t>
+  </si>
+  <si>
+    <t>G1421</t>
+  </si>
+  <si>
+    <t>CBE_094</t>
+  </si>
+  <si>
+    <t>CBE_095</t>
+  </si>
+  <si>
+    <t>G1432</t>
+  </si>
+  <si>
+    <t>CBE_096</t>
+  </si>
+  <si>
+    <t>G1429</t>
+  </si>
+  <si>
+    <t>CBE_097</t>
+  </si>
+  <si>
+    <t>G1439</t>
+  </si>
+  <si>
+    <t>CBE_098</t>
+  </si>
+  <si>
+    <t>G1438</t>
+  </si>
+  <si>
+    <t>CBE_099</t>
+  </si>
+  <si>
+    <t>G1436</t>
+  </si>
+  <si>
+    <t>CBE_100</t>
+  </si>
+  <si>
+    <t>G1437</t>
+  </si>
+  <si>
+    <t>CBE_101</t>
+  </si>
+  <si>
+    <t>CBE_102</t>
+  </si>
+  <si>
+    <t>G1415</t>
+  </si>
+  <si>
+    <t>CBE_103</t>
+  </si>
+  <si>
+    <t>G1414</t>
+  </si>
+  <si>
+    <t>CBE_104</t>
+  </si>
+  <si>
+    <t>G1430</t>
+  </si>
+  <si>
+    <t>CBE_105</t>
+  </si>
+  <si>
+    <t>G1428</t>
+  </si>
+  <si>
+    <t>CBE_106</t>
+  </si>
+  <si>
+    <t>G1427</t>
+  </si>
+  <si>
+    <t>CBE_107</t>
+  </si>
+  <si>
+    <t>G1423</t>
+  </si>
+  <si>
+    <t>CBE_108</t>
+  </si>
+  <si>
+    <t>G1424</t>
+  </si>
+  <si>
+    <t>CBE_109</t>
+  </si>
+  <si>
+    <t>G1425</t>
   </si>
   <si>
     <t>Site_ID</t>
@@ -57366,204 +57666,1625 @@
       </c>
     </row>
     <row r="1504">
-      <c r="A1504" s="24"/>
-      <c r="B1504" s="7"/>
+      <c r="A1504" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1504" s="7" t="s">
+        <v>2432</v>
+      </c>
+      <c r="C1504" s="7" t="s">
+        <v>2433</v>
+      </c>
+      <c r="D1504" s="7">
+        <v>107.0</v>
+      </c>
+      <c r="E1504" s="8">
+        <v>0.6506944444444445</v>
+      </c>
+      <c r="F1504" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1504" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1504" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1504" s="11">
+        <v>17.7741150185466</v>
+      </c>
+      <c r="K1504" s="11">
+        <v>-64.8114669229835</v>
+      </c>
     </row>
     <row r="1505">
-      <c r="A1505" s="24"/>
-      <c r="B1505" s="7"/>
+      <c r="A1505" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1505" s="7" t="s">
+        <v>2435</v>
+      </c>
+      <c r="C1505" s="7" t="s">
+        <v>2436</v>
+      </c>
+      <c r="D1505" s="7">
+        <v>43.0</v>
+      </c>
+      <c r="E1505" s="8">
+        <v>0.6527777777777778</v>
+      </c>
+      <c r="F1505" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1505" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1505" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1505" s="11">
+        <v>17.7741808164865</v>
+      </c>
+      <c r="K1505" s="11">
+        <v>-64.8114428669214</v>
+      </c>
     </row>
     <row r="1506">
-      <c r="A1506" s="24"/>
-      <c r="B1506" s="7"/>
+      <c r="A1506" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1506" s="7" t="s">
+        <v>2437</v>
+      </c>
+      <c r="C1506" s="7" t="s">
+        <v>2438</v>
+      </c>
+      <c r="D1506" s="7">
+        <v>66.0</v>
+      </c>
+      <c r="E1506" s="8">
+        <v>0.6548611111111111</v>
+      </c>
+      <c r="F1506" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1506" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1506" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1506" s="11">
+        <v>17.7742346283048</v>
+      </c>
+      <c r="K1506" s="11">
+        <v>-64.8114955052733</v>
+      </c>
     </row>
     <row r="1507">
-      <c r="A1507" s="24"/>
-      <c r="B1507" s="7"/>
+      <c r="A1507" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1507" s="7" t="s">
+        <v>2439</v>
+      </c>
+      <c r="C1507" s="7" t="s">
+        <v>2440</v>
+      </c>
+      <c r="D1507" s="7">
+        <v>72.0</v>
+      </c>
+      <c r="E1507" s="8">
+        <v>0.6569444444444444</v>
+      </c>
+      <c r="F1507" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1507" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1507" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1507" s="11">
+        <v>17.7742358855903</v>
+      </c>
+      <c r="K1507" s="11">
+        <v>-64.8114695213735</v>
+      </c>
     </row>
     <row r="1508">
-      <c r="A1508" s="24"/>
-      <c r="B1508" s="7"/>
+      <c r="A1508" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1508" s="7" t="s">
+        <v>2441</v>
+      </c>
+      <c r="C1508" s="7" t="s">
+        <v>2442</v>
+      </c>
+      <c r="D1508" s="7">
+        <v>21.0</v>
+      </c>
+      <c r="E1508" s="8">
+        <v>0.6597222222222222</v>
+      </c>
+      <c r="F1508" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1508" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1508" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1508" s="11">
+        <v>17.7742948103696</v>
+      </c>
+      <c r="K1508" s="11">
+        <v>-64.8114882130176</v>
+      </c>
     </row>
     <row r="1509">
-      <c r="A1509" s="24"/>
-      <c r="B1509" s="7"/>
+      <c r="A1509" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1509" s="7" t="s">
+        <v>2443</v>
+      </c>
+      <c r="C1509" s="7" t="s">
+        <v>2444</v>
+      </c>
+      <c r="D1509" s="7">
+        <v>32.0</v>
+      </c>
+      <c r="E1509" s="8">
+        <v>0.6618055555555555</v>
+      </c>
+      <c r="F1509" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1509" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1509" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1509" s="11">
+        <v>17.774288021028</v>
+      </c>
+      <c r="K1509" s="11">
+        <v>-64.8115694336593</v>
+      </c>
+      <c r="M1509" s="7" t="s">
+        <v>2445</v>
+      </c>
     </row>
     <row r="1510">
-      <c r="A1510" s="24"/>
-      <c r="B1510" s="7"/>
+      <c r="A1510" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1510" s="7" t="s">
+        <v>2446</v>
+      </c>
+      <c r="C1510" s="7" t="s">
+        <v>2447</v>
+      </c>
+      <c r="D1510" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="E1510" s="8">
+        <v>0.6638888888888889</v>
+      </c>
+      <c r="F1510" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1510" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1510" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1510" s="11">
+        <v>17.7742544934154</v>
+      </c>
+      <c r="K1510" s="11">
+        <v>-64.811592483893</v>
+      </c>
     </row>
     <row r="1511">
-      <c r="A1511" s="24"/>
-      <c r="B1511" s="7"/>
+      <c r="A1511" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1511" s="7" t="s">
+        <v>2448</v>
+      </c>
+      <c r="C1511" s="7" t="s">
+        <v>2449</v>
+      </c>
+      <c r="D1511" s="7">
+        <v>41.0</v>
+      </c>
+      <c r="E1511" s="8">
+        <v>0.6673611111111111</v>
+      </c>
+      <c r="F1511" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1511" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1511" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1511" s="11">
+        <v>17.7742600254714</v>
+      </c>
+      <c r="K1511" s="11">
+        <v>-64.8116624727845</v>
+      </c>
     </row>
     <row r="1512">
-      <c r="A1512" s="24"/>
-      <c r="B1512" s="7"/>
+      <c r="A1512" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1512" s="7" t="s">
+        <v>2450</v>
+      </c>
+      <c r="C1512" s="7" t="s">
+        <v>2451</v>
+      </c>
+      <c r="D1512" s="7">
+        <v>216.0</v>
+      </c>
+      <c r="E1512" s="8">
+        <v>0.6694444444444444</v>
+      </c>
+      <c r="F1512" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1512" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1512" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1512" s="11">
+        <v>17.7742316946387</v>
+      </c>
+      <c r="K1512" s="11">
+        <v>-64.8116837628186</v>
+      </c>
     </row>
     <row r="1513">
-      <c r="A1513" s="24"/>
-      <c r="B1513" s="7"/>
+      <c r="A1513" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1513" s="7" t="s">
+        <v>2452</v>
+      </c>
+      <c r="C1513" s="7" t="s">
+        <v>2453</v>
+      </c>
+      <c r="D1513" s="7">
+        <v>13.0</v>
+      </c>
+      <c r="E1513" s="8">
+        <v>0.675</v>
+      </c>
+      <c r="F1513" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1513" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1513" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1513" s="11">
+        <v>17.7743574231863</v>
+      </c>
+      <c r="K1513" s="11">
+        <v>-64.8118025343865</v>
+      </c>
+      <c r="M1513" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1514">
-      <c r="A1514" s="24"/>
-      <c r="B1514" s="7"/>
+      <c r="A1514" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1514" s="7" t="s">
+        <v>2454</v>
+      </c>
+      <c r="C1514" s="7" t="s">
+        <v>2453</v>
+      </c>
+      <c r="D1514" s="7">
+        <v>202.0</v>
+      </c>
+      <c r="E1514" s="8">
+        <v>0.6756944444444445</v>
+      </c>
+      <c r="F1514" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1514" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1514" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1514" s="11">
+        <v>17.7743057068437</v>
+      </c>
+      <c r="K1514" s="11">
+        <v>-64.8118135984987</v>
+      </c>
+      <c r="M1514" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1515">
-      <c r="A1515" s="24"/>
-      <c r="B1515" s="7"/>
+      <c r="A1515" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1515" s="7" t="s">
+        <v>2455</v>
+      </c>
+      <c r="C1515" s="7" t="s">
+        <v>2456</v>
+      </c>
+      <c r="D1515" s="7">
+        <v>211.0</v>
+      </c>
+      <c r="E1515" s="8">
+        <v>0.6777777777777778</v>
+      </c>
+      <c r="F1515" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1515" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1515" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1515" s="11">
+        <v>17.7743260748684</v>
+      </c>
+      <c r="K1515" s="11">
+        <v>-64.8118099942803</v>
+      </c>
     </row>
     <row r="1516">
-      <c r="A1516" s="24"/>
-      <c r="B1516" s="7"/>
+      <c r="A1516" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1516" s="7" t="s">
+        <v>2457</v>
+      </c>
+      <c r="C1516" s="7" t="s">
+        <v>2458</v>
+      </c>
+      <c r="D1516" s="7">
+        <v>112.0</v>
+      </c>
+      <c r="E1516" s="8">
+        <v>0.6819444444444445</v>
+      </c>
+      <c r="F1516" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1516" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1516" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1516" s="11">
+        <v>17.7744952216744</v>
+      </c>
+      <c r="K1516" s="11">
+        <v>-64.8116724472493</v>
+      </c>
     </row>
     <row r="1517">
-      <c r="A1517" s="24"/>
-      <c r="B1517" s="7"/>
+      <c r="A1517" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1517" s="7" t="s">
+        <v>2459</v>
+      </c>
+      <c r="C1517" s="7" t="s">
+        <v>2460</v>
+      </c>
+      <c r="D1517" s="7">
+        <v>110.0</v>
+      </c>
+      <c r="E1517" s="8">
+        <v>0.6854166666666667</v>
+      </c>
+      <c r="F1517" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1517" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1517" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1517" s="11">
+        <v>17.7745740115643</v>
+      </c>
+      <c r="K1517" s="11">
+        <v>-64.8116115946323</v>
+      </c>
     </row>
     <row r="1518">
-      <c r="A1518" s="24"/>
-      <c r="B1518" s="7"/>
+      <c r="A1518" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1518" s="7" t="s">
+        <v>2461</v>
+      </c>
+      <c r="C1518" s="7" t="s">
+        <v>2462</v>
+      </c>
+      <c r="D1518" s="7">
+        <v>101.0</v>
+      </c>
+      <c r="E1518" s="8">
+        <v>0.6868055555555556</v>
+      </c>
+      <c r="F1518" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1518" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1518" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1518" s="11">
+        <v>17.7746434975415</v>
+      </c>
+      <c r="K1518" s="11">
+        <v>-64.8115561064333</v>
+      </c>
     </row>
     <row r="1519">
-      <c r="A1519" s="24"/>
-      <c r="B1519" s="7"/>
+      <c r="A1519" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1519" s="7" t="s">
+        <v>2463</v>
+      </c>
+      <c r="C1519" s="7" t="s">
+        <v>2464</v>
+      </c>
+      <c r="D1519" s="7">
+        <v>88.0</v>
+      </c>
+      <c r="E1519" s="8">
+        <v>0.6895833333333333</v>
+      </c>
+      <c r="F1519" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1519" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1519" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1519" s="11">
+        <v>17.7747575752437</v>
+      </c>
+      <c r="K1519" s="11">
+        <v>-64.8114904761314</v>
+      </c>
     </row>
     <row r="1520">
-      <c r="A1520" s="24"/>
-      <c r="B1520" s="7"/>
+      <c r="A1520" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1520" s="7" t="s">
+        <v>2465</v>
+      </c>
+      <c r="C1520" s="7" t="s">
+        <v>2466</v>
+      </c>
+      <c r="D1520" s="7">
+        <v>79.0</v>
+      </c>
+      <c r="E1520" s="8">
+        <v>0.6916666666666667</v>
+      </c>
+      <c r="F1520" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1520" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1520" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1520" s="11">
+        <v>17.7747127320617</v>
+      </c>
+      <c r="K1520" s="11">
+        <v>-64.8114499077201</v>
+      </c>
     </row>
     <row r="1521">
-      <c r="A1521" s="24"/>
-      <c r="B1521" s="7"/>
+      <c r="A1521" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1521" s="7" t="s">
+        <v>2467</v>
+      </c>
+      <c r="C1521" s="7" t="s">
+        <v>2468</v>
+      </c>
+      <c r="D1521" s="7">
+        <v>116.0</v>
+      </c>
+      <c r="E1521" s="8">
+        <v>0.6951388888888889</v>
+      </c>
+      <c r="F1521" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1521" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1521" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1521" s="11">
+        <v>17.7746916934848</v>
+      </c>
+      <c r="K1521" s="11">
+        <v>-64.8114053998142</v>
+      </c>
     </row>
     <row r="1522">
-      <c r="A1522" s="24"/>
-      <c r="B1522" s="7"/>
+      <c r="A1522" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1522" s="7" t="s">
+        <v>2469</v>
+      </c>
+      <c r="C1522" s="7" t="s">
+        <v>2470</v>
+      </c>
+      <c r="D1522" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="E1522" s="8">
+        <v>0.6972222222222222</v>
+      </c>
+      <c r="F1522" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1522" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1522" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1522" s="11">
+        <v>17.7747521270067</v>
+      </c>
+      <c r="K1522" s="11">
+        <v>-64.8114374186844</v>
+      </c>
     </row>
     <row r="1523">
-      <c r="A1523" s="24"/>
-      <c r="B1523" s="7"/>
+      <c r="A1523" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1523" s="7" t="s">
+        <v>2471</v>
+      </c>
+      <c r="C1523" s="7" t="s">
+        <v>2472</v>
+      </c>
+      <c r="D1523" s="7">
+        <v>45.0</v>
+      </c>
+      <c r="E1523" s="8">
+        <v>0.6993055555555555</v>
+      </c>
+      <c r="F1523" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1523" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1523" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1523" s="11">
+        <v>17.7747517079115</v>
+      </c>
+      <c r="K1523" s="11">
+        <v>-64.8114345688373</v>
+      </c>
     </row>
     <row r="1524">
-      <c r="A1524" s="24"/>
-      <c r="B1524" s="7"/>
+      <c r="A1524" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1524" s="7" t="s">
+        <v>2473</v>
+      </c>
+      <c r="C1524" s="7" t="s">
+        <v>2474</v>
+      </c>
+      <c r="D1524" s="7">
+        <v>22.0</v>
+      </c>
+      <c r="E1524" s="8">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="F1524" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1524" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1524" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1524" s="11">
+        <v>17.7748670428991</v>
+      </c>
+      <c r="K1524" s="11">
+        <v>-64.8113789968193</v>
+      </c>
     </row>
     <row r="1525">
-      <c r="A1525" s="24"/>
-      <c r="B1525" s="7"/>
+      <c r="A1525" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1525" s="7" t="s">
+        <v>2475</v>
+      </c>
+      <c r="C1525" s="7" t="s">
+        <v>2476</v>
+      </c>
+      <c r="D1525" s="7">
+        <v>7.0</v>
+      </c>
+      <c r="E1525" s="8">
+        <v>0.7034722222222223</v>
+      </c>
+      <c r="F1525" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1525" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1525" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1525" s="11">
+        <v>17.7747859898955</v>
+      </c>
+      <c r="K1525" s="11">
+        <v>-64.8113153781742</v>
+      </c>
     </row>
     <row r="1526">
-      <c r="A1526" s="24"/>
-      <c r="B1526" s="7"/>
+      <c r="A1526" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1526" s="7" t="s">
+        <v>2477</v>
+      </c>
+      <c r="C1526" s="7" t="s">
+        <v>2478</v>
+      </c>
+      <c r="D1526" s="7">
+        <v>118.0</v>
+      </c>
+      <c r="E1526" s="8">
+        <v>0.7076388888888889</v>
+      </c>
+      <c r="F1526" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1526" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1526" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1526" s="11">
+        <v>17.7748868241906</v>
+      </c>
+      <c r="K1526" s="11">
+        <v>-64.8111893981695</v>
+      </c>
     </row>
     <row r="1527">
-      <c r="A1527" s="24"/>
-      <c r="B1527" s="7"/>
+      <c r="A1527" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1527" s="7" t="s">
+        <v>2479</v>
+      </c>
+      <c r="C1527" s="7" t="s">
+        <v>2480</v>
+      </c>
+      <c r="D1527" s="7">
+        <v>36.0</v>
+      </c>
+      <c r="E1527" s="8">
+        <v>0.7104166666666667</v>
+      </c>
+      <c r="F1527" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1527" s="7" t="s">
+        <v>2434</v>
+      </c>
+      <c r="H1527" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1527" s="11">
+        <v>17.7749977167696</v>
+      </c>
+      <c r="K1527" s="11">
+        <v>-64.8111036513001</v>
+      </c>
     </row>
     <row r="1528">
-      <c r="A1528" s="24"/>
-      <c r="B1528" s="7"/>
+      <c r="A1528" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1528" s="7" t="s">
+        <v>2481</v>
+      </c>
+      <c r="C1528" s="7" t="s">
+        <v>2482</v>
+      </c>
+      <c r="D1528" s="7">
+        <v>40.0</v>
+      </c>
+      <c r="E1528" s="8">
+        <v>0.6506944444444445</v>
+      </c>
+      <c r="F1528" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1528" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1528" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1528" s="11">
+        <v>17.7741150185466</v>
+      </c>
+      <c r="K1528" s="11">
+        <v>-64.8114669229835</v>
+      </c>
     </row>
     <row r="1529">
-      <c r="A1529" s="24"/>
-      <c r="B1529" s="7"/>
+      <c r="A1529" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1529" s="7" t="s">
+        <v>2483</v>
+      </c>
+      <c r="C1529" s="7" t="s">
+        <v>2484</v>
+      </c>
+      <c r="D1529" s="7">
+        <v>102.0</v>
+      </c>
+      <c r="E1529" s="8">
+        <v>0.6527777777777778</v>
+      </c>
+      <c r="F1529" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1529" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1529" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1529" s="11">
+        <v>17.7741808164865</v>
+      </c>
+      <c r="K1529" s="11">
+        <v>-64.8114428669214</v>
+      </c>
     </row>
     <row r="1530">
-      <c r="A1530" s="24"/>
-      <c r="B1530" s="7"/>
+      <c r="A1530" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1530" s="7" t="s">
+        <v>2485</v>
+      </c>
+      <c r="C1530" s="7" t="s">
+        <v>2486</v>
+      </c>
+      <c r="D1530" s="7">
+        <v>209.0</v>
+      </c>
+      <c r="E1530" s="8">
+        <v>0.6548611111111111</v>
+      </c>
+      <c r="F1530" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1530" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1530" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1530" s="11">
+        <v>17.7742346283048</v>
+      </c>
+      <c r="K1530" s="11">
+        <v>-64.8114955052733</v>
+      </c>
+      <c r="M1530" s="7" t="s">
+        <v>2487</v>
+      </c>
     </row>
     <row r="1531">
-      <c r="A1531" s="24"/>
-      <c r="B1531" s="7"/>
+      <c r="A1531" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1531" s="7" t="s">
+        <v>2488</v>
+      </c>
+      <c r="C1531" s="7" t="s">
+        <v>2489</v>
+      </c>
+      <c r="D1531" s="7">
+        <v>25.0</v>
+      </c>
+      <c r="E1531" s="8">
+        <v>0.6569444444444444</v>
+      </c>
+      <c r="F1531" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1531" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1531" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1531" s="11">
+        <v>17.7742358855903</v>
+      </c>
+      <c r="K1531" s="11">
+        <v>-64.8114695213735</v>
+      </c>
     </row>
     <row r="1532">
-      <c r="A1532" s="24"/>
-      <c r="B1532" s="7"/>
+      <c r="A1532" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1532" s="7" t="s">
+        <v>2490</v>
+      </c>
+      <c r="C1532" s="7" t="s">
+        <v>2491</v>
+      </c>
+      <c r="D1532" s="7">
+        <v>75.0</v>
+      </c>
+      <c r="E1532" s="8">
+        <v>0.6597222222222222</v>
+      </c>
+      <c r="F1532" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1532" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1532" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1532" s="11">
+        <v>17.7742948103696</v>
+      </c>
+      <c r="K1532" s="11">
+        <v>-64.8114882130176</v>
+      </c>
     </row>
     <row r="1533">
-      <c r="A1533" s="24"/>
-      <c r="B1533" s="7"/>
+      <c r="A1533" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1533" s="7" t="s">
+        <v>2492</v>
+      </c>
+      <c r="C1533" s="7" t="s">
+        <v>2493</v>
+      </c>
+      <c r="D1533" s="7">
+        <v>108.0</v>
+      </c>
+      <c r="E1533" s="8">
+        <v>0.6618055555555555</v>
+      </c>
+      <c r="F1533" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1533" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1533" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1533" s="11">
+        <v>17.774288021028</v>
+      </c>
+      <c r="K1533" s="11">
+        <v>-64.8115694336593</v>
+      </c>
     </row>
     <row r="1534">
-      <c r="A1534" s="24"/>
-      <c r="B1534" s="7"/>
+      <c r="A1534" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1534" s="7" t="s">
+        <v>2494</v>
+      </c>
+      <c r="C1534" s="7" t="s">
+        <v>2495</v>
+      </c>
+      <c r="D1534" s="7">
+        <v>210.0</v>
+      </c>
+      <c r="E1534" s="8">
+        <v>0.6645833333333333</v>
+      </c>
+      <c r="F1534" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1534" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1534" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1534" s="11">
+        <v>17.7742934692651</v>
+      </c>
+      <c r="K1534" s="11">
+        <v>-64.8116089962423</v>
+      </c>
     </row>
     <row r="1535">
-      <c r="A1535" s="24"/>
-      <c r="B1535" s="7"/>
+      <c r="A1535" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1535" s="7" t="s">
+        <v>2496</v>
+      </c>
+      <c r="C1535" s="7" t="s">
+        <v>2497</v>
+      </c>
+      <c r="D1535" s="7">
+        <v>9.0</v>
+      </c>
+      <c r="E1535" s="8">
+        <v>0.6659722222222222</v>
+      </c>
+      <c r="F1535" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1535" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1535" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1535" s="11">
+        <v>17.7742081414908</v>
+      </c>
+      <c r="K1535" s="11">
+        <v>-64.811650570482</v>
+      </c>
     </row>
     <row r="1536">
-      <c r="A1536" s="24"/>
-      <c r="B1536" s="7"/>
+      <c r="A1536" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1536" s="7" t="s">
+        <v>2498</v>
+      </c>
+      <c r="C1536" s="7" t="s">
+        <v>2499</v>
+      </c>
+      <c r="D1536" s="7">
+        <v>20.0</v>
+      </c>
+      <c r="E1536" s="8">
+        <v>0.66875</v>
+      </c>
+      <c r="F1536" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1536" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1536" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1536" s="11">
+        <v>17.7742355503142</v>
+      </c>
+      <c r="K1536" s="11">
+        <v>-64.8116674181074</v>
+      </c>
+      <c r="M1536" s="7" t="s">
+        <v>2487</v>
+      </c>
     </row>
     <row r="1537">
-      <c r="A1537" s="24"/>
-      <c r="B1537" s="7"/>
+      <c r="A1537" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1537" s="7" t="s">
+        <v>2500</v>
+      </c>
+      <c r="C1537" s="7" t="s">
+        <v>2501</v>
+      </c>
+      <c r="D1537" s="7">
+        <v>44.0</v>
+      </c>
+      <c r="E1537" s="8">
+        <v>0.6715277777777777</v>
+      </c>
+      <c r="F1537" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1537" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1537" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1537" s="11">
+        <v>17.7742580138147</v>
+      </c>
+      <c r="K1537" s="11">
+        <v>-64.8117861058563</v>
+      </c>
+      <c r="M1537" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1538">
-      <c r="A1538" s="24"/>
-      <c r="B1538" s="7"/>
+      <c r="A1538" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1538" s="7" t="s">
+        <v>2502</v>
+      </c>
+      <c r="C1538" s="7" t="s">
+        <v>2501</v>
+      </c>
+      <c r="D1538" s="7">
+        <v>52.0</v>
+      </c>
+      <c r="E1538" s="8">
+        <v>0.6715277777777777</v>
+      </c>
+      <c r="F1538" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1538" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1538" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1538" s="11">
+        <v>17.7742580138147</v>
+      </c>
+      <c r="K1538" s="11">
+        <v>-64.8117861058563</v>
+      </c>
+      <c r="M1538" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1539">
-      <c r="A1539" s="24"/>
-      <c r="B1539" s="7"/>
+      <c r="A1539" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1539" s="7" t="s">
+        <v>2503</v>
+      </c>
+      <c r="C1539" s="7" t="s">
+        <v>2504</v>
+      </c>
+      <c r="D1539" s="7">
+        <v>23.0</v>
+      </c>
+      <c r="E1539" s="8">
+        <v>0.6743055555555556</v>
+      </c>
+      <c r="F1539" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1539" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1539" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1539" s="11">
+        <v>17.7743527293205</v>
+      </c>
+      <c r="K1539" s="11">
+        <v>-64.8119244910777</v>
+      </c>
     </row>
     <row r="1540">
-      <c r="A1540" s="24"/>
-      <c r="B1540" s="7"/>
+      <c r="A1540" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1540" s="7" t="s">
+        <v>2505</v>
+      </c>
+      <c r="C1540" s="7" t="s">
+        <v>2506</v>
+      </c>
+      <c r="D1540" s="7">
+        <v>27.0</v>
+      </c>
+      <c r="E1540" s="8">
+        <v>0.6763888888888889</v>
+      </c>
+      <c r="F1540" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1540" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1540" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1540" s="11">
+        <v>17.7743105683476</v>
+      </c>
+      <c r="K1540" s="11">
+        <v>-64.8117943201214</v>
+      </c>
     </row>
     <row r="1541">
-      <c r="A1541" s="24"/>
-      <c r="B1541" s="7"/>
+      <c r="A1541" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1541" s="7" t="s">
+        <v>2507</v>
+      </c>
+      <c r="C1541" s="7" t="s">
+        <v>2508</v>
+      </c>
+      <c r="D1541" s="7">
+        <v>37.0</v>
+      </c>
+      <c r="E1541" s="8">
+        <v>0.6784722222222223</v>
+      </c>
+      <c r="F1541" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1541" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1541" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1541" s="11">
+        <v>17.7743202913553</v>
+      </c>
+      <c r="K1541" s="11">
+        <v>-64.8117186315358</v>
+      </c>
     </row>
     <row r="1542">
-      <c r="A1542" s="24"/>
-      <c r="B1542" s="7"/>
+      <c r="A1542" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1542" s="7" t="s">
+        <v>2509</v>
+      </c>
+      <c r="C1542" s="7" t="s">
+        <v>2510</v>
+      </c>
+      <c r="D1542" s="7">
+        <v>218.0</v>
+      </c>
+      <c r="E1542" s="8">
+        <v>0.68125</v>
+      </c>
+      <c r="F1542" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1542" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1542" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1542" s="11">
+        <v>17.7744473610073</v>
+      </c>
+      <c r="K1542" s="11">
+        <v>-64.811716619879</v>
+      </c>
     </row>
     <row r="1543">
-      <c r="A1543" s="24"/>
-      <c r="B1543" s="7"/>
+      <c r="A1543" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1543" s="7" t="s">
+        <v>2511</v>
+      </c>
+      <c r="C1543" s="7" t="s">
+        <v>2512</v>
+      </c>
+      <c r="D1543" s="7">
+        <v>200.0</v>
+      </c>
+      <c r="E1543" s="8">
+        <v>0.6833333333333333</v>
+      </c>
+      <c r="F1543" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1543" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1543" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1543" s="11">
+        <v>17.7745056152344</v>
+      </c>
+      <c r="K1543" s="11">
+        <v>-64.8116385005414</v>
+      </c>
     </row>
     <row r="1544">
-      <c r="A1544" s="24"/>
-      <c r="B1544" s="7"/>
+      <c r="A1544" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1544" s="7" t="s">
+        <v>2513</v>
+      </c>
+      <c r="C1544" s="7" t="s">
+        <v>2514</v>
+      </c>
+      <c r="D1544" s="7">
+        <v>77.0</v>
+      </c>
+      <c r="E1544" s="8">
+        <v>0.6854166666666667</v>
+      </c>
+      <c r="F1544" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1544" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1544" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1544" s="11">
+        <v>17.7745740115643</v>
+      </c>
+      <c r="K1544" s="11">
+        <v>-64.8116115946323</v>
+      </c>
     </row>
     <row r="1545">
-      <c r="A1545" s="24"/>
-      <c r="B1545" s="7"/>
+      <c r="A1545" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1545" s="7" t="s">
+        <v>2515</v>
+      </c>
+      <c r="C1545" s="7" t="s">
+        <v>2514</v>
+      </c>
+      <c r="D1545" s="7">
+        <v>29.0</v>
+      </c>
+      <c r="E1545" s="8">
+        <v>0.6854166666666667</v>
+      </c>
+      <c r="F1545" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1545" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1545" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1545" s="11">
+        <v>17.7745740115643</v>
+      </c>
+      <c r="K1545" s="11">
+        <v>-64.8116115946323</v>
+      </c>
     </row>
     <row r="1546">
-      <c r="A1546" s="24"/>
-      <c r="B1546" s="7"/>
+      <c r="A1546" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1546" s="7" t="s">
+        <v>2516</v>
+      </c>
+      <c r="C1546" s="7" t="s">
+        <v>2517</v>
+      </c>
+      <c r="D1546" s="7">
+        <v>104.0</v>
+      </c>
+      <c r="E1546" s="8">
+        <v>0.6881944444444444</v>
+      </c>
+      <c r="F1546" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1546" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1546" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1546" s="11">
+        <v>17.7747007459402</v>
+      </c>
+      <c r="K1546" s="11">
+        <v>-64.8115267697722</v>
+      </c>
     </row>
     <row r="1547">
-      <c r="A1547" s="24"/>
-      <c r="B1547" s="7"/>
+      <c r="A1547" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1547" s="7" t="s">
+        <v>2518</v>
+      </c>
+      <c r="C1547" s="7" t="s">
+        <v>2519</v>
+      </c>
+      <c r="D1547" s="7">
+        <v>115.0</v>
+      </c>
+      <c r="E1547" s="8">
+        <v>0.6895833333333333</v>
+      </c>
+      <c r="F1547" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1547" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1547" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1547" s="11">
+        <v>17.7747575752437</v>
+      </c>
+      <c r="K1547" s="11">
+        <v>-64.8114904761314</v>
+      </c>
     </row>
     <row r="1548">
-      <c r="A1548" s="24"/>
-      <c r="B1548" s="7"/>
+      <c r="A1548" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1548" s="7" t="s">
+        <v>2520</v>
+      </c>
+      <c r="C1548" s="7" t="s">
+        <v>2521</v>
+      </c>
+      <c r="D1548" s="7">
+        <v>120.0</v>
+      </c>
+      <c r="E1548" s="8">
+        <v>0.6916666666666667</v>
+      </c>
+      <c r="F1548" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1548" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1548" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1548" s="11">
+        <v>17.7747127320617</v>
+      </c>
+      <c r="K1548" s="11">
+        <v>-64.8114499077201</v>
+      </c>
     </row>
     <row r="1549">
-      <c r="A1549" s="24"/>
-      <c r="B1549" s="7"/>
+      <c r="A1549" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1549" s="7" t="s">
+        <v>2522</v>
+      </c>
+      <c r="C1549" s="7" t="s">
+        <v>2523</v>
+      </c>
+      <c r="D1549" s="7">
+        <v>15.0</v>
+      </c>
+      <c r="E1549" s="8">
+        <v>0.6930555555555555</v>
+      </c>
+      <c r="F1549" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1549" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1549" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1549" s="11">
+        <v>17.774692280218</v>
+      </c>
+      <c r="K1549" s="11">
+        <v>-64.8114665877074</v>
+      </c>
     </row>
     <row r="1550">
-      <c r="A1550" s="24"/>
-      <c r="B1550" s="7"/>
+      <c r="A1550" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1550" s="7" t="s">
+        <v>2524</v>
+      </c>
+      <c r="C1550" s="7" t="s">
+        <v>2525</v>
+      </c>
+      <c r="D1550" s="7">
+        <v>38.0</v>
+      </c>
+      <c r="E1550" s="8">
+        <v>0.6965277777777777</v>
+      </c>
+      <c r="F1550" s="7" t="s">
+        <v>1197</v>
+      </c>
+      <c r="G1550" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1550" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1550" s="11">
+        <v>17.774716168642</v>
+      </c>
+      <c r="K1550" s="11">
+        <v>-64.8114317189902</v>
+      </c>
     </row>
     <row r="1551">
-      <c r="A1551" s="24"/>
-      <c r="B1551" s="7"/>
+      <c r="A1551" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1551" s="7" t="s">
+        <v>2526</v>
+      </c>
+      <c r="C1551" s="7" t="s">
+        <v>2527</v>
+      </c>
+      <c r="D1551" s="7">
+        <v>113.0</v>
+      </c>
+      <c r="E1551" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="F1551" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1551" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1551" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1551" s="11">
+        <v>17.7746872510761</v>
+      </c>
+      <c r="K1551" s="11">
+        <v>-64.8113798350096</v>
+      </c>
     </row>
     <row r="1552">
-      <c r="A1552" s="24"/>
-      <c r="B1552" s="7"/>
+      <c r="A1552" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1552" s="7" t="s">
+        <v>2528</v>
+      </c>
+      <c r="C1552" s="7" t="s">
+        <v>2529</v>
+      </c>
+      <c r="D1552" s="7">
+        <v>47.0</v>
+      </c>
+      <c r="E1552" s="8">
+        <v>0.7027777777777777</v>
+      </c>
+      <c r="F1552" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1552" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1552" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1552" s="11">
+        <v>17.7747962158173</v>
+      </c>
+      <c r="K1552" s="11">
+        <v>-64.8113378416747</v>
+      </c>
     </row>
     <row r="1553">
-      <c r="A1553" s="24"/>
-      <c r="B1553" s="7"/>
+      <c r="A1553" s="6">
+        <v>44738.0</v>
+      </c>
+      <c r="B1553" s="7" t="s">
+        <v>2530</v>
+      </c>
+      <c r="C1553" s="7" t="s">
+        <v>2531</v>
+      </c>
+      <c r="D1553" s="7">
+        <v>71.0</v>
+      </c>
+      <c r="E1553" s="8">
+        <v>0.7083333333333334</v>
+      </c>
+      <c r="F1553" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1553" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1553" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1553" s="11">
+        <v>17.7748895902187</v>
+      </c>
+      <c r="K1553" s="11">
+        <v>-64.8111925832927</v>
+      </c>
     </row>
     <row r="1554">
       <c r="A1554" s="24"/>
@@ -59362,19 +61083,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>2432</v>
+        <v>2532</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2433</v>
+        <v>2533</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2434</v>
+        <v>2534</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2435</v>
+        <v>2535</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2436</v>
+        <v>2536</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>7</v>
@@ -59398,21 +61119,21 @@
         <v>51</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>2437</v>
+        <v>2537</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>145</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>2438</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>2439</v>
+        <v>2539</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2440</v>
+        <v>2540</v>
       </c>
       <c r="C2" s="7">
         <v>7.0</v>
@@ -59424,33 +61145,33 @@
         <v>44688.0</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>2441</v>
+        <v>2541</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>2441</v>
+        <v>2541</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>2441</v>
+        <v>2541</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>2441</v>
+        <v>2541</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>2441</v>
+        <v>2541</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>2442</v>
+        <v>2542</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>2443</v>
+        <v>2543</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>2444</v>
+        <v>2544</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2445</v>
+        <v>2545</v>
       </c>
       <c r="C3" s="7">
         <v>25.0</v>
@@ -59461,10 +61182,10 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>2446</v>
+        <v>2546</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="C4" s="7">
         <v>15.0</v>
@@ -59476,18 +61197,18 @@
         <v>44690.0</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>2448</v>
+        <v>2548</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>2449</v>
+        <v>2549</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2450</v>
+        <v>2550</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2451</v>
+        <v>2551</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>20</v>
@@ -59495,10 +61216,10 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>2452</v>
+        <v>2552</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2453</v>
+        <v>2553</v>
       </c>
       <c r="C6" s="7">
         <v>20.0</v>
@@ -59530,10 +61251,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>2454</v>
+        <v>2554</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2455</v>
+        <v>2555</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>78</v>
@@ -59565,7 +61286,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2439</v>
+        <v>2539</v>
       </c>
       <c r="C2" s="7">
         <v>2.0</v>
@@ -59594,7 +61315,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2446</v>
+        <v>2546</v>
       </c>
       <c r="C3" s="7">
         <v>5.0</v>
@@ -59623,7 +61344,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2444</v>
+        <v>2544</v>
       </c>
       <c r="F4" s="7">
         <v>17.0</v>
@@ -59646,7 +61367,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2452</v>
+        <v>2552</v>
       </c>
       <c r="F5" s="7">
         <v>6.0</v>
@@ -59669,7 +61390,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2456</v>
+        <v>2556</v>
       </c>
       <c r="F6" s="7">
         <v>11.0</v>
@@ -59712,16 +61433,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="26" t="s">
-        <v>2457</v>
+        <v>2557</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>2458</v>
+        <v>2558</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>2459</v>
+        <v>2559</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>12</v>
@@ -59751,7 +61472,7 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B2" s="6">
         <v>44690.0</v>
@@ -59766,7 +61487,7 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B3" s="6">
         <v>44690.0</v>
@@ -59781,7 +61502,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B4" s="6">
         <v>44690.0</v>
@@ -59796,7 +61517,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B5" s="6">
         <v>44690.0</v>
@@ -59811,7 +61532,7 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B6" s="6">
         <v>44690.0</v>
@@ -59826,7 +61547,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B7" s="6">
         <v>44690.0</v>
@@ -59841,7 +61562,7 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B8" s="6">
         <v>44690.0</v>
@@ -59856,7 +61577,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B9" s="6">
         <v>44690.0</v>
@@ -59871,7 +61592,7 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B10" s="6">
         <v>44690.0</v>
@@ -59886,7 +61607,7 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B11" s="6">
         <v>44690.0</v>
@@ -59901,7 +61622,7 @@
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B12" s="6">
         <v>44690.0</v>
@@ -59916,7 +61637,7 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B13" s="6">
         <v>44690.0</v>
@@ -59931,7 +61652,7 @@
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B14" s="6">
         <v>44690.0</v>
@@ -59946,7 +61667,7 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B15" s="6">
         <v>44690.0</v>
@@ -59961,7 +61682,7 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B16" s="6">
         <v>44690.0</v>
@@ -59976,7 +61697,7 @@
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B17" s="6">
         <v>44690.0</v>
@@ -59992,7 +61713,7 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B18" s="6">
         <v>44690.0</v>
@@ -60008,7 +61729,7 @@
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B19" s="6">
         <v>44690.0</v>
@@ -60023,7 +61744,7 @@
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B20" s="6">
         <v>44690.0</v>
@@ -60038,7 +61759,7 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B21" s="6">
         <v>44690.0</v>
@@ -60053,7 +61774,7 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B22" s="6">
         <v>44690.0</v>
@@ -60068,7 +61789,7 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B23" s="6">
         <v>44690.0</v>
@@ -60083,7 +61804,7 @@
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B24" s="6">
         <v>44690.0</v>
@@ -60098,7 +61819,7 @@
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B25" s="6">
         <v>44690.0</v>
@@ -60113,7 +61834,7 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B26" s="6">
         <v>44690.0</v>
@@ -60128,7 +61849,7 @@
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B27" s="6">
         <v>44690.0</v>
@@ -60143,7 +61864,7 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B28" s="6">
         <v>44690.0</v>
@@ -60158,7 +61879,7 @@
     </row>
     <row r="29">
       <c r="A29" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B29" s="6">
         <v>44690.0</v>
@@ -60173,7 +61894,7 @@
     </row>
     <row r="30">
       <c r="A30" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B30" s="6">
         <v>44690.0</v>
@@ -60188,7 +61909,7 @@
     </row>
     <row r="31">
       <c r="A31" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B31" s="6">
         <v>44690.0</v>
@@ -60203,7 +61924,7 @@
     </row>
     <row r="32">
       <c r="A32" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B32" s="6">
         <v>44690.0</v>
@@ -60218,7 +61939,7 @@
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B33" s="6">
         <v>44690.0</v>
@@ -60233,7 +61954,7 @@
     </row>
     <row r="34">
       <c r="A34" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B34" s="6">
         <v>44690.0</v>
@@ -60248,7 +61969,7 @@
     </row>
     <row r="35">
       <c r="A35" s="7" t="s">
-        <v>2447</v>
+        <v>2547</v>
       </c>
       <c r="B35" s="6">
         <v>44690.0</v>
@@ -60263,7 +61984,7 @@
     </row>
     <row r="36">
       <c r="A36" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B36" s="6">
         <v>44704.0</v>
@@ -60278,7 +61999,7 @@
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B37" s="6">
         <v>44704.0</v>
@@ -60293,7 +62014,7 @@
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B38" s="6">
         <v>44704.0</v>
@@ -60305,12 +62026,12 @@
         <v>22.0</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>2461</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B39" s="6">
         <v>44704.0</v>
@@ -60325,7 +62046,7 @@
     </row>
     <row r="40">
       <c r="A40" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B40" s="6">
         <v>44704.0</v>
@@ -60337,12 +62058,12 @@
         <v>34.0</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>2461</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B41" s="6">
         <v>44704.0</v>
@@ -60357,7 +62078,7 @@
     </row>
     <row r="42">
       <c r="A42" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B42" s="6">
         <v>44704.0</v>
@@ -60372,7 +62093,7 @@
     </row>
     <row r="43">
       <c r="A43" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B43" s="6">
         <v>44704.0</v>
@@ -60387,7 +62108,7 @@
     </row>
     <row r="44">
       <c r="A44" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B44" s="6">
         <v>44704.0</v>
@@ -60399,12 +62120,12 @@
         <v>6.0</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>2461</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B45" s="6">
         <v>44704.0</v>
@@ -60419,7 +62140,7 @@
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B46" s="6">
         <v>44704.0</v>
@@ -60434,7 +62155,7 @@
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B47" s="6">
         <v>44704.0</v>
@@ -60449,7 +62170,7 @@
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B48" s="6">
         <v>44704.0</v>
@@ -60464,7 +62185,7 @@
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B49" s="6">
         <v>44704.0</v>
@@ -60479,7 +62200,7 @@
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B50" s="6">
         <v>44704.0</v>
@@ -60494,7 +62215,7 @@
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B51" s="6">
         <v>44704.0</v>
@@ -60509,7 +62230,7 @@
     </row>
     <row r="52">
       <c r="A52" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B52" s="6">
         <v>44704.0</v>
@@ -60524,7 +62245,7 @@
     </row>
     <row r="53">
       <c r="A53" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B53" s="6">
         <v>44704.0</v>
@@ -60539,7 +62260,7 @@
     </row>
     <row r="54">
       <c r="A54" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B54" s="6">
         <v>44704.0</v>
@@ -60554,7 +62275,7 @@
     </row>
     <row r="55">
       <c r="A55" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B55" s="6">
         <v>44704.0</v>
@@ -60569,7 +62290,7 @@
     </row>
     <row r="56">
       <c r="A56" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B56" s="6">
         <v>44704.0</v>
@@ -60584,7 +62305,7 @@
     </row>
     <row r="57">
       <c r="A57" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B57" s="6">
         <v>44704.0</v>
@@ -60599,7 +62320,7 @@
     </row>
     <row r="58">
       <c r="A58" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B58" s="6">
         <v>44704.0</v>
@@ -60614,7 +62335,7 @@
     </row>
     <row r="59">
       <c r="A59" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B59" s="6">
         <v>44704.0</v>
@@ -60629,7 +62350,7 @@
     </row>
     <row r="60">
       <c r="A60" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B60" s="6">
         <v>44704.0</v>
@@ -60644,7 +62365,7 @@
     </row>
     <row r="61">
       <c r="A61" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B61" s="6">
         <v>44704.0</v>
@@ -60659,7 +62380,7 @@
     </row>
     <row r="62">
       <c r="A62" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B62" s="6">
         <v>44704.0</v>
@@ -60674,7 +62395,7 @@
     </row>
     <row r="63">
       <c r="A63" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B63" s="6">
         <v>44704.0</v>
@@ -60689,7 +62410,7 @@
     </row>
     <row r="64">
       <c r="A64" s="7" t="s">
-        <v>2460</v>
+        <v>2560</v>
       </c>
       <c r="B64" s="6">
         <v>44704.0</v>
@@ -60704,7 +62425,7 @@
     </row>
     <row r="65">
       <c r="A65" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B65" s="6">
         <v>44704.0</v>
@@ -60719,7 +62440,7 @@
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B66" s="6">
         <v>44704.0</v>
@@ -60734,7 +62455,7 @@
     </row>
     <row r="67">
       <c r="A67" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B67" s="6">
         <v>44704.0</v>
@@ -60749,7 +62470,7 @@
     </row>
     <row r="68">
       <c r="A68" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B68" s="6">
         <v>44704.0</v>
@@ -60764,7 +62485,7 @@
     </row>
     <row r="69">
       <c r="A69" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B69" s="6">
         <v>44704.0</v>
@@ -60779,7 +62500,7 @@
     </row>
     <row r="70">
       <c r="A70" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B70" s="6">
         <v>44704.0</v>
@@ -60794,7 +62515,7 @@
     </row>
     <row r="71">
       <c r="A71" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B71" s="6">
         <v>44704.0</v>
@@ -60809,7 +62530,7 @@
     </row>
     <row r="72">
       <c r="A72" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B72" s="6">
         <v>44704.0</v>
@@ -60824,7 +62545,7 @@
     </row>
     <row r="73">
       <c r="A73" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B73" s="6">
         <v>44704.0</v>
@@ -60839,7 +62560,7 @@
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B74" s="6">
         <v>44704.0</v>
@@ -60854,7 +62575,7 @@
     </row>
     <row r="75">
       <c r="A75" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B75" s="6">
         <v>44704.0</v>
@@ -60869,7 +62590,7 @@
     </row>
     <row r="76">
       <c r="A76" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B76" s="6">
         <v>44704.0</v>
@@ -60884,7 +62605,7 @@
     </row>
     <row r="77">
       <c r="A77" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B77" s="6">
         <v>44704.0</v>
@@ -60899,7 +62620,7 @@
     </row>
     <row r="78">
       <c r="A78" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B78" s="6">
         <v>44704.0</v>
@@ -60914,7 +62635,7 @@
     </row>
     <row r="79">
       <c r="A79" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B79" s="6">
         <v>44704.0</v>
@@ -60929,7 +62650,7 @@
     </row>
     <row r="80">
       <c r="A80" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B80" s="6">
         <v>44704.0</v>
@@ -60944,7 +62665,7 @@
     </row>
     <row r="81">
       <c r="A81" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B81" s="6">
         <v>44704.0</v>
@@ -60959,7 +62680,7 @@
     </row>
     <row r="82">
       <c r="A82" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B82" s="6">
         <v>44704.0</v>
@@ -60974,7 +62695,7 @@
     </row>
     <row r="83">
       <c r="A83" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B83" s="6">
         <v>44704.0</v>
@@ -60989,7 +62710,7 @@
     </row>
     <row r="84">
       <c r="A84" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B84" s="6">
         <v>44704.0</v>
@@ -61004,7 +62725,7 @@
     </row>
     <row r="85">
       <c r="A85" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B85" s="6">
         <v>44704.0</v>
@@ -61019,7 +62740,7 @@
     </row>
     <row r="86">
       <c r="A86" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B86" s="6">
         <v>44704.0</v>
@@ -61034,7 +62755,7 @@
     </row>
     <row r="87">
       <c r="A87" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B87" s="6">
         <v>44704.0</v>
@@ -61049,7 +62770,7 @@
     </row>
     <row r="88">
       <c r="A88" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B88" s="6">
         <v>44704.0</v>
@@ -61064,7 +62785,7 @@
     </row>
     <row r="89">
       <c r="A89" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B89" s="6">
         <v>44704.0</v>
@@ -61079,7 +62800,7 @@
     </row>
     <row r="90">
       <c r="A90" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B90" s="6">
         <v>44704.0</v>
@@ -61094,7 +62815,7 @@
     </row>
     <row r="91">
       <c r="A91" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B91" s="6">
         <v>44704.0</v>
@@ -61109,7 +62830,7 @@
     </row>
     <row r="92">
       <c r="A92" s="7" t="s">
-        <v>2462</v>
+        <v>2562</v>
       </c>
       <c r="B92" s="6">
         <v>44704.0</v>
@@ -61124,7 +62845,7 @@
     </row>
     <row r="93">
       <c r="A93" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B93" s="6">
         <v>44705.0</v>
@@ -61139,7 +62860,7 @@
     </row>
     <row r="94">
       <c r="A94" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B94" s="6">
         <v>44705.0</v>
@@ -61154,7 +62875,7 @@
     </row>
     <row r="95">
       <c r="A95" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B95" s="6">
         <v>44705.0</v>
@@ -61169,7 +62890,7 @@
     </row>
     <row r="96">
       <c r="A96" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B96" s="6">
         <v>44705.0</v>
@@ -61184,7 +62905,7 @@
     </row>
     <row r="97">
       <c r="A97" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B97" s="6">
         <v>44705.0</v>
@@ -61199,7 +62920,7 @@
     </row>
     <row r="98">
       <c r="A98" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B98" s="6">
         <v>44705.0</v>
@@ -61214,7 +62935,7 @@
     </row>
     <row r="99">
       <c r="A99" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B99" s="6">
         <v>44705.0</v>
@@ -61229,7 +62950,7 @@
     </row>
     <row r="100">
       <c r="A100" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B100" s="6">
         <v>44705.0</v>
@@ -61244,7 +62965,7 @@
     </row>
     <row r="101">
       <c r="A101" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B101" s="6">
         <v>44705.0</v>
@@ -61259,7 +62980,7 @@
     </row>
     <row r="102">
       <c r="A102" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B102" s="6">
         <v>44705.0</v>
@@ -61274,7 +62995,7 @@
     </row>
     <row r="103">
       <c r="A103" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B103" s="6">
         <v>44705.0</v>
@@ -61289,7 +63010,7 @@
     </row>
     <row r="104">
       <c r="A104" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B104" s="6">
         <v>44705.0</v>
@@ -61304,7 +63025,7 @@
     </row>
     <row r="105">
       <c r="A105" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B105" s="6">
         <v>44705.0</v>
@@ -61319,7 +63040,7 @@
     </row>
     <row r="106">
       <c r="A106" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B106" s="6">
         <v>44705.0</v>
@@ -61334,7 +63055,7 @@
     </row>
     <row r="107">
       <c r="A107" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B107" s="6">
         <v>44705.0</v>
@@ -61349,7 +63070,7 @@
     </row>
     <row r="108">
       <c r="A108" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B108" s="6">
         <v>44705.0</v>
@@ -61364,7 +63085,7 @@
     </row>
     <row r="109">
       <c r="A109" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B109" s="6">
         <v>44705.0</v>
@@ -61379,7 +63100,7 @@
     </row>
     <row r="110">
       <c r="A110" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B110" s="6">
         <v>44705.0</v>
@@ -61394,7 +63115,7 @@
     </row>
     <row r="111">
       <c r="A111" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B111" s="6">
         <v>44705.0</v>
@@ -61409,7 +63130,7 @@
     </row>
     <row r="112">
       <c r="A112" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B112" s="6">
         <v>44705.0</v>
@@ -61424,7 +63145,7 @@
     </row>
     <row r="113">
       <c r="A113" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B113" s="6">
         <v>44705.0</v>
@@ -61439,7 +63160,7 @@
     </row>
     <row r="114">
       <c r="A114" s="7" t="s">
-        <v>2463</v>
+        <v>2563</v>
       </c>
       <c r="B114" s="6">
         <v>44705.0</v>
@@ -61454,7 +63175,7 @@
     </row>
     <row r="115">
       <c r="A115" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B115" s="6">
         <v>44708.0</v>
@@ -61469,7 +63190,7 @@
     </row>
     <row r="116">
       <c r="A116" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B116" s="6">
         <v>44708.0</v>
@@ -61484,7 +63205,7 @@
     </row>
     <row r="117">
       <c r="A117" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B117" s="6">
         <v>44708.0</v>
@@ -61499,7 +63220,7 @@
     </row>
     <row r="118">
       <c r="A118" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B118" s="6">
         <v>44708.0</v>
@@ -61511,12 +63232,12 @@
         <v>39.0</v>
       </c>
       <c r="E118" s="29" t="s">
-        <v>2461</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B119" s="6">
         <v>44708.0</v>
@@ -61531,7 +63252,7 @@
     </row>
     <row r="120">
       <c r="A120" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B120" s="6">
         <v>44708.0</v>
@@ -61546,7 +63267,7 @@
     </row>
     <row r="121">
       <c r="A121" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B121" s="6">
         <v>44708.0</v>
@@ -61561,7 +63282,7 @@
     </row>
     <row r="122">
       <c r="A122" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B122" s="6">
         <v>44708.0</v>
@@ -61576,7 +63297,7 @@
     </row>
     <row r="123">
       <c r="A123" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B123" s="6">
         <v>44708.0</v>
@@ -61591,7 +63312,7 @@
     </row>
     <row r="124">
       <c r="A124" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B124" s="6">
         <v>44708.0</v>
@@ -61606,7 +63327,7 @@
     </row>
     <row r="125">
       <c r="A125" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B125" s="6">
         <v>44708.0</v>
@@ -61621,7 +63342,7 @@
     </row>
     <row r="126">
       <c r="A126" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B126" s="6">
         <v>44708.0</v>
@@ -61636,7 +63357,7 @@
     </row>
     <row r="127">
       <c r="A127" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B127" s="6">
         <v>44708.0</v>
@@ -61648,12 +63369,12 @@
         <v>11.0</v>
       </c>
       <c r="E127" s="29" t="s">
-        <v>2461</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B128" s="6">
         <v>44708.0</v>
@@ -61668,7 +63389,7 @@
     </row>
     <row r="129">
       <c r="A129" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B129" s="6">
         <v>44708.0</v>
@@ -61680,12 +63401,12 @@
         <v>40.0</v>
       </c>
       <c r="E129" s="29" t="s">
-        <v>2461</v>
+        <v>2561</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B130" s="6">
         <v>44708.0</v>
@@ -61700,7 +63421,7 @@
     </row>
     <row r="131">
       <c r="A131" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B131" s="6">
         <v>44708.0</v>
@@ -61715,7 +63436,7 @@
     </row>
     <row r="132">
       <c r="A132" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B132" s="6">
         <v>44708.0</v>
@@ -61730,7 +63451,7 @@
     </row>
     <row r="133">
       <c r="A133" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="B133" s="6">
         <v>44708.0</v>
@@ -61745,7 +63466,7 @@
     </row>
     <row r="134">
       <c r="A134" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B134" s="6">
         <v>44713.0</v>
@@ -61757,12 +63478,12 @@
         <v>1298</v>
       </c>
       <c r="E134" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B135" s="6">
         <v>44713.0</v>
@@ -61774,12 +63495,12 @@
         <v>1300</v>
       </c>
       <c r="E135" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B136" s="6">
         <v>44713.0</v>
@@ -61791,12 +63512,12 @@
         <v>1302</v>
       </c>
       <c r="E136" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B137" s="6">
         <v>44713.0</v>
@@ -61808,12 +63529,12 @@
         <v>1304</v>
       </c>
       <c r="E137" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B138" s="6">
         <v>44713.0</v>
@@ -61825,12 +63546,12 @@
         <v>1306</v>
       </c>
       <c r="E138" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B139" s="6">
         <v>44713.0</v>
@@ -61842,12 +63563,12 @@
         <v>1309</v>
       </c>
       <c r="E139" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B140" s="6">
         <v>44713.0</v>
@@ -61859,12 +63580,12 @@
         <v>1312</v>
       </c>
       <c r="E140" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B141" s="6">
         <v>44713.0</v>
@@ -61876,12 +63597,12 @@
         <v>1315</v>
       </c>
       <c r="E141" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B142" s="6">
         <v>44713.0</v>
@@ -61893,12 +63614,12 @@
         <v>1318</v>
       </c>
       <c r="E142" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B143" s="6">
         <v>44713.0</v>
@@ -61910,12 +63631,12 @@
         <v>1321</v>
       </c>
       <c r="E143" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B144" s="6">
         <v>44713.0</v>
@@ -61927,12 +63648,12 @@
         <v>1323</v>
       </c>
       <c r="E144" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B145" s="6">
         <v>44713.0</v>
@@ -61944,12 +63665,12 @@
         <v>1325</v>
       </c>
       <c r="E145" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B146" s="6">
         <v>44713.0</v>
@@ -61961,12 +63682,12 @@
         <v>1327</v>
       </c>
       <c r="E146" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B147" s="6">
         <v>44713.0</v>
@@ -61978,12 +63699,12 @@
         <v>1329</v>
       </c>
       <c r="E147" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B148" s="6">
         <v>44713.0</v>
@@ -61995,12 +63716,12 @@
         <v>1331</v>
       </c>
       <c r="E148" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B149" s="6">
         <v>44713.0</v>
@@ -62012,12 +63733,12 @@
         <v>1333</v>
       </c>
       <c r="E149" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B150" s="6">
         <v>44713.0</v>
@@ -62029,12 +63750,12 @@
         <v>1335</v>
       </c>
       <c r="E150" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B151" s="6">
         <v>44713.0</v>
@@ -62046,12 +63767,12 @@
         <v>1337</v>
       </c>
       <c r="E151" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B152" s="6">
         <v>44713.0</v>
@@ -62063,12 +63784,12 @@
         <v>1340</v>
       </c>
       <c r="E152" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B153" s="6">
         <v>44713.0</v>
@@ -62080,12 +63801,12 @@
         <v>1342</v>
       </c>
       <c r="E153" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B154" s="6">
         <v>44713.0</v>
@@ -62097,12 +63818,12 @@
         <v>1344</v>
       </c>
       <c r="E154" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B155" s="6">
         <v>44713.0</v>
@@ -62114,12 +63835,12 @@
         <v>1346</v>
       </c>
       <c r="E155" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B156" s="6">
         <v>44713.0</v>
@@ -62131,12 +63852,12 @@
         <v>1348</v>
       </c>
       <c r="E156" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="7" t="s">
-        <v>2465</v>
+        <v>2565</v>
       </c>
       <c r="B157" s="6">
         <v>44713.0</v>
@@ -62148,7 +63869,7 @@
         <v>1350</v>
       </c>
       <c r="E157" s="29" t="s">
-        <v>2466</v>
+        <v>2566</v>
       </c>
     </row>
     <row r="158">
@@ -64700,22 +66421,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2467</v>
+        <v>2567</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2468</v>
+        <v>2568</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2469</v>
+        <v>2569</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2470</v>
+        <v>2570</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>2471</v>
+        <v>2571</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>2472</v>
+        <v>2572</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>12</v>
@@ -64726,17 +66447,17 @@
         <v>44690.0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2473</v>
+        <v>2573</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>2446</v>
+        <v>2546</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7" t="s">
-        <v>2474</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="3">
@@ -64744,7 +66465,7 @@
         <v>44692.0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2475</v>
+        <v>2575</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="7" t="s">
@@ -64765,10 +66486,10 @@
         <v>44694.0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2476</v>
+        <v>2576</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>2452</v>
+        <v>2552</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
@@ -64783,7 +66504,7 @@
         <v>2.5</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>2477</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="5">
@@ -64791,10 +66512,10 @@
         <v>44695.0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2478</v>
+        <v>2578</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2456</v>
+        <v>2556</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -64814,10 +66535,10 @@
         <v>44697.0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2479</v>
+        <v>2579</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>2480</v>
+        <v>2580</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -64837,10 +66558,10 @@
         <v>44698.0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>2464</v>
+        <v>2564</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>2481</v>
+        <v>2581</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -64860,10 +66581,10 @@
         <v>44726.0</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>2482</v>
+        <v>2582</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>2483</v>
+        <v>2583</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>1353</v>

</xml_diff>

<commit_message>
Updated data and counts and KML file with Butler Bay samples from 27Jun2022
</commit_message>
<xml_diff>
--- a/Data/Genotype_Samples_2022.xlsx
+++ b/Data/Genotype_Samples_2022.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8606" uniqueCount="2584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8924" uniqueCount="2694">
   <si>
     <t>Date</t>
   </si>
@@ -7611,6 +7611,336 @@
   </si>
   <si>
     <t>G1425</t>
+  </si>
+  <si>
+    <t>BUT_051</t>
+  </si>
+  <si>
+    <t>G1638</t>
+  </si>
+  <si>
+    <t>BUT_052</t>
+  </si>
+  <si>
+    <t>BUT_053</t>
+  </si>
+  <si>
+    <t>G1650</t>
+  </si>
+  <si>
+    <t>BUT_054</t>
+  </si>
+  <si>
+    <t>G1649</t>
+  </si>
+  <si>
+    <t>BUT_055</t>
+  </si>
+  <si>
+    <t>BUT_056</t>
+  </si>
+  <si>
+    <t>BUT_057</t>
+  </si>
+  <si>
+    <t>G1640</t>
+  </si>
+  <si>
+    <t>BUT_058</t>
+  </si>
+  <si>
+    <t>BUT_059</t>
+  </si>
+  <si>
+    <t>BUT_060</t>
+  </si>
+  <si>
+    <t>G1639</t>
+  </si>
+  <si>
+    <t>BUT_061</t>
+  </si>
+  <si>
+    <t>G1630</t>
+  </si>
+  <si>
+    <t>BUT_062</t>
+  </si>
+  <si>
+    <t>G1629</t>
+  </si>
+  <si>
+    <t>BUT_063</t>
+  </si>
+  <si>
+    <t>G1693</t>
+  </si>
+  <si>
+    <t>BUT_064</t>
+  </si>
+  <si>
+    <t>BUT_065</t>
+  </si>
+  <si>
+    <t>G1400</t>
+  </si>
+  <si>
+    <t>BUT_066</t>
+  </si>
+  <si>
+    <t>G1399</t>
+  </si>
+  <si>
+    <t>BUT_067</t>
+  </si>
+  <si>
+    <t>G1870</t>
+  </si>
+  <si>
+    <t>BUT_068</t>
+  </si>
+  <si>
+    <t>G1822</t>
+  </si>
+  <si>
+    <t>Maybe OFRA</t>
+  </si>
+  <si>
+    <t>BUT_069</t>
+  </si>
+  <si>
+    <t>G1823</t>
+  </si>
+  <si>
+    <t>BUT_070</t>
+  </si>
+  <si>
+    <t>G1824</t>
+  </si>
+  <si>
+    <t>BUT_071</t>
+  </si>
+  <si>
+    <t>G1825</t>
+  </si>
+  <si>
+    <t>BUT_072</t>
+  </si>
+  <si>
+    <t>G1831</t>
+  </si>
+  <si>
+    <t>BUT_073</t>
+  </si>
+  <si>
+    <t>G1901</t>
+  </si>
+  <si>
+    <t>BUT_074</t>
+  </si>
+  <si>
+    <t>BUT_075</t>
+  </si>
+  <si>
+    <t>G1681</t>
+  </si>
+  <si>
+    <t>BUT_076</t>
+  </si>
+  <si>
+    <t>G1691</t>
+  </si>
+  <si>
+    <t>BUT_077</t>
+  </si>
+  <si>
+    <t>BUT_078</t>
+  </si>
+  <si>
+    <t>G1683</t>
+  </si>
+  <si>
+    <t>BUT_079</t>
+  </si>
+  <si>
+    <t>BUT_080</t>
+  </si>
+  <si>
+    <t>G1684</t>
+  </si>
+  <si>
+    <t>BUT_081</t>
+  </si>
+  <si>
+    <t>G1685</t>
+  </si>
+  <si>
+    <t>BUT_082</t>
+  </si>
+  <si>
+    <t>G1682</t>
+  </si>
+  <si>
+    <t>BUT_083</t>
+  </si>
+  <si>
+    <t>G1933</t>
+  </si>
+  <si>
+    <t>BUT_084</t>
+  </si>
+  <si>
+    <t>BUT_085</t>
+  </si>
+  <si>
+    <t>G1675</t>
+  </si>
+  <si>
+    <t>BUT_086</t>
+  </si>
+  <si>
+    <t>G1922</t>
+  </si>
+  <si>
+    <t>BUT_087</t>
+  </si>
+  <si>
+    <t>G1932</t>
+  </si>
+  <si>
+    <t>BUT_088</t>
+  </si>
+  <si>
+    <t>G1923</t>
+  </si>
+  <si>
+    <t>BUT_089</t>
+  </si>
+  <si>
+    <t>G1911</t>
+  </si>
+  <si>
+    <t>BUT_090</t>
+  </si>
+  <si>
+    <t>G1902</t>
+  </si>
+  <si>
+    <t>BUT_091</t>
+  </si>
+  <si>
+    <t>G1904</t>
+  </si>
+  <si>
+    <t>BUT_092</t>
+  </si>
+  <si>
+    <t>G1913</t>
+  </si>
+  <si>
+    <t>BUT_093</t>
+  </si>
+  <si>
+    <t>G1903</t>
+  </si>
+  <si>
+    <t>BUT_094</t>
+  </si>
+  <si>
+    <t>G1692</t>
+  </si>
+  <si>
+    <t>BUT_095</t>
+  </si>
+  <si>
+    <t>G1446</t>
+  </si>
+  <si>
+    <t>BUT_096</t>
+  </si>
+  <si>
+    <t>G1447</t>
+  </si>
+  <si>
+    <t>BUT_097</t>
+  </si>
+  <si>
+    <t>G1448</t>
+  </si>
+  <si>
+    <t>BUT_098</t>
+  </si>
+  <si>
+    <t>G1449</t>
+  </si>
+  <si>
+    <t>BUT_099</t>
+  </si>
+  <si>
+    <t>BUT_100</t>
+  </si>
+  <si>
+    <t>G1440</t>
+  </si>
+  <si>
+    <t>BUT_101</t>
+  </si>
+  <si>
+    <t>G1642</t>
+  </si>
+  <si>
+    <t>BUT_102</t>
+  </si>
+  <si>
+    <t>G1643</t>
+  </si>
+  <si>
+    <t>BUT_103</t>
+  </si>
+  <si>
+    <t>G1645</t>
+  </si>
+  <si>
+    <t>BUT_104</t>
+  </si>
+  <si>
+    <t>G1644</t>
+  </si>
+  <si>
+    <t>BUT_105</t>
+  </si>
+  <si>
+    <t>G1632</t>
+  </si>
+  <si>
+    <t>BUT_106</t>
+  </si>
+  <si>
+    <t>G1624</t>
+  </si>
+  <si>
+    <t>BUT_107</t>
+  </si>
+  <si>
+    <t>G1992</t>
+  </si>
+  <si>
+    <t>BUT_108</t>
+  </si>
+  <si>
+    <t>G1994</t>
+  </si>
+  <si>
+    <t>BUT_109</t>
+  </si>
+  <si>
+    <t>G1993</t>
+  </si>
+  <si>
+    <t>BUT_110</t>
+  </si>
+  <si>
+    <t>G1225</t>
   </si>
   <si>
     <t>Site_ID</t>
@@ -59287,244 +59617,1978 @@
       </c>
     </row>
     <row r="1554">
-      <c r="A1554" s="24"/>
-      <c r="B1554" s="7"/>
+      <c r="A1554" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1554" s="7" t="s">
+        <v>2532</v>
+      </c>
+      <c r="C1554" s="7" t="s">
+        <v>2533</v>
+      </c>
+      <c r="D1554" s="7">
+        <v>68.0</v>
+      </c>
+      <c r="E1554" s="8">
+        <v>0.6027777777777777</v>
+      </c>
+      <c r="F1554" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1554" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1554" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1554" s="11">
+        <v>17.7482140157372</v>
+      </c>
+      <c r="K1554" s="11">
+        <v>-64.8954167962074</v>
+      </c>
+      <c r="M1554" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1555">
-      <c r="A1555" s="24"/>
-      <c r="B1555" s="7"/>
+      <c r="A1555" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1555" s="7" t="s">
+        <v>2534</v>
+      </c>
+      <c r="C1555" s="7" t="s">
+        <v>2533</v>
+      </c>
+      <c r="D1555" s="7">
+        <v>78.0</v>
+      </c>
+      <c r="E1555" s="8">
+        <v>0.6027777777777777</v>
+      </c>
+      <c r="F1555" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1555" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1555" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1555" s="11">
+        <v>17.7482140157372</v>
+      </c>
+      <c r="K1555" s="11">
+        <v>-64.8954167962074</v>
+      </c>
+      <c r="M1555" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1556">
-      <c r="A1556" s="24"/>
-      <c r="B1556" s="7"/>
+      <c r="A1556" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1556" s="7" t="s">
+        <v>2535</v>
+      </c>
+      <c r="C1556" s="7" t="s">
+        <v>2536</v>
+      </c>
+      <c r="D1556" s="7">
+        <v>55.0</v>
+      </c>
+      <c r="E1556" s="8">
+        <v>0.6055555555555555</v>
+      </c>
+      <c r="F1556" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1556" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1556" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1556" s="11">
+        <v>17.7482475433499</v>
+      </c>
+      <c r="K1556" s="11">
+        <v>-64.8953851964325</v>
+      </c>
     </row>
     <row r="1557">
-      <c r="A1557" s="24"/>
-      <c r="B1557" s="7"/>
+      <c r="A1557" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1557" s="7" t="s">
+        <v>2537</v>
+      </c>
+      <c r="C1557" s="7" t="s">
+        <v>2538</v>
+      </c>
+      <c r="D1557" s="7">
+        <v>59.0</v>
+      </c>
+      <c r="E1557" s="8">
+        <v>0.6083333333333333</v>
+      </c>
+      <c r="F1557" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1557" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1557" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1557" s="11">
+        <v>17.7483414206654</v>
+      </c>
+      <c r="K1557" s="11">
+        <v>-64.8953454662114</v>
+      </c>
+      <c r="M1557" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1558">
-      <c r="A1558" s="24"/>
-      <c r="B1558" s="7"/>
+      <c r="A1558" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1558" s="7" t="s">
+        <v>2539</v>
+      </c>
+      <c r="C1558" s="7" t="s">
+        <v>2538</v>
+      </c>
+      <c r="D1558" s="7">
+        <v>64.0</v>
+      </c>
+      <c r="E1558" s="8">
+        <v>0.6083333333333333</v>
+      </c>
+      <c r="F1558" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1558" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1558" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1558" s="11">
+        <v>17.7483414206654</v>
+      </c>
+      <c r="K1558" s="11">
+        <v>-64.8953454662114</v>
+      </c>
+      <c r="M1558" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1559">
-      <c r="A1559" s="24"/>
-      <c r="B1559" s="7"/>
+      <c r="A1559" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1559" s="7" t="s">
+        <v>2540</v>
+      </c>
+      <c r="C1559" s="7" t="s">
+        <v>2538</v>
+      </c>
+      <c r="D1559" s="7">
+        <v>65.0</v>
+      </c>
+      <c r="E1559" s="8">
+        <v>0.6083333333333333</v>
+      </c>
+      <c r="F1559" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1559" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1559" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1559" s="11">
+        <v>17.7483414206654</v>
+      </c>
+      <c r="K1559" s="11">
+        <v>-64.8953454662114</v>
+      </c>
+      <c r="M1559" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1560">
-      <c r="A1560" s="24"/>
-      <c r="B1560" s="7"/>
+      <c r="A1560" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1560" s="7" t="s">
+        <v>2541</v>
+      </c>
+      <c r="C1560" s="7" t="s">
+        <v>2542</v>
+      </c>
+      <c r="D1560" s="7">
+        <v>83.0</v>
+      </c>
+      <c r="E1560" s="8">
+        <v>0.6138888888888889</v>
+      </c>
+      <c r="F1560" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1560" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1560" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1560" s="11">
+        <v>17.7484437637031</v>
+      </c>
+      <c r="K1560" s="11">
+        <v>-64.8953509982675</v>
+      </c>
+      <c r="M1560" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1561">
-      <c r="A1561" s="24"/>
-      <c r="B1561" s="7"/>
+      <c r="A1561" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1561" s="7" t="s">
+        <v>2543</v>
+      </c>
+      <c r="C1561" s="7" t="s">
+        <v>2542</v>
+      </c>
+      <c r="D1561" s="7">
+        <v>62.0</v>
+      </c>
+      <c r="E1561" s="8">
+        <v>0.6138888888888889</v>
+      </c>
+      <c r="F1561" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1561" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1561" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1561" s="11">
+        <v>17.7484437637031</v>
+      </c>
+      <c r="K1561" s="11">
+        <v>-64.8953509982675</v>
+      </c>
+      <c r="M1561" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1562">
-      <c r="A1562" s="24"/>
-      <c r="B1562" s="7"/>
+      <c r="A1562" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1562" s="7" t="s">
+        <v>2544</v>
+      </c>
+      <c r="C1562" s="7" t="s">
+        <v>2542</v>
+      </c>
+      <c r="D1562" s="7">
+        <v>63.0</v>
+      </c>
+      <c r="E1562" s="8">
+        <v>0.6138888888888889</v>
+      </c>
+      <c r="F1562" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1562" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1562" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1562" s="11">
+        <v>17.7484437637031</v>
+      </c>
+      <c r="K1562" s="11">
+        <v>-64.8953509982675</v>
+      </c>
+      <c r="M1562" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1563">
-      <c r="A1563" s="24"/>
-      <c r="B1563" s="7"/>
+      <c r="A1563" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1563" s="7" t="s">
+        <v>2545</v>
+      </c>
+      <c r="C1563" s="7" t="s">
+        <v>2546</v>
+      </c>
+      <c r="D1563" s="7">
+        <v>56.0</v>
+      </c>
+      <c r="E1563" s="8">
+        <v>0.6173611111111111</v>
+      </c>
+      <c r="F1563" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1563" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1563" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1563" s="11">
+        <v>17.7484285924584</v>
+      </c>
+      <c r="K1563" s="11">
+        <v>-64.8953059874475</v>
+      </c>
     </row>
     <row r="1564">
-      <c r="A1564" s="24"/>
-      <c r="B1564" s="7"/>
+      <c r="A1564" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1564" s="7" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C1564" s="7" t="s">
+        <v>2548</v>
+      </c>
+      <c r="D1564" s="7">
+        <v>61.0</v>
+      </c>
+      <c r="E1564" s="8">
+        <v>0.6201388888888889</v>
+      </c>
+      <c r="F1564" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1564" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1564" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1564" s="11">
+        <v>17.7484655566514</v>
+      </c>
+      <c r="K1564" s="11">
+        <v>-64.8952542711049</v>
+      </c>
     </row>
     <row r="1565">
-      <c r="A1565" s="24"/>
-      <c r="B1565" s="7"/>
+      <c r="A1565" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1565" s="7" t="s">
+        <v>2549</v>
+      </c>
+      <c r="C1565" s="7" t="s">
+        <v>2550</v>
+      </c>
+      <c r="D1565" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="E1565" s="8">
+        <v>0.6229166666666667</v>
+      </c>
+      <c r="F1565" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1565" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1565" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1565" s="11">
+        <v>17.7484828233719</v>
+      </c>
+      <c r="K1565" s="11">
+        <v>-64.8951424565166</v>
+      </c>
     </row>
     <row r="1566">
-      <c r="A1566" s="24"/>
-      <c r="B1566" s="7"/>
+      <c r="A1566" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1566" s="7" t="s">
+        <v>2551</v>
+      </c>
+      <c r="C1566" s="7" t="s">
+        <v>2552</v>
+      </c>
+      <c r="D1566" s="7">
+        <v>67.0</v>
+      </c>
+      <c r="E1566" s="8">
+        <v>0.6256944444444444</v>
+      </c>
+      <c r="F1566" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1566" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1566" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1566" s="11">
+        <v>17.7485399879515</v>
+      </c>
+      <c r="K1566" s="11">
+        <v>-64.8950883094221</v>
+      </c>
     </row>
     <row r="1567">
-      <c r="A1567" s="24"/>
-      <c r="B1567" s="7"/>
+      <c r="A1567" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1567" s="7" t="s">
+        <v>2553</v>
+      </c>
+      <c r="C1567" s="7" t="s">
+        <v>2552</v>
+      </c>
+      <c r="D1567" s="7">
+        <v>74.0</v>
+      </c>
+      <c r="E1567" s="8">
+        <v>0.6256944444444444</v>
+      </c>
+      <c r="F1567" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1567" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1567" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1567" s="11">
+        <v>17.7485399879515</v>
+      </c>
+      <c r="K1567" s="11">
+        <v>-64.8950883094221</v>
+      </c>
     </row>
     <row r="1568">
-      <c r="A1568" s="24"/>
-      <c r="B1568" s="7"/>
+      <c r="A1568" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1568" s="7" t="s">
+        <v>2554</v>
+      </c>
+      <c r="C1568" s="7" t="s">
+        <v>2555</v>
+      </c>
+      <c r="D1568" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="E1568" s="8">
+        <v>0.6291666666666667</v>
+      </c>
+      <c r="F1568" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1568" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1568" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1568" s="11">
+        <v>17.7486114855856</v>
+      </c>
+      <c r="K1568" s="11">
+        <v>-64.8950015567243</v>
+      </c>
     </row>
     <row r="1569">
-      <c r="A1569" s="24"/>
-      <c r="B1569" s="7"/>
+      <c r="A1569" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1569" s="7" t="s">
+        <v>2556</v>
+      </c>
+      <c r="C1569" s="7" t="s">
+        <v>2557</v>
+      </c>
+      <c r="D1569" s="7">
+        <v>51.0</v>
+      </c>
+      <c r="E1569" s="8">
+        <v>0.63125</v>
+      </c>
+      <c r="F1569" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1569" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1569" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1569" s="11">
+        <v>17.7486492879689</v>
+      </c>
+      <c r="K1569" s="11">
+        <v>-64.8950449749827</v>
+      </c>
     </row>
     <row r="1570">
-      <c r="A1570" s="24"/>
-      <c r="B1570" s="7"/>
+      <c r="A1570" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1570" s="7" t="s">
+        <v>2558</v>
+      </c>
+      <c r="C1570" s="7" t="s">
+        <v>2559</v>
+      </c>
+      <c r="D1570" s="7">
+        <v>70.0</v>
+      </c>
+      <c r="E1570" s="8">
+        <v>0.6326388888888889</v>
+      </c>
+      <c r="F1570" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1570" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1570" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1570" s="11">
+        <v>17.7487155050039</v>
+      </c>
+      <c r="K1570" s="11">
+        <v>-64.8949163965881</v>
+      </c>
     </row>
     <row r="1571">
-      <c r="A1571" s="24"/>
-      <c r="B1571" s="7"/>
+      <c r="A1571" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1571" s="7" t="s">
+        <v>2560</v>
+      </c>
+      <c r="C1571" s="7" t="s">
+        <v>2561</v>
+      </c>
+      <c r="D1571" s="7">
+        <v>89.0</v>
+      </c>
+      <c r="E1571" s="8">
+        <v>0.6354166666666666</v>
+      </c>
+      <c r="F1571" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1571" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1571" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1571" s="11">
+        <v>17.7487280778587</v>
+      </c>
+      <c r="K1571" s="11">
+        <v>-64.8948508501053</v>
+      </c>
+      <c r="M1571" s="7" t="s">
+        <v>2562</v>
+      </c>
     </row>
     <row r="1572">
-      <c r="A1572" s="24"/>
-      <c r="B1572" s="7"/>
+      <c r="A1572" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1572" s="7" t="s">
+        <v>2563</v>
+      </c>
+      <c r="C1572" s="7" t="s">
+        <v>2564</v>
+      </c>
+      <c r="D1572" s="7">
+        <v>49.0</v>
+      </c>
+      <c r="E1572" s="8">
+        <v>0.6368055555555555</v>
+      </c>
+      <c r="F1572" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1572" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1572" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1572" s="11">
+        <v>17.7487666346133</v>
+      </c>
+      <c r="K1572" s="11">
+        <v>-64.8948106169701</v>
+      </c>
     </row>
     <row r="1573">
-      <c r="A1573" s="24"/>
-      <c r="B1573" s="7"/>
+      <c r="A1573" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1573" s="7" t="s">
+        <v>2565</v>
+      </c>
+      <c r="C1573" s="7" t="s">
+        <v>2566</v>
+      </c>
+      <c r="D1573" s="7">
+        <v>82.0</v>
+      </c>
+      <c r="E1573" s="8">
+        <v>0.6388888888888888</v>
+      </c>
+      <c r="F1573" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1573" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1573" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1573" s="11">
+        <v>17.7488360367715</v>
+      </c>
+      <c r="K1573" s="11">
+        <v>-64.8947388678789</v>
+      </c>
     </row>
     <row r="1574">
-      <c r="A1574" s="24"/>
-      <c r="B1574" s="7"/>
+      <c r="A1574" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1574" s="7" t="s">
+        <v>2567</v>
+      </c>
+      <c r="C1574" s="7" t="s">
+        <v>2568</v>
+      </c>
+      <c r="D1574" s="7">
+        <v>87.0</v>
+      </c>
+      <c r="E1574" s="8">
+        <v>0.6416666666666667</v>
+      </c>
+      <c r="F1574" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1574" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1574" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1574" s="11">
+        <v>17.7488667145371</v>
+      </c>
+      <c r="K1574" s="11">
+        <v>-64.8947242833674</v>
+      </c>
+      <c r="M1574" s="7" t="s">
+        <v>2562</v>
+      </c>
     </row>
     <row r="1575">
-      <c r="A1575" s="24"/>
-      <c r="B1575" s="7"/>
+      <c r="A1575" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1575" s="7" t="s">
+        <v>2569</v>
+      </c>
+      <c r="C1575" s="7" t="s">
+        <v>2570</v>
+      </c>
+      <c r="D1575" s="7">
+        <v>53.0</v>
+      </c>
+      <c r="E1575" s="8">
+        <v>0.6444444444444445</v>
+      </c>
+      <c r="F1575" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1575" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1575" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1575" s="11">
+        <v>17.7490955404937</v>
+      </c>
+      <c r="K1575" s="11">
+        <v>-64.8946817032993</v>
+      </c>
     </row>
     <row r="1576">
-      <c r="A1576" s="24"/>
-      <c r="B1576" s="7"/>
+      <c r="A1576" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1576" s="7" t="s">
+        <v>2571</v>
+      </c>
+      <c r="C1576" s="7" t="s">
+        <v>2572</v>
+      </c>
+      <c r="D1576" s="7">
+        <v>73.0</v>
+      </c>
+      <c r="E1576" s="8">
+        <v>0.6013888888888889</v>
+      </c>
+      <c r="F1576" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1576" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1576" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1576" s="11">
+        <v>17.7482290193439</v>
+      </c>
+      <c r="K1576" s="11">
+        <v>-64.8954230826348</v>
+      </c>
+      <c r="M1576" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1577">
-      <c r="A1577" s="24"/>
-      <c r="B1577" s="7"/>
+      <c r="A1577" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1577" s="7" t="s">
+        <v>2573</v>
+      </c>
+      <c r="C1577" s="7" t="s">
+        <v>2572</v>
+      </c>
+      <c r="D1577" s="7">
+        <v>109.0</v>
+      </c>
+      <c r="E1577" s="8">
+        <v>0.6013888888888889</v>
+      </c>
+      <c r="F1577" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1577" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1577" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1577" s="11">
+        <v>17.7482290193439</v>
+      </c>
+      <c r="K1577" s="11">
+        <v>-64.8954230826348</v>
+      </c>
+      <c r="M1577" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1578">
-      <c r="A1578" s="24"/>
-      <c r="B1578" s="7"/>
+      <c r="A1578" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1578" s="7" t="s">
+        <v>2574</v>
+      </c>
+      <c r="C1578" s="7" t="s">
+        <v>2575</v>
+      </c>
+      <c r="D1578" s="7">
+        <v>215.0</v>
+      </c>
+      <c r="E1578" s="8">
+        <v>0.6034722222222222</v>
+      </c>
+      <c r="F1578" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1578" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1578" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1578" s="11">
+        <v>17.7482377365232</v>
+      </c>
+      <c r="K1578" s="11">
+        <v>-64.8953943327069</v>
+      </c>
     </row>
     <row r="1579">
-      <c r="A1579" s="24"/>
-      <c r="B1579" s="7"/>
+      <c r="A1579" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1579" s="7" t="s">
+        <v>2576</v>
+      </c>
+      <c r="C1579" s="7" t="s">
+        <v>2577</v>
+      </c>
+      <c r="D1579" s="7">
+        <v>205.0</v>
+      </c>
+      <c r="E1579" s="8">
+        <v>0.6076388888888888</v>
+      </c>
+      <c r="F1579" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1579" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1579" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1579" s="11">
+        <v>17.7483394090086</v>
+      </c>
+      <c r="K1579" s="11">
+        <v>-64.8953413590789</v>
+      </c>
+      <c r="M1579" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1580">
-      <c r="A1580" s="24"/>
-      <c r="B1580" s="7"/>
+      <c r="A1580" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1580" s="7" t="s">
+        <v>2578</v>
+      </c>
+      <c r="C1580" s="7" t="s">
+        <v>2577</v>
+      </c>
+      <c r="D1580" s="7">
+        <v>208.0</v>
+      </c>
+      <c r="E1580" s="8">
+        <v>0.6076388888888888</v>
+      </c>
+      <c r="F1580" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1580" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1580" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1580" s="11">
+        <v>17.7483394090086</v>
+      </c>
+      <c r="K1580" s="11">
+        <v>-64.8953413590789</v>
+      </c>
+      <c r="M1580" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1581">
-      <c r="A1581" s="24"/>
-      <c r="B1581" s="7"/>
+      <c r="A1581" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1581" s="7" t="s">
+        <v>2579</v>
+      </c>
+      <c r="C1581" s="7" t="s">
+        <v>2580</v>
+      </c>
+      <c r="D1581" s="7">
+        <v>34.0</v>
+      </c>
+      <c r="E1581" s="8">
+        <v>0.6111111111111112</v>
+      </c>
+      <c r="F1581" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1581" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1581" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1581" s="11">
+        <v>17.7484451886266</v>
+      </c>
+      <c r="K1581" s="11">
+        <v>-64.8953516688198</v>
+      </c>
+      <c r="M1581" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1582">
-      <c r="A1582" s="24"/>
-      <c r="B1582" s="7"/>
+      <c r="A1582" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1582" s="7" t="s">
+        <v>2581</v>
+      </c>
+      <c r="C1582" s="7" t="s">
+        <v>2580</v>
+      </c>
+      <c r="D1582" s="7">
+        <v>84.0</v>
+      </c>
+      <c r="E1582" s="8">
+        <v>0.6111111111111112</v>
+      </c>
+      <c r="F1582" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1582" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1582" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1582" s="11">
+        <v>17.7484451886266</v>
+      </c>
+      <c r="K1582" s="11">
+        <v>-64.8953516688198</v>
+      </c>
+      <c r="M1582" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1583">
-      <c r="A1583" s="24"/>
-      <c r="B1583" s="7"/>
+      <c r="A1583" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1583" s="7" t="s">
+        <v>2582</v>
+      </c>
+      <c r="C1583" s="7" t="s">
+        <v>2583</v>
+      </c>
+      <c r="D1583" s="7">
+        <v>12.0</v>
+      </c>
+      <c r="E1583" s="8">
+        <v>0.6145833333333334</v>
+      </c>
+      <c r="F1583" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1583" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1583" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1583" s="11">
+        <v>17.7484462782741</v>
+      </c>
+      <c r="K1583" s="11">
+        <v>-64.8953433707356</v>
+      </c>
     </row>
     <row r="1584">
-      <c r="A1584" s="24"/>
-      <c r="B1584" s="7"/>
+      <c r="A1584" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1584" s="7" t="s">
+        <v>2584</v>
+      </c>
+      <c r="C1584" s="7" t="s">
+        <v>2585</v>
+      </c>
+      <c r="D1584" s="7">
+        <v>201.0</v>
+      </c>
+      <c r="E1584" s="8">
+        <v>0.6159722222222223</v>
+      </c>
+      <c r="F1584" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1584" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1584" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1584" s="11">
+        <v>17.7484419196844</v>
+      </c>
+      <c r="K1584" s="11">
+        <v>-64.8953146208078</v>
+      </c>
     </row>
     <row r="1585">
-      <c r="A1585" s="24"/>
-      <c r="B1585" s="7"/>
+      <c r="A1585" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1585" s="7" t="s">
+        <v>2586</v>
+      </c>
+      <c r="C1585" s="7" t="s">
+        <v>2587</v>
+      </c>
+      <c r="D1585" s="7">
+        <v>28.0</v>
+      </c>
+      <c r="E1585" s="8">
+        <v>0.61875</v>
+      </c>
+      <c r="F1585" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1585" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1585" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1585" s="11">
+        <v>17.7484643831849</v>
+      </c>
+      <c r="K1585" s="11">
+        <v>-64.8952508345246</v>
+      </c>
     </row>
     <row r="1586">
-      <c r="A1586" s="24"/>
-      <c r="B1586" s="7"/>
+      <c r="A1586" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1586" s="7" t="s">
+        <v>2588</v>
+      </c>
+      <c r="C1586" s="7" t="s">
+        <v>2589</v>
+      </c>
+      <c r="D1586" s="7">
+        <v>69.0</v>
+      </c>
+      <c r="E1586" s="8">
+        <v>0.6201388888888889</v>
+      </c>
+      <c r="F1586" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1586" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1586" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1586" s="11">
+        <v>17.7484655566514</v>
+      </c>
+      <c r="K1586" s="11">
+        <v>-64.8952542711049</v>
+      </c>
+      <c r="M1586" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1587">
-      <c r="A1587" s="24"/>
-      <c r="B1587" s="7"/>
+      <c r="A1587" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1587" s="7" t="s">
+        <v>2590</v>
+      </c>
+      <c r="C1587" s="7" t="s">
+        <v>2589</v>
+      </c>
+      <c r="D1587" s="7">
+        <v>19.0</v>
+      </c>
+      <c r="E1587" s="8">
+        <v>0.6201388888888889</v>
+      </c>
+      <c r="F1587" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1587" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1587" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1587" s="11">
+        <v>17.7484655566514</v>
+      </c>
+      <c r="K1587" s="11">
+        <v>-64.8952542711049</v>
+      </c>
+      <c r="M1587" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="1588">
-      <c r="A1588" s="24"/>
-      <c r="B1588" s="7"/>
+      <c r="A1588" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1588" s="7" t="s">
+        <v>2591</v>
+      </c>
+      <c r="C1588" s="7" t="s">
+        <v>2592</v>
+      </c>
+      <c r="D1588" s="7">
+        <v>8.0</v>
+      </c>
+      <c r="E1588" s="8">
+        <v>0.6236111111111111</v>
+      </c>
+      <c r="F1588" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1588" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1588" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1588" s="11">
+        <v>17.7484876010567</v>
+      </c>
+      <c r="K1588" s="11">
+        <v>-64.8951628245413</v>
+      </c>
     </row>
     <row r="1589">
-      <c r="A1589" s="24"/>
-      <c r="B1589" s="7"/>
+      <c r="A1589" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1589" s="7" t="s">
+        <v>2593</v>
+      </c>
+      <c r="C1589" s="7" t="s">
+        <v>2594</v>
+      </c>
+      <c r="D1589" s="7">
+        <v>31.0</v>
+      </c>
+      <c r="E1589" s="8">
+        <v>0.625</v>
+      </c>
+      <c r="F1589" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1589" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1589" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1589" s="11">
+        <v>17.7484846673906</v>
+      </c>
+      <c r="K1589" s="11">
+        <v>-64.8951682727784</v>
+      </c>
     </row>
     <row r="1590">
-      <c r="A1590" s="24"/>
-      <c r="B1590" s="7"/>
+      <c r="A1590" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1590" s="7" t="s">
+        <v>2595</v>
+      </c>
+      <c r="C1590" s="7" t="s">
+        <v>2596</v>
+      </c>
+      <c r="D1590" s="7">
+        <v>86.0</v>
+      </c>
+      <c r="E1590" s="8">
+        <v>0.6277777777777778</v>
+      </c>
+      <c r="F1590" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1590" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1590" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1590" s="11">
+        <v>17.7485959790647</v>
+      </c>
+      <c r="K1590" s="11">
+        <v>-64.895066684112</v>
+      </c>
     </row>
     <row r="1591">
-      <c r="A1591" s="24"/>
-      <c r="B1591" s="7"/>
+      <c r="A1591" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1591" s="7" t="s">
+        <v>2597</v>
+      </c>
+      <c r="C1591" s="7" t="s">
+        <v>2598</v>
+      </c>
+      <c r="D1591" s="7">
+        <v>57.0</v>
+      </c>
+      <c r="E1591" s="8">
+        <v>0.6305555555555555</v>
+      </c>
+      <c r="F1591" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1591" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1591" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1591" s="11">
+        <v>17.7486501261592</v>
+      </c>
+      <c r="K1591" s="11">
+        <v>-64.8950396943837</v>
+      </c>
     </row>
     <row r="1592">
-      <c r="A1592" s="24"/>
-      <c r="B1592" s="7"/>
+      <c r="A1592" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1592" s="7" t="s">
+        <v>2599</v>
+      </c>
+      <c r="C1592" s="7" t="s">
+        <v>2600</v>
+      </c>
+      <c r="D1592" s="7">
+        <v>58.0</v>
+      </c>
+      <c r="E1592" s="8">
+        <v>0.6326388888888889</v>
+      </c>
+      <c r="F1592" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1592" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1592" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1592" s="11">
+        <v>17.7487155050039</v>
+      </c>
+      <c r="K1592" s="11">
+        <v>-64.8949163965881</v>
+      </c>
     </row>
     <row r="1593">
-      <c r="A1593" s="24"/>
-      <c r="B1593" s="7"/>
+      <c r="A1593" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1593" s="7" t="s">
+        <v>2601</v>
+      </c>
+      <c r="C1593" s="7" t="s">
+        <v>2602</v>
+      </c>
+      <c r="D1593" s="7">
+        <v>46.0</v>
+      </c>
+      <c r="E1593" s="8">
+        <v>0.6347222222222222</v>
+      </c>
+      <c r="F1593" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1593" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1593" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1593" s="11">
+        <v>17.748728999868</v>
+      </c>
+      <c r="K1593" s="11">
+        <v>-64.8948388639838</v>
+      </c>
     </row>
     <row r="1594">
-      <c r="A1594" s="24"/>
-      <c r="B1594" s="7"/>
+      <c r="A1594" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1594" s="7" t="s">
+        <v>2603</v>
+      </c>
+      <c r="C1594" s="7" t="s">
+        <v>2604</v>
+      </c>
+      <c r="D1594" s="7">
+        <v>204.0</v>
+      </c>
+      <c r="E1594" s="8">
+        <v>0.6368055555555555</v>
+      </c>
+      <c r="F1594" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1594" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1594" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1594" s="11">
+        <v>17.7487666346133</v>
+      </c>
+      <c r="K1594" s="11">
+        <v>-64.8948106169701</v>
+      </c>
     </row>
     <row r="1595">
-      <c r="A1595" s="24"/>
-      <c r="B1595" s="7"/>
+      <c r="A1595" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1595" s="7" t="s">
+        <v>2605</v>
+      </c>
+      <c r="C1595" s="7" t="s">
+        <v>2606</v>
+      </c>
+      <c r="D1595" s="7">
+        <v>207.0</v>
+      </c>
+      <c r="E1595" s="8">
+        <v>0.6395833333333333</v>
+      </c>
+      <c r="F1595" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1595" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1595" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1595" s="11">
+        <v>17.7488629426807</v>
+      </c>
+      <c r="K1595" s="11">
+        <v>-64.8947229422629</v>
+      </c>
     </row>
     <row r="1596">
-      <c r="A1596" s="24"/>
-      <c r="B1596" s="7"/>
+      <c r="A1596" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1596" s="7" t="s">
+        <v>2607</v>
+      </c>
+      <c r="C1596" s="7" t="s">
+        <v>2608</v>
+      </c>
+      <c r="D1596" s="7">
+        <v>35.0</v>
+      </c>
+      <c r="E1596" s="8">
+        <v>0.6430555555555556</v>
+      </c>
+      <c r="F1596" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1596" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1596" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1596" s="11">
+        <v>17.7490700595081</v>
+      </c>
+      <c r="K1596" s="11">
+        <v>-64.8946494329721</v>
+      </c>
     </row>
     <row r="1597">
-      <c r="A1597" s="24"/>
-      <c r="B1597" s="7"/>
+      <c r="A1597" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1597" s="7" t="s">
+        <v>2609</v>
+      </c>
+      <c r="C1597" s="7" t="s">
+        <v>2610</v>
+      </c>
+      <c r="D1597" s="7">
+        <v>186.0</v>
+      </c>
+      <c r="E1597" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="F1597" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1597" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1597" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1597" s="11">
+        <v>17.7482741139829</v>
+      </c>
+      <c r="K1597" s="11">
+        <v>-64.8954167962074</v>
+      </c>
     </row>
     <row r="1598">
-      <c r="A1598" s="24"/>
-      <c r="B1598" s="7"/>
+      <c r="A1598" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1598" s="7" t="s">
+        <v>2611</v>
+      </c>
+      <c r="C1598" s="7" t="s">
+        <v>2612</v>
+      </c>
+      <c r="D1598" s="7">
+        <v>106.0</v>
+      </c>
+      <c r="E1598" s="8">
+        <v>0.6041666666666666</v>
+      </c>
+      <c r="F1598" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1598" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1598" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1598" s="11">
+        <v>17.7482265047729</v>
+      </c>
+      <c r="K1598" s="11">
+        <v>-64.8954010382295</v>
+      </c>
     </row>
     <row r="1599">
-      <c r="A1599" s="24"/>
-      <c r="B1599" s="7"/>
+      <c r="A1599" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1599" s="7" t="s">
+        <v>2613</v>
+      </c>
+      <c r="C1599" s="7" t="s">
+        <v>2614</v>
+      </c>
+      <c r="D1599" s="7">
+        <v>40.0</v>
+      </c>
+      <c r="E1599" s="8">
+        <v>0.6069444444444444</v>
+      </c>
+      <c r="F1599" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1599" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1599" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1599" s="11">
+        <v>17.7483435161412</v>
+      </c>
+      <c r="K1599" s="11">
+        <v>-64.895341778174</v>
+      </c>
     </row>
     <row r="1600">
-      <c r="A1600" s="24"/>
-      <c r="B1600" s="7"/>
+      <c r="A1600" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1600" s="7" t="s">
+        <v>2615</v>
+      </c>
+      <c r="C1600" s="7" t="s">
+        <v>2616</v>
+      </c>
+      <c r="D1600" s="7">
+        <v>17.0</v>
+      </c>
+      <c r="E1600" s="8">
+        <v>0.6104166666666667</v>
+      </c>
+      <c r="F1600" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1600" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1600" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1600" s="11">
+        <v>17.7484475355595</v>
+      </c>
+      <c r="K1600" s="11">
+        <v>-64.8953476455063</v>
+      </c>
     </row>
     <row r="1601">
-      <c r="A1601" s="24"/>
-      <c r="B1601" s="7"/>
+      <c r="A1601" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1601" s="7" t="s">
+        <v>2617</v>
+      </c>
+      <c r="C1601" s="7" t="s">
+        <v>2618</v>
+      </c>
+      <c r="D1601" s="7">
+        <v>6.0</v>
+      </c>
+      <c r="E1601" s="8">
+        <v>0.6125</v>
+      </c>
+      <c r="F1601" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1601" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1601" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1601" s="11">
+        <v>17.748451475054</v>
+      </c>
+      <c r="K1601" s="11">
+        <v>-64.8953460529447</v>
+      </c>
     </row>
     <row r="1602">
-      <c r="A1602" s="24"/>
-      <c r="B1602" s="7"/>
+      <c r="A1602" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1602" s="7" t="s">
+        <v>2619</v>
+      </c>
+      <c r="C1602" s="7" t="s">
+        <v>2618</v>
+      </c>
+      <c r="D1602" s="7">
+        <v>105.0</v>
+      </c>
+      <c r="E1602" s="8">
+        <v>0.6138888888888889</v>
+      </c>
+      <c r="F1602" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1602" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1602" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1602" s="11">
+        <v>17.7484437637031</v>
+      </c>
+      <c r="K1602" s="11">
+        <v>-64.8953509982675</v>
+      </c>
     </row>
     <row r="1603">
-      <c r="A1603" s="24"/>
-      <c r="B1603" s="7"/>
+      <c r="A1603" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1603" s="7" t="s">
+        <v>2620</v>
+      </c>
+      <c r="C1603" s="7" t="s">
+        <v>2621</v>
+      </c>
+      <c r="D1603" s="7">
+        <v>206.0</v>
+      </c>
+      <c r="E1603" s="8">
+        <v>0.6159722222222223</v>
+      </c>
+      <c r="F1603" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1603" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1603" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1603" s="11">
+        <v>17.7484419196844</v>
+      </c>
+      <c r="K1603" s="11">
+        <v>-64.8953146208078</v>
+      </c>
     </row>
     <row r="1604">
-      <c r="A1604" s="24"/>
-      <c r="B1604" s="7"/>
+      <c r="A1604" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1604" s="7" t="s">
+        <v>2622</v>
+      </c>
+      <c r="C1604" s="7" t="s">
+        <v>2623</v>
+      </c>
+      <c r="D1604" s="7">
+        <v>212.0</v>
+      </c>
+      <c r="E1604" s="8">
+        <v>0.6194444444444445</v>
+      </c>
+      <c r="F1604" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1604" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1604" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1604" s="11">
+        <v>17.7484916243702</v>
+      </c>
+      <c r="K1604" s="11">
+        <v>-64.8952579591423</v>
+      </c>
     </row>
     <row r="1605">
-      <c r="A1605" s="24"/>
-      <c r="B1605" s="7"/>
+      <c r="A1605" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1605" s="7" t="s">
+        <v>2624</v>
+      </c>
+      <c r="C1605" s="7" t="s">
+        <v>2625</v>
+      </c>
+      <c r="D1605" s="7">
+        <v>76.0</v>
+      </c>
+      <c r="E1605" s="8">
+        <v>0.6236111111111111</v>
+      </c>
+      <c r="F1605" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1605" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1605" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1605" s="11">
+        <v>17.7484876010567</v>
+      </c>
+      <c r="K1605" s="11">
+        <v>-64.8951628245413</v>
+      </c>
     </row>
     <row r="1606">
-      <c r="A1606" s="24"/>
-      <c r="B1606" s="7"/>
+      <c r="A1606" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1606" s="7" t="s">
+        <v>2626</v>
+      </c>
+      <c r="C1606" s="7" t="s">
+        <v>2627</v>
+      </c>
+      <c r="D1606" s="7">
+        <v>26.0</v>
+      </c>
+      <c r="E1606" s="8">
+        <v>0.6270833333333333</v>
+      </c>
+      <c r="F1606" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1606" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1606" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1606" s="11">
+        <v>17.7485849987715</v>
+      </c>
+      <c r="K1606" s="11">
+        <v>-64.8950594756752</v>
+      </c>
     </row>
     <row r="1607">
-      <c r="A1607" s="24"/>
-      <c r="B1607" s="7"/>
+      <c r="A1607" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1607" s="7" t="s">
+        <v>2628</v>
+      </c>
+      <c r="C1607" s="7" t="s">
+        <v>2629</v>
+      </c>
+      <c r="D1607" s="7">
+        <v>213.0</v>
+      </c>
+      <c r="E1607" s="8">
+        <v>0.6298611111111111</v>
+      </c>
+      <c r="F1607" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1607" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1607" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1607" s="11">
+        <v>17.748647108674</v>
+      </c>
+      <c r="K1607" s="11">
+        <v>-64.8950434662402</v>
+      </c>
     </row>
     <row r="1608">
-      <c r="A1608" s="24"/>
-      <c r="B1608" s="7"/>
+      <c r="A1608" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1608" s="7" t="s">
+        <v>2630</v>
+      </c>
+      <c r="C1608" s="7" t="s">
+        <v>2631</v>
+      </c>
+      <c r="D1608" s="7">
+        <v>214.0</v>
+      </c>
+      <c r="E1608" s="8">
+        <v>0.6340277777777777</v>
+      </c>
+      <c r="F1608" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1608" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1608" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1608" s="11">
+        <v>17.7487243060023</v>
+      </c>
+      <c r="K1608" s="11">
+        <v>-64.8948411270976</v>
+      </c>
     </row>
     <row r="1609">
-      <c r="A1609" s="24"/>
-      <c r="B1609" s="7"/>
+      <c r="A1609" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1609" s="7" t="s">
+        <v>2632</v>
+      </c>
+      <c r="C1609" s="7" t="s">
+        <v>2633</v>
+      </c>
+      <c r="D1609" s="7">
+        <v>10.0</v>
+      </c>
+      <c r="E1609" s="8">
+        <v>0.6368055555555555</v>
+      </c>
+      <c r="F1609" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1609" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1609" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1609" s="11">
+        <v>17.7487666346133</v>
+      </c>
+      <c r="K1609" s="11">
+        <v>-64.8948106169701</v>
+      </c>
     </row>
     <row r="1610">
-      <c r="A1610" s="24"/>
-      <c r="B1610" s="7"/>
+      <c r="A1610" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1610" s="7" t="s">
+        <v>2634</v>
+      </c>
+      <c r="C1610" s="7" t="s">
+        <v>2635</v>
+      </c>
+      <c r="D1610" s="7">
+        <v>119.0</v>
+      </c>
+      <c r="E1610" s="8">
+        <v>0.6402777777777777</v>
+      </c>
+      <c r="F1610" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1610" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1610" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1610" s="11">
+        <v>17.7488640323281</v>
+      </c>
+      <c r="K1610" s="11">
+        <v>-64.8947230260819</v>
+      </c>
     </row>
     <row r="1611">
-      <c r="A1611" s="24"/>
-      <c r="B1611" s="7"/>
+      <c r="A1611" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1611" s="7" t="s">
+        <v>2636</v>
+      </c>
+      <c r="C1611" s="7" t="s">
+        <v>2637</v>
+      </c>
+      <c r="D1611" s="7">
+        <v>90.0</v>
+      </c>
+      <c r="E1611" s="8">
+        <v>0.6444444444444445</v>
+      </c>
+      <c r="F1611" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1611" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1611" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1611" s="11">
+        <v>17.7490955404937</v>
+      </c>
+      <c r="K1611" s="11">
+        <v>-64.8946817032993</v>
+      </c>
     </row>
     <row r="1612">
-      <c r="A1612" s="24"/>
-      <c r="B1612" s="7"/>
+      <c r="A1612" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1612" s="7" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C1612" s="7" t="s">
+        <v>2639</v>
+      </c>
+      <c r="D1612" s="7">
+        <v>203.0</v>
+      </c>
+      <c r="E1612" s="8">
+        <v>0.6479166666666667</v>
+      </c>
+      <c r="F1612" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1612" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1612" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1612" s="11">
+        <v>17.7491916809231</v>
+      </c>
+      <c r="K1612" s="11">
+        <v>-64.8945810366422</v>
+      </c>
     </row>
     <row r="1613">
-      <c r="A1613" s="24"/>
-      <c r="B1613" s="7"/>
+      <c r="A1613" s="6">
+        <v>44739.0</v>
+      </c>
+      <c r="B1613" s="7" t="s">
+        <v>2640</v>
+      </c>
+      <c r="C1613" s="7" t="s">
+        <v>2641</v>
+      </c>
+      <c r="D1613" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="E1613" s="8">
+        <v>0.6506944444444445</v>
+      </c>
+      <c r="F1613" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1613" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1613" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1613" s="11">
+        <v>17.7492107078433</v>
+      </c>
+      <c r="K1613" s="11">
+        <v>-64.8945775162429</v>
+      </c>
     </row>
     <row r="1614">
       <c r="A1614" s="24"/>
@@ -61083,19 +63147,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>2532</v>
+        <v>2642</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2533</v>
+        <v>2643</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2534</v>
+        <v>2644</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2535</v>
+        <v>2645</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2536</v>
+        <v>2646</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>7</v>
@@ -61119,21 +63183,21 @@
         <v>51</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>2537</v>
+        <v>2647</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>145</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>2538</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>2539</v>
+        <v>2649</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2540</v>
+        <v>2650</v>
       </c>
       <c r="C2" s="7">
         <v>7.0</v>
@@ -61145,33 +63209,33 @@
         <v>44688.0</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>2541</v>
+        <v>2651</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>2541</v>
+        <v>2651</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>2541</v>
+        <v>2651</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>2541</v>
+        <v>2651</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>2541</v>
+        <v>2651</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>2542</v>
+        <v>2652</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>2543</v>
+        <v>2653</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>2544</v>
+        <v>2654</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2545</v>
+        <v>2655</v>
       </c>
       <c r="C3" s="7">
         <v>25.0</v>
@@ -61182,10 +63246,10 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>2546</v>
+        <v>2656</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="C4" s="7">
         <v>15.0</v>
@@ -61197,18 +63261,18 @@
         <v>44690.0</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>2548</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>2549</v>
+        <v>2659</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2550</v>
+        <v>2660</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2551</v>
+        <v>2661</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>20</v>
@@ -61216,10 +63280,10 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>2552</v>
+        <v>2662</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2553</v>
+        <v>2663</v>
       </c>
       <c r="C6" s="7">
         <v>20.0</v>
@@ -61251,10 +63315,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>2554</v>
+        <v>2664</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2555</v>
+        <v>2665</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>78</v>
@@ -61286,7 +63350,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2539</v>
+        <v>2649</v>
       </c>
       <c r="C2" s="7">
         <v>2.0</v>
@@ -61315,7 +63379,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2546</v>
+        <v>2656</v>
       </c>
       <c r="C3" s="7">
         <v>5.0</v>
@@ -61344,7 +63408,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2544</v>
+        <v>2654</v>
       </c>
       <c r="F4" s="7">
         <v>17.0</v>
@@ -61367,7 +63431,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2552</v>
+        <v>2662</v>
       </c>
       <c r="F5" s="7">
         <v>6.0</v>
@@ -61390,7 +63454,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2556</v>
+        <v>2666</v>
       </c>
       <c r="F6" s="7">
         <v>11.0</v>
@@ -61433,16 +63497,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="26" t="s">
-        <v>2557</v>
+        <v>2667</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>2558</v>
+        <v>2668</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>2559</v>
+        <v>2669</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>12</v>
@@ -61472,7 +63536,7 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B2" s="6">
         <v>44690.0</v>
@@ -61487,7 +63551,7 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B3" s="6">
         <v>44690.0</v>
@@ -61502,7 +63566,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B4" s="6">
         <v>44690.0</v>
@@ -61517,7 +63581,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B5" s="6">
         <v>44690.0</v>
@@ -61532,7 +63596,7 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B6" s="6">
         <v>44690.0</v>
@@ -61547,7 +63611,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B7" s="6">
         <v>44690.0</v>
@@ -61562,7 +63626,7 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B8" s="6">
         <v>44690.0</v>
@@ -61577,7 +63641,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B9" s="6">
         <v>44690.0</v>
@@ -61592,7 +63656,7 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B10" s="6">
         <v>44690.0</v>
@@ -61607,7 +63671,7 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B11" s="6">
         <v>44690.0</v>
@@ -61622,7 +63686,7 @@
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B12" s="6">
         <v>44690.0</v>
@@ -61637,7 +63701,7 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B13" s="6">
         <v>44690.0</v>
@@ -61652,7 +63716,7 @@
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B14" s="6">
         <v>44690.0</v>
@@ -61667,7 +63731,7 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B15" s="6">
         <v>44690.0</v>
@@ -61682,7 +63746,7 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B16" s="6">
         <v>44690.0</v>
@@ -61697,7 +63761,7 @@
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B17" s="6">
         <v>44690.0</v>
@@ -61713,7 +63777,7 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B18" s="6">
         <v>44690.0</v>
@@ -61729,7 +63793,7 @@
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B19" s="6">
         <v>44690.0</v>
@@ -61744,7 +63808,7 @@
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B20" s="6">
         <v>44690.0</v>
@@ -61759,7 +63823,7 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B21" s="6">
         <v>44690.0</v>
@@ -61774,7 +63838,7 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B22" s="6">
         <v>44690.0</v>
@@ -61789,7 +63853,7 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B23" s="6">
         <v>44690.0</v>
@@ -61804,7 +63868,7 @@
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B24" s="6">
         <v>44690.0</v>
@@ -61819,7 +63883,7 @@
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B25" s="6">
         <v>44690.0</v>
@@ -61834,7 +63898,7 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B26" s="6">
         <v>44690.0</v>
@@ -61849,7 +63913,7 @@
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B27" s="6">
         <v>44690.0</v>
@@ -61864,7 +63928,7 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B28" s="6">
         <v>44690.0</v>
@@ -61879,7 +63943,7 @@
     </row>
     <row r="29">
       <c r="A29" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B29" s="6">
         <v>44690.0</v>
@@ -61894,7 +63958,7 @@
     </row>
     <row r="30">
       <c r="A30" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B30" s="6">
         <v>44690.0</v>
@@ -61909,7 +63973,7 @@
     </row>
     <row r="31">
       <c r="A31" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B31" s="6">
         <v>44690.0</v>
@@ -61924,7 +63988,7 @@
     </row>
     <row r="32">
       <c r="A32" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B32" s="6">
         <v>44690.0</v>
@@ -61939,7 +64003,7 @@
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B33" s="6">
         <v>44690.0</v>
@@ -61954,7 +64018,7 @@
     </row>
     <row r="34">
       <c r="A34" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B34" s="6">
         <v>44690.0</v>
@@ -61969,7 +64033,7 @@
     </row>
     <row r="35">
       <c r="A35" s="7" t="s">
-        <v>2547</v>
+        <v>2657</v>
       </c>
       <c r="B35" s="6">
         <v>44690.0</v>
@@ -61984,7 +64048,7 @@
     </row>
     <row r="36">
       <c r="A36" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B36" s="6">
         <v>44704.0</v>
@@ -61999,7 +64063,7 @@
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B37" s="6">
         <v>44704.0</v>
@@ -62014,7 +64078,7 @@
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B38" s="6">
         <v>44704.0</v>
@@ -62026,12 +64090,12 @@
         <v>22.0</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>2561</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B39" s="6">
         <v>44704.0</v>
@@ -62046,7 +64110,7 @@
     </row>
     <row r="40">
       <c r="A40" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B40" s="6">
         <v>44704.0</v>
@@ -62058,12 +64122,12 @@
         <v>34.0</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>2561</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B41" s="6">
         <v>44704.0</v>
@@ -62078,7 +64142,7 @@
     </row>
     <row r="42">
       <c r="A42" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B42" s="6">
         <v>44704.0</v>
@@ -62093,7 +64157,7 @@
     </row>
     <row r="43">
       <c r="A43" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B43" s="6">
         <v>44704.0</v>
@@ -62108,7 +64172,7 @@
     </row>
     <row r="44">
       <c r="A44" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B44" s="6">
         <v>44704.0</v>
@@ -62120,12 +64184,12 @@
         <v>6.0</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>2561</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B45" s="6">
         <v>44704.0</v>
@@ -62140,7 +64204,7 @@
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B46" s="6">
         <v>44704.0</v>
@@ -62155,7 +64219,7 @@
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B47" s="6">
         <v>44704.0</v>
@@ -62170,7 +64234,7 @@
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B48" s="6">
         <v>44704.0</v>
@@ -62185,7 +64249,7 @@
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B49" s="6">
         <v>44704.0</v>
@@ -62200,7 +64264,7 @@
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B50" s="6">
         <v>44704.0</v>
@@ -62215,7 +64279,7 @@
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B51" s="6">
         <v>44704.0</v>
@@ -62230,7 +64294,7 @@
     </row>
     <row r="52">
       <c r="A52" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B52" s="6">
         <v>44704.0</v>
@@ -62245,7 +64309,7 @@
     </row>
     <row r="53">
       <c r="A53" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B53" s="6">
         <v>44704.0</v>
@@ -62260,7 +64324,7 @@
     </row>
     <row r="54">
       <c r="A54" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B54" s="6">
         <v>44704.0</v>
@@ -62275,7 +64339,7 @@
     </row>
     <row r="55">
       <c r="A55" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B55" s="6">
         <v>44704.0</v>
@@ -62290,7 +64354,7 @@
     </row>
     <row r="56">
       <c r="A56" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B56" s="6">
         <v>44704.0</v>
@@ -62305,7 +64369,7 @@
     </row>
     <row r="57">
       <c r="A57" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B57" s="6">
         <v>44704.0</v>
@@ -62320,7 +64384,7 @@
     </row>
     <row r="58">
       <c r="A58" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B58" s="6">
         <v>44704.0</v>
@@ -62335,7 +64399,7 @@
     </row>
     <row r="59">
       <c r="A59" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B59" s="6">
         <v>44704.0</v>
@@ -62350,7 +64414,7 @@
     </row>
     <row r="60">
       <c r="A60" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B60" s="6">
         <v>44704.0</v>
@@ -62365,7 +64429,7 @@
     </row>
     <row r="61">
       <c r="A61" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B61" s="6">
         <v>44704.0</v>
@@ -62380,7 +64444,7 @@
     </row>
     <row r="62">
       <c r="A62" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B62" s="6">
         <v>44704.0</v>
@@ -62395,7 +64459,7 @@
     </row>
     <row r="63">
       <c r="A63" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B63" s="6">
         <v>44704.0</v>
@@ -62410,7 +64474,7 @@
     </row>
     <row r="64">
       <c r="A64" s="7" t="s">
-        <v>2560</v>
+        <v>2670</v>
       </c>
       <c r="B64" s="6">
         <v>44704.0</v>
@@ -62425,7 +64489,7 @@
     </row>
     <row r="65">
       <c r="A65" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B65" s="6">
         <v>44704.0</v>
@@ -62440,7 +64504,7 @@
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B66" s="6">
         <v>44704.0</v>
@@ -62455,7 +64519,7 @@
     </row>
     <row r="67">
       <c r="A67" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B67" s="6">
         <v>44704.0</v>
@@ -62470,7 +64534,7 @@
     </row>
     <row r="68">
       <c r="A68" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B68" s="6">
         <v>44704.0</v>
@@ -62485,7 +64549,7 @@
     </row>
     <row r="69">
       <c r="A69" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B69" s="6">
         <v>44704.0</v>
@@ -62500,7 +64564,7 @@
     </row>
     <row r="70">
       <c r="A70" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B70" s="6">
         <v>44704.0</v>
@@ -62515,7 +64579,7 @@
     </row>
     <row r="71">
       <c r="A71" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B71" s="6">
         <v>44704.0</v>
@@ -62530,7 +64594,7 @@
     </row>
     <row r="72">
       <c r="A72" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B72" s="6">
         <v>44704.0</v>
@@ -62545,7 +64609,7 @@
     </row>
     <row r="73">
       <c r="A73" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B73" s="6">
         <v>44704.0</v>
@@ -62560,7 +64624,7 @@
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B74" s="6">
         <v>44704.0</v>
@@ -62575,7 +64639,7 @@
     </row>
     <row r="75">
       <c r="A75" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B75" s="6">
         <v>44704.0</v>
@@ -62590,7 +64654,7 @@
     </row>
     <row r="76">
       <c r="A76" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B76" s="6">
         <v>44704.0</v>
@@ -62605,7 +64669,7 @@
     </row>
     <row r="77">
       <c r="A77" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B77" s="6">
         <v>44704.0</v>
@@ -62620,7 +64684,7 @@
     </row>
     <row r="78">
       <c r="A78" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B78" s="6">
         <v>44704.0</v>
@@ -62635,7 +64699,7 @@
     </row>
     <row r="79">
       <c r="A79" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B79" s="6">
         <v>44704.0</v>
@@ -62650,7 +64714,7 @@
     </row>
     <row r="80">
       <c r="A80" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B80" s="6">
         <v>44704.0</v>
@@ -62665,7 +64729,7 @@
     </row>
     <row r="81">
       <c r="A81" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B81" s="6">
         <v>44704.0</v>
@@ -62680,7 +64744,7 @@
     </row>
     <row r="82">
       <c r="A82" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B82" s="6">
         <v>44704.0</v>
@@ -62695,7 +64759,7 @@
     </row>
     <row r="83">
       <c r="A83" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B83" s="6">
         <v>44704.0</v>
@@ -62710,7 +64774,7 @@
     </row>
     <row r="84">
       <c r="A84" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B84" s="6">
         <v>44704.0</v>
@@ -62725,7 +64789,7 @@
     </row>
     <row r="85">
       <c r="A85" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B85" s="6">
         <v>44704.0</v>
@@ -62740,7 +64804,7 @@
     </row>
     <row r="86">
       <c r="A86" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B86" s="6">
         <v>44704.0</v>
@@ -62755,7 +64819,7 @@
     </row>
     <row r="87">
       <c r="A87" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B87" s="6">
         <v>44704.0</v>
@@ -62770,7 +64834,7 @@
     </row>
     <row r="88">
       <c r="A88" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B88" s="6">
         <v>44704.0</v>
@@ -62785,7 +64849,7 @@
     </row>
     <row r="89">
       <c r="A89" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B89" s="6">
         <v>44704.0</v>
@@ -62800,7 +64864,7 @@
     </row>
     <row r="90">
       <c r="A90" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B90" s="6">
         <v>44704.0</v>
@@ -62815,7 +64879,7 @@
     </row>
     <row r="91">
       <c r="A91" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B91" s="6">
         <v>44704.0</v>
@@ -62830,7 +64894,7 @@
     </row>
     <row r="92">
       <c r="A92" s="7" t="s">
-        <v>2562</v>
+        <v>2672</v>
       </c>
       <c r="B92" s="6">
         <v>44704.0</v>
@@ -62845,7 +64909,7 @@
     </row>
     <row r="93">
       <c r="A93" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B93" s="6">
         <v>44705.0</v>
@@ -62860,7 +64924,7 @@
     </row>
     <row r="94">
       <c r="A94" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B94" s="6">
         <v>44705.0</v>
@@ -62875,7 +64939,7 @@
     </row>
     <row r="95">
       <c r="A95" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B95" s="6">
         <v>44705.0</v>
@@ -62890,7 +64954,7 @@
     </row>
     <row r="96">
       <c r="A96" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B96" s="6">
         <v>44705.0</v>
@@ -62905,7 +64969,7 @@
     </row>
     <row r="97">
       <c r="A97" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B97" s="6">
         <v>44705.0</v>
@@ -62920,7 +64984,7 @@
     </row>
     <row r="98">
       <c r="A98" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B98" s="6">
         <v>44705.0</v>
@@ -62935,7 +64999,7 @@
     </row>
     <row r="99">
       <c r="A99" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B99" s="6">
         <v>44705.0</v>
@@ -62950,7 +65014,7 @@
     </row>
     <row r="100">
       <c r="A100" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B100" s="6">
         <v>44705.0</v>
@@ -62965,7 +65029,7 @@
     </row>
     <row r="101">
       <c r="A101" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B101" s="6">
         <v>44705.0</v>
@@ -62980,7 +65044,7 @@
     </row>
     <row r="102">
       <c r="A102" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B102" s="6">
         <v>44705.0</v>
@@ -62995,7 +65059,7 @@
     </row>
     <row r="103">
       <c r="A103" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B103" s="6">
         <v>44705.0</v>
@@ -63010,7 +65074,7 @@
     </row>
     <row r="104">
       <c r="A104" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B104" s="6">
         <v>44705.0</v>
@@ -63025,7 +65089,7 @@
     </row>
     <row r="105">
       <c r="A105" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B105" s="6">
         <v>44705.0</v>
@@ -63040,7 +65104,7 @@
     </row>
     <row r="106">
       <c r="A106" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B106" s="6">
         <v>44705.0</v>
@@ -63055,7 +65119,7 @@
     </row>
     <row r="107">
       <c r="A107" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B107" s="6">
         <v>44705.0</v>
@@ -63070,7 +65134,7 @@
     </row>
     <row r="108">
       <c r="A108" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B108" s="6">
         <v>44705.0</v>
@@ -63085,7 +65149,7 @@
     </row>
     <row r="109">
       <c r="A109" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B109" s="6">
         <v>44705.0</v>
@@ -63100,7 +65164,7 @@
     </row>
     <row r="110">
       <c r="A110" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B110" s="6">
         <v>44705.0</v>
@@ -63115,7 +65179,7 @@
     </row>
     <row r="111">
       <c r="A111" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B111" s="6">
         <v>44705.0</v>
@@ -63130,7 +65194,7 @@
     </row>
     <row r="112">
       <c r="A112" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B112" s="6">
         <v>44705.0</v>
@@ -63145,7 +65209,7 @@
     </row>
     <row r="113">
       <c r="A113" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B113" s="6">
         <v>44705.0</v>
@@ -63160,7 +65224,7 @@
     </row>
     <row r="114">
       <c r="A114" s="7" t="s">
-        <v>2563</v>
+        <v>2673</v>
       </c>
       <c r="B114" s="6">
         <v>44705.0</v>
@@ -63175,7 +65239,7 @@
     </row>
     <row r="115">
       <c r="A115" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B115" s="6">
         <v>44708.0</v>
@@ -63190,7 +65254,7 @@
     </row>
     <row r="116">
       <c r="A116" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B116" s="6">
         <v>44708.0</v>
@@ -63205,7 +65269,7 @@
     </row>
     <row r="117">
       <c r="A117" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B117" s="6">
         <v>44708.0</v>
@@ -63220,7 +65284,7 @@
     </row>
     <row r="118">
       <c r="A118" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B118" s="6">
         <v>44708.0</v>
@@ -63232,12 +65296,12 @@
         <v>39.0</v>
       </c>
       <c r="E118" s="29" t="s">
-        <v>2561</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B119" s="6">
         <v>44708.0</v>
@@ -63252,7 +65316,7 @@
     </row>
     <row r="120">
       <c r="A120" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B120" s="6">
         <v>44708.0</v>
@@ -63267,7 +65331,7 @@
     </row>
     <row r="121">
       <c r="A121" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B121" s="6">
         <v>44708.0</v>
@@ -63282,7 +65346,7 @@
     </row>
     <row r="122">
       <c r="A122" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B122" s="6">
         <v>44708.0</v>
@@ -63297,7 +65361,7 @@
     </row>
     <row r="123">
       <c r="A123" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B123" s="6">
         <v>44708.0</v>
@@ -63312,7 +65376,7 @@
     </row>
     <row r="124">
       <c r="A124" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B124" s="6">
         <v>44708.0</v>
@@ -63327,7 +65391,7 @@
     </row>
     <row r="125">
       <c r="A125" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B125" s="6">
         <v>44708.0</v>
@@ -63342,7 +65406,7 @@
     </row>
     <row r="126">
       <c r="A126" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B126" s="6">
         <v>44708.0</v>
@@ -63357,7 +65421,7 @@
     </row>
     <row r="127">
       <c r="A127" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B127" s="6">
         <v>44708.0</v>
@@ -63369,12 +65433,12 @@
         <v>11.0</v>
       </c>
       <c r="E127" s="29" t="s">
-        <v>2561</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B128" s="6">
         <v>44708.0</v>
@@ -63389,7 +65453,7 @@
     </row>
     <row r="129">
       <c r="A129" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B129" s="6">
         <v>44708.0</v>
@@ -63401,12 +65465,12 @@
         <v>40.0</v>
       </c>
       <c r="E129" s="29" t="s">
-        <v>2561</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B130" s="6">
         <v>44708.0</v>
@@ -63421,7 +65485,7 @@
     </row>
     <row r="131">
       <c r="A131" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B131" s="6">
         <v>44708.0</v>
@@ -63436,7 +65500,7 @@
     </row>
     <row r="132">
       <c r="A132" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B132" s="6">
         <v>44708.0</v>
@@ -63451,7 +65515,7 @@
     </row>
     <row r="133">
       <c r="A133" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="B133" s="6">
         <v>44708.0</v>
@@ -63466,7 +65530,7 @@
     </row>
     <row r="134">
       <c r="A134" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B134" s="6">
         <v>44713.0</v>
@@ -63478,12 +65542,12 @@
         <v>1298</v>
       </c>
       <c r="E134" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B135" s="6">
         <v>44713.0</v>
@@ -63495,12 +65559,12 @@
         <v>1300</v>
       </c>
       <c r="E135" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B136" s="6">
         <v>44713.0</v>
@@ -63512,12 +65576,12 @@
         <v>1302</v>
       </c>
       <c r="E136" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B137" s="6">
         <v>44713.0</v>
@@ -63529,12 +65593,12 @@
         <v>1304</v>
       </c>
       <c r="E137" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B138" s="6">
         <v>44713.0</v>
@@ -63546,12 +65610,12 @@
         <v>1306</v>
       </c>
       <c r="E138" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B139" s="6">
         <v>44713.0</v>
@@ -63563,12 +65627,12 @@
         <v>1309</v>
       </c>
       <c r="E139" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B140" s="6">
         <v>44713.0</v>
@@ -63580,12 +65644,12 @@
         <v>1312</v>
       </c>
       <c r="E140" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B141" s="6">
         <v>44713.0</v>
@@ -63597,12 +65661,12 @@
         <v>1315</v>
       </c>
       <c r="E141" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B142" s="6">
         <v>44713.0</v>
@@ -63614,12 +65678,12 @@
         <v>1318</v>
       </c>
       <c r="E142" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B143" s="6">
         <v>44713.0</v>
@@ -63631,12 +65695,12 @@
         <v>1321</v>
       </c>
       <c r="E143" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B144" s="6">
         <v>44713.0</v>
@@ -63648,12 +65712,12 @@
         <v>1323</v>
       </c>
       <c r="E144" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B145" s="6">
         <v>44713.0</v>
@@ -63665,12 +65729,12 @@
         <v>1325</v>
       </c>
       <c r="E145" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B146" s="6">
         <v>44713.0</v>
@@ -63682,12 +65746,12 @@
         <v>1327</v>
       </c>
       <c r="E146" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B147" s="6">
         <v>44713.0</v>
@@ -63699,12 +65763,12 @@
         <v>1329</v>
       </c>
       <c r="E147" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B148" s="6">
         <v>44713.0</v>
@@ -63716,12 +65780,12 @@
         <v>1331</v>
       </c>
       <c r="E148" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B149" s="6">
         <v>44713.0</v>
@@ -63733,12 +65797,12 @@
         <v>1333</v>
       </c>
       <c r="E149" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B150" s="6">
         <v>44713.0</v>
@@ -63750,12 +65814,12 @@
         <v>1335</v>
       </c>
       <c r="E150" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B151" s="6">
         <v>44713.0</v>
@@ -63767,12 +65831,12 @@
         <v>1337</v>
       </c>
       <c r="E151" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B152" s="6">
         <v>44713.0</v>
@@ -63784,12 +65848,12 @@
         <v>1340</v>
       </c>
       <c r="E152" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B153" s="6">
         <v>44713.0</v>
@@ -63801,12 +65865,12 @@
         <v>1342</v>
       </c>
       <c r="E153" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B154" s="6">
         <v>44713.0</v>
@@ -63818,12 +65882,12 @@
         <v>1344</v>
       </c>
       <c r="E154" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B155" s="6">
         <v>44713.0</v>
@@ -63835,12 +65899,12 @@
         <v>1346</v>
       </c>
       <c r="E155" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B156" s="6">
         <v>44713.0</v>
@@ -63852,12 +65916,12 @@
         <v>1348</v>
       </c>
       <c r="E156" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="7" t="s">
-        <v>2565</v>
+        <v>2675</v>
       </c>
       <c r="B157" s="6">
         <v>44713.0</v>
@@ -63869,7 +65933,7 @@
         <v>1350</v>
       </c>
       <c r="E157" s="29" t="s">
-        <v>2566</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="158">
@@ -66421,22 +68485,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2567</v>
+        <v>2677</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2568</v>
+        <v>2678</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2569</v>
+        <v>2679</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2570</v>
+        <v>2680</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>2571</v>
+        <v>2681</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>2572</v>
+        <v>2682</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>12</v>
@@ -66447,17 +68511,17 @@
         <v>44690.0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2573</v>
+        <v>2683</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>2546</v>
+        <v>2656</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7" t="s">
-        <v>2574</v>
+        <v>2684</v>
       </c>
     </row>
     <row r="3">
@@ -66465,7 +68529,7 @@
         <v>44692.0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2575</v>
+        <v>2685</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="7" t="s">
@@ -66486,10 +68550,10 @@
         <v>44694.0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2576</v>
+        <v>2686</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>2552</v>
+        <v>2662</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
@@ -66504,7 +68568,7 @@
         <v>2.5</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>2577</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="5">
@@ -66512,10 +68576,10 @@
         <v>44695.0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2578</v>
+        <v>2688</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2556</v>
+        <v>2666</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -66535,10 +68599,10 @@
         <v>44697.0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2579</v>
+        <v>2689</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>2580</v>
+        <v>2690</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -66558,10 +68622,10 @@
         <v>44698.0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>2564</v>
+        <v>2674</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>2581</v>
+        <v>2691</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -66581,10 +68645,10 @@
         <v>44726.0</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>2582</v>
+        <v>2692</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>2583</v>
+        <v>2693</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>1353</v>

</xml_diff>

<commit_message>
Updated counts and gps for 28Jun2022 from Deep End Beach (DEB)
</commit_message>
<xml_diff>
--- a/Data/Genotype_Samples_2022.xlsx
+++ b/Data/Genotype_Samples_2022.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8924" uniqueCount="2694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9254" uniqueCount="2797">
   <si>
     <t>Date</t>
   </si>
@@ -7941,6 +7941,315 @@
   </si>
   <si>
     <t>G1225</t>
+  </si>
+  <si>
+    <t>DEB_001</t>
+  </si>
+  <si>
+    <t>G1459</t>
+  </si>
+  <si>
+    <t>DEB_002</t>
+  </si>
+  <si>
+    <t>DEB_003</t>
+  </si>
+  <si>
+    <t>G1460</t>
+  </si>
+  <si>
+    <t>DEB_004</t>
+  </si>
+  <si>
+    <t>DEB_005</t>
+  </si>
+  <si>
+    <t>G1470</t>
+  </si>
+  <si>
+    <t>slight disease</t>
+  </si>
+  <si>
+    <t>DEB_006</t>
+  </si>
+  <si>
+    <t>DEB_007</t>
+  </si>
+  <si>
+    <t>G1469</t>
+  </si>
+  <si>
+    <t>DEB_008</t>
+  </si>
+  <si>
+    <t>G1480</t>
+  </si>
+  <si>
+    <t>DEB_009</t>
+  </si>
+  <si>
+    <t>DEB_010</t>
+  </si>
+  <si>
+    <t>G1458</t>
+  </si>
+  <si>
+    <t>DEB_011</t>
+  </si>
+  <si>
+    <t>DEB_012</t>
+  </si>
+  <si>
+    <t>DEB_013</t>
+  </si>
+  <si>
+    <t>G1490</t>
+  </si>
+  <si>
+    <t>DEB_014</t>
+  </si>
+  <si>
+    <t>pale</t>
+  </si>
+  <si>
+    <t>DEB_015</t>
+  </si>
+  <si>
+    <t>DEB_016</t>
+  </si>
+  <si>
+    <t>G1468</t>
+  </si>
+  <si>
+    <t>DEB_017</t>
+  </si>
+  <si>
+    <t>DEB_018</t>
+  </si>
+  <si>
+    <t>G1488</t>
+  </si>
+  <si>
+    <t>DEB_019</t>
+  </si>
+  <si>
+    <t>G1489</t>
+  </si>
+  <si>
+    <t>DEB_020</t>
+  </si>
+  <si>
+    <t>DEB_021</t>
+  </si>
+  <si>
+    <t>DEB_022</t>
+  </si>
+  <si>
+    <t>G1479</t>
+  </si>
+  <si>
+    <t>DEB_023</t>
+  </si>
+  <si>
+    <t>DEB_024</t>
+  </si>
+  <si>
+    <t>DEB_025</t>
+  </si>
+  <si>
+    <t>G1498</t>
+  </si>
+  <si>
+    <t>DEB_026</t>
+  </si>
+  <si>
+    <t>DEB_027</t>
+  </si>
+  <si>
+    <t>G1499</t>
+  </si>
+  <si>
+    <t>DEB_028</t>
+  </si>
+  <si>
+    <t>DEB_029</t>
+  </si>
+  <si>
+    <t>DEB_030</t>
+  </si>
+  <si>
+    <t>G1478</t>
+  </si>
+  <si>
+    <t>DEB_031</t>
+  </si>
+  <si>
+    <t>G1500</t>
+  </si>
+  <si>
+    <t>DEB_032</t>
+  </si>
+  <si>
+    <t>G1456</t>
+  </si>
+  <si>
+    <t>DEB_033</t>
+  </si>
+  <si>
+    <t>G1457</t>
+  </si>
+  <si>
+    <t>DEB_034</t>
+  </si>
+  <si>
+    <t>G1495</t>
+  </si>
+  <si>
+    <t>DEB_035</t>
+  </si>
+  <si>
+    <t>DEB_036</t>
+  </si>
+  <si>
+    <t>DEB_037</t>
+  </si>
+  <si>
+    <t>G1494</t>
+  </si>
+  <si>
+    <t>DEB_038</t>
+  </si>
+  <si>
+    <t>G1493</t>
+  </si>
+  <si>
+    <t>DEB_039</t>
+  </si>
+  <si>
+    <t>DEB_040</t>
+  </si>
+  <si>
+    <t>G1452</t>
+  </si>
+  <si>
+    <t>DEB_041</t>
+  </si>
+  <si>
+    <t>G1492</t>
+  </si>
+  <si>
+    <t>DEB_042</t>
+  </si>
+  <si>
+    <t>DEB_043</t>
+  </si>
+  <si>
+    <t>G1453</t>
+  </si>
+  <si>
+    <t>DEB_044</t>
+  </si>
+  <si>
+    <t>DEB_045</t>
+  </si>
+  <si>
+    <t>G1461</t>
+  </si>
+  <si>
+    <t>DEB_046</t>
+  </si>
+  <si>
+    <t>DEB_047</t>
+  </si>
+  <si>
+    <t>G1462</t>
+  </si>
+  <si>
+    <t>DEB_048</t>
+  </si>
+  <si>
+    <t>G1454</t>
+  </si>
+  <si>
+    <t>DEB_049</t>
+  </si>
+  <si>
+    <t>DEB_050</t>
+  </si>
+  <si>
+    <t>G1463</t>
+  </si>
+  <si>
+    <t>DEB_051</t>
+  </si>
+  <si>
+    <t>DEB_052</t>
+  </si>
+  <si>
+    <t>G1455</t>
+  </si>
+  <si>
+    <t>DEB_053</t>
+  </si>
+  <si>
+    <t>G1464</t>
+  </si>
+  <si>
+    <t>DEB_054</t>
+  </si>
+  <si>
+    <t>DEB_055</t>
+  </si>
+  <si>
+    <t>G1471</t>
+  </si>
+  <si>
+    <t>DEB_056</t>
+  </si>
+  <si>
+    <t>G1465</t>
+  </si>
+  <si>
+    <t>DEB_057</t>
+  </si>
+  <si>
+    <t>G1481</t>
+  </si>
+  <si>
+    <t>DEB_058</t>
+  </si>
+  <si>
+    <t>G1472</t>
+  </si>
+  <si>
+    <t>DEB_059</t>
+  </si>
+  <si>
+    <t>DEB_060</t>
+  </si>
+  <si>
+    <t>DEB_061</t>
+  </si>
+  <si>
+    <t>G1473</t>
+  </si>
+  <si>
+    <t>DEB_062</t>
+  </si>
+  <si>
+    <t>G1482</t>
+  </si>
+  <si>
+    <t>DEB_063</t>
+  </si>
+  <si>
+    <t>G1474</t>
+  </si>
+  <si>
+    <t>DEB_064</t>
+  </si>
+  <si>
+    <t>G1475</t>
   </si>
   <si>
     <t>Site_ID</t>
@@ -61591,263 +61900,2085 @@
       </c>
     </row>
     <row r="1614">
-      <c r="A1614" s="24"/>
-      <c r="B1614" s="7"/>
+      <c r="A1614" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1614" s="7" t="s">
+        <v>2642</v>
+      </c>
+      <c r="C1614" s="7" t="s">
+        <v>2643</v>
+      </c>
+      <c r="D1614" s="7">
+        <v>58.0</v>
+      </c>
+      <c r="E1614" s="8">
+        <v>0.5034722222222222</v>
+      </c>
+      <c r="F1614" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1614" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1614" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1614" s="11">
+        <v>17.7610717713833</v>
+      </c>
+      <c r="K1614" s="11">
+        <v>-64.6690336614847</v>
+      </c>
     </row>
     <row r="1615">
-      <c r="A1615" s="24"/>
-      <c r="B1615" s="7"/>
+      <c r="A1615" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1615" s="7" t="s">
+        <v>2644</v>
+      </c>
+      <c r="C1615" s="7" t="s">
+        <v>2643</v>
+      </c>
+      <c r="D1615" s="7">
+        <v>35.0</v>
+      </c>
+      <c r="E1615" s="8">
+        <v>0.5034722222222222</v>
+      </c>
+      <c r="F1615" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1615" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1615" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1615" s="11">
+        <v>17.7610717713833</v>
+      </c>
+      <c r="K1615" s="11">
+        <v>-64.6690336614847</v>
+      </c>
     </row>
     <row r="1616">
-      <c r="A1616" s="24"/>
-      <c r="B1616" s="7"/>
+      <c r="A1616" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1616" s="7" t="s">
+        <v>2645</v>
+      </c>
+      <c r="C1616" s="7" t="s">
+        <v>2646</v>
+      </c>
+      <c r="D1616" s="7">
+        <v>57.0</v>
+      </c>
+      <c r="E1616" s="8">
+        <v>0.5076388888888889</v>
+      </c>
+      <c r="F1616" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1616" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1616" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1616" s="11">
+        <v>17.7611262537539</v>
+      </c>
+      <c r="K1616" s="11">
+        <v>-64.6691091824323</v>
+      </c>
     </row>
     <row r="1617">
-      <c r="A1617" s="24"/>
-      <c r="B1617" s="7"/>
+      <c r="A1617" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1617" s="7" t="s">
+        <v>2647</v>
+      </c>
+      <c r="C1617" s="7" t="s">
+        <v>2646</v>
+      </c>
+      <c r="D1617" s="7">
+        <v>204.0</v>
+      </c>
+      <c r="E1617" s="8">
+        <v>0.5076388888888889</v>
+      </c>
+      <c r="F1617" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1617" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1617" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1617" s="11">
+        <v>17.7611262537539</v>
+      </c>
+      <c r="K1617" s="11">
+        <v>-64.6691091824323</v>
+      </c>
     </row>
     <row r="1618">
-      <c r="A1618" s="24"/>
-      <c r="B1618" s="7"/>
+      <c r="A1618" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1618" s="7" t="s">
+        <v>2648</v>
+      </c>
+      <c r="C1618" s="7" t="s">
+        <v>2649</v>
+      </c>
+      <c r="D1618" s="7">
+        <v>205.0</v>
+      </c>
+      <c r="E1618" s="8">
+        <v>0.5111111111111111</v>
+      </c>
+      <c r="F1618" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1618" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1618" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1618" s="11">
+        <v>17.7611826639622</v>
+      </c>
+      <c r="K1618" s="11">
+        <v>-64.6691217552871</v>
+      </c>
+      <c r="M1618" s="7" t="s">
+        <v>2650</v>
+      </c>
     </row>
     <row r="1619">
-      <c r="A1619" s="24"/>
-      <c r="B1619" s="7"/>
+      <c r="A1619" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1619" s="7" t="s">
+        <v>2651</v>
+      </c>
+      <c r="C1619" s="7" t="s">
+        <v>2649</v>
+      </c>
+      <c r="D1619" s="7">
+        <v>19.0</v>
+      </c>
+      <c r="E1619" s="8">
+        <v>0.5111111111111111</v>
+      </c>
+      <c r="F1619" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1619" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1619" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1619" s="11">
+        <v>17.7611826639622</v>
+      </c>
+      <c r="K1619" s="11">
+        <v>-64.6691217552871</v>
+      </c>
     </row>
     <row r="1620">
-      <c r="A1620" s="24"/>
-      <c r="B1620" s="7"/>
+      <c r="A1620" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1620" s="7" t="s">
+        <v>2652</v>
+      </c>
+      <c r="C1620" s="7" t="s">
+        <v>2653</v>
+      </c>
+      <c r="D1620" s="7">
+        <v>208.0</v>
+      </c>
+      <c r="E1620" s="8">
+        <v>0.5145833333333333</v>
+      </c>
+      <c r="F1620" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1620" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1620" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1620" s="11">
+        <v>17.761211078614</v>
+      </c>
+      <c r="K1620" s="11">
+        <v>-64.6691859606653</v>
+      </c>
+      <c r="M1620" s="7" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="1621">
-      <c r="A1621" s="24"/>
-      <c r="B1621" s="7"/>
+      <c r="A1621" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1621" s="7" t="s">
+        <v>2654</v>
+      </c>
+      <c r="C1621" s="7" t="s">
+        <v>2655</v>
+      </c>
+      <c r="D1621" s="7">
+        <v>8.0</v>
+      </c>
+      <c r="E1621" s="8">
+        <v>0.5173611111111112</v>
+      </c>
+      <c r="F1621" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1621" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1621" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1621" s="11">
+        <v>17.7611965779215</v>
+      </c>
+      <c r="K1621" s="11">
+        <v>-64.6692260261625</v>
+      </c>
     </row>
     <row r="1622">
-      <c r="A1622" s="24"/>
-      <c r="B1622" s="7"/>
+      <c r="A1622" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1622" s="7" t="s">
+        <v>2656</v>
+      </c>
+      <c r="C1622" s="7" t="s">
+        <v>2655</v>
+      </c>
+      <c r="D1622" s="7">
+        <v>207.0</v>
+      </c>
+      <c r="E1622" s="8">
+        <v>0.5173611111111112</v>
+      </c>
+      <c r="F1622" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1622" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1622" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1622" s="11">
+        <v>17.7611965779215</v>
+      </c>
+      <c r="K1622" s="11">
+        <v>-64.6692260261625</v>
+      </c>
     </row>
     <row r="1623">
-      <c r="A1623" s="24"/>
-      <c r="B1623" s="7"/>
+      <c r="A1623" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1623" s="7" t="s">
+        <v>2657</v>
+      </c>
+      <c r="C1623" s="7" t="s">
+        <v>2658</v>
+      </c>
+      <c r="D1623" s="7">
+        <v>31.0</v>
+      </c>
+      <c r="E1623" s="8">
+        <v>0.5208333333333334</v>
+      </c>
+      <c r="F1623" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1623" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1623" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1623" s="11">
+        <v>17.7611949853599</v>
+      </c>
+      <c r="K1623" s="11">
+        <v>-64.6692491602153</v>
+      </c>
     </row>
     <row r="1624">
-      <c r="A1624" s="24"/>
-      <c r="B1624" s="7"/>
+      <c r="A1624" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1624" s="7" t="s">
+        <v>2659</v>
+      </c>
+      <c r="C1624" s="7" t="s">
+        <v>2658</v>
+      </c>
+      <c r="D1624" s="7">
+        <v>73.0</v>
+      </c>
+      <c r="E1624" s="8">
+        <v>0.5208333333333334</v>
+      </c>
+      <c r="F1624" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1624" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1624" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1624" s="11">
+        <v>17.7611949853599</v>
+      </c>
+      <c r="K1624" s="11">
+        <v>-64.6692491602153</v>
+      </c>
     </row>
     <row r="1625">
-      <c r="A1625" s="24"/>
-      <c r="B1625" s="7"/>
+      <c r="A1625" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1625" s="7" t="s">
+        <v>2660</v>
+      </c>
+      <c r="C1625" s="7" t="s">
+        <v>2658</v>
+      </c>
+      <c r="D1625" s="7">
+        <v>109.0</v>
+      </c>
+      <c r="E1625" s="8">
+        <v>0.5208333333333334</v>
+      </c>
+      <c r="F1625" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1625" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1625" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1625" s="11">
+        <v>17.7611949853599</v>
+      </c>
+      <c r="K1625" s="11">
+        <v>-64.6692491602153</v>
+      </c>
     </row>
     <row r="1626">
-      <c r="A1626" s="24"/>
-      <c r="B1626" s="7"/>
+      <c r="A1626" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1626" s="7" t="s">
+        <v>2661</v>
+      </c>
+      <c r="C1626" s="7" t="s">
+        <v>2662</v>
+      </c>
+      <c r="D1626" s="7">
+        <v>28.0</v>
+      </c>
+      <c r="E1626" s="8">
+        <v>0.5263888888888889</v>
+      </c>
+      <c r="F1626" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1626" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1626" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1626" s="11">
+        <v>17.7612430974841</v>
+      </c>
+      <c r="K1626" s="11">
+        <v>-64.6692791674286</v>
+      </c>
+      <c r="M1626" s="7" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="1627">
-      <c r="A1627" s="24"/>
-      <c r="B1627" s="7"/>
+      <c r="A1627" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1627" s="7" t="s">
+        <v>2663</v>
+      </c>
+      <c r="C1627" s="7" t="s">
+        <v>2662</v>
+      </c>
+      <c r="D1627" s="7">
+        <v>84.0</v>
+      </c>
+      <c r="E1627" s="8">
+        <v>0.5263888888888889</v>
+      </c>
+      <c r="F1627" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1627" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1627" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1627" s="11">
+        <v>17.7612430974841</v>
+      </c>
+      <c r="K1627" s="11">
+        <v>-64.6692791674286</v>
+      </c>
+      <c r="M1627" s="7" t="s">
+        <v>2664</v>
+      </c>
     </row>
     <row r="1628">
-      <c r="A1628" s="24"/>
-      <c r="B1628" s="7"/>
+      <c r="A1628" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1628" s="7" t="s">
+        <v>2665</v>
+      </c>
+      <c r="C1628" s="7" t="s">
+        <v>2662</v>
+      </c>
+      <c r="D1628" s="7">
+        <v>69.0</v>
+      </c>
+      <c r="E1628" s="8">
+        <v>0.5263888888888889</v>
+      </c>
+      <c r="F1628" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1628" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1628" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1628" s="11">
+        <v>17.7612430974841</v>
+      </c>
+      <c r="K1628" s="11">
+        <v>-64.6692791674286</v>
+      </c>
     </row>
     <row r="1629">
-      <c r="A1629" s="24"/>
-      <c r="B1629" s="7"/>
+      <c r="A1629" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1629" s="7" t="s">
+        <v>2666</v>
+      </c>
+      <c r="C1629" s="7" t="s">
+        <v>2667</v>
+      </c>
+      <c r="D1629" s="7">
+        <v>215.0</v>
+      </c>
+      <c r="E1629" s="8">
+        <v>0.5326388888888889</v>
+      </c>
+      <c r="F1629" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1629" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1629" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1629" s="11">
+        <v>17.7611707616597</v>
+      </c>
+      <c r="K1629" s="11">
+        <v>-64.6693577896804</v>
+      </c>
     </row>
     <row r="1630">
-      <c r="A1630" s="24"/>
-      <c r="B1630" s="7"/>
+      <c r="A1630" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1630" s="7" t="s">
+        <v>2668</v>
+      </c>
+      <c r="C1630" s="7" t="s">
+        <v>2667</v>
+      </c>
+      <c r="D1630" s="7">
+        <v>12.0</v>
+      </c>
+      <c r="E1630" s="8">
+        <v>0.5326388888888889</v>
+      </c>
+      <c r="F1630" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1630" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1630" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1630" s="11">
+        <v>17.7611707616597</v>
+      </c>
+      <c r="K1630" s="11">
+        <v>-64.6693577896804</v>
+      </c>
     </row>
     <row r="1631">
-      <c r="A1631" s="24"/>
-      <c r="B1631" s="7"/>
+      <c r="A1631" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1631" s="7" t="s">
+        <v>2669</v>
+      </c>
+      <c r="C1631" s="7" t="s">
+        <v>2670</v>
+      </c>
+      <c r="D1631" s="7">
+        <v>86.0</v>
+      </c>
+      <c r="E1631" s="8">
+        <v>0.5361111111111111</v>
+      </c>
+      <c r="F1631" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1631" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1631" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1631" s="11">
+        <v>17.7611497230828</v>
+      </c>
+      <c r="K1631" s="11">
+        <v>-64.6693789120764</v>
+      </c>
     </row>
     <row r="1632">
-      <c r="A1632" s="24"/>
-      <c r="B1632" s="7"/>
+      <c r="A1632" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1632" s="7" t="s">
+        <v>2671</v>
+      </c>
+      <c r="C1632" s="7" t="s">
+        <v>2672</v>
+      </c>
+      <c r="D1632" s="7">
+        <v>46.0</v>
+      </c>
+      <c r="E1632" s="8">
+        <v>0.5388888888888889</v>
+      </c>
+      <c r="F1632" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1632" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1632" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1632" s="11">
+        <v>17.7611365634948</v>
+      </c>
+      <c r="K1632" s="11">
+        <v>-64.6693878807127</v>
+      </c>
     </row>
     <row r="1633">
-      <c r="A1633" s="24"/>
-      <c r="B1633" s="7"/>
+      <c r="A1633" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1633" s="7" t="s">
+        <v>2673</v>
+      </c>
+      <c r="C1633" s="7" t="s">
+        <v>2672</v>
+      </c>
+      <c r="D1633" s="7">
+        <v>201.0</v>
+      </c>
+      <c r="E1633" s="8">
+        <v>0.5388888888888889</v>
+      </c>
+      <c r="F1633" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1633" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1633" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1633" s="11">
+        <v>17.7611365634948</v>
+      </c>
+      <c r="K1633" s="11">
+        <v>-64.6693878807127</v>
+      </c>
     </row>
     <row r="1634">
-      <c r="A1634" s="24"/>
-      <c r="B1634" s="7"/>
+      <c r="A1634" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1634" s="7" t="s">
+        <v>2674</v>
+      </c>
+      <c r="C1634" s="7" t="s">
+        <v>2672</v>
+      </c>
+      <c r="D1634" s="7">
+        <v>34.0</v>
+      </c>
+      <c r="E1634" s="8">
+        <v>0.5388888888888889</v>
+      </c>
+      <c r="F1634" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1634" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1634" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1634" s="11">
+        <v>17.7611365634948</v>
+      </c>
+      <c r="K1634" s="11">
+        <v>-64.6693878807127</v>
+      </c>
     </row>
     <row r="1635">
-      <c r="A1635" s="24"/>
-      <c r="B1635" s="7"/>
+      <c r="A1635" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1635" s="7" t="s">
+        <v>2675</v>
+      </c>
+      <c r="C1635" s="7" t="s">
+        <v>2676</v>
+      </c>
+      <c r="D1635" s="7">
+        <v>67.0</v>
+      </c>
+      <c r="E1635" s="8">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="F1635" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1635" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1635" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1635" s="11">
+        <v>17.7612726017833</v>
+      </c>
+      <c r="K1635" s="11">
+        <v>-64.6695821732283</v>
+      </c>
+      <c r="M1635" s="7" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="1636">
-      <c r="A1636" s="24"/>
-      <c r="B1636" s="7"/>
+      <c r="A1636" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1636" s="7" t="s">
+        <v>2677</v>
+      </c>
+      <c r="C1636" s="7" t="s">
+        <v>2676</v>
+      </c>
+      <c r="D1636" s="7">
+        <v>62.0</v>
+      </c>
+      <c r="E1636" s="8">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="F1636" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1636" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1636" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1636" s="11">
+        <v>17.7612726017833</v>
+      </c>
+      <c r="K1636" s="11">
+        <v>-64.6695821732283</v>
+      </c>
     </row>
     <row r="1637">
-      <c r="A1637" s="24"/>
-      <c r="B1637" s="7"/>
+      <c r="A1637" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1637" s="7" t="s">
+        <v>2678</v>
+      </c>
+      <c r="C1637" s="7" t="s">
+        <v>2676</v>
+      </c>
+      <c r="D1637" s="7">
+        <v>50.0</v>
+      </c>
+      <c r="E1637" s="8">
+        <v>0.5527777777777778</v>
+      </c>
+      <c r="F1637" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1637" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1637" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1637" s="11">
+        <v>17.7612726017833</v>
+      </c>
+      <c r="K1637" s="11">
+        <v>-64.6695821732283</v>
+      </c>
     </row>
     <row r="1638">
-      <c r="A1638" s="24"/>
-      <c r="B1638" s="7"/>
+      <c r="A1638" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1638" s="7" t="s">
+        <v>2679</v>
+      </c>
+      <c r="C1638" s="7" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D1638" s="7">
+        <v>83.0</v>
+      </c>
+      <c r="E1638" s="8">
+        <v>0.5597222222222222</v>
+      </c>
+      <c r="F1638" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1638" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1638" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1638" s="11">
+        <v>17.761353822425</v>
+      </c>
+      <c r="K1638" s="11">
+        <v>-64.669829774648</v>
+      </c>
     </row>
     <row r="1639">
-      <c r="A1639" s="24"/>
-      <c r="B1639" s="7"/>
+      <c r="A1639" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1639" s="7" t="s">
+        <v>2681</v>
+      </c>
+      <c r="C1639" s="7" t="s">
+        <v>2680</v>
+      </c>
+      <c r="D1639" s="7">
+        <v>89.0</v>
+      </c>
+      <c r="E1639" s="8">
+        <v>0.5597222222222222</v>
+      </c>
+      <c r="F1639" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1639" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1639" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1639" s="11">
+        <v>17.761353822425</v>
+      </c>
+      <c r="K1639" s="11">
+        <v>-64.669829774648</v>
+      </c>
     </row>
     <row r="1640">
-      <c r="A1640" s="24"/>
-      <c r="B1640" s="7"/>
+      <c r="A1640" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1640" s="7" t="s">
+        <v>2682</v>
+      </c>
+      <c r="C1640" s="7" t="s">
+        <v>2683</v>
+      </c>
+      <c r="D1640" s="7">
+        <v>82.0</v>
+      </c>
+      <c r="E1640" s="8">
+        <v>0.5638888888888889</v>
+      </c>
+      <c r="F1640" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1640" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1640" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1640" s="11">
+        <v>17.7613549120724</v>
+      </c>
+      <c r="K1640" s="11">
+        <v>-64.6697098296136</v>
+      </c>
     </row>
     <row r="1641">
-      <c r="A1641" s="24"/>
-      <c r="B1641" s="7"/>
+      <c r="A1641" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1641" s="7" t="s">
+        <v>2684</v>
+      </c>
+      <c r="C1641" s="7" t="s">
+        <v>2683</v>
+      </c>
+      <c r="D1641" s="7">
+        <v>119.0</v>
+      </c>
+      <c r="E1641" s="8">
+        <v>0.5638888888888889</v>
+      </c>
+      <c r="F1641" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1641" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1641" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1641" s="11">
+        <v>17.7613549120724</v>
+      </c>
+      <c r="K1641" s="11">
+        <v>-64.6697098296136</v>
+      </c>
     </row>
     <row r="1642">
-      <c r="A1642" s="24"/>
-      <c r="B1642" s="7"/>
+      <c r="A1642" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1642" s="7" t="s">
+        <v>2685</v>
+      </c>
+      <c r="C1642" s="7" t="s">
+        <v>2683</v>
+      </c>
+      <c r="D1642" s="7">
+        <v>81.0</v>
+      </c>
+      <c r="E1642" s="8">
+        <v>0.5638888888888889</v>
+      </c>
+      <c r="F1642" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1642" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1642" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1642" s="11">
+        <v>17.7613549120724</v>
+      </c>
+      <c r="K1642" s="11">
+        <v>-64.6697098296136</v>
+      </c>
     </row>
     <row r="1643">
-      <c r="A1643" s="24"/>
-      <c r="B1643" s="7"/>
+      <c r="A1643" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1643" s="7" t="s">
+        <v>2686</v>
+      </c>
+      <c r="C1643" s="7" t="s">
+        <v>2687</v>
+      </c>
+      <c r="D1643" s="7">
+        <v>26.0</v>
+      </c>
+      <c r="E1643" s="8">
+        <v>0.56875</v>
+      </c>
+      <c r="F1643" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1643" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1643" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1643" s="11">
+        <v>17.7612990885973</v>
+      </c>
+      <c r="K1643" s="11">
+        <v>-64.6697099134326</v>
+      </c>
+      <c r="M1643" s="7" t="s">
+        <v>2487</v>
+      </c>
     </row>
     <row r="1644">
-      <c r="A1644" s="24"/>
-      <c r="B1644" s="7"/>
+      <c r="A1644" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1644" s="7" t="s">
+        <v>2688</v>
+      </c>
+      <c r="C1644" s="7" t="s">
+        <v>2689</v>
+      </c>
+      <c r="D1644" s="7">
+        <v>105.0</v>
+      </c>
+      <c r="E1644" s="8">
+        <v>0.5715277777777777</v>
+      </c>
+      <c r="F1644" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1644" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1644" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1644" s="11">
+        <v>17.7613663114607</v>
+      </c>
+      <c r="K1644" s="11">
+        <v>-64.6697364002466</v>
+      </c>
     </row>
     <row r="1645">
-      <c r="A1645" s="24"/>
-      <c r="B1645" s="7"/>
+      <c r="A1645" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1645" s="7" t="s">
+        <v>2690</v>
+      </c>
+      <c r="C1645" s="7" t="s">
+        <v>2691</v>
+      </c>
+      <c r="D1645" s="7">
+        <v>65.0</v>
+      </c>
+      <c r="E1645" s="8">
+        <v>0.5736111111111111</v>
+      </c>
+      <c r="F1645" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1645" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1645" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1645" s="11">
+        <v>17.7613851707429</v>
+      </c>
+      <c r="K1645" s="11">
+        <v>-64.6697949897498</v>
+      </c>
     </row>
     <row r="1646">
-      <c r="A1646" s="24"/>
-      <c r="B1646" s="7"/>
+      <c r="A1646" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1646" s="7" t="s">
+        <v>2692</v>
+      </c>
+      <c r="C1646" s="7" t="s">
+        <v>2693</v>
+      </c>
+      <c r="D1646" s="7">
+        <v>209.0</v>
+      </c>
+      <c r="E1646" s="8">
+        <v>0.5034722222222222</v>
+      </c>
+      <c r="F1646" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1646" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1646" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1646" s="11">
+        <v>17.7610717713833</v>
+      </c>
+      <c r="K1646" s="11">
+        <v>-64.6690336614847</v>
+      </c>
     </row>
     <row r="1647">
-      <c r="A1647" s="24"/>
-      <c r="B1647" s="7"/>
+      <c r="A1647" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1647" s="7" t="s">
+        <v>2694</v>
+      </c>
+      <c r="C1647" s="7" t="s">
+        <v>2695</v>
+      </c>
+      <c r="D1647" s="7">
+        <v>20.0</v>
+      </c>
+      <c r="E1647" s="8">
+        <v>0.5069444444444444</v>
+      </c>
+      <c r="F1647" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1647" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1647" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1647" s="11">
+        <v>17.7611308638006</v>
+      </c>
+      <c r="K1647" s="11">
+        <v>-64.6691228449345</v>
+      </c>
     </row>
     <row r="1648">
-      <c r="A1648" s="24"/>
-      <c r="B1648" s="7"/>
+      <c r="A1648" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1648" s="7" t="s">
+        <v>2696</v>
+      </c>
+      <c r="C1648" s="7" t="s">
+        <v>2695</v>
+      </c>
+      <c r="D1648" s="7">
+        <v>200.0</v>
+      </c>
+      <c r="E1648" s="8">
+        <v>0.5069444444444444</v>
+      </c>
+      <c r="F1648" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1648" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1648" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1648" s="11">
+        <v>17.7611308638006</v>
+      </c>
+      <c r="K1648" s="11">
+        <v>-64.6691228449345</v>
+      </c>
     </row>
     <row r="1649">
-      <c r="A1649" s="24"/>
-      <c r="B1649" s="7"/>
+      <c r="A1649" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1649" s="7" t="s">
+        <v>2697</v>
+      </c>
+      <c r="C1649" s="7" t="s">
+        <v>2695</v>
+      </c>
+      <c r="D1649" s="7">
+        <v>108.0</v>
+      </c>
+      <c r="E1649" s="8">
+        <v>0.5069444444444444</v>
+      </c>
+      <c r="F1649" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1649" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1649" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1649" s="11">
+        <v>17.7611308638006</v>
+      </c>
+      <c r="K1649" s="11">
+        <v>-64.6691228449345</v>
+      </c>
     </row>
     <row r="1650">
-      <c r="A1650" s="24"/>
-      <c r="B1650" s="7"/>
+      <c r="A1650" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1650" s="7" t="s">
+        <v>2698</v>
+      </c>
+      <c r="C1650" s="7" t="s">
+        <v>2699</v>
+      </c>
+      <c r="D1650" s="7">
+        <v>9.0</v>
+      </c>
+      <c r="E1650" s="8">
+        <v>0.5125</v>
+      </c>
+      <c r="F1650" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1650" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1650" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1650" s="11">
+        <v>17.7611739467829</v>
+      </c>
+      <c r="K1650" s="11">
+        <v>-64.6691372618079</v>
+      </c>
+      <c r="M1650" s="7" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="1651">
-      <c r="A1651" s="24"/>
-      <c r="B1651" s="7"/>
+      <c r="A1651" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1651" s="7" t="s">
+        <v>2700</v>
+      </c>
+      <c r="C1651" s="7" t="s">
+        <v>2701</v>
+      </c>
+      <c r="D1651" s="7">
+        <v>21.0</v>
+      </c>
+      <c r="E1651" s="8">
+        <v>0.5152777777777777</v>
+      </c>
+      <c r="F1651" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1651" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1651" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1651" s="11">
+        <v>17.7612050436437</v>
+      </c>
+      <c r="K1651" s="11">
+        <v>-64.6691792551428</v>
+      </c>
     </row>
     <row r="1652">
-      <c r="A1652" s="24"/>
-      <c r="B1652" s="7"/>
+      <c r="A1652" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1652" s="7" t="s">
+        <v>2702</v>
+      </c>
+      <c r="C1652" s="7" t="s">
+        <v>2701</v>
+      </c>
+      <c r="D1652" s="7">
+        <v>77.0</v>
+      </c>
+      <c r="E1652" s="8">
+        <v>0.5152777777777777</v>
+      </c>
+      <c r="F1652" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1652" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1652" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1652" s="11">
+        <v>17.7612050436437</v>
+      </c>
+      <c r="K1652" s="11">
+        <v>-64.6691792551428</v>
+      </c>
     </row>
     <row r="1653">
-      <c r="A1653" s="24"/>
-      <c r="B1653" s="7"/>
+      <c r="A1653" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1653" s="7" t="s">
+        <v>2703</v>
+      </c>
+      <c r="C1653" s="7" t="s">
+        <v>2704</v>
+      </c>
+      <c r="D1653" s="7">
+        <v>25.0</v>
+      </c>
+      <c r="E1653" s="8">
+        <v>0.51875</v>
+      </c>
+      <c r="F1653" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1653" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1653" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1653" s="11">
+        <v>17.7611985895783</v>
+      </c>
+      <c r="K1653" s="11">
+        <v>-64.6692328993231</v>
+      </c>
     </row>
     <row r="1654">
-      <c r="A1654" s="24"/>
-      <c r="B1654" s="7"/>
+      <c r="A1654" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1654" s="7" t="s">
+        <v>2705</v>
+      </c>
+      <c r="C1654" s="7" t="s">
+        <v>2706</v>
+      </c>
+      <c r="D1654" s="7">
+        <v>104.0</v>
+      </c>
+      <c r="E1654" s="8">
+        <v>0.5208333333333334</v>
+      </c>
+      <c r="F1654" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1654" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1654" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1654" s="11">
+        <v>17.7611949853599</v>
+      </c>
+      <c r="K1654" s="11">
+        <v>-64.6692491602153</v>
+      </c>
     </row>
     <row r="1655">
-      <c r="A1655" s="24"/>
-      <c r="B1655" s="7"/>
+      <c r="A1655" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1655" s="7" t="s">
+        <v>2707</v>
+      </c>
+      <c r="C1655" s="7" t="s">
+        <v>2706</v>
+      </c>
+      <c r="D1655" s="7">
+        <v>23.0</v>
+      </c>
+      <c r="E1655" s="8">
+        <v>0.5208333333333334</v>
+      </c>
+      <c r="F1655" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1655" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1655" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1655" s="11">
+        <v>17.7611949853599</v>
+      </c>
+      <c r="K1655" s="11">
+        <v>-64.6692491602153</v>
+      </c>
     </row>
     <row r="1656">
-      <c r="A1656" s="24"/>
-      <c r="B1656" s="7"/>
+      <c r="A1656" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1656" s="7" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C1656" s="7" t="s">
+        <v>2709</v>
+      </c>
+      <c r="D1656" s="7">
+        <v>71.0</v>
+      </c>
+      <c r="E1656" s="8">
+        <v>0.525</v>
+      </c>
+      <c r="F1656" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1656" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1656" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1656" s="11">
+        <v>17.7612446900457</v>
+      </c>
+      <c r="K1656" s="11">
+        <v>-64.6692719589919</v>
+      </c>
     </row>
     <row r="1657">
-      <c r="A1657" s="24"/>
-      <c r="B1657" s="7"/>
+      <c r="A1657" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1657" s="7" t="s">
+        <v>2710</v>
+      </c>
+      <c r="C1657" s="7" t="s">
+        <v>2709</v>
+      </c>
+      <c r="D1657" s="7">
+        <v>29.0</v>
+      </c>
+      <c r="E1657" s="8">
+        <v>0.525</v>
+      </c>
+      <c r="F1657" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1657" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1657" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1657" s="11">
+        <v>17.7612446900457</v>
+      </c>
+      <c r="K1657" s="11">
+        <v>-64.6692719589919</v>
+      </c>
     </row>
     <row r="1658">
-      <c r="A1658" s="24"/>
-      <c r="B1658" s="7"/>
+      <c r="A1658" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1658" s="7" t="s">
+        <v>2711</v>
+      </c>
+      <c r="C1658" s="7" t="s">
+        <v>2712</v>
+      </c>
+      <c r="D1658" s="7">
+        <v>27.0</v>
+      </c>
+      <c r="E1658" s="8">
+        <v>0.5277777777777778</v>
+      </c>
+      <c r="F1658" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1658" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1658" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1658" s="11">
+        <v>17.761258604005</v>
+      </c>
+      <c r="K1658" s="11">
+        <v>-64.6692894771695</v>
+      </c>
     </row>
     <row r="1659">
-      <c r="A1659" s="24"/>
-      <c r="B1659" s="7"/>
+      <c r="A1659" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1659" s="7" t="s">
+        <v>2713</v>
+      </c>
+      <c r="C1659" s="7" t="s">
+        <v>2712</v>
+      </c>
+      <c r="D1659" s="7">
+        <v>75.0</v>
+      </c>
+      <c r="E1659" s="8">
+        <v>0.5277777777777778</v>
+      </c>
+      <c r="F1659" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1659" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1659" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1659" s="11">
+        <v>17.761258604005</v>
+      </c>
+      <c r="K1659" s="11">
+        <v>-64.6692894771695</v>
+      </c>
     </row>
     <row r="1660">
-      <c r="A1660" s="24"/>
-      <c r="B1660" s="7"/>
+      <c r="A1660" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1660" s="7" t="s">
+        <v>2714</v>
+      </c>
+      <c r="C1660" s="7" t="s">
+        <v>2715</v>
+      </c>
+      <c r="D1660" s="7">
+        <v>38.0</v>
+      </c>
+      <c r="E1660" s="8">
+        <v>0.5305555555555556</v>
+      </c>
+      <c r="F1660" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1660" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1660" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1660" s="11">
+        <v>17.7611906267703</v>
+      </c>
+      <c r="K1660" s="11">
+        <v>-64.6693940833211</v>
+      </c>
     </row>
     <row r="1661">
-      <c r="A1661" s="24"/>
-      <c r="B1661" s="7"/>
+      <c r="A1661" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1661" s="7" t="s">
+        <v>2716</v>
+      </c>
+      <c r="C1661" s="7" t="s">
+        <v>2717</v>
+      </c>
+      <c r="D1661" s="7">
+        <v>40.0</v>
+      </c>
+      <c r="E1661" s="8">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="F1661" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1661" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1661" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1661" s="11">
+        <v>17.7611791435629</v>
+      </c>
+      <c r="K1661" s="11">
+        <v>-64.6693612262607</v>
+      </c>
     </row>
     <row r="1662">
-      <c r="A1662" s="24"/>
-      <c r="B1662" s="7"/>
+      <c r="A1662" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1662" s="7" t="s">
+        <v>2718</v>
+      </c>
+      <c r="C1662" s="7" t="s">
+        <v>2717</v>
+      </c>
+      <c r="D1662" s="7">
+        <v>115.0</v>
+      </c>
+      <c r="E1662" s="8">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="F1662" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1662" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1662" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1662" s="11">
+        <v>17.7611791435629</v>
+      </c>
+      <c r="K1662" s="11">
+        <v>-64.6693612262607</v>
+      </c>
     </row>
     <row r="1663">
-      <c r="A1663" s="24"/>
-      <c r="B1663" s="7"/>
+      <c r="A1663" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1663" s="7" t="s">
+        <v>2719</v>
+      </c>
+      <c r="C1663" s="7" t="s">
+        <v>2720</v>
+      </c>
+      <c r="D1663" s="7">
+        <v>44.0</v>
+      </c>
+      <c r="E1663" s="8">
+        <v>0.5368055555555555</v>
+      </c>
+      <c r="F1663" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1663" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1663" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1663" s="11">
+        <v>17.7611365634948</v>
+      </c>
+      <c r="K1663" s="11">
+        <v>-64.669380672276</v>
+      </c>
+      <c r="M1663" s="7" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="1664">
-      <c r="A1664" s="24"/>
-      <c r="B1664" s="7"/>
+      <c r="A1664" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1664" s="7" t="s">
+        <v>2721</v>
+      </c>
+      <c r="C1664" s="7" t="s">
+        <v>2720</v>
+      </c>
+      <c r="D1664" s="7">
+        <v>15.0</v>
+      </c>
+      <c r="E1664" s="8">
+        <v>0.5368055555555555</v>
+      </c>
+      <c r="F1664" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1664" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1664" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1664" s="11">
+        <v>17.7611365634948</v>
+      </c>
+      <c r="K1664" s="11">
+        <v>-64.669380672276</v>
+      </c>
     </row>
     <row r="1665">
-      <c r="A1665" s="24"/>
-      <c r="B1665" s="7"/>
+      <c r="A1665" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1665" s="7" t="s">
+        <v>2722</v>
+      </c>
+      <c r="C1665" s="7" t="s">
+        <v>2723</v>
+      </c>
+      <c r="D1665" s="7">
+        <v>113.0</v>
+      </c>
+      <c r="E1665" s="8">
+        <v>0.5416666666666666</v>
+      </c>
+      <c r="F1665" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1665" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1665" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1665" s="11">
+        <v>17.7612943947315</v>
+      </c>
+      <c r="K1665" s="11">
+        <v>-64.669526014477</v>
+      </c>
     </row>
     <row r="1666">
-      <c r="A1666" s="24"/>
-      <c r="B1666" s="7"/>
+      <c r="A1666" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1666" s="7" t="s">
+        <v>2724</v>
+      </c>
+      <c r="C1666" s="7" t="s">
+        <v>2725</v>
+      </c>
+      <c r="D1666" s="7">
+        <v>52.0</v>
+      </c>
+      <c r="E1666" s="8">
+        <v>0.5451388888888888</v>
+      </c>
+      <c r="F1666" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1666" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1666" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1666" s="11">
+        <v>17.7612741943449</v>
+      </c>
+      <c r="K1666" s="11">
+        <v>-64.6695165429264</v>
+      </c>
     </row>
     <row r="1667">
-      <c r="A1667" s="24"/>
-      <c r="B1667" s="7"/>
+      <c r="A1667" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1667" s="7" t="s">
+        <v>2726</v>
+      </c>
+      <c r="C1667" s="7" t="s">
+        <v>2725</v>
+      </c>
+      <c r="D1667" s="7">
+        <v>210.0</v>
+      </c>
+      <c r="E1667" s="8">
+        <v>0.5451388888888888</v>
+      </c>
+      <c r="F1667" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1667" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1667" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1667" s="11">
+        <v>17.7612741943449</v>
+      </c>
+      <c r="K1667" s="11">
+        <v>-64.6695165429264</v>
+      </c>
     </row>
     <row r="1668">
-      <c r="A1668" s="24"/>
-      <c r="B1668" s="7"/>
+      <c r="A1668" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1668" s="7" t="s">
+        <v>2727</v>
+      </c>
+      <c r="C1668" s="7" t="s">
+        <v>2728</v>
+      </c>
+      <c r="D1668" s="7">
+        <v>79.0</v>
+      </c>
+      <c r="E1668" s="8">
+        <v>0.5520833333333334</v>
+      </c>
+      <c r="F1668" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1668" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1668" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1668" s="11">
+        <v>17.7612788043916</v>
+      </c>
+      <c r="K1668" s="11">
+        <v>-64.6695646550506</v>
+      </c>
+      <c r="M1668" s="7" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="1669">
-      <c r="A1669" s="24"/>
-      <c r="B1669" s="7"/>
+      <c r="A1669" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1669" s="7" t="s">
+        <v>2729</v>
+      </c>
+      <c r="C1669" s="7" t="s">
+        <v>2730</v>
+      </c>
+      <c r="D1669" s="7">
+        <v>101.0</v>
+      </c>
+      <c r="E1669" s="8">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="F1669" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1669" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1669" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1669" s="11">
+        <v>17.7613029442728</v>
+      </c>
+      <c r="K1669" s="11">
+        <v>-64.6697175409645</v>
+      </c>
     </row>
     <row r="1670">
-      <c r="A1670" s="24"/>
-      <c r="B1670" s="7"/>
+      <c r="A1670" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1670" s="7" t="s">
+        <v>2731</v>
+      </c>
+      <c r="C1670" s="7" t="s">
+        <v>2732</v>
+      </c>
+      <c r="D1670" s="7">
+        <v>218.0</v>
+      </c>
+      <c r="E1670" s="8">
+        <v>0.5569444444444445</v>
+      </c>
+      <c r="F1670" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1670" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1670" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1670" s="11">
+        <v>17.7612934727222</v>
+      </c>
+      <c r="K1670" s="11">
+        <v>-64.6697255875915</v>
+      </c>
+      <c r="M1670" s="7" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="1671">
-      <c r="A1671" s="24"/>
-      <c r="B1671" s="7"/>
+      <c r="A1671" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1671" s="7" t="s">
+        <v>2733</v>
+      </c>
+      <c r="C1671" s="7" t="s">
+        <v>2734</v>
+      </c>
+      <c r="D1671" s="7">
+        <v>120.0</v>
+      </c>
+      <c r="E1671" s="8">
+        <v>0.5631944444444444</v>
+      </c>
+      <c r="F1671" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1671" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1671" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1671" s="11">
+        <v>17.7613733522594</v>
+      </c>
+      <c r="K1671" s="11">
+        <v>-64.66971879825</v>
+      </c>
     </row>
     <row r="1672">
-      <c r="A1672" s="24"/>
-      <c r="B1672" s="7"/>
+      <c r="A1672" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1672" s="7" t="s">
+        <v>2735</v>
+      </c>
+      <c r="C1672" s="7" t="s">
+        <v>2734</v>
+      </c>
+      <c r="D1672" s="7">
+        <v>37.0</v>
+      </c>
+      <c r="E1672" s="8">
+        <v>0.5631944444444444</v>
+      </c>
+      <c r="F1672" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1672" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1672" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1672" s="11">
+        <v>17.7613733522594</v>
+      </c>
+      <c r="K1672" s="11">
+        <v>-64.66971879825</v>
+      </c>
     </row>
     <row r="1673">
-      <c r="A1673" s="24"/>
-      <c r="B1673" s="7"/>
+      <c r="A1673" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1673" s="7" t="s">
+        <v>2736</v>
+      </c>
+      <c r="C1673" s="7" t="s">
+        <v>2734</v>
+      </c>
+      <c r="D1673" s="7">
+        <v>80.0</v>
+      </c>
+      <c r="E1673" s="8">
+        <v>0.5631944444444444</v>
+      </c>
+      <c r="F1673" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1673" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1673" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1673" s="11">
+        <v>17.7613733522594</v>
+      </c>
+      <c r="K1673" s="11">
+        <v>-64.66971879825</v>
+      </c>
     </row>
     <row r="1674">
-      <c r="A1674" s="24"/>
-      <c r="B1674" s="7"/>
+      <c r="A1674" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1674" s="7" t="s">
+        <v>2737</v>
+      </c>
+      <c r="C1674" s="7" t="s">
+        <v>2738</v>
+      </c>
+      <c r="D1674" s="7">
+        <v>202.0</v>
+      </c>
+      <c r="E1674" s="8">
+        <v>0.5722222222222222</v>
+      </c>
+      <c r="F1674" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1674" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1674" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1674" s="11">
+        <v>17.7613554988056</v>
+      </c>
+      <c r="K1674" s="11">
+        <v>-64.6697285212576</v>
+      </c>
     </row>
     <row r="1675">
-      <c r="A1675" s="24"/>
-      <c r="B1675" s="7"/>
+      <c r="A1675" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1675" s="7" t="s">
+        <v>2739</v>
+      </c>
+      <c r="C1675" s="7" t="s">
+        <v>2740</v>
+      </c>
+      <c r="D1675" s="7">
+        <v>211.0</v>
+      </c>
+      <c r="E1675" s="8">
+        <v>0.575</v>
+      </c>
+      <c r="F1675" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1675" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1675" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1675" s="11">
+        <v>17.7613783814013</v>
+      </c>
+      <c r="K1675" s="11">
+        <v>-64.6698147710413</v>
+      </c>
     </row>
     <row r="1676">
-      <c r="A1676" s="24"/>
-      <c r="B1676" s="7"/>
+      <c r="A1676" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1676" s="7" t="s">
+        <v>2741</v>
+      </c>
+      <c r="C1676" s="7" t="s">
+        <v>2742</v>
+      </c>
+      <c r="D1676" s="7">
+        <v>47.0</v>
+      </c>
+      <c r="E1676" s="8">
+        <v>0.5770833333333333</v>
+      </c>
+      <c r="F1676" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1676" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1676" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1676" s="11">
+        <v>17.7613442670554</v>
+      </c>
+      <c r="K1676" s="11">
+        <v>-64.6698367316276</v>
+      </c>
     </row>
     <row r="1677">
-      <c r="A1677" s="24"/>
-      <c r="B1677" s="7"/>
+      <c r="A1677" s="6">
+        <v>44740.0</v>
+      </c>
+      <c r="B1677" s="7" t="s">
+        <v>2743</v>
+      </c>
+      <c r="C1677" s="7" t="s">
+        <v>2744</v>
+      </c>
+      <c r="D1677" s="7">
+        <v>41.0</v>
+      </c>
+      <c r="E1677" s="8">
+        <v>0.5784722222222223</v>
+      </c>
+      <c r="F1677" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1677" s="7" t="s">
+        <v>1338</v>
+      </c>
+      <c r="H1677" s="7" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J1677" s="11">
+        <v>17.7613560855389</v>
+      </c>
+      <c r="K1677" s="11">
+        <v>-64.6698047965765</v>
+      </c>
     </row>
     <row r="1678">
-      <c r="A1678" s="24"/>
+      <c r="A1678" s="6"/>
       <c r="B1678" s="7"/>
     </row>
     <row r="1679">
@@ -63147,19 +65278,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>2642</v>
+        <v>2745</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2643</v>
+        <v>2746</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2644</v>
+        <v>2747</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2645</v>
+        <v>2748</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2646</v>
+        <v>2749</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>7</v>
@@ -63183,21 +65314,21 @@
         <v>51</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>2647</v>
+        <v>2750</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>145</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>2648</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>2649</v>
+        <v>2752</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2650</v>
+        <v>2753</v>
       </c>
       <c r="C2" s="7">
         <v>7.0</v>
@@ -63209,33 +65340,33 @@
         <v>44688.0</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>2651</v>
+        <v>2754</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>2651</v>
+        <v>2754</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>2651</v>
+        <v>2754</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>2651</v>
+        <v>2754</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>2651</v>
+        <v>2754</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>2652</v>
+        <v>2755</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>2653</v>
+        <v>2756</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>2654</v>
+        <v>2757</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2655</v>
+        <v>2758</v>
       </c>
       <c r="C3" s="7">
         <v>25.0</v>
@@ -63246,10 +65377,10 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>2656</v>
+        <v>2759</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="C4" s="7">
         <v>15.0</v>
@@ -63261,18 +65392,18 @@
         <v>44690.0</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>2658</v>
+        <v>2761</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>2659</v>
+        <v>2762</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2660</v>
+        <v>2763</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2661</v>
+        <v>2764</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>20</v>
@@ -63280,10 +65411,10 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>2662</v>
+        <v>2765</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2663</v>
+        <v>2766</v>
       </c>
       <c r="C6" s="7">
         <v>20.0</v>
@@ -63315,10 +65446,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="7" t="s">
-        <v>2664</v>
+        <v>2767</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2665</v>
+        <v>2768</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>78</v>
@@ -63350,7 +65481,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2649</v>
+        <v>2752</v>
       </c>
       <c r="C2" s="7">
         <v>2.0</v>
@@ -63379,7 +65510,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2656</v>
+        <v>2759</v>
       </c>
       <c r="C3" s="7">
         <v>5.0</v>
@@ -63408,7 +65539,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2654</v>
+        <v>2757</v>
       </c>
       <c r="F4" s="7">
         <v>17.0</v>
@@ -63431,7 +65562,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2662</v>
+        <v>2765</v>
       </c>
       <c r="F5" s="7">
         <v>6.0</v>
@@ -63454,7 +65585,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2666</v>
+        <v>2769</v>
       </c>
       <c r="F6" s="7">
         <v>11.0</v>
@@ -63497,16 +65628,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="26" t="s">
-        <v>2667</v>
+        <v>2770</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>2668</v>
+        <v>2771</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>2669</v>
+        <v>2772</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>12</v>
@@ -63536,7 +65667,7 @@
     </row>
     <row r="2">
       <c r="A2" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B2" s="6">
         <v>44690.0</v>
@@ -63551,7 +65682,7 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B3" s="6">
         <v>44690.0</v>
@@ -63566,7 +65697,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B4" s="6">
         <v>44690.0</v>
@@ -63581,7 +65712,7 @@
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B5" s="6">
         <v>44690.0</v>
@@ -63596,7 +65727,7 @@
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B6" s="6">
         <v>44690.0</v>
@@ -63611,7 +65742,7 @@
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B7" s="6">
         <v>44690.0</v>
@@ -63626,7 +65757,7 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B8" s="6">
         <v>44690.0</v>
@@ -63641,7 +65772,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B9" s="6">
         <v>44690.0</v>
@@ -63656,7 +65787,7 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B10" s="6">
         <v>44690.0</v>
@@ -63671,7 +65802,7 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B11" s="6">
         <v>44690.0</v>
@@ -63686,7 +65817,7 @@
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B12" s="6">
         <v>44690.0</v>
@@ -63701,7 +65832,7 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B13" s="6">
         <v>44690.0</v>
@@ -63716,7 +65847,7 @@
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B14" s="6">
         <v>44690.0</v>
@@ -63731,7 +65862,7 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B15" s="6">
         <v>44690.0</v>
@@ -63746,7 +65877,7 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B16" s="6">
         <v>44690.0</v>
@@ -63761,7 +65892,7 @@
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B17" s="6">
         <v>44690.0</v>
@@ -63777,7 +65908,7 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B18" s="6">
         <v>44690.0</v>
@@ -63793,7 +65924,7 @@
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B19" s="6">
         <v>44690.0</v>
@@ -63808,7 +65939,7 @@
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B20" s="6">
         <v>44690.0</v>
@@ -63823,7 +65954,7 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B21" s="6">
         <v>44690.0</v>
@@ -63838,7 +65969,7 @@
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B22" s="6">
         <v>44690.0</v>
@@ -63853,7 +65984,7 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B23" s="6">
         <v>44690.0</v>
@@ -63868,7 +65999,7 @@
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B24" s="6">
         <v>44690.0</v>
@@ -63883,7 +66014,7 @@
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B25" s="6">
         <v>44690.0</v>
@@ -63898,7 +66029,7 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B26" s="6">
         <v>44690.0</v>
@@ -63913,7 +66044,7 @@
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B27" s="6">
         <v>44690.0</v>
@@ -63928,7 +66059,7 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B28" s="6">
         <v>44690.0</v>
@@ -63943,7 +66074,7 @@
     </row>
     <row r="29">
       <c r="A29" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B29" s="6">
         <v>44690.0</v>
@@ -63958,7 +66089,7 @@
     </row>
     <row r="30">
       <c r="A30" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B30" s="6">
         <v>44690.0</v>
@@ -63973,7 +66104,7 @@
     </row>
     <row r="31">
       <c r="A31" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B31" s="6">
         <v>44690.0</v>
@@ -63988,7 +66119,7 @@
     </row>
     <row r="32">
       <c r="A32" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B32" s="6">
         <v>44690.0</v>
@@ -64003,7 +66134,7 @@
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B33" s="6">
         <v>44690.0</v>
@@ -64018,7 +66149,7 @@
     </row>
     <row r="34">
       <c r="A34" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B34" s="6">
         <v>44690.0</v>
@@ -64033,7 +66164,7 @@
     </row>
     <row r="35">
       <c r="A35" s="7" t="s">
-        <v>2657</v>
+        <v>2760</v>
       </c>
       <c r="B35" s="6">
         <v>44690.0</v>
@@ -64048,7 +66179,7 @@
     </row>
     <row r="36">
       <c r="A36" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B36" s="6">
         <v>44704.0</v>
@@ -64063,7 +66194,7 @@
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B37" s="6">
         <v>44704.0</v>
@@ -64078,7 +66209,7 @@
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B38" s="6">
         <v>44704.0</v>
@@ -64090,12 +66221,12 @@
         <v>22.0</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>2671</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B39" s="6">
         <v>44704.0</v>
@@ -64110,7 +66241,7 @@
     </row>
     <row r="40">
       <c r="A40" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B40" s="6">
         <v>44704.0</v>
@@ -64122,12 +66253,12 @@
         <v>34.0</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>2671</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B41" s="6">
         <v>44704.0</v>
@@ -64142,7 +66273,7 @@
     </row>
     <row r="42">
       <c r="A42" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B42" s="6">
         <v>44704.0</v>
@@ -64157,7 +66288,7 @@
     </row>
     <row r="43">
       <c r="A43" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B43" s="6">
         <v>44704.0</v>
@@ -64172,7 +66303,7 @@
     </row>
     <row r="44">
       <c r="A44" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B44" s="6">
         <v>44704.0</v>
@@ -64184,12 +66315,12 @@
         <v>6.0</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>2671</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B45" s="6">
         <v>44704.0</v>
@@ -64204,7 +66335,7 @@
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B46" s="6">
         <v>44704.0</v>
@@ -64219,7 +66350,7 @@
     </row>
     <row r="47">
       <c r="A47" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B47" s="6">
         <v>44704.0</v>
@@ -64234,7 +66365,7 @@
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B48" s="6">
         <v>44704.0</v>
@@ -64249,7 +66380,7 @@
     </row>
     <row r="49">
       <c r="A49" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B49" s="6">
         <v>44704.0</v>
@@ -64264,7 +66395,7 @@
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B50" s="6">
         <v>44704.0</v>
@@ -64279,7 +66410,7 @@
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B51" s="6">
         <v>44704.0</v>
@@ -64294,7 +66425,7 @@
     </row>
     <row r="52">
       <c r="A52" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B52" s="6">
         <v>44704.0</v>
@@ -64309,7 +66440,7 @@
     </row>
     <row r="53">
       <c r="A53" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B53" s="6">
         <v>44704.0</v>
@@ -64324,7 +66455,7 @@
     </row>
     <row r="54">
       <c r="A54" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B54" s="6">
         <v>44704.0</v>
@@ -64339,7 +66470,7 @@
     </row>
     <row r="55">
       <c r="A55" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B55" s="6">
         <v>44704.0</v>
@@ -64354,7 +66485,7 @@
     </row>
     <row r="56">
       <c r="A56" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B56" s="6">
         <v>44704.0</v>
@@ -64369,7 +66500,7 @@
     </row>
     <row r="57">
       <c r="A57" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B57" s="6">
         <v>44704.0</v>
@@ -64384,7 +66515,7 @@
     </row>
     <row r="58">
       <c r="A58" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B58" s="6">
         <v>44704.0</v>
@@ -64399,7 +66530,7 @@
     </row>
     <row r="59">
       <c r="A59" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B59" s="6">
         <v>44704.0</v>
@@ -64414,7 +66545,7 @@
     </row>
     <row r="60">
       <c r="A60" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B60" s="6">
         <v>44704.0</v>
@@ -64429,7 +66560,7 @@
     </row>
     <row r="61">
       <c r="A61" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B61" s="6">
         <v>44704.0</v>
@@ -64444,7 +66575,7 @@
     </row>
     <row r="62">
       <c r="A62" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B62" s="6">
         <v>44704.0</v>
@@ -64459,7 +66590,7 @@
     </row>
     <row r="63">
       <c r="A63" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B63" s="6">
         <v>44704.0</v>
@@ -64474,7 +66605,7 @@
     </row>
     <row r="64">
       <c r="A64" s="7" t="s">
-        <v>2670</v>
+        <v>2773</v>
       </c>
       <c r="B64" s="6">
         <v>44704.0</v>
@@ -64489,7 +66620,7 @@
     </row>
     <row r="65">
       <c r="A65" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B65" s="6">
         <v>44704.0</v>
@@ -64504,7 +66635,7 @@
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B66" s="6">
         <v>44704.0</v>
@@ -64519,7 +66650,7 @@
     </row>
     <row r="67">
       <c r="A67" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B67" s="6">
         <v>44704.0</v>
@@ -64534,7 +66665,7 @@
     </row>
     <row r="68">
       <c r="A68" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B68" s="6">
         <v>44704.0</v>
@@ -64549,7 +66680,7 @@
     </row>
     <row r="69">
       <c r="A69" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B69" s="6">
         <v>44704.0</v>
@@ -64564,7 +66695,7 @@
     </row>
     <row r="70">
       <c r="A70" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B70" s="6">
         <v>44704.0</v>
@@ -64579,7 +66710,7 @@
     </row>
     <row r="71">
       <c r="A71" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B71" s="6">
         <v>44704.0</v>
@@ -64594,7 +66725,7 @@
     </row>
     <row r="72">
       <c r="A72" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B72" s="6">
         <v>44704.0</v>
@@ -64609,7 +66740,7 @@
     </row>
     <row r="73">
       <c r="A73" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B73" s="6">
         <v>44704.0</v>
@@ -64624,7 +66755,7 @@
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B74" s="6">
         <v>44704.0</v>
@@ -64639,7 +66770,7 @@
     </row>
     <row r="75">
       <c r="A75" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B75" s="6">
         <v>44704.0</v>
@@ -64654,7 +66785,7 @@
     </row>
     <row r="76">
       <c r="A76" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B76" s="6">
         <v>44704.0</v>
@@ -64669,7 +66800,7 @@
     </row>
     <row r="77">
       <c r="A77" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B77" s="6">
         <v>44704.0</v>
@@ -64684,7 +66815,7 @@
     </row>
     <row r="78">
       <c r="A78" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B78" s="6">
         <v>44704.0</v>
@@ -64699,7 +66830,7 @@
     </row>
     <row r="79">
       <c r="A79" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B79" s="6">
         <v>44704.0</v>
@@ -64714,7 +66845,7 @@
     </row>
     <row r="80">
       <c r="A80" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B80" s="6">
         <v>44704.0</v>
@@ -64729,7 +66860,7 @@
     </row>
     <row r="81">
       <c r="A81" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B81" s="6">
         <v>44704.0</v>
@@ -64744,7 +66875,7 @@
     </row>
     <row r="82">
       <c r="A82" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B82" s="6">
         <v>44704.0</v>
@@ -64759,7 +66890,7 @@
     </row>
     <row r="83">
       <c r="A83" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B83" s="6">
         <v>44704.0</v>
@@ -64774,7 +66905,7 @@
     </row>
     <row r="84">
       <c r="A84" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B84" s="6">
         <v>44704.0</v>
@@ -64789,7 +66920,7 @@
     </row>
     <row r="85">
       <c r="A85" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B85" s="6">
         <v>44704.0</v>
@@ -64804,7 +66935,7 @@
     </row>
     <row r="86">
       <c r="A86" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B86" s="6">
         <v>44704.0</v>
@@ -64819,7 +66950,7 @@
     </row>
     <row r="87">
       <c r="A87" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B87" s="6">
         <v>44704.0</v>
@@ -64834,7 +66965,7 @@
     </row>
     <row r="88">
       <c r="A88" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B88" s="6">
         <v>44704.0</v>
@@ -64849,7 +66980,7 @@
     </row>
     <row r="89">
       <c r="A89" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B89" s="6">
         <v>44704.0</v>
@@ -64864,7 +66995,7 @@
     </row>
     <row r="90">
       <c r="A90" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B90" s="6">
         <v>44704.0</v>
@@ -64879,7 +67010,7 @@
     </row>
     <row r="91">
       <c r="A91" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B91" s="6">
         <v>44704.0</v>
@@ -64894,7 +67025,7 @@
     </row>
     <row r="92">
       <c r="A92" s="7" t="s">
-        <v>2672</v>
+        <v>2775</v>
       </c>
       <c r="B92" s="6">
         <v>44704.0</v>
@@ -64909,7 +67040,7 @@
     </row>
     <row r="93">
       <c r="A93" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B93" s="6">
         <v>44705.0</v>
@@ -64924,7 +67055,7 @@
     </row>
     <row r="94">
       <c r="A94" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B94" s="6">
         <v>44705.0</v>
@@ -64939,7 +67070,7 @@
     </row>
     <row r="95">
       <c r="A95" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B95" s="6">
         <v>44705.0</v>
@@ -64954,7 +67085,7 @@
     </row>
     <row r="96">
       <c r="A96" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B96" s="6">
         <v>44705.0</v>
@@ -64969,7 +67100,7 @@
     </row>
     <row r="97">
       <c r="A97" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B97" s="6">
         <v>44705.0</v>
@@ -64984,7 +67115,7 @@
     </row>
     <row r="98">
       <c r="A98" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B98" s="6">
         <v>44705.0</v>
@@ -64999,7 +67130,7 @@
     </row>
     <row r="99">
       <c r="A99" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B99" s="6">
         <v>44705.0</v>
@@ -65014,7 +67145,7 @@
     </row>
     <row r="100">
       <c r="A100" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B100" s="6">
         <v>44705.0</v>
@@ -65029,7 +67160,7 @@
     </row>
     <row r="101">
       <c r="A101" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B101" s="6">
         <v>44705.0</v>
@@ -65044,7 +67175,7 @@
     </row>
     <row r="102">
       <c r="A102" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B102" s="6">
         <v>44705.0</v>
@@ -65059,7 +67190,7 @@
     </row>
     <row r="103">
       <c r="A103" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B103" s="6">
         <v>44705.0</v>
@@ -65074,7 +67205,7 @@
     </row>
     <row r="104">
       <c r="A104" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B104" s="6">
         <v>44705.0</v>
@@ -65089,7 +67220,7 @@
     </row>
     <row r="105">
       <c r="A105" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B105" s="6">
         <v>44705.0</v>
@@ -65104,7 +67235,7 @@
     </row>
     <row r="106">
       <c r="A106" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B106" s="6">
         <v>44705.0</v>
@@ -65119,7 +67250,7 @@
     </row>
     <row r="107">
       <c r="A107" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B107" s="6">
         <v>44705.0</v>
@@ -65134,7 +67265,7 @@
     </row>
     <row r="108">
       <c r="A108" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B108" s="6">
         <v>44705.0</v>
@@ -65149,7 +67280,7 @@
     </row>
     <row r="109">
       <c r="A109" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B109" s="6">
         <v>44705.0</v>
@@ -65164,7 +67295,7 @@
     </row>
     <row r="110">
       <c r="A110" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B110" s="6">
         <v>44705.0</v>
@@ -65179,7 +67310,7 @@
     </row>
     <row r="111">
       <c r="A111" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B111" s="6">
         <v>44705.0</v>
@@ -65194,7 +67325,7 @@
     </row>
     <row r="112">
       <c r="A112" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B112" s="6">
         <v>44705.0</v>
@@ -65209,7 +67340,7 @@
     </row>
     <row r="113">
       <c r="A113" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B113" s="6">
         <v>44705.0</v>
@@ -65224,7 +67355,7 @@
     </row>
     <row r="114">
       <c r="A114" s="7" t="s">
-        <v>2673</v>
+        <v>2776</v>
       </c>
       <c r="B114" s="6">
         <v>44705.0</v>
@@ -65239,7 +67370,7 @@
     </row>
     <row r="115">
       <c r="A115" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B115" s="6">
         <v>44708.0</v>
@@ -65254,7 +67385,7 @@
     </row>
     <row r="116">
       <c r="A116" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B116" s="6">
         <v>44708.0</v>
@@ -65269,7 +67400,7 @@
     </row>
     <row r="117">
       <c r="A117" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B117" s="6">
         <v>44708.0</v>
@@ -65284,7 +67415,7 @@
     </row>
     <row r="118">
       <c r="A118" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B118" s="6">
         <v>44708.0</v>
@@ -65296,12 +67427,12 @@
         <v>39.0</v>
       </c>
       <c r="E118" s="29" t="s">
-        <v>2671</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B119" s="6">
         <v>44708.0</v>
@@ -65316,7 +67447,7 @@
     </row>
     <row r="120">
       <c r="A120" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B120" s="6">
         <v>44708.0</v>
@@ -65331,7 +67462,7 @@
     </row>
     <row r="121">
       <c r="A121" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B121" s="6">
         <v>44708.0</v>
@@ -65346,7 +67477,7 @@
     </row>
     <row r="122">
       <c r="A122" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B122" s="6">
         <v>44708.0</v>
@@ -65361,7 +67492,7 @@
     </row>
     <row r="123">
       <c r="A123" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B123" s="6">
         <v>44708.0</v>
@@ -65376,7 +67507,7 @@
     </row>
     <row r="124">
       <c r="A124" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B124" s="6">
         <v>44708.0</v>
@@ -65391,7 +67522,7 @@
     </row>
     <row r="125">
       <c r="A125" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B125" s="6">
         <v>44708.0</v>
@@ -65406,7 +67537,7 @@
     </row>
     <row r="126">
       <c r="A126" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B126" s="6">
         <v>44708.0</v>
@@ -65421,7 +67552,7 @@
     </row>
     <row r="127">
       <c r="A127" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B127" s="6">
         <v>44708.0</v>
@@ -65433,12 +67564,12 @@
         <v>11.0</v>
       </c>
       <c r="E127" s="29" t="s">
-        <v>2671</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B128" s="6">
         <v>44708.0</v>
@@ -65453,7 +67584,7 @@
     </row>
     <row r="129">
       <c r="A129" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B129" s="6">
         <v>44708.0</v>
@@ -65465,12 +67596,12 @@
         <v>40.0</v>
       </c>
       <c r="E129" s="29" t="s">
-        <v>2671</v>
+        <v>2774</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B130" s="6">
         <v>44708.0</v>
@@ -65485,7 +67616,7 @@
     </row>
     <row r="131">
       <c r="A131" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B131" s="6">
         <v>44708.0</v>
@@ -65500,7 +67631,7 @@
     </row>
     <row r="132">
       <c r="A132" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B132" s="6">
         <v>44708.0</v>
@@ -65515,7 +67646,7 @@
     </row>
     <row r="133">
       <c r="A133" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="B133" s="6">
         <v>44708.0</v>
@@ -65530,7 +67661,7 @@
     </row>
     <row r="134">
       <c r="A134" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B134" s="6">
         <v>44713.0</v>
@@ -65542,12 +67673,12 @@
         <v>1298</v>
       </c>
       <c r="E134" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B135" s="6">
         <v>44713.0</v>
@@ -65559,12 +67690,12 @@
         <v>1300</v>
       </c>
       <c r="E135" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B136" s="6">
         <v>44713.0</v>
@@ -65576,12 +67707,12 @@
         <v>1302</v>
       </c>
       <c r="E136" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B137" s="6">
         <v>44713.0</v>
@@ -65593,12 +67724,12 @@
         <v>1304</v>
       </c>
       <c r="E137" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B138" s="6">
         <v>44713.0</v>
@@ -65610,12 +67741,12 @@
         <v>1306</v>
       </c>
       <c r="E138" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B139" s="6">
         <v>44713.0</v>
@@ -65627,12 +67758,12 @@
         <v>1309</v>
       </c>
       <c r="E139" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B140" s="6">
         <v>44713.0</v>
@@ -65644,12 +67775,12 @@
         <v>1312</v>
       </c>
       <c r="E140" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B141" s="6">
         <v>44713.0</v>
@@ -65661,12 +67792,12 @@
         <v>1315</v>
       </c>
       <c r="E141" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B142" s="6">
         <v>44713.0</v>
@@ -65678,12 +67809,12 @@
         <v>1318</v>
       </c>
       <c r="E142" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B143" s="6">
         <v>44713.0</v>
@@ -65695,12 +67826,12 @@
         <v>1321</v>
       </c>
       <c r="E143" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B144" s="6">
         <v>44713.0</v>
@@ -65712,12 +67843,12 @@
         <v>1323</v>
       </c>
       <c r="E144" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B145" s="6">
         <v>44713.0</v>
@@ -65729,12 +67860,12 @@
         <v>1325</v>
       </c>
       <c r="E145" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B146" s="6">
         <v>44713.0</v>
@@ -65746,12 +67877,12 @@
         <v>1327</v>
       </c>
       <c r="E146" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B147" s="6">
         <v>44713.0</v>
@@ -65763,12 +67894,12 @@
         <v>1329</v>
       </c>
       <c r="E147" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B148" s="6">
         <v>44713.0</v>
@@ -65780,12 +67911,12 @@
         <v>1331</v>
       </c>
       <c r="E148" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B149" s="6">
         <v>44713.0</v>
@@ -65797,12 +67928,12 @@
         <v>1333</v>
       </c>
       <c r="E149" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B150" s="6">
         <v>44713.0</v>
@@ -65814,12 +67945,12 @@
         <v>1335</v>
       </c>
       <c r="E150" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B151" s="6">
         <v>44713.0</v>
@@ -65831,12 +67962,12 @@
         <v>1337</v>
       </c>
       <c r="E151" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B152" s="6">
         <v>44713.0</v>
@@ -65848,12 +67979,12 @@
         <v>1340</v>
       </c>
       <c r="E152" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B153" s="6">
         <v>44713.0</v>
@@ -65865,12 +67996,12 @@
         <v>1342</v>
       </c>
       <c r="E153" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B154" s="6">
         <v>44713.0</v>
@@ -65882,12 +68013,12 @@
         <v>1344</v>
       </c>
       <c r="E154" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B155" s="6">
         <v>44713.0</v>
@@ -65899,12 +68030,12 @@
         <v>1346</v>
       </c>
       <c r="E155" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B156" s="6">
         <v>44713.0</v>
@@ -65916,12 +68047,12 @@
         <v>1348</v>
       </c>
       <c r="E156" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="7" t="s">
-        <v>2675</v>
+        <v>2778</v>
       </c>
       <c r="B157" s="6">
         <v>44713.0</v>
@@ -65933,7 +68064,7 @@
         <v>1350</v>
       </c>
       <c r="E157" s="29" t="s">
-        <v>2676</v>
+        <v>2779</v>
       </c>
     </row>
     <row r="158">
@@ -68485,22 +70616,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>2677</v>
+        <v>2780</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2678</v>
+        <v>2781</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2679</v>
+        <v>2782</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>2680</v>
+        <v>2783</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>2681</v>
+        <v>2784</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>2682</v>
+        <v>2785</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>12</v>
@@ -68511,17 +70642,17 @@
         <v>44690.0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>2683</v>
+        <v>2786</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>2656</v>
+        <v>2759</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7" t="s">
-        <v>2684</v>
+        <v>2787</v>
       </c>
     </row>
     <row r="3">
@@ -68529,7 +70660,7 @@
         <v>44692.0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2685</v>
+        <v>2788</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="7" t="s">
@@ -68550,10 +70681,10 @@
         <v>44694.0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2686</v>
+        <v>2789</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>2662</v>
+        <v>2765</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>20</v>
@@ -68568,7 +70699,7 @@
         <v>2.5</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>2687</v>
+        <v>2790</v>
       </c>
     </row>
     <row r="5">
@@ -68576,10 +70707,10 @@
         <v>44695.0</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>2688</v>
+        <v>2791</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>2666</v>
+        <v>2769</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -68599,10 +70730,10 @@
         <v>44697.0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>2689</v>
+        <v>2792</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>2690</v>
+        <v>2793</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -68622,10 +70753,10 @@
         <v>44698.0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>2674</v>
+        <v>2777</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>2691</v>
+        <v>2794</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -68645,10 +70776,10 @@
         <v>44726.0</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>2692</v>
+        <v>2795</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>2693</v>
+        <v>2796</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>1353</v>

</xml_diff>